<commit_message>
US1351 - Implemented addReports action and added method stubs for different Compliance report actions to enable reading test cases from Excel
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCases.xlsx
+++ b/selenium-wd/data/TestCases.xlsx
@@ -9,18 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="910" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="910" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="TestCases-Reports" sheetId="1" r:id="rId1"/>
+    <sheet name="TestCases-CmpReports" sheetId="1" r:id="rId1"/>
     <sheet name="TestCases-DriverView" sheetId="6" r:id="rId2"/>
-    <sheet name="TestCases-Reports-TestSteps" sheetId="3" r:id="rId3"/>
+    <sheet name="TestCases-CmpReports-TestSteps" sheetId="3" r:id="rId3"/>
     <sheet name="TestCases-DriverView-TestSteps" sheetId="7" r:id="rId4"/>
     <sheet name="Page Objects And Actions" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="AdministrationPage">'Page Objects And Actions'!$B$2:$B$50</definedName>
-    <definedName name="ComplianceReportsPage">'Page Objects And Actions'!$C$2:$C$50</definedName>
+    <definedName name="ComplianceReportsPage">'Page Objects And Actions'!$C$2:$C$149</definedName>
     <definedName name="DriverViewPage">'Page Objects And Actions'!$D$2:$D$132</definedName>
     <definedName name="EULAPage">'Page Objects And Actions'!$E$2:$E$50</definedName>
     <definedName name="FleetMapPage">'Page Objects And Actions'!$F$2:$F$50</definedName>
@@ -203,7 +203,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="321">
   <si>
     <t>ID</t>
   </si>
@@ -313,63 +313,15 @@
     <t>WebElement</t>
   </si>
   <si>
-    <t>openManageReports</t>
-  </si>
-  <si>
-    <t>performSearch</t>
-  </si>
-  <si>
-    <t>setRecordsPerPage</t>
-  </si>
-  <si>
-    <t>navigateToPageNo</t>
-  </si>
-  <si>
-    <t>navigateToFirstPage</t>
-  </si>
-  <si>
-    <t>navigateToLastPage</t>
-  </si>
-  <si>
-    <t>navigateToNextPage</t>
-  </si>
-  <si>
-    <t>navigateToPrevPage</t>
-  </si>
-  <si>
-    <t>openAddNewReports</t>
-  </si>
-  <si>
-    <t>submitNewReport</t>
-  </si>
-  <si>
-    <t>addNewReport</t>
-  </si>
-  <si>
     <t>deleteReport</t>
   </si>
   <si>
-    <t>copyReport</t>
-  </si>
-  <si>
-    <t>copyReportModifyDetails</t>
-  </si>
-  <si>
     <t>findReport</t>
   </si>
   <si>
-    <t>resubmitReport</t>
-  </si>
-  <si>
     <t>investigateReport</t>
   </si>
   <si>
-    <t>validateInvestigatePDFReport</t>
-  </si>
-  <si>
-    <t>validatePDFFiles</t>
-  </si>
-  <si>
     <t>clickById</t>
   </si>
   <si>
@@ -932,6 +884,288 @@
   </si>
   <si>
     <t>clickOnHeaderInfoBox</t>
+  </si>
+  <si>
+    <t>addSurveyToReport</t>
+  </si>
+  <si>
+    <t>cancelInProgressReport</t>
+  </si>
+  <si>
+    <t>clickOnCancelButton</t>
+  </si>
+  <si>
+    <t>clickOnOKButton</t>
+  </si>
+  <si>
+    <t>clickOnCopyButton</t>
+  </si>
+  <si>
+    <t>clickOnDeleteButton</t>
+  </si>
+  <si>
+    <t>clickOnComplianceViewerButton</t>
+  </si>
+  <si>
+    <t>clickOnInvestigateButton</t>
+  </si>
+  <si>
+    <t>clickOnInvestigatePDFButton</t>
+  </si>
+  <si>
+    <t>clickOnResubmitButton</t>
+  </si>
+  <si>
+    <t>clickThumbnailInViewer</t>
+  </si>
+  <si>
+    <t>clickOnConfirmDeleteReport</t>
+  </si>
+  <si>
+    <t>clickOnCancelConfirmDeleteReport</t>
+  </si>
+  <si>
+    <t>createNewReport</t>
+  </si>
+  <si>
+    <t>enterReportTitle</t>
+  </si>
+  <si>
+    <t>selectCustomer</t>
+  </si>
+  <si>
+    <t>selectTimeZone</t>
+  </si>
+  <si>
+    <t>enterExclusionRadius</t>
+  </si>
+  <si>
+    <t>selectReportMode</t>
+  </si>
+  <si>
+    <t>enterCustomBoundaryUsingAreaSelector</t>
+  </si>
+  <si>
+    <t>enterCustomBoundaryUsingTextFields</t>
+  </si>
+  <si>
+    <t>enterCustomerBoundaryUsingAreaSelector</t>
+  </si>
+  <si>
+    <t>enterCustomerBoundaryUsingTextFields</t>
+  </si>
+  <si>
+    <t>selectSurveySelectorSurveyor</t>
+  </si>
+  <si>
+    <t>enterSurveySelectorUsername</t>
+  </si>
+  <si>
+    <t>enterSurveySelectorTag</t>
+  </si>
+  <si>
+    <t>selectSurveySelectorStartDateTime</t>
+  </si>
+  <si>
+    <t>selectSurveySelectorEndDateTime</t>
+  </si>
+  <si>
+    <t>selectSurveySelectorSurveyModeFilter</t>
+  </si>
+  <si>
+    <t>checkSurveySelectorGeographicFilter</t>
+  </si>
+  <si>
+    <t>clickOnSurveySelectorSearchButton</t>
+  </si>
+  <si>
+    <t>enterFOVOpacity</t>
+  </si>
+  <si>
+    <t>enterLISAOpacity</t>
+  </si>
+  <si>
+    <t>enterPDFImageWidth</t>
+  </si>
+  <si>
+    <t>enterPDFImageHeight</t>
+  </si>
+  <si>
+    <t>addDefaultView</t>
+  </si>
+  <si>
+    <t>addNewView</t>
+  </si>
+  <si>
+    <t>selectViewLayersAsset</t>
+  </si>
+  <si>
+    <t>selectViewLayersBoundary</t>
+  </si>
+  <si>
+    <t>selectTabularPDFContent</t>
+  </si>
+  <si>
+    <t>openNewReportPage</t>
+  </si>
+  <si>
+    <t>searchForSurveyByKeyword</t>
+  </si>
+  <si>
+    <t>sortRecordsBy</t>
+  </si>
+  <si>
+    <t>verifyPDFThumbnailIsShownInComplianceViewer</t>
+  </si>
+  <si>
+    <t>verifyPDFZIPThumbnailIsShownInComplianceViewer</t>
+  </si>
+  <si>
+    <t>verifyShapeZIPThumbnailIsShownInComplianceViewer</t>
+  </si>
+  <si>
+    <t>verifyMetaDataZIPThumbnailIsShownInComplianceViewer</t>
+  </si>
+  <si>
+    <t>verifyView1ThumbnailIsShownInComplianceViewer</t>
+  </si>
+  <si>
+    <t>verifyView2ThumbnailIsShownInComplianceViewer</t>
+  </si>
+  <si>
+    <t>verifyView3ThumbnailIsShownInComplianceViewer</t>
+  </si>
+  <si>
+    <t>verifyView4ThumbnailIsShownInComplianceViewer</t>
+  </si>
+  <si>
+    <t>verifyView5ThumbnailIsShownInComplianceViewer</t>
+  </si>
+  <si>
+    <t>verifyView6ThumbnailIsShownInComplianceViewer</t>
+  </si>
+  <si>
+    <t>verifyView7ThumbnailIsShownInComplianceViewer</t>
+  </si>
+  <si>
+    <t>verifyPDFThumbnailDownloadFromComplianceViewer</t>
+  </si>
+  <si>
+    <t>verifyPDFZIPThumbnailDownloadFromComplianceViewer</t>
+  </si>
+  <si>
+    <t>verifyShapeZIPThumbnailDownloadFromComplianceViewer</t>
+  </si>
+  <si>
+    <t>verifyMetaDataZIPThumbnailDownloadFromComplianceViewer</t>
+  </si>
+  <si>
+    <t>verifyView1ThumbnailDownloadFromComplianceViewer</t>
+  </si>
+  <si>
+    <t>verifyView2ThumbnailDownloadFromComplianceViewer</t>
+  </si>
+  <si>
+    <t>verifyView3ThumbnailDownloadFromComplianceViewer</t>
+  </si>
+  <si>
+    <t>verifyView4ThumbnailDownloadFromComplianceViewer</t>
+  </si>
+  <si>
+    <t>verifyView5ThumbnailDownloadFromComplianceViewer</t>
+  </si>
+  <si>
+    <t>verifyView6ThumbnailDownloadFromComplianceViewer</t>
+  </si>
+  <si>
+    <t>verifyView7ThumbnailDownloadFromComplianceViewer</t>
+  </si>
+  <si>
+    <t>verifyInvestigatePDFDownload</t>
+  </si>
+  <si>
+    <t>verifySearchedSurveyIsShown</t>
+  </si>
+  <si>
+    <t>verifyCopyButtonIsDisplayed</t>
+  </si>
+  <si>
+    <t>verifyDeleteButtonIsDisplayed</t>
+  </si>
+  <si>
+    <t>verifyComplianceViewerButtonIsDisplayed</t>
+  </si>
+  <si>
+    <t>verifyInvestigateButtonIsDisplayed</t>
+  </si>
+  <si>
+    <t>verifyInvestigatePDFButtonIsDisplayed</t>
+  </si>
+  <si>
+    <t>verifyResubmitButtonIsDisplayed</t>
+  </si>
+  <si>
+    <t>verifyPDFZipFilesAreCorrect</t>
+  </si>
+  <si>
+    <t>verifyShapeZIPFilesAreCorrect</t>
+  </si>
+  <si>
+    <t>verifyMetaDataZIPFilesAreCorrect</t>
+  </si>
+  <si>
+    <t>verifyReportPDFMatches</t>
+  </si>
+  <si>
+    <t>verifyReportThumbnailMatches</t>
+  </si>
+  <si>
+    <t>verifySearchedSurveysMatchTag</t>
+  </si>
+  <si>
+    <t>verifySearchedSurveysMatchDateRange</t>
+  </si>
+  <si>
+    <t>verifySearchedSurveysMatchSurveyorUnit</t>
+  </si>
+  <si>
+    <t>verifySearchedSurveysAreForLastXDays</t>
+  </si>
+  <si>
+    <t>verifyShapeFilesHaveCorrectData</t>
+  </si>
+  <si>
+    <t>verifyMetaDataFilesHaveCorrectData</t>
+  </si>
+  <si>
+    <t>verifyRequiredFieldsAreShownInRed</t>
+  </si>
+  <si>
+    <t>verifyComplianceViewerViewCountEquals</t>
+  </si>
+  <si>
+    <t>Generate compliance report with all default values/filters selected and download it</t>
+  </si>
+  <si>
+    <t>TC146</t>
+  </si>
+  <si>
+    <t>1,6</t>
+  </si>
+  <si>
+    <t>Login as Picarro Admin</t>
+  </si>
+  <si>
+    <t>Open compliance report page</t>
+  </si>
+  <si>
+    <t>Create new compliance report page</t>
+  </si>
+  <si>
+    <t>Report generated successfully</t>
+  </si>
+  <si>
+    <t>Click Compliance PDF (ZIP)</t>
   </si>
 </sst>
 </file>
@@ -988,7 +1222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1005,6 +1239,7 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1285,10 +1520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1321,6 +1556,23 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>314</v>
+      </c>
+      <c r="C2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D2" t="s">
+        <v>315</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -1332,7 +1584,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1370,10 +1622,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="D2">
         <v>3</v>
@@ -1390,10 +1642,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1434,12 +1686,111 @@
         <v>6</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>217</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="8">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>316</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>317</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="8">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>240</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="8">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>320</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>234</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="8">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>319</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>300</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576">
       <formula1>PageObject_Name</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D423">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D424">
       <formula1>INDIRECT(C2)</formula1>
     </dataValidation>
   </dataValidations>
@@ -1452,7 +1803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
@@ -1499,13 +1850,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -1513,13 +1864,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="G3" s="5">
         <v>6</v>
@@ -1530,13 +1881,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>231</v>
+        <v>215</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="G4" s="5">
         <v>3</v>
@@ -1547,13 +1898,13 @@
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>232</v>
+        <v>216</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -1561,13 +1912,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1575,13 +1926,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="G7" s="5">
         <v>3</v>
@@ -1592,13 +1943,13 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -1606,13 +1957,13 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -1620,13 +1971,13 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -1634,13 +1985,13 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -1648,13 +1999,13 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
     </row>
     <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -1662,13 +2013,13 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -1676,13 +2027,13 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -1690,13 +2041,13 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="C15" t="s">
         <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -1704,13 +2055,13 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="C16" t="s">
         <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -1718,13 +2069,13 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="C17" t="s">
         <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -1732,13 +2083,13 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="C18" t="s">
         <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -1746,13 +2097,13 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="C19" t="s">
         <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -1760,13 +2111,13 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="C20" t="s">
         <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -1774,13 +2125,13 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="C21" t="s">
         <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -1788,13 +2139,13 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="C22" t="s">
         <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -1802,13 +2153,13 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="C23" t="s">
         <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
     </row>
     <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -1816,13 +2167,13 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="C24" t="s">
         <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -1830,13 +2181,13 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>191</v>
+        <v>175</v>
       </c>
       <c r="C25" t="s">
         <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
     </row>
     <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -1844,13 +2195,13 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="C26" t="s">
         <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
     </row>
     <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -1858,13 +2209,13 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="C27" t="s">
         <v>10</v>
       </c>
       <c r="D27" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -1872,13 +2223,13 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="C28" t="s">
         <v>10</v>
       </c>
       <c r="D28" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -1886,13 +2237,13 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="C29" t="s">
         <v>10</v>
       </c>
       <c r="D29" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1900,13 +2251,13 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="C30" t="s">
         <v>10</v>
       </c>
       <c r="D30" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -1914,13 +2265,13 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="C31" t="s">
         <v>10</v>
       </c>
       <c r="D31" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -1928,13 +2279,13 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="C32" t="s">
         <v>10</v>
       </c>
       <c r="D32" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1942,13 +2293,13 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="C33" t="s">
         <v>10</v>
       </c>
       <c r="D33" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1956,13 +2307,13 @@
         <v>1</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="C34" t="s">
         <v>10</v>
       </c>
       <c r="D34" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1970,13 +2321,13 @@
         <v>1</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="C35" t="s">
         <v>10</v>
       </c>
       <c r="D35" t="s">
-        <v>225</v>
+        <v>209</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1984,13 +2335,13 @@
         <v>1</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="C36" t="s">
         <v>10</v>
       </c>
       <c r="D36" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="F36" s="3"/>
     </row>
@@ -1999,13 +2350,13 @@
         <v>1</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="C37" t="s">
         <v>10</v>
       </c>
       <c r="D37" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -2013,13 +2364,13 @@
         <v>1</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="C38" t="s">
         <v>10</v>
       </c>
       <c r="D38" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -2027,13 +2378,13 @@
         <v>1</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="C39" t="s">
         <v>10</v>
       </c>
       <c r="D39" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -2041,13 +2392,13 @@
         <v>1</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="C40" t="s">
         <v>10</v>
       </c>
       <c r="D40" t="s">
-        <v>221</v>
+        <v>205</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -2055,13 +2406,13 @@
         <v>1</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="C41" t="s">
         <v>10</v>
       </c>
       <c r="D41" t="s">
-        <v>221</v>
+        <v>205</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -2069,13 +2420,13 @@
         <v>1</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="C42" t="s">
         <v>10</v>
       </c>
       <c r="D42" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -2083,13 +2434,13 @@
         <v>1</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="C43" t="s">
         <v>10</v>
       </c>
       <c r="D43" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -2097,13 +2448,13 @@
         <v>1</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="C44" t="s">
         <v>10</v>
       </c>
       <c r="D44" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -2111,13 +2462,13 @@
         <v>1</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="C45" t="s">
         <v>10</v>
       </c>
       <c r="D45" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -2151,15 +2502,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="D139" sqref="D138:D139"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.77734375" customWidth="1"/>
-    <col min="3" max="3" width="29.33203125" customWidth="1"/>
+    <col min="3" max="3" width="53.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="11" width="23" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="23.33203125" bestFit="1" customWidth="1"/>
@@ -2251,70 +2602,70 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>262</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E2" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="F2" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="G2" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="H2" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="I2" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="J2" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="K2" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="L2" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="M2" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="N2" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="O2" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="P2" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="Q2" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="R2" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="S2" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="T2" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="U2" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="V2" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="W2" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
@@ -2322,70 +2673,70 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>263</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="F3" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="G3" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="H3" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="I3" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="J3" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="K3" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="L3" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="M3" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="N3" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="O3" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="P3" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="Q3" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="R3" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="S3" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="T3" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="U3" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="V3" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="W3" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
@@ -2393,70 +2744,70 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>227</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="E4" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="F4" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="G4" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="H4" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="I4" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="J4" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="K4" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="L4" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="M4" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="N4" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="O4" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="P4" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="Q4" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="R4" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="S4" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="T4" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="U4" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="V4" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="W4" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
@@ -2464,70 +2815,70 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>228</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="F5" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="G5" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="H5" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="I5" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="J5" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="K5" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="L5" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="M5" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="N5" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="O5" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="P5" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="Q5" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="R5" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="S5" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="T5" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="U5" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="V5" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="W5" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
@@ -2535,70 +2886,70 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>256</v>
       </c>
       <c r="D6" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="E6" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="F6" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="G6" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="H6" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="I6" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="J6" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="K6" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="L6" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="M6" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="N6" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="O6" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="P6" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="Q6" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="R6" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="S6" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="T6" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="U6" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="V6" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="W6" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
@@ -2606,70 +2957,70 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="E7" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="F7" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="G7" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="H7" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="I7" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="J7" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="K7" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="L7" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="M7" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="N7" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="O7" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="P7" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="Q7" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="R7" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="S7" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="T7" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="U7" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="V7" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="W7" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.3">
@@ -2677,70 +3028,70 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" t="s">
+        <v>217</v>
+      </c>
+      <c r="F8" t="s">
+        <v>217</v>
+      </c>
+      <c r="G8" t="s">
+        <v>217</v>
+      </c>
+      <c r="H8" t="s">
         <v>49</v>
       </c>
-      <c r="D8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E8" t="s">
-        <v>233</v>
-      </c>
-      <c r="F8" t="s">
-        <v>233</v>
-      </c>
-      <c r="G8" t="s">
-        <v>233</v>
-      </c>
-      <c r="H8" t="s">
-        <v>65</v>
-      </c>
       <c r="I8" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="J8" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="K8" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="L8" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="M8" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="N8" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="O8" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="P8" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="Q8" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="R8" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="S8" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="T8" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="U8" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="V8" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="W8" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
@@ -2748,70 +3099,70 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="E9" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="F9" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="G9" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="H9" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="I9" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="J9" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="K9" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="L9" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="M9" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="N9" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="O9" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="P9" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="Q9" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="R9" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="S9" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="T9" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="U9" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="V9" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="W9" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
@@ -2819,70 +3170,70 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="E10" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="F10" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="G10" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="H10" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="I10" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="J10" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="K10" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="L10" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="M10" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="N10" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="O10" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="P10" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="Q10" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="R10" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="S10" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="T10" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="U10" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="V10" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="W10" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.3">
@@ -2890,70 +3241,70 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>59</v>
+        <v>229</v>
       </c>
       <c r="D11" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="E11" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="F11" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="G11" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="H11" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="I11" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="J11" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="K11" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="L11" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="M11" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="N11" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="O11" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="P11" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="Q11" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="R11" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="S11" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="T11" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="U11" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="V11" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="W11" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
@@ -2961,70 +3312,70 @@
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
-        <v>60</v>
+        <v>239</v>
       </c>
       <c r="D12" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="E12" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="F12" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="G12" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="H12" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="I12" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="J12" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="K12" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="L12" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="M12" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="N12" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="O12" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="P12" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="Q12" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="R12" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="S12" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="T12" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="U12" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="V12" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="W12" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.3">
@@ -3032,13 +3383,13 @@
         <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>233</v>
       </c>
       <c r="D13" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="H13" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.3">
@@ -3046,13 +3397,13 @@
         <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>238</v>
       </c>
       <c r="D14" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="H14" t="s">
-        <v>228</v>
+        <v>212</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.3">
@@ -3060,13 +3411,13 @@
         <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>231</v>
       </c>
       <c r="D15" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="H15" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.3">
@@ -3074,10 +3425,10 @@
         <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>232</v>
       </c>
       <c r="D16" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -3085,10 +3436,10 @@
         <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>234</v>
       </c>
       <c r="D17" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -3096,10 +3447,10 @@
         <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>235</v>
       </c>
       <c r="D18" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -3107,10 +3458,10 @@
         <v>25</v>
       </c>
       <c r="C19" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D19" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -3118,10 +3469,10 @@
         <v>26</v>
       </c>
       <c r="C20" t="s">
-        <v>44</v>
+        <v>236</v>
       </c>
       <c r="D20" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -3129,10 +3480,10 @@
         <v>27</v>
       </c>
       <c r="C21" t="s">
-        <v>36</v>
+        <v>257</v>
       </c>
       <c r="D21" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -3140,10 +3491,10 @@
         <v>28</v>
       </c>
       <c r="C22" t="s">
-        <v>37</v>
+        <v>237</v>
       </c>
       <c r="D22" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -3151,614 +3502,824 @@
         <v>29</v>
       </c>
       <c r="C23" t="s">
-        <v>51</v>
+        <v>240</v>
       </c>
       <c r="D23" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="D24" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
-        <v>62</v>
+        <v>246</v>
       </c>
       <c r="D25" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
-        <v>63</v>
+        <v>247</v>
       </c>
       <c r="D26" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
+        <v>248</v>
+      </c>
+      <c r="D27" t="s">
         <v>64</v>
-      </c>
-      <c r="D27" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
-        <v>38</v>
+        <v>249</v>
       </c>
       <c r="D28" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
-        <v>45</v>
+        <v>244</v>
       </c>
       <c r="D29" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C30" t="s">
-        <v>53</v>
+        <v>258</v>
       </c>
       <c r="D30" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
-        <v>54</v>
+        <v>259</v>
       </c>
       <c r="D31" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>261</v>
+      </c>
+      <c r="D32" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>260</v>
+      </c>
+      <c r="D33" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C34" t="s">
+        <v>241</v>
+      </c>
+      <c r="D34" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C35" t="s">
+        <v>252</v>
+      </c>
+      <c r="D35" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C36" t="s">
+        <v>251</v>
+      </c>
+      <c r="D36" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>37</v>
+      </c>
+      <c r="D37" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="38" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C38" t="s">
+        <v>43</v>
+      </c>
+      <c r="D38" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="39" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C39" t="s">
+        <v>44</v>
+      </c>
+      <c r="D39" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C40" t="s">
+        <v>38</v>
+      </c>
+      <c r="D40" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="41" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C41" t="s">
+        <v>217</v>
+      </c>
+      <c r="D41" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="42" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C42" t="s">
+        <v>267</v>
+      </c>
+      <c r="D42" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="43" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C43" t="s">
+        <v>268</v>
+      </c>
+      <c r="D43" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="44" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C44" t="s">
+        <v>242</v>
+      </c>
+      <c r="D44" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="45" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C45" t="s">
+        <v>45</v>
+      </c>
+      <c r="D45" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="46" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D46" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="47" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C47" t="s">
+        <v>47</v>
+      </c>
+      <c r="D47" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="48" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C48" t="s">
+        <v>48</v>
+      </c>
+      <c r="D48" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
+        <v>245</v>
+      </c>
+      <c r="D49" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C50" t="s">
+        <v>254</v>
+      </c>
+      <c r="D50" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C51" t="s">
+        <v>253</v>
+      </c>
+      <c r="D51" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C52" t="s">
+        <v>255</v>
+      </c>
+      <c r="D52" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="53" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C53" t="s">
+        <v>250</v>
+      </c>
+      <c r="D53" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="54" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C54" t="s">
+        <v>266</v>
+      </c>
+      <c r="D54" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="55" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C55" t="s">
+        <v>243</v>
+      </c>
+      <c r="D55" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="56" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C56" t="s">
+        <v>264</v>
+      </c>
+      <c r="D56" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C57" t="s">
+        <v>265</v>
+      </c>
+      <c r="D57" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="58" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C58" t="s">
+        <v>269</v>
+      </c>
+      <c r="D58" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="59" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C59" t="s">
+        <v>296</v>
+      </c>
+      <c r="D59" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="60" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C60" t="s">
+        <v>312</v>
+      </c>
+      <c r="D60" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="61" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C61" t="s">
+        <v>294</v>
+      </c>
+      <c r="D61" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="62" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C62" t="s">
+        <v>295</v>
+      </c>
+      <c r="D62" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="63" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C63" t="s">
+        <v>297</v>
+      </c>
+      <c r="D63" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="64" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C64" t="s">
+        <v>298</v>
+      </c>
+      <c r="D64" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D32" t="s">
+    <row r="65" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C65" t="s">
+        <v>292</v>
+      </c>
+      <c r="D65" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="66" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C66" t="s">
+        <v>310</v>
+      </c>
+      <c r="D66" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="67" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C67" t="s">
+        <v>302</v>
+      </c>
+      <c r="D67" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="68" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C68" t="s">
+        <v>284</v>
+      </c>
+      <c r="D68" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D33" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D34" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D35" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D36" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D37" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D38" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D39" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D40" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D41" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D42" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D43" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D44" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D45" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D46" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D47" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D48" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D49" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D50" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D51" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D52" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D53" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D54" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D55" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D56" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D57" t="s">
+    <row r="69" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C69" t="s">
+        <v>273</v>
+      </c>
+      <c r="D69" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C70" t="s">
+        <v>281</v>
+      </c>
+      <c r="D70" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C71" t="s">
+        <v>270</v>
+      </c>
+      <c r="D71" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="72" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C72" t="s">
+        <v>300</v>
+      </c>
+      <c r="D72" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="73" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C73" t="s">
+        <v>282</v>
+      </c>
+      <c r="D73" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="74" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C74" t="s">
+        <v>271</v>
+      </c>
+      <c r="D74" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="75" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C75" t="s">
+        <v>303</v>
+      </c>
+      <c r="D75" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="76" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C76" t="s">
+        <v>304</v>
+      </c>
+      <c r="D76" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="77" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C77" t="s">
+        <v>311</v>
+      </c>
+      <c r="D77" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="78" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C78" t="s">
+        <v>299</v>
+      </c>
+      <c r="D78" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="79" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C79" t="s">
+        <v>293</v>
+      </c>
+      <c r="D79" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="80" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C80" t="s">
+        <v>308</v>
+      </c>
+      <c r="D80" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="81" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C81" t="s">
+        <v>306</v>
+      </c>
+      <c r="D81" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="82" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C82" t="s">
+        <v>307</v>
+      </c>
+      <c r="D82" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="83" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C83" t="s">
+        <v>305</v>
+      </c>
+      <c r="D83" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="84" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C84" t="s">
+        <v>309</v>
+      </c>
+      <c r="D84" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="85" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C85" t="s">
+        <v>301</v>
+      </c>
+      <c r="D85" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="86" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C86" t="s">
+        <v>283</v>
+      </c>
+      <c r="D86" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="87" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C87" t="s">
+        <v>272</v>
+      </c>
+      <c r="D87" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="88" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C88" t="s">
+        <v>285</v>
+      </c>
+      <c r="D88" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="89" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C89" t="s">
+        <v>274</v>
+      </c>
+      <c r="D89" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="90" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C90" t="s">
+        <v>286</v>
+      </c>
+      <c r="D90" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="91" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C91" t="s">
+        <v>275</v>
+      </c>
+      <c r="D91" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="92" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C92" t="s">
+        <v>287</v>
+      </c>
+      <c r="D92" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="93" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C93" t="s">
+        <v>276</v>
+      </c>
+      <c r="D93" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="94" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C94" t="s">
+        <v>288</v>
+      </c>
+      <c r="D94" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="95" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C95" t="s">
+        <v>277</v>
+      </c>
+      <c r="D95" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="96" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C96" t="s">
+        <v>289</v>
+      </c>
+      <c r="D96" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="97" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C97" t="s">
+        <v>278</v>
+      </c>
+      <c r="D97" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="98" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C98" t="s">
+        <v>290</v>
+      </c>
+      <c r="D98" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="99" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C99" t="s">
+        <v>279</v>
+      </c>
+      <c r="D99" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="100" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C100" t="s">
+        <v>291</v>
+      </c>
+      <c r="D100" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="101" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C101" t="s">
+        <v>280</v>
+      </c>
+      <c r="D101" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="102" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D102" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D58" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D59" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D60" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D61" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D62" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D63" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="64" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D64" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D65" t="s">
+    <row r="103" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D103" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D66" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D67" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D68" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D69" t="s">
+    <row r="104" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D104" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D70" t="s">
+    <row r="105" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D105" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D71" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D72" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D73" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D74" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D75" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D76" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D77" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D78" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D79" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D80" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D81" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D82" t="s">
+    <row r="106" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D106" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D83" t="s">
+    <row r="107" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D107" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D84" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D85" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="86" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D86" t="s">
+    <row r="108" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D108" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D87" t="s">
+    <row r="109" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D109" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="88" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D88" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="89" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D89" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="90" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D90" t="s">
+    <row r="110" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D110" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="91" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D91" t="s">
+    <row r="111" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D111" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="92" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D92" t="s">
+    <row r="112" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D112" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="93" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D93" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="94" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D94" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="95" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D95" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="96" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D96" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D97" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D98" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D99" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="100" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D100" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="101" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D101" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="102" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D102" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="103" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D103" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="104" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D104" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="105" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D105" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="106" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D106" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="107" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D107" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="108" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D108" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="109" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D109" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="110" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D110" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="111" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D111" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="112" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D112" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="113" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D113" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
     </row>
     <row r="114" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D114" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
     </row>
     <row r="115" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D115" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
     </row>
     <row r="116" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D116" t="s">
-        <v>221</v>
+        <v>205</v>
       </c>
     </row>
     <row r="117" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D117" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
     </row>
     <row r="118" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D118" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
     </row>
     <row r="119" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D119" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
     </row>
     <row r="120" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D120" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
     </row>
     <row r="121" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D121" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
     </row>
     <row r="122" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D122" t="s">
-        <v>217</v>
+        <v>201</v>
       </c>
     </row>
     <row r="123" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D123" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
     </row>
     <row r="124" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D124" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
     </row>
     <row r="125" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D125" t="s">
-        <v>240</v>
+        <v>224</v>
       </c>
     </row>
     <row r="126" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D126" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
     </row>
     <row r="127" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D127" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
     </row>
     <row r="128" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D128" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
     </row>
     <row r="129" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D129" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
     </row>
     <row r="130" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D130" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
     </row>
     <row r="131" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D131" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
     </row>
     <row r="132" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D132" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
     </row>
     <row r="133" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D133" t="s">
-        <v>235</v>
+        <v>219</v>
       </c>
     </row>
     <row r="134" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D134" t="s">
-        <v>236</v>
+        <v>220</v>
       </c>
     </row>
     <row r="135" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D135" t="s">
-        <v>237</v>
+        <v>221</v>
       </c>
     </row>
     <row r="136" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D136" t="s">
-        <v>238</v>
+        <v>222</v>
       </c>
     </row>
     <row r="137" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D137" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
     </row>
     <row r="138" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D138" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="D2:D132">
-    <sortCondition ref="D132"/>
+  <sortState ref="C2:C102">
+    <sortCondition ref="C102"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Test case and page action/page modal classes for TC256,TC302,TC777
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCases.xlsx
+++ b/selenium-wd/data/TestCases.xlsx
@@ -203,7 +203,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="338">
   <si>
     <t>ID</t>
   </si>
@@ -1202,13 +1202,28 @@
   </si>
   <si>
     <t>verifyUncertaintyValueIsFormattedCorrectly</t>
+  </si>
+  <si>
+    <t>openStartSurveyModalDialog</t>
+  </si>
+  <si>
+    <t>clickOnShutdownButton</t>
+  </si>
+  <si>
+    <t>verifySurveyTagInStartSurveyDialogEquals</t>
+  </si>
+  <si>
+    <t>verifyStartSurveyButtonFromSurveyDialogIsEnabled</t>
+  </si>
+  <si>
+    <t>verifyStartSurveyButtonFromSurveyDialogIsDisabled</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1239,7 +1254,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1265,7 +1286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1288,6 +1309,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2737,10 +2759,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:W138"/>
+  <dimension ref="A1:W143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B98" workbookViewId="0">
-      <selection activeCell="C104" sqref="C104:C106"/>
+    <sheetView tabSelected="1" topLeftCell="B120" workbookViewId="0">
+      <selection activeCell="D143" sqref="D143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4569,6 +4591,31 @@
         <v>225</v>
       </c>
     </row>
+    <row r="139" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D139" s="12" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="140" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D140" s="12" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="141" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D141" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="142" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D142" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="143" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D143" t="s">
+        <v>337</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="C2:C103">
     <sortCondition ref="C103"/>

</xml_diff>

<commit_message>
Initial set of changes for adding additional driver view test cases using Page actions
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCases.xlsx
+++ b/selenium-wd/data/TestCases.xlsx
@@ -9,19 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="910" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="910" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases-CmpReports" sheetId="1" r:id="rId1"/>
-    <sheet name="TestCases-DriverView" sheetId="6" r:id="rId2"/>
-    <sheet name="TestCases-CmpReports-TestSteps" sheetId="3" r:id="rId3"/>
+    <sheet name="TestCases-CmpReports-TestSteps" sheetId="3" r:id="rId2"/>
+    <sheet name="TestCases-DriverView" sheetId="6" r:id="rId3"/>
     <sheet name="TestCases-DriverView-TestSteps" sheetId="7" r:id="rId4"/>
     <sheet name="Page Objects And Actions" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="AdministrationPage">'Page Objects And Actions'!$B$2:$B$50</definedName>
     <definedName name="ComplianceReportsPage">'Page Objects And Actions'!$C$2:$C$149</definedName>
-    <definedName name="DriverViewPage">'Page Objects And Actions'!$D$2:$D$132</definedName>
+    <definedName name="DriverViewPage">'Page Objects And Actions'!$D$2:$D$133</definedName>
     <definedName name="EULAPage">'Page Objects And Actions'!$E$2:$E$50</definedName>
     <definedName name="FleetMapPage">'Page Objects And Actions'!$F$2:$F$50</definedName>
     <definedName name="HomePage">'Page Objects And Actions'!$G$2:$G$50</definedName>
@@ -35,12 +35,13 @@
     <definedName name="ManageSurveyorPage">'Page Objects And Actions'!$N$2:$N$50</definedName>
     <definedName name="ManageUsersPage">'Page Objects And Actions'!$P$2:$P$50</definedName>
     <definedName name="MeasurementSessionsPage">'Page Objects And Actions'!$Q$2:$Q$50</definedName>
-    <definedName name="PageObject_Name">'Page Objects And Actions'!$A$2:$A$23</definedName>
+    <definedName name="PageObject_Name">'Page Objects And Actions'!$A$2:$A$24</definedName>
     <definedName name="PrimePage">'Page Objects And Actions'!$R$2:$R$50</definedName>
     <definedName name="ReferenceGasReportsPage">'Page Objects And Actions'!$S$2:$S$50</definedName>
     <definedName name="SendFeedbackPage">'Page Objects And Actions'!$T$2:$T$50</definedName>
     <definedName name="SurveyorHistoryReportsPage">'Page Objects And Actions'!$V$2:$V$50</definedName>
     <definedName name="SurveyorSystemsPage">'Page Objects And Actions'!$U$2:$U$50</definedName>
+    <definedName name="TestEnvironment">'Page Objects And Actions'!$X$2:$X$11</definedName>
     <definedName name="UserFeedbackPage">'Page Objects And Actions'!$W$2:$W$50</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -95,43 +96,6 @@
     <author>Shirish Pulikkal</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Shirish Pulikkal:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-To specify range use: {n:m} .. For eg. "3:5"
-To specify beginning use: {n:} .. For eg "3:" will runs tests for all rows starting from row 3.
-To specify a specific row: {n} .. For eg "3" will run test ONLY for row 3.
-To specify random rows: {n1,n2,n3} .. For eg "1,3,15" will run test for rows 1, 3 and 15.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Shirish Pulikkal</author>
-  </authors>
-  <commentList>
     <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
@@ -157,6 +121,43 @@
 To specify a specific row: {n} .. For eg "3" will run test ONLY for row 3.
 To specify random rows: {n1,n2,n3} .. For eg "1,3,15" will run test for rows 1, 3 and 15.
 </t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Shirish Pulikkal</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Shirish Pulikkal:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+To specify range use: {n:m} .. For eg. "3:5"
+To specify beginning use: {n:} .. For eg "3:" will runs tests for all rows starting from row 3.
+To specify a specific row: {n} .. For eg "3" will run test ONLY for row 3.
+To specify random rows: {n1,n2,n3} .. For eg "1,3,15" will run test for rows 1, 3 and 15.</t>
         </r>
       </text>
     </comment>
@@ -203,7 +204,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="348">
   <si>
     <t>ID</t>
   </si>
@@ -859,9 +860,6 @@
     <t>open</t>
   </si>
   <si>
-    <t>startSimulatorScript</t>
-  </si>
-  <si>
     <t>verifyMapSwitchOn</t>
   </si>
   <si>
@@ -1217,6 +1215,39 @@
   </si>
   <si>
     <t>verifyStartSurveyButtonFromSurveyDialogIsDisabled</t>
+  </si>
+  <si>
+    <t>clickOnPicarroLogoButton</t>
+  </si>
+  <si>
+    <t>verifyPageLoaded</t>
+  </si>
+  <si>
+    <t>verifySystemShutdownButtonIsDisplayed</t>
+  </si>
+  <si>
+    <t>verifySurveyInfoTimeLabelEquals</t>
+  </si>
+  <si>
+    <t>verifySurveyInfoTimeLabelStartsWith</t>
+  </si>
+  <si>
+    <t>TestEnvironment</t>
+  </si>
+  <si>
+    <t>switchAnalyzer</t>
+  </si>
+  <si>
+    <t>startSimulator</t>
+  </si>
+  <si>
+    <t>stopSimulator</t>
+  </si>
+  <si>
+    <t>verifyAnalyzerIsRunning</t>
+  </si>
+  <si>
+    <t>verifyAnalyzerIsShutdown</t>
   </si>
 </sst>
 </file>
@@ -1632,10 +1663,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D2">
         <v>6</v>
@@ -1649,10 +1680,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>319</v>
+      </c>
+      <c r="C3" t="s">
         <v>320</v>
-      </c>
-      <c r="C3" t="s">
-        <v>321</v>
       </c>
       <c r="D3">
         <v>6</v>
@@ -1666,10 +1697,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="11" t="s">
+        <v>325</v>
+      </c>
+      <c r="C4" t="s">
         <v>326</v>
-      </c>
-      <c r="C4" t="s">
-        <v>327</v>
       </c>
       <c r="D4">
         <v>6</v>
@@ -1683,10 +1714,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C5" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D5">
         <v>6</v>
@@ -1702,6 +1733,299 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:H15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.77734375" style="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="59.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.77734375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.77734375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.44140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.33203125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.44140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="20.21875" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>217</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="8">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>313</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>314</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="8">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>315</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>239</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="8">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>317</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>233</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="8">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>316</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>318</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>213</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>217</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="8">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>313</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="8">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>314</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="8">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>315</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>239</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="8">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>317</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>233</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="8">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>316</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>318</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="8">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>323</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>321</v>
+      </c>
+      <c r="E14">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="8">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>324</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
+        <v>322</v>
+      </c>
+      <c r="G15">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576">
+      <formula1>PageObject_Name</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D424">
+      <formula1>INDIRECT(C2)</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F2"/>
@@ -1763,306 +2087,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:H15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="2.77734375" style="7" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="59.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.77734375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.77734375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.44140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.44140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="20.21875" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="8">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>213</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>217</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="8">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>314</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>315</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="8">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>316</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>240</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="8">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>318</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>234</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="8">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
-        <v>317</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" t="s">
-        <v>319</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="8">
-        <v>2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>213</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" t="s">
-        <v>217</v>
-      </c>
-      <c r="G8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="8">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>314</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="8">
-        <v>2</v>
-      </c>
-      <c r="B10" t="s">
-        <v>315</v>
-      </c>
-      <c r="C10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="8">
-        <v>2</v>
-      </c>
-      <c r="B11" t="s">
-        <v>316</v>
-      </c>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" t="s">
-        <v>240</v>
-      </c>
-      <c r="G11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="8">
-        <v>2</v>
-      </c>
-      <c r="B12" t="s">
-        <v>318</v>
-      </c>
-      <c r="C12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" t="s">
-        <v>234</v>
-      </c>
-      <c r="G12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="8">
-        <v>2</v>
-      </c>
-      <c r="B13" t="s">
-        <v>317</v>
-      </c>
-      <c r="C13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" t="s">
-        <v>319</v>
-      </c>
-      <c r="G13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="8">
-        <v>2</v>
-      </c>
-      <c r="B14" t="s">
-        <v>324</v>
-      </c>
-      <c r="C14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" t="s">
-        <v>322</v>
-      </c>
-      <c r="E14">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="8">
-        <v>2</v>
-      </c>
-      <c r="B15" t="s">
-        <v>325</v>
-      </c>
-      <c r="C15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" t="s">
-        <v>323</v>
-      </c>
-      <c r="G15">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576">
-      <formula1>PageObject_Name</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D424">
-      <formula1>INDIRECT(C2)</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2142,10 +2173,10 @@
         <v>215</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>342</v>
       </c>
       <c r="D4" t="s">
-        <v>218</v>
+        <v>343</v>
       </c>
       <c r="G4" s="5">
         <v>3</v>
@@ -2759,10 +2790,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:W143"/>
+  <dimension ref="A1:X147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B120" workbookViewId="0">
-      <selection activeCell="D143" sqref="D143"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="X6" sqref="X6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2782,10 +2813,10 @@
     <col min="20" max="20" width="27.21875" customWidth="1" collapsed="1"/>
     <col min="21" max="21" width="31.5546875" customWidth="1" collapsed="1"/>
     <col min="22" max="22" width="28.21875" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="28" customWidth="1" collapsed="1"/>
+    <col min="23" max="24" width="28" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -2855,8 +2886,11 @@
       <c r="W1" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X1" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -2864,7 +2898,7 @@
         <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D2" t="s">
         <v>39</v>
@@ -2926,8 +2960,11 @@
       <c r="W2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X2" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2935,7 +2972,7 @@
         <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D3" t="s">
         <v>41</v>
@@ -2997,8 +3034,11 @@
       <c r="W3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X3" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -3006,7 +3046,7 @@
         <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D4" t="s">
         <v>40</v>
@@ -3068,8 +3108,11 @@
       <c r="W4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X4" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -3077,7 +3120,7 @@
         <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D5" t="s">
         <v>42</v>
@@ -3139,8 +3182,11 @@
       <c r="W5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X5" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -3148,7 +3194,7 @@
         <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D6" t="s">
         <v>50</v>
@@ -3211,7 +3257,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -3282,7 +3328,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -3353,7 +3399,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -3424,7 +3470,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -3495,7 +3541,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -3503,7 +3549,7 @@
         <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D11" t="s">
         <v>55</v>
@@ -3566,7 +3612,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -3574,7 +3620,7 @@
         <v>48</v>
       </c>
       <c r="C12" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D12" t="s">
         <v>56</v>
@@ -3637,12 +3683,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D13" t="s">
         <v>57</v>
@@ -3651,12 +3697,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D14" t="s">
         <v>58</v>
@@ -3665,12 +3711,12 @@
         <v>212</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D15" t="s">
         <v>59</v>
@@ -3679,12 +3725,12 @@
         <v>211</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D16" t="s">
         <v>60</v>
@@ -3695,10 +3741,10 @@
         <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
+        <v>337</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -3706,10 +3752,10 @@
         <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -3717,10 +3763,10 @@
         <v>25</v>
       </c>
       <c r="C19" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -3728,10 +3774,10 @@
         <v>26</v>
       </c>
       <c r="C20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D20" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -3739,10 +3785,10 @@
         <v>27</v>
       </c>
       <c r="C21" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -3750,10 +3796,10 @@
         <v>28</v>
       </c>
       <c r="C22" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D22" t="s">
-        <v>217</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -3761,63 +3807,66 @@
         <v>29</v>
       </c>
       <c r="C23" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D23" t="s">
-        <v>45</v>
+        <v>217</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>342</v>
+      </c>
       <c r="C24" t="s">
         <v>36</v>
       </c>
       <c r="D24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D27" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D29" t="s">
-        <v>218</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C30" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D30" t="s">
         <v>66</v>
@@ -3825,7 +3874,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D31" t="s">
         <v>135</v>
@@ -3833,7 +3882,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C32" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D32" t="s">
         <v>136</v>
@@ -3841,7 +3890,7 @@
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C33" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D33" t="s">
         <v>154</v>
@@ -3849,7 +3898,7 @@
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C34" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D34" t="s">
         <v>153</v>
@@ -3857,7 +3906,7 @@
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C35" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D35" t="s">
         <v>155</v>
@@ -3905,7 +3954,7 @@
     </row>
     <row r="41" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C41" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D41" t="s">
         <v>139</v>
@@ -3913,7 +3962,7 @@
     </row>
     <row r="42" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C42" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D42" t="s">
         <v>140</v>
@@ -3921,7 +3970,7 @@
     </row>
     <row r="43" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C43" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D43" t="s">
         <v>141</v>
@@ -3961,7 +4010,7 @@
     </row>
     <row r="48" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C48" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D48" t="s">
         <v>160</v>
@@ -3969,7 +4018,7 @@
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C49" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D49" t="s">
         <v>125</v>
@@ -3977,7 +4026,7 @@
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D50" t="s">
         <v>126</v>
@@ -3985,7 +4034,7 @@
     </row>
     <row r="51" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C51" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D51" t="s">
         <v>146</v>
@@ -3993,7 +4042,7 @@
     </row>
     <row r="52" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C52" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D52" t="s">
         <v>145</v>
@@ -4001,7 +4050,7 @@
     </row>
     <row r="53" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C53" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D53" t="s">
         <v>147</v>
@@ -4009,7 +4058,7 @@
     </row>
     <row r="54" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C54" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D54" t="s">
         <v>148</v>
@@ -4017,7 +4066,7 @@
     </row>
     <row r="55" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C55" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D55" t="s">
         <v>149</v>
@@ -4025,7 +4074,7 @@
     </row>
     <row r="56" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D56" t="s">
         <v>150</v>
@@ -4033,7 +4082,7 @@
     </row>
     <row r="57" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C57" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D57" t="s">
         <v>67</v>
@@ -4041,7 +4090,7 @@
     </row>
     <row r="58" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C58" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D58" t="s">
         <v>128</v>
@@ -4049,7 +4098,7 @@
     </row>
     <row r="59" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C59" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D59" t="s">
         <v>127</v>
@@ -4057,7 +4106,7 @@
     </row>
     <row r="60" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C60" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D60" t="s">
         <v>129</v>
@@ -4065,7 +4114,7 @@
     </row>
     <row r="61" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C61" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D61" t="s">
         <v>130</v>
@@ -4073,7 +4122,7 @@
     </row>
     <row r="62" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C62" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D62" t="s">
         <v>131</v>
@@ -4081,7 +4130,7 @@
     </row>
     <row r="63" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C63" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D63" t="s">
         <v>132</v>
@@ -4089,7 +4138,7 @@
     </row>
     <row r="64" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C64" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D64" t="s">
         <v>151</v>
@@ -4097,7 +4146,7 @@
     </row>
     <row r="65" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C65" s="10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D65" t="s">
         <v>68</v>
@@ -4105,7 +4154,7 @@
     </row>
     <row r="66" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C66" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D66" t="s">
         <v>133</v>
@@ -4113,7 +4162,7 @@
     </row>
     <row r="67" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C67" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D67" t="s">
         <v>134</v>
@@ -4121,7 +4170,7 @@
     </row>
     <row r="68" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C68" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D68" t="s">
         <v>152</v>
@@ -4129,7 +4178,7 @@
     </row>
     <row r="69" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C69" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D69" t="s">
         <v>69</v>
@@ -4137,7 +4186,7 @@
     </row>
     <row r="70" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C70" s="10" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D70" t="s">
         <v>70</v>
@@ -4145,7 +4194,7 @@
     </row>
     <row r="71" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C71" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D71" t="s">
         <v>191</v>
@@ -4153,7 +4202,7 @@
     </row>
     <row r="72" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C72" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D72" t="s">
         <v>183</v>
@@ -4161,7 +4210,7 @@
     </row>
     <row r="73" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C73" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D73" t="s">
         <v>192</v>
@@ -4169,7 +4218,7 @@
     </row>
     <row r="74" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C74" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D74" t="s">
         <v>184</v>
@@ -4177,7 +4226,7 @@
     </row>
     <row r="75" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C75" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D75" t="s">
         <v>189</v>
@@ -4185,7 +4234,7 @@
     </row>
     <row r="76" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C76" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D76" t="s">
         <v>181</v>
@@ -4193,7 +4242,7 @@
     </row>
     <row r="77" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C77" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D77" t="s">
         <v>209</v>
@@ -4201,7 +4250,7 @@
     </row>
     <row r="78" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C78" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D78" t="s">
         <v>188</v>
@@ -4209,7 +4258,7 @@
     </row>
     <row r="79" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C79" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D79" t="s">
         <v>180</v>
@@ -4217,7 +4266,7 @@
     </row>
     <row r="80" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C80" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D80" t="s">
         <v>193</v>
@@ -4225,7 +4274,7 @@
     </row>
     <row r="81" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C81" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D81" t="s">
         <v>185</v>
@@ -4233,7 +4282,7 @@
     </row>
     <row r="82" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C82" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D82" t="s">
         <v>71</v>
@@ -4241,7 +4290,7 @@
     </row>
     <row r="83" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C83" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D83" t="s">
         <v>72</v>
@@ -4249,7 +4298,7 @@
     </row>
     <row r="84" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C84" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D84" t="s">
         <v>196</v>
@@ -4257,7 +4306,7 @@
     </row>
     <row r="85" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C85" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D85" t="s">
         <v>194</v>
@@ -4265,7 +4314,7 @@
     </row>
     <row r="86" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C86" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D86" t="s">
         <v>73</v>
@@ -4273,7 +4322,7 @@
     </row>
     <row r="87" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C87" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D87" t="s">
         <v>74</v>
@@ -4281,7 +4330,7 @@
     </row>
     <row r="88" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C88" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D88" t="s">
         <v>190</v>
@@ -4289,7 +4338,7 @@
     </row>
     <row r="89" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C89" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D89" t="s">
         <v>182</v>
@@ -4297,7 +4346,7 @@
     </row>
     <row r="90" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C90" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D90" t="s">
         <v>75</v>
@@ -4305,7 +4354,7 @@
     </row>
     <row r="91" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C91" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D91" t="s">
         <v>76</v>
@@ -4313,7 +4362,7 @@
     </row>
     <row r="92" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C92" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D92" t="s">
         <v>77</v>
@@ -4321,7 +4370,7 @@
     </row>
     <row r="93" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C93" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D93" t="s">
         <v>78</v>
@@ -4329,7 +4378,7 @@
     </row>
     <row r="94" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C94" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D94" t="s">
         <v>79</v>
@@ -4337,7 +4386,7 @@
     </row>
     <row r="95" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C95" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D95" t="s">
         <v>80</v>
@@ -4345,7 +4394,7 @@
     </row>
     <row r="96" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C96" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D96" t="s">
         <v>187</v>
@@ -4353,7 +4402,7 @@
     </row>
     <row r="97" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C97" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D97" t="s">
         <v>179</v>
@@ -4361,7 +4410,7 @@
     </row>
     <row r="98" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C98" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D98" t="s">
         <v>186</v>
@@ -4369,7 +4418,7 @@
     </row>
     <row r="99" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C99" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D99" t="s">
         <v>178</v>
@@ -4377,243 +4426,263 @@
     </row>
     <row r="100" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C100" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D100" t="s">
-        <v>81</v>
+        <v>338</v>
       </c>
     </row>
     <row r="101" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C101" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D101" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="102" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C102" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D102" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="103" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C103" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D103" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="104" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C104" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D104" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="105" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C105" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D105" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="106" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C106" s="9" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D106" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="107" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D107" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="108" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D108" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="109" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D109" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="110" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D110" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="111" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D111" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="112" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D112" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="113" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D113" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="114" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D114" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="115" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D115" t="s">
-        <v>206</v>
+        <v>95</v>
       </c>
     </row>
     <row r="116" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D116" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="117" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D117" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
     </row>
     <row r="118" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D118" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="119" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D119" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="120" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D120" t="s">
-        <v>199</v>
+        <v>210</v>
       </c>
     </row>
     <row r="121" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D121" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="122" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D122" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="123" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D123" t="s">
-        <v>223</v>
+        <v>340</v>
       </c>
     </row>
     <row r="124" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D124" t="s">
-        <v>202</v>
+        <v>341</v>
       </c>
     </row>
     <row r="125" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D125" t="s">
-        <v>224</v>
+        <v>201</v>
       </c>
     </row>
     <row r="126" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D126" t="s">
-        <v>203</v>
+        <v>222</v>
       </c>
     </row>
     <row r="127" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D127" t="s">
-        <v>96</v>
+        <v>202</v>
       </c>
     </row>
     <row r="128" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D128" t="s">
-        <v>97</v>
+        <v>223</v>
       </c>
     </row>
     <row r="129" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D129" t="s">
-        <v>98</v>
+        <v>203</v>
       </c>
     </row>
     <row r="130" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D130" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="131" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D131" t="s">
-        <v>197</v>
+        <v>97</v>
       </c>
     </row>
     <row r="132" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D132" t="s">
-        <v>195</v>
+        <v>339</v>
       </c>
     </row>
     <row r="133" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D133" t="s">
-        <v>219</v>
+        <v>98</v>
       </c>
     </row>
     <row r="134" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D134" t="s">
-        <v>220</v>
+        <v>99</v>
       </c>
     </row>
     <row r="135" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D135" t="s">
-        <v>221</v>
+        <v>197</v>
       </c>
     </row>
     <row r="136" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D136" t="s">
-        <v>222</v>
+        <v>195</v>
       </c>
     </row>
     <row r="137" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D137" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
     </row>
     <row r="138" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D138" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="139" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D139" s="12" t="s">
-        <v>333</v>
+      <c r="D139" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="140" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D140" s="12" t="s">
-        <v>335</v>
+      <c r="D140" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="141" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D141" t="s">
-        <v>334</v>
+        <v>225</v>
       </c>
     </row>
     <row r="142" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D142" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="143" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D143" s="12" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="144" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D144" s="12" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="145" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D145" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="146" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D146" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="147" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D147" t="s">
         <v>336</v>
-      </c>
-    </row>
-    <row r="143" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D143" t="s">
-        <v>337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added few driver view tests from US1533 + Fixed failing sanity automation tests - CheckBrokenPages
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCases.xlsx
+++ b/selenium-wd/data/TestCases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="910" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="910" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases-CmpReports" sheetId="1" r:id="rId1"/>
@@ -204,7 +204,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1389" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1391" uniqueCount="405">
   <si>
     <t>ID</t>
   </si>
@@ -1413,6 +1413,12 @@
   </si>
   <si>
     <t>Click GIS - Turn ON All Assets &amp; Boundaries</t>
+  </si>
+  <si>
+    <t>turnOffAllDisplayOptions</t>
+  </si>
+  <si>
+    <t>turnOnAllDisplayOptions</t>
   </si>
 </sst>
 </file>
@@ -2385,7 +2391,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:H238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+    <sheetView topLeftCell="A102" workbookViewId="0">
       <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
@@ -6756,10 +6762,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:X160"/>
+  <dimension ref="A1:X162"/>
   <sheetViews>
-    <sheetView topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="D160" sqref="D160"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="D166" sqref="D166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7914,7 +7920,7 @@
         <v>202</v>
       </c>
       <c r="D40" s="17" t="s">
-        <v>132</v>
+        <v>403</v>
       </c>
     </row>
     <row r="41" spans="3:4" x14ac:dyDescent="0.3">
@@ -7922,7 +7928,7 @@
         <v>250</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="42" spans="3:4" x14ac:dyDescent="0.3">
@@ -7930,7 +7936,7 @@
         <v>251</v>
       </c>
       <c r="D42" s="17" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43" spans="3:4" x14ac:dyDescent="0.3">
@@ -7938,7 +7944,7 @@
         <v>226</v>
       </c>
       <c r="D43" s="17" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="44" spans="3:4" x14ac:dyDescent="0.3">
@@ -7946,7 +7952,7 @@
         <v>45</v>
       </c>
       <c r="D44" s="17" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="45" spans="3:4" x14ac:dyDescent="0.3">
@@ -7954,7 +7960,7 @@
         <v>46</v>
       </c>
       <c r="D45" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="46" spans="3:4" x14ac:dyDescent="0.3">
@@ -7962,7 +7968,7 @@
         <v>47</v>
       </c>
       <c r="D46" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="47" spans="3:4" x14ac:dyDescent="0.3">
@@ -7970,7 +7976,7 @@
         <v>48</v>
       </c>
       <c r="D47" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="48" spans="3:4" x14ac:dyDescent="0.3">
@@ -7978,7 +7984,7 @@
         <v>229</v>
       </c>
       <c r="D48" s="17" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.3">
@@ -7986,7 +7992,7 @@
         <v>237</v>
       </c>
       <c r="D49" s="17" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.3">
@@ -7994,7 +8000,7 @@
         <v>236</v>
       </c>
       <c r="D50" s="17" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="51" spans="3:4" x14ac:dyDescent="0.3">
@@ -8002,7 +8008,7 @@
         <v>238</v>
       </c>
       <c r="D51" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="52" spans="3:4" x14ac:dyDescent="0.3">
@@ -8010,7 +8016,7 @@
         <v>233</v>
       </c>
       <c r="D52" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="53" spans="3:4" x14ac:dyDescent="0.3">
@@ -8018,7 +8024,7 @@
         <v>249</v>
       </c>
       <c r="D53" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="54" spans="3:4" x14ac:dyDescent="0.3">
@@ -8026,7 +8032,7 @@
         <v>227</v>
       </c>
       <c r="D54" s="17" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
     </row>
     <row r="55" spans="3:4" x14ac:dyDescent="0.3">
@@ -8034,7 +8040,7 @@
         <v>247</v>
       </c>
       <c r="D55" s="17" t="s">
-        <v>345</v>
+        <v>156</v>
       </c>
     </row>
     <row r="56" spans="3:4" x14ac:dyDescent="0.3">
@@ -8042,7 +8048,7 @@
         <v>248</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>140</v>
+        <v>345</v>
       </c>
     </row>
     <row r="57" spans="3:4" x14ac:dyDescent="0.3">
@@ -8050,7 +8056,7 @@
         <v>252</v>
       </c>
       <c r="D57" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="58" spans="3:4" x14ac:dyDescent="0.3">
@@ -8058,7 +8064,7 @@
         <v>279</v>
       </c>
       <c r="D58" s="17" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
     </row>
     <row r="59" spans="3:4" x14ac:dyDescent="0.3">
@@ -8066,7 +8072,7 @@
         <v>295</v>
       </c>
       <c r="D59" s="17" t="s">
-        <v>395</v>
+        <v>157</v>
       </c>
     </row>
     <row r="60" spans="3:4" x14ac:dyDescent="0.3">
@@ -8074,7 +8080,7 @@
         <v>277</v>
       </c>
       <c r="D60" s="17" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="61" spans="3:4" x14ac:dyDescent="0.3">
@@ -8082,7 +8088,7 @@
         <v>278</v>
       </c>
       <c r="D61" s="17" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="62" spans="3:4" x14ac:dyDescent="0.3">
@@ -8090,7 +8096,7 @@
         <v>280</v>
       </c>
       <c r="D62" s="17" t="s">
-        <v>122</v>
+        <v>396</v>
       </c>
     </row>
     <row r="63" spans="3:4" x14ac:dyDescent="0.3">
@@ -8098,7 +8104,7 @@
         <v>281</v>
       </c>
       <c r="D63" s="17" t="s">
-        <v>123</v>
+        <v>404</v>
       </c>
     </row>
     <row r="64" spans="3:4" x14ac:dyDescent="0.3">
@@ -8106,7 +8112,7 @@
         <v>275</v>
       </c>
       <c r="D64" s="17" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
     </row>
     <row r="65" spans="3:4" x14ac:dyDescent="0.3">
@@ -8114,7 +8120,7 @@
         <v>306</v>
       </c>
       <c r="D65" s="17" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
     </row>
     <row r="66" spans="3:4" x14ac:dyDescent="0.3">
@@ -8122,7 +8128,7 @@
         <v>293</v>
       </c>
       <c r="D66" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="67" spans="3:4" x14ac:dyDescent="0.3">
@@ -8130,7 +8136,7 @@
         <v>285</v>
       </c>
       <c r="D67" s="17" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="68" spans="3:4" x14ac:dyDescent="0.3">
@@ -8138,7 +8144,7 @@
         <v>267</v>
       </c>
       <c r="D68" s="17" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="69" spans="3:4" x14ac:dyDescent="0.3">
@@ -8146,7 +8152,7 @@
         <v>256</v>
       </c>
       <c r="D69" s="17" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="70" spans="3:4" x14ac:dyDescent="0.3">
@@ -8154,7 +8160,7 @@
         <v>307</v>
       </c>
       <c r="D70" s="17" t="s">
-        <v>67</v>
+        <v>146</v>
       </c>
     </row>
     <row r="71" spans="3:4" x14ac:dyDescent="0.3">
@@ -8162,7 +8168,7 @@
         <v>264</v>
       </c>
       <c r="D71" s="17" t="s">
-        <v>125</v>
+        <v>147</v>
       </c>
     </row>
     <row r="72" spans="3:4" x14ac:dyDescent="0.3">
@@ -8170,7 +8176,7 @@
         <v>253</v>
       </c>
       <c r="D72" s="17" t="s">
-        <v>124</v>
+        <v>67</v>
       </c>
     </row>
     <row r="73" spans="3:4" x14ac:dyDescent="0.3">
@@ -8178,7 +8184,7 @@
         <v>283</v>
       </c>
       <c r="D73" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="74" spans="3:4" x14ac:dyDescent="0.3">
@@ -8186,7 +8192,7 @@
         <v>303</v>
       </c>
       <c r="D74" s="17" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="75" spans="3:4" x14ac:dyDescent="0.3">
@@ -8194,7 +8200,7 @@
         <v>265</v>
       </c>
       <c r="D75" s="17" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="76" spans="3:4" x14ac:dyDescent="0.3">
@@ -8202,7 +8208,7 @@
         <v>254</v>
       </c>
       <c r="D76" s="17" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="77" spans="3:4" x14ac:dyDescent="0.3">
@@ -8210,7 +8216,7 @@
         <v>286</v>
       </c>
       <c r="D77" s="17" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
     </row>
     <row r="78" spans="3:4" x14ac:dyDescent="0.3">
@@ -8218,7 +8224,7 @@
         <v>287</v>
       </c>
       <c r="D78" s="17" t="s">
-        <v>344</v>
+        <v>129</v>
       </c>
     </row>
     <row r="79" spans="3:4" x14ac:dyDescent="0.3">
@@ -8226,7 +8232,7 @@
         <v>294</v>
       </c>
       <c r="D79" s="17" t="s">
-        <v>68</v>
+        <v>148</v>
       </c>
     </row>
     <row r="80" spans="3:4" x14ac:dyDescent="0.3">
@@ -8234,7 +8240,7 @@
         <v>282</v>
       </c>
       <c r="D80" s="17" t="s">
-        <v>130</v>
+        <v>344</v>
       </c>
     </row>
     <row r="81" spans="3:4" x14ac:dyDescent="0.3">
@@ -8242,7 +8248,7 @@
         <v>276</v>
       </c>
       <c r="D81" s="17" t="s">
-        <v>131</v>
+        <v>68</v>
       </c>
     </row>
     <row r="82" spans="3:4" x14ac:dyDescent="0.3">
@@ -8250,7 +8256,7 @@
         <v>291</v>
       </c>
       <c r="D82" s="17" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
     </row>
     <row r="83" spans="3:4" x14ac:dyDescent="0.3">
@@ -8258,7 +8264,7 @@
         <v>289</v>
       </c>
       <c r="D83" s="17" t="s">
-        <v>69</v>
+        <v>131</v>
       </c>
     </row>
     <row r="84" spans="3:4" x14ac:dyDescent="0.3">
@@ -8266,7 +8272,7 @@
         <v>290</v>
       </c>
       <c r="D84" s="17" t="s">
-        <v>70</v>
+        <v>149</v>
       </c>
     </row>
     <row r="85" spans="3:4" x14ac:dyDescent="0.3">
@@ -8274,7 +8280,7 @@
         <v>288</v>
       </c>
       <c r="D85" s="17" t="s">
-        <v>178</v>
+        <v>69</v>
       </c>
     </row>
     <row r="86" spans="3:4" x14ac:dyDescent="0.3">
@@ -8282,7 +8288,7 @@
         <v>292</v>
       </c>
       <c r="D86" s="17" t="s">
-        <v>170</v>
+        <v>70</v>
       </c>
     </row>
     <row r="87" spans="3:4" x14ac:dyDescent="0.3">
@@ -8290,7 +8296,7 @@
         <v>284</v>
       </c>
       <c r="D87" s="17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="88" spans="3:4" x14ac:dyDescent="0.3">
@@ -8298,7 +8304,7 @@
         <v>266</v>
       </c>
       <c r="D88" s="17" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="89" spans="3:4" x14ac:dyDescent="0.3">
@@ -8306,7 +8312,7 @@
         <v>255</v>
       </c>
       <c r="D89" s="17" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="90" spans="3:4" x14ac:dyDescent="0.3">
@@ -8314,7 +8320,7 @@
         <v>268</v>
       </c>
       <c r="D90" s="17" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="91" spans="3:4" x14ac:dyDescent="0.3">
@@ -8322,7 +8328,7 @@
         <v>257</v>
       </c>
       <c r="D91" s="17" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
     </row>
     <row r="92" spans="3:4" x14ac:dyDescent="0.3">
@@ -8330,7 +8336,7 @@
         <v>269</v>
       </c>
       <c r="D92" s="17" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="93" spans="3:4" x14ac:dyDescent="0.3">
@@ -8338,7 +8344,7 @@
         <v>258</v>
       </c>
       <c r="D93" s="17" t="s">
-        <v>167</v>
+        <v>194</v>
       </c>
     </row>
     <row r="94" spans="3:4" x14ac:dyDescent="0.3">
@@ -8346,7 +8352,7 @@
         <v>270</v>
       </c>
       <c r="D94" s="17" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="95" spans="3:4" x14ac:dyDescent="0.3">
@@ -8354,7 +8360,7 @@
         <v>259</v>
       </c>
       <c r="D95" s="17" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="96" spans="3:4" x14ac:dyDescent="0.3">
@@ -8362,7 +8368,7 @@
         <v>271</v>
       </c>
       <c r="D96" s="17" t="s">
-        <v>71</v>
+        <v>180</v>
       </c>
     </row>
     <row r="97" spans="3:4" x14ac:dyDescent="0.3">
@@ -8370,7 +8376,7 @@
         <v>260</v>
       </c>
       <c r="D97" s="17" t="s">
-        <v>72</v>
+        <v>172</v>
       </c>
     </row>
     <row r="98" spans="3:4" x14ac:dyDescent="0.3">
@@ -8378,7 +8384,7 @@
         <v>272</v>
       </c>
       <c r="D98" s="17" t="s">
-        <v>183</v>
+        <v>71</v>
       </c>
     </row>
     <row r="99" spans="3:4" x14ac:dyDescent="0.3">
@@ -8386,7 +8392,7 @@
         <v>261</v>
       </c>
       <c r="D99" s="17" t="s">
-        <v>181</v>
+        <v>72</v>
       </c>
     </row>
     <row r="100" spans="3:4" x14ac:dyDescent="0.3">
@@ -8394,7 +8400,7 @@
         <v>273</v>
       </c>
       <c r="D100" s="17" t="s">
-        <v>73</v>
+        <v>183</v>
       </c>
     </row>
     <row r="101" spans="3:4" x14ac:dyDescent="0.3">
@@ -8402,7 +8408,7 @@
         <v>262</v>
       </c>
       <c r="D101" s="17" t="s">
-        <v>74</v>
+        <v>181</v>
       </c>
     </row>
     <row r="102" spans="3:4" x14ac:dyDescent="0.3">
@@ -8410,7 +8416,7 @@
         <v>274</v>
       </c>
       <c r="D102" s="17" t="s">
-        <v>177</v>
+        <v>73</v>
       </c>
     </row>
     <row r="103" spans="3:4" x14ac:dyDescent="0.3">
@@ -8418,7 +8424,7 @@
         <v>263</v>
       </c>
       <c r="D103" s="17" t="s">
-        <v>169</v>
+        <v>74</v>
       </c>
     </row>
     <row r="104" spans="3:4" x14ac:dyDescent="0.3">
@@ -8426,7 +8432,7 @@
         <v>314</v>
       </c>
       <c r="D104" s="17" t="s">
-        <v>75</v>
+        <v>177</v>
       </c>
     </row>
     <row r="105" spans="3:4" x14ac:dyDescent="0.3">
@@ -8434,7 +8440,7 @@
         <v>315</v>
       </c>
       <c r="D105" s="17" t="s">
-        <v>76</v>
+        <v>169</v>
       </c>
     </row>
     <row r="106" spans="3:4" x14ac:dyDescent="0.3">
@@ -8442,282 +8448,292 @@
         <v>316</v>
       </c>
       <c r="D106" s="17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="107" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D107" s="17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="108" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D108" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="109" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D109" s="17" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="110" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D110" s="17" t="s">
-        <v>174</v>
+        <v>79</v>
       </c>
     </row>
     <row r="111" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D111" s="17" t="s">
-        <v>166</v>
+        <v>80</v>
       </c>
     </row>
     <row r="112" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D112" s="17" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="113" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D113" s="17" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="114" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D114" s="17" t="s">
-        <v>204</v>
+        <v>173</v>
       </c>
     </row>
     <row r="115" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D115" s="17" t="s">
-        <v>203</v>
+        <v>165</v>
       </c>
     </row>
     <row r="116" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D116" s="17" t="s">
-        <v>390</v>
+        <v>204</v>
       </c>
     </row>
     <row r="117" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D117" s="17" t="s">
-        <v>323</v>
+        <v>203</v>
       </c>
     </row>
     <row r="118" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D118" s="17" t="s">
-        <v>81</v>
+        <v>390</v>
       </c>
     </row>
     <row r="119" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D119" s="17" t="s">
-        <v>82</v>
+        <v>323</v>
       </c>
     </row>
     <row r="120" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D120" s="17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="121" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D121" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="122" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D122" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="123" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D123" s="17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="124" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D124" s="17" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="125" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D125" s="17" t="s">
-        <v>391</v>
+        <v>86</v>
       </c>
     </row>
     <row r="126" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D126" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="127" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D127" s="17" t="s">
-        <v>89</v>
+        <v>391</v>
       </c>
     </row>
     <row r="128" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D128" s="17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="129" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D129" s="17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="130" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D130" s="17" t="s">
-        <v>321</v>
+        <v>90</v>
       </c>
     </row>
     <row r="131" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D131" s="17" t="s">
-        <v>320</v>
+        <v>91</v>
       </c>
     </row>
     <row r="132" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D132" s="17" t="s">
-        <v>92</v>
+        <v>321</v>
       </c>
     </row>
     <row r="133" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D133" s="17" t="s">
-        <v>93</v>
+        <v>320</v>
       </c>
     </row>
     <row r="134" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D134" s="17" t="s">
-        <v>209</v>
+        <v>92</v>
       </c>
     </row>
     <row r="135" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D135" s="17" t="s">
-        <v>205</v>
+        <v>93</v>
       </c>
     </row>
     <row r="136" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D136" s="17" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="137" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D137" s="17" t="s">
-        <v>94</v>
+        <v>205</v>
       </c>
     </row>
     <row r="138" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D138" s="17" t="s">
-        <v>95</v>
+        <v>206</v>
       </c>
     </row>
     <row r="139" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D139" s="17" t="s">
-        <v>193</v>
+        <v>94</v>
       </c>
     </row>
     <row r="140" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D140" s="17" t="s">
-        <v>192</v>
+        <v>95</v>
       </c>
     </row>
     <row r="141" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D141" s="17" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
     </row>
     <row r="142" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D142" s="17" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="143" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D143" s="17" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
     </row>
     <row r="144" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D144" s="17" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
     </row>
     <row r="145" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D145" s="17" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
     </row>
     <row r="146" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D146" s="17" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="147" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D147" s="17" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
     </row>
     <row r="148" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D148" s="17" t="s">
-        <v>325</v>
+        <v>188</v>
       </c>
     </row>
     <row r="149" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D149" s="17" t="s">
-        <v>326</v>
+        <v>207</v>
       </c>
     </row>
     <row r="150" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D150" s="17" t="s">
-        <v>189</v>
+        <v>325</v>
       </c>
     </row>
     <row r="151" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D151" s="17" t="s">
-        <v>208</v>
+        <v>326</v>
       </c>
     </row>
     <row r="152" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D152" s="17" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="153" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D153" s="17" t="s">
-        <v>319</v>
+        <v>208</v>
       </c>
     </row>
     <row r="154" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D154" s="17" t="s">
-        <v>96</v>
+        <v>190</v>
       </c>
     </row>
     <row r="155" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D155" s="17" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
     </row>
     <row r="156" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D156" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="157" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D157" s="17" t="s">
-        <v>98</v>
+        <v>324</v>
       </c>
     </row>
     <row r="158" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D158" s="17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="159" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D159" s="17" t="s">
-        <v>184</v>
+        <v>98</v>
       </c>
     </row>
     <row r="160" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D160" s="17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="161" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D161" s="17" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="162" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D162" s="17" t="s">
         <v>182</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="D2:D160">
-    <sortCondition ref="D160"/>
+  <sortState ref="D2:D162">
+    <sortCondition ref="D162"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed code review comments
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCases.xlsx
+++ b/selenium-wd/data/TestCases.xlsx
@@ -204,7 +204,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1392" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1393" uniqueCount="407">
   <si>
     <t>ID</t>
   </si>
@@ -1422,6 +1422,9 @@
   </si>
   <si>
     <t>refreshPage</t>
+  </si>
+  <si>
+    <t>verifyDriverViewPageIsOpened</t>
   </si>
 </sst>
 </file>
@@ -6765,10 +6768,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:X163"/>
+  <dimension ref="A1:X164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="D163" sqref="D2:D163"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="D164" sqref="D164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8739,6 +8742,11 @@
         <v>182</v>
       </c>
     </row>
+    <row r="164" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D164" s="17" t="s">
+        <v>406</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="D2:D163">
     <sortCondition ref="D163"/>

</xml_diff>

<commit_message>
Adding Test cases xlsx
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCases.xlsx
+++ b/selenium-wd/data/TestCases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9396" tabRatio="910" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9396" tabRatio="910" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases-CmpReports" sheetId="1" r:id="rId1"/>
@@ -2481,8 +2481,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2545,8 +2545,8 @@
       <c r="D3" s="13">
         <v>3</v>
       </c>
-      <c r="E3" s="13" t="b">
-        <v>0</v>
+      <c r="E3" s="26" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -2563,7 +2563,7 @@
         <v>4</v>
       </c>
       <c r="E4" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -2580,7 +2580,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -2597,7 +2597,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -2614,7 +2614,7 @@
         <v>8</v>
       </c>
       <c r="E7" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -2631,7 +2631,7 @@
         <v>8</v>
       </c>
       <c r="E8" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -2648,7 +2648,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -2665,7 +2665,7 @@
         <v>8</v>
       </c>
       <c r="E10" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -2682,7 +2682,7 @@
         <v>8</v>
       </c>
       <c r="E11" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -2699,7 +2699,7 @@
         <v>8</v>
       </c>
       <c r="E12" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -2716,7 +2716,7 @@
         <v>8</v>
       </c>
       <c r="E13" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -2733,7 +2733,7 @@
         <v>8</v>
       </c>
       <c r="E14" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -2750,7 +2750,7 @@
         <v>8</v>
       </c>
       <c r="E15" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2765,7 +2765,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:H614"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Test cases for Picarro admin - Set-I + Lat/Long boundary selection control
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCases.xlsx
+++ b/selenium-wd/data/TestCases.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\surveyor-qa\selenium-wd\data\"/>
     </mc:Choice>
@@ -46,7 +46,7 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -204,7 +204,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2609" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2614" uniqueCount="481">
   <si>
     <t>ID</t>
   </si>
@@ -1644,12 +1644,16 @@
   </si>
   <si>
     <t>Zoom Level: 17</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2081,12 +2085,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="46.21875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.77734375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.21875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="28" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="2.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="46.21875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="23.77734375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="21.21875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="28.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -2194,14 +2198,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="59.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.77734375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.77734375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.44140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.44140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="20.21875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="2.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="59.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.77734375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.77734375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.44140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="20.21875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -2487,12 +2491,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.5546875" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="68" style="13" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.33203125" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="6.21875" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="26.6640625" style="13" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="21" width="2.77734375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="13" width="15.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="13" width="68.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="13" width="9.33203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="13" width="6.21875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="13" width="26.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -2531,6 +2535,9 @@
       <c r="E2" s="26" t="b">
         <v>1</v>
       </c>
+      <c r="F2" t="s">
+        <v>480</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A3" s="22">
@@ -2548,6 +2555,9 @@
       <c r="E3" s="26" t="b">
         <v>1</v>
       </c>
+      <c r="F3" t="s">
+        <v>480</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="22">
@@ -2565,6 +2575,9 @@
       <c r="E4" s="26" t="b">
         <v>1</v>
       </c>
+      <c r="F4" t="s">
+        <v>480</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="22">
@@ -2582,6 +2595,9 @@
       <c r="E5" s="26" t="b">
         <v>1</v>
       </c>
+      <c r="F5" t="s">
+        <v>480</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="22">
@@ -2598,6 +2614,9 @@
       </c>
       <c r="E6" s="26" t="b">
         <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -2771,14 +2790,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="38.77734375" style="12" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.44140625" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="38.33203125" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.77734375" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.77734375" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.5546875" style="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18.77734375" style="13" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="11" width="2.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="12" width="38.77734375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="13" width="12.44140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="13" width="38.33203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="13" width="11.77734375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="13" width="8.77734375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="14" width="15.5546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="13" width="18.77734375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -14111,7 +14130,7 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -14136,15 +14155,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.21875" style="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.44140625" style="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="49.88671875" style="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="45.21875" style="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="14" width="22.44140625" style="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="25.21875" style="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="21" width="22.44140625" style="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="24.21875" style="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="24" width="22.44140625" style="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="17" width="25.21875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="17" width="22.44140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="17" width="49.88671875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="17" width="45.21875" collapsed="true"/>
+    <col min="5" max="14" bestFit="true" customWidth="true" style="17" width="22.44140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="17" width="25.21875" collapsed="true"/>
+    <col min="16" max="21" bestFit="true" customWidth="true" style="17" width="22.44140625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="17" width="24.21875" collapsed="true"/>
+    <col min="23" max="24" bestFit="true" customWidth="true" style="17" width="22.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Made fixes to DriverView tests
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCases.xlsx
+++ b/selenium-wd/data/TestCases.xlsx
@@ -204,7 +204,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2737" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2715" uniqueCount="481">
   <si>
     <t>ID</t>
   </si>
@@ -1643,26 +1643,17 @@
     <t>Start Analyzer</t>
   </si>
   <si>
-    <t>FAIL</t>
-  </si>
-  <si>
-    <t>PASS</t>
-  </si>
-  <si>
     <t>CHECK DISABLED: DE1484</t>
   </si>
   <si>
     <t>Run the survey for 20 seconds</t>
-  </si>
-  <si>
-    <t>When adding field notes &amp; VerifyLISAIsShownOnMap</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1724,13 +1715,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1744,17 +1728,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1771,12 +1750,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1837,15 +1815,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2531,10 +2506,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2581,11 +2556,10 @@
         <v>3</v>
       </c>
       <c r="E2" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" s="31" t="s">
-        <v>480</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
     </row>
     <row r="3" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A3" s="22">
@@ -2601,11 +2575,9 @@
         <v>3</v>
       </c>
       <c r="E3" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" s="31" t="s">
-        <v>480</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F3" s="26"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="22">
@@ -2623,12 +2595,7 @@
       <c r="E4" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="F4" s="32" t="s">
-        <v>479</v>
-      </c>
-      <c r="G4" t="s">
-        <v>171</v>
-      </c>
+      <c r="F4" s="26"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="22">
@@ -2644,14 +2611,10 @@
         <v>7</v>
       </c>
       <c r="E5" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" s="32" t="s">
-        <v>479</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>171</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F5" s="26"/>
+      <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="22">
@@ -2667,14 +2630,10 @@
         <v>7</v>
       </c>
       <c r="E6" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F6" s="32" t="s">
-        <v>479</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>171</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F6" s="26"/>
+      <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="22">
@@ -2690,14 +2649,10 @@
         <v>8</v>
       </c>
       <c r="E7" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F7" s="32" t="s">
-        <v>479</v>
-      </c>
-      <c r="G7" t="s">
-        <v>166</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F7" s="26"/>
+      <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="24">
@@ -2713,14 +2668,9 @@
         <v>8</v>
       </c>
       <c r="E8" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F8" s="32" t="s">
-        <v>479</v>
-      </c>
-      <c r="G8" t="s">
-        <v>166</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F8" s="26"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="24">
@@ -2736,11 +2686,9 @@
         <v>8</v>
       </c>
       <c r="E9" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F9" s="31" t="s">
-        <v>480</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F9" s="26"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="24">
@@ -2756,11 +2704,9 @@
         <v>8</v>
       </c>
       <c r="E10" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F10" s="31" t="s">
-        <v>480</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F10" s="26"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="24">
@@ -2776,14 +2722,9 @@
         <v>8</v>
       </c>
       <c r="E11" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F11" s="32" t="s">
-        <v>479</v>
-      </c>
-      <c r="G11" t="s">
-        <v>171</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F11" s="26"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="24">
@@ -2799,14 +2740,10 @@
         <v>8</v>
       </c>
       <c r="E12" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F12" s="32" t="s">
-        <v>479</v>
-      </c>
-      <c r="G12" s="26" t="s">
-        <v>483</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="24">
@@ -2822,11 +2759,9 @@
         <v>8</v>
       </c>
       <c r="E13" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F13" s="31" t="s">
-        <v>480</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F13" s="26"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="24">
@@ -2842,14 +2777,9 @@
         <v>8</v>
       </c>
       <c r="E14" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F14" s="32" t="s">
-        <v>479</v>
-      </c>
-      <c r="G14" t="s">
-        <v>171</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F14" s="26"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="24">
@@ -2865,11 +2795,21 @@
         <v>8</v>
       </c>
       <c r="E15" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F15" s="31" t="s">
-        <v>480</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F15" s="26"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F16" s="26"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F17" s="26"/>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F18" s="26"/>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F19" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2883,8 +2823,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:H642"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="D166" sqref="D166"/>
+    <sheetView tabSelected="1" topLeftCell="A279" workbookViewId="0">
+      <selection activeCell="A308" sqref="A308"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2992,19 +2932,17 @@
         <v>1</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>200</v>
+        <v>460</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>327</v>
+        <v>10</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="E6" s="26"/>
       <c r="F6" s="26"/>
-      <c r="G6" s="27">
-        <v>3</v>
-      </c>
+      <c r="G6" s="27"/>
       <c r="H6" s="26"/>
     </row>
     <row r="7" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3012,17 +2950,19 @@
         <v>1</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>460</v>
+        <v>200</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>10</v>
+        <v>327</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="E7" s="26"/>
       <c r="F7" s="26"/>
-      <c r="G7" s="27"/>
+      <c r="G7" s="27">
+        <v>3</v>
+      </c>
       <c r="H7" s="26"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -3461,7 +3401,7 @@
         <v>1</v>
       </c>
       <c r="H35" s="30" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
@@ -3749,19 +3689,17 @@
         <v>2</v>
       </c>
       <c r="B52" s="25" t="s">
-        <v>200</v>
+        <v>460</v>
       </c>
       <c r="C52" s="26" t="s">
-        <v>327</v>
+        <v>10</v>
       </c>
       <c r="D52" s="26" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="E52" s="26"/>
       <c r="F52" s="26"/>
-      <c r="G52" s="27">
-        <v>3</v>
-      </c>
+      <c r="G52" s="27"/>
       <c r="H52" s="26"/>
     </row>
     <row r="53" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3769,17 +3707,19 @@
         <v>2</v>
       </c>
       <c r="B53" s="25" t="s">
-        <v>460</v>
+        <v>200</v>
       </c>
       <c r="C53" s="26" t="s">
-        <v>10</v>
+        <v>327</v>
       </c>
       <c r="D53" s="26" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="E53" s="26"/>
       <c r="F53" s="26"/>
-      <c r="G53" s="27"/>
+      <c r="G53" s="27">
+        <v>3</v>
+      </c>
       <c r="H53" s="26"/>
     </row>
     <row r="54" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -4238,7 +4178,7 @@
         <v>1</v>
       </c>
       <c r="H78" s="30" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="79" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -4628,19 +4568,17 @@
         <v>3</v>
       </c>
       <c r="B99" s="25" t="s">
-        <v>200</v>
+        <v>460</v>
       </c>
       <c r="C99" s="26" t="s">
-        <v>327</v>
+        <v>10</v>
       </c>
       <c r="D99" s="26" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="E99" s="26"/>
       <c r="F99" s="26"/>
-      <c r="G99" s="27">
-        <v>3</v>
-      </c>
+      <c r="G99" s="27"/>
       <c r="H99" s="26"/>
     </row>
     <row r="100" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -4648,17 +4586,19 @@
         <v>3</v>
       </c>
       <c r="B100" s="25" t="s">
-        <v>460</v>
+        <v>200</v>
       </c>
       <c r="C100" s="26" t="s">
-        <v>10</v>
+        <v>327</v>
       </c>
       <c r="D100" s="26" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="E100" s="26"/>
       <c r="F100" s="26"/>
-      <c r="G100" s="27"/>
+      <c r="G100" s="27">
+        <v>3</v>
+      </c>
       <c r="H100" s="26"/>
     </row>
     <row r="101" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -4740,7 +4680,7 @@
         <v>3</v>
       </c>
       <c r="B105" s="13" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C105" s="13" t="s">
         <v>327</v>
@@ -5062,7 +5002,7 @@
       </c>
       <c r="G122" s="14"/>
       <c r="H122" s="30" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="123" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -5416,19 +5356,17 @@
         <v>4</v>
       </c>
       <c r="B141" s="25" t="s">
-        <v>200</v>
+        <v>460</v>
       </c>
       <c r="C141" s="26" t="s">
-        <v>327</v>
+        <v>10</v>
       </c>
       <c r="D141" s="26" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="E141" s="26"/>
       <c r="F141" s="26"/>
-      <c r="G141" s="27">
-        <v>3</v>
-      </c>
+      <c r="G141" s="27"/>
       <c r="H141" s="26"/>
     </row>
     <row r="142" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -5436,17 +5374,19 @@
         <v>4</v>
       </c>
       <c r="B142" s="25" t="s">
-        <v>460</v>
+        <v>200</v>
       </c>
       <c r="C142" s="26" t="s">
-        <v>10</v>
+        <v>327</v>
       </c>
       <c r="D142" s="26" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="E142" s="26"/>
       <c r="F142" s="26"/>
-      <c r="G142" s="27"/>
+      <c r="G142" s="27">
+        <v>3</v>
+      </c>
       <c r="H142" s="26"/>
     </row>
     <row r="143" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -5528,7 +5468,7 @@
         <v>4</v>
       </c>
       <c r="B147" s="13" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C147" s="13" t="s">
         <v>327</v>
@@ -5850,7 +5790,7 @@
       </c>
       <c r="G164" s="14"/>
       <c r="H164" s="30" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="165" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -6204,19 +6144,17 @@
         <v>5</v>
       </c>
       <c r="B183" s="25" t="s">
-        <v>200</v>
+        <v>460</v>
       </c>
       <c r="C183" s="26" t="s">
-        <v>327</v>
+        <v>10</v>
       </c>
       <c r="D183" s="26" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="E183" s="26"/>
       <c r="F183" s="26"/>
-      <c r="G183" s="27">
-        <v>3</v>
-      </c>
+      <c r="G183" s="27"/>
       <c r="H183" s="26"/>
     </row>
     <row r="184" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -6224,17 +6162,19 @@
         <v>5</v>
       </c>
       <c r="B184" s="25" t="s">
-        <v>460</v>
+        <v>200</v>
       </c>
       <c r="C184" s="26" t="s">
-        <v>10</v>
+        <v>327</v>
       </c>
       <c r="D184" s="26" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="E184" s="26"/>
       <c r="F184" s="26"/>
-      <c r="G184" s="27"/>
+      <c r="G184" s="27">
+        <v>3</v>
+      </c>
       <c r="H184" s="26"/>
     </row>
     <row r="185" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -6316,7 +6256,7 @@
         <v>5</v>
       </c>
       <c r="B189" s="13" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C189" s="13" t="s">
         <v>327</v>
@@ -6638,7 +6578,7 @@
       </c>
       <c r="G206" s="14"/>
       <c r="H206" s="30" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="207" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -6992,19 +6932,17 @@
         <v>6</v>
       </c>
       <c r="B225" s="25" t="s">
-        <v>200</v>
+        <v>460</v>
       </c>
       <c r="C225" s="26" t="s">
-        <v>327</v>
+        <v>10</v>
       </c>
       <c r="D225" s="26" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="E225" s="26"/>
       <c r="F225" s="26"/>
-      <c r="G225" s="27">
-        <v>3</v>
-      </c>
+      <c r="G225" s="27"/>
       <c r="H225" s="26"/>
     </row>
     <row r="226" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -7012,17 +6950,19 @@
         <v>6</v>
       </c>
       <c r="B226" s="25" t="s">
-        <v>460</v>
+        <v>200</v>
       </c>
       <c r="C226" s="26" t="s">
-        <v>10</v>
+        <v>327</v>
       </c>
       <c r="D226" s="26" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="E226" s="26"/>
       <c r="F226" s="26"/>
-      <c r="G226" s="27"/>
+      <c r="G226" s="27">
+        <v>3</v>
+      </c>
       <c r="H226" s="26"/>
     </row>
     <row r="227" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -7104,7 +7044,7 @@
         <v>6</v>
       </c>
       <c r="B231" s="13" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C231" s="13" t="s">
         <v>327</v>
@@ -7426,7 +7366,7 @@
       </c>
       <c r="G248" s="14"/>
       <c r="H248" s="30" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="249" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -7780,19 +7720,17 @@
         <v>7</v>
       </c>
       <c r="B267" s="25" t="s">
-        <v>200</v>
+        <v>460</v>
       </c>
       <c r="C267" s="26" t="s">
-        <v>327</v>
+        <v>10</v>
       </c>
       <c r="D267" s="26" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="E267" s="26"/>
       <c r="F267" s="26"/>
-      <c r="G267" s="27">
-        <v>3</v>
-      </c>
+      <c r="G267" s="27"/>
       <c r="H267" s="26"/>
     </row>
     <row r="268" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -7800,17 +7738,19 @@
         <v>7</v>
       </c>
       <c r="B268" s="25" t="s">
-        <v>460</v>
+        <v>200</v>
       </c>
       <c r="C268" s="26" t="s">
-        <v>10</v>
+        <v>327</v>
       </c>
       <c r="D268" s="26" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="E268" s="26"/>
       <c r="F268" s="26"/>
-      <c r="G268" s="27"/>
+      <c r="G268" s="27">
+        <v>3</v>
+      </c>
       <c r="H268" s="26"/>
     </row>
     <row r="269" spans="1:8" x14ac:dyDescent="0.3">
@@ -7892,7 +7832,7 @@
         <v>7</v>
       </c>
       <c r="B273" s="26" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C273" s="26" t="s">
         <v>327</v>
@@ -8394,7 +8334,7 @@
       </c>
       <c r="G300" s="27"/>
       <c r="H300" s="30" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="301" spans="1:8" x14ac:dyDescent="0.3">
@@ -8768,19 +8708,17 @@
         <v>8</v>
       </c>
       <c r="B320" s="25" t="s">
-        <v>200</v>
+        <v>460</v>
       </c>
       <c r="C320" s="26" t="s">
-        <v>327</v>
+        <v>10</v>
       </c>
       <c r="D320" s="26" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="E320" s="26"/>
       <c r="F320" s="26"/>
-      <c r="G320" s="27">
-        <v>3</v>
-      </c>
+      <c r="G320" s="27"/>
       <c r="H320" s="26"/>
     </row>
     <row r="321" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -8788,17 +8726,19 @@
         <v>8</v>
       </c>
       <c r="B321" s="25" t="s">
-        <v>460</v>
+        <v>200</v>
       </c>
       <c r="C321" s="26" t="s">
-        <v>10</v>
+        <v>327</v>
       </c>
       <c r="D321" s="26" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="E321" s="26"/>
       <c r="F321" s="26"/>
-      <c r="G321" s="27"/>
+      <c r="G321" s="27">
+        <v>3</v>
+      </c>
       <c r="H321" s="26"/>
     </row>
     <row r="322" spans="1:8" x14ac:dyDescent="0.3">
@@ -8880,7 +8820,7 @@
         <v>8</v>
       </c>
       <c r="B326" s="26" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C326" s="26" t="s">
         <v>327</v>
@@ -9437,7 +9377,7 @@
       </c>
       <c r="G356" s="27"/>
       <c r="H356" s="30" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="357" spans="1:8" x14ac:dyDescent="0.3">
@@ -9831,19 +9771,17 @@
         <v>9</v>
       </c>
       <c r="B377" s="25" t="s">
-        <v>200</v>
+        <v>460</v>
       </c>
       <c r="C377" s="26" t="s">
-        <v>327</v>
+        <v>10</v>
       </c>
       <c r="D377" s="26" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="E377" s="26"/>
       <c r="F377" s="26"/>
-      <c r="G377" s="27">
-        <v>3</v>
-      </c>
+      <c r="G377" s="27"/>
       <c r="H377" s="26"/>
     </row>
     <row r="378" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -9851,17 +9789,19 @@
         <v>9</v>
       </c>
       <c r="B378" s="25" t="s">
-        <v>460</v>
+        <v>200</v>
       </c>
       <c r="C378" s="26" t="s">
-        <v>10</v>
+        <v>327</v>
       </c>
       <c r="D378" s="26" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="E378" s="26"/>
       <c r="F378" s="26"/>
-      <c r="G378" s="27"/>
+      <c r="G378" s="27">
+        <v>3</v>
+      </c>
       <c r="H378" s="26"/>
     </row>
     <row r="379" spans="1:8" x14ac:dyDescent="0.3">
@@ -9943,7 +9883,7 @@
         <v>9</v>
       </c>
       <c r="B383" s="26" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C383" s="26" t="s">
         <v>327</v>
@@ -10265,7 +10205,7 @@
       </c>
       <c r="G400" s="27"/>
       <c r="H400" s="30" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="401" spans="1:8" x14ac:dyDescent="0.3">
@@ -10637,19 +10577,17 @@
         <v>10</v>
       </c>
       <c r="B420" s="25" t="s">
-        <v>200</v>
+        <v>460</v>
       </c>
       <c r="C420" s="26" t="s">
-        <v>327</v>
+        <v>10</v>
       </c>
       <c r="D420" s="26" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="E420" s="26"/>
       <c r="F420" s="26"/>
-      <c r="G420" s="27">
-        <v>3</v>
-      </c>
+      <c r="G420" s="27"/>
       <c r="H420" s="26"/>
     </row>
     <row r="421" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -10657,17 +10595,19 @@
         <v>10</v>
       </c>
       <c r="B421" s="25" t="s">
-        <v>460</v>
+        <v>200</v>
       </c>
       <c r="C421" s="26" t="s">
-        <v>10</v>
+        <v>327</v>
       </c>
       <c r="D421" s="26" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="E421" s="26"/>
       <c r="F421" s="26"/>
-      <c r="G421" s="27"/>
+      <c r="G421" s="27">
+        <v>3</v>
+      </c>
       <c r="H421" s="26"/>
     </row>
     <row r="422" spans="1:8" x14ac:dyDescent="0.3">
@@ -10749,7 +10689,7 @@
         <v>10</v>
       </c>
       <c r="B426" s="26" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C426" s="26" t="s">
         <v>327</v>
@@ -11144,7 +11084,7 @@
       </c>
       <c r="G447" s="27"/>
       <c r="H447" s="30" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="448" spans="1:8" x14ac:dyDescent="0.3">
@@ -11518,19 +11458,17 @@
         <v>11</v>
       </c>
       <c r="B467" s="25" t="s">
-        <v>200</v>
+        <v>460</v>
       </c>
       <c r="C467" s="26" t="s">
-        <v>327</v>
+        <v>10</v>
       </c>
       <c r="D467" s="26" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="E467" s="26"/>
       <c r="F467" s="26"/>
-      <c r="G467" s="27">
-        <v>3</v>
-      </c>
+      <c r="G467" s="27"/>
       <c r="H467" s="26"/>
     </row>
     <row r="468" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -11538,17 +11476,19 @@
         <v>11</v>
       </c>
       <c r="B468" s="25" t="s">
-        <v>460</v>
+        <v>200</v>
       </c>
       <c r="C468" s="26" t="s">
-        <v>10</v>
+        <v>327</v>
       </c>
       <c r="D468" s="26" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="E468" s="26"/>
       <c r="F468" s="26"/>
-      <c r="G468" s="27"/>
+      <c r="G468" s="27">
+        <v>3</v>
+      </c>
       <c r="H468" s="26"/>
     </row>
     <row r="469" spans="1:8" x14ac:dyDescent="0.3">
@@ -11630,7 +11570,7 @@
         <v>11</v>
       </c>
       <c r="B473" s="26" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C473" s="26" t="s">
         <v>327</v>
@@ -12025,7 +11965,7 @@
       </c>
       <c r="G494" s="27"/>
       <c r="H494" s="30" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="495" spans="1:8" x14ac:dyDescent="0.3">
@@ -12399,19 +12339,17 @@
         <v>12</v>
       </c>
       <c r="B514" s="25" t="s">
-        <v>200</v>
+        <v>460</v>
       </c>
       <c r="C514" s="26" t="s">
-        <v>327</v>
+        <v>10</v>
       </c>
       <c r="D514" s="26" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="E514" s="26"/>
       <c r="F514" s="26"/>
-      <c r="G514" s="27">
-        <v>3</v>
-      </c>
+      <c r="G514" s="27"/>
       <c r="H514" s="26"/>
     </row>
     <row r="515" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -12419,17 +12357,19 @@
         <v>12</v>
       </c>
       <c r="B515" s="25" t="s">
-        <v>460</v>
+        <v>200</v>
       </c>
       <c r="C515" s="26" t="s">
-        <v>10</v>
+        <v>327</v>
       </c>
       <c r="D515" s="26" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="E515" s="26"/>
       <c r="F515" s="26"/>
-      <c r="G515" s="27"/>
+      <c r="G515" s="27">
+        <v>3</v>
+      </c>
       <c r="H515" s="26"/>
     </row>
     <row r="516" spans="1:8" x14ac:dyDescent="0.3">
@@ -12511,7 +12451,7 @@
         <v>12</v>
       </c>
       <c r="B520" s="26" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C520" s="26" t="s">
         <v>327</v>
@@ -12833,7 +12773,7 @@
       </c>
       <c r="G537" s="27"/>
       <c r="H537" s="30" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="538" spans="1:8" x14ac:dyDescent="0.3">
@@ -13205,19 +13145,17 @@
         <v>13</v>
       </c>
       <c r="B557" s="25" t="s">
-        <v>200</v>
+        <v>460</v>
       </c>
       <c r="C557" s="26" t="s">
-        <v>327</v>
+        <v>10</v>
       </c>
       <c r="D557" s="26" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="E557" s="26"/>
       <c r="F557" s="26"/>
-      <c r="G557" s="27">
-        <v>3</v>
-      </c>
+      <c r="G557" s="27"/>
       <c r="H557" s="26"/>
     </row>
     <row r="558" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -13225,17 +13163,19 @@
         <v>13</v>
       </c>
       <c r="B558" s="25" t="s">
-        <v>460</v>
+        <v>200</v>
       </c>
       <c r="C558" s="26" t="s">
-        <v>10</v>
+        <v>327</v>
       </c>
       <c r="D558" s="26" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="E558" s="26"/>
       <c r="F558" s="26"/>
-      <c r="G558" s="27"/>
+      <c r="G558" s="27">
+        <v>3</v>
+      </c>
       <c r="H558" s="26"/>
     </row>
     <row r="559" spans="1:8" x14ac:dyDescent="0.3">
@@ -13317,7 +13257,7 @@
         <v>13</v>
       </c>
       <c r="B563" s="26" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C563" s="26" t="s">
         <v>327</v>
@@ -13712,7 +13652,7 @@
       </c>
       <c r="G584" s="27"/>
       <c r="H584" s="30" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="585" spans="1:8" x14ac:dyDescent="0.3">
@@ -14086,19 +14026,17 @@
         <v>14</v>
       </c>
       <c r="B604" s="25" t="s">
-        <v>200</v>
+        <v>460</v>
       </c>
       <c r="C604" s="26" t="s">
-        <v>327</v>
+        <v>10</v>
       </c>
       <c r="D604" s="26" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="E604" s="26"/>
       <c r="F604" s="26"/>
-      <c r="G604" s="27">
-        <v>3</v>
-      </c>
+      <c r="G604" s="27"/>
       <c r="H604" s="26"/>
     </row>
     <row r="605" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -14106,17 +14044,19 @@
         <v>14</v>
       </c>
       <c r="B605" s="25" t="s">
-        <v>460</v>
+        <v>200</v>
       </c>
       <c r="C605" s="26" t="s">
-        <v>10</v>
+        <v>327</v>
       </c>
       <c r="D605" s="26" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="E605" s="26"/>
       <c r="F605" s="26"/>
-      <c r="G605" s="27"/>
+      <c r="G605" s="27">
+        <v>3</v>
+      </c>
       <c r="H605" s="26"/>
     </row>
     <row r="606" spans="1:8" x14ac:dyDescent="0.3">
@@ -14198,7 +14138,7 @@
         <v>14</v>
       </c>
       <c r="B610" s="26" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C610" s="26" t="s">
         <v>327</v>
@@ -14520,7 +14460,7 @@
       </c>
       <c r="G627" s="27"/>
       <c r="H627" s="30" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="628" spans="1:8" x14ac:dyDescent="0.3">
@@ -14813,10 +14753,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D608:D609 D271:D272 D324:D325 D381:D382 D424:D425 D471:D472 D518:D519 D561:D562 D557:D558 D267:D268 D320:D321 D377:D378 D420:D421 D467:D468 D514:D515 D604:D605 D2:D262 D327:D328 D427:D428 D474:D475 D564:D565">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D608:D609 D271:D272 D324:D325 D381:D382 D424:D425 D471:D472 D518:D519 D561:D562 D267:D268 D327:D328 D427:D428 D474:D475 D564:D565 D604:D605 D320:D321 D377:D378 D420:D421 D467:D468 D514:D515 D557:D558 D2:D223 D224:D262">
       <formula1>INDIRECT(C2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C4248">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C223 C224:C4248">
       <formula1>PageObject_Name</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Changes in Driver/Observer/Survey view page models and other classes to support test case actions
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCases.xlsx
+++ b/selenium-wd/data/TestCases.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\surveyor-qa\selenium-wd\data\"/>
     </mc:Choice>
@@ -46,7 +46,7 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -204,7 +204,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2715" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2717" uniqueCount="482">
   <si>
     <t>ID</t>
   </si>
@@ -1647,12 +1647,16 @@
   </si>
   <si>
     <t>Run the survey for 20 seconds</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2108,12 +2112,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="46.21875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.77734375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.21875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="28" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="2.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="46.21875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="23.77734375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="21.21875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="28.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -2221,14 +2225,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="59.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.77734375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.77734375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.44140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.44140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="20.21875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="2.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="59.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.77734375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.77734375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.44140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="20.21875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -2514,12 +2518,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.5546875" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="68" style="13" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.33203125" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="6.21875" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="26.6640625" style="13" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="21" width="2.77734375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="13" width="15.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="13" width="68.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="13" width="9.33203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="13" width="6.21875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="13" width="26.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -2558,7 +2562,9 @@
       <c r="E2" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="F2" s="26"/>
+      <c r="F2" t="s">
+        <v>481</v>
+      </c>
       <c r="G2" s="26"/>
     </row>
     <row r="3" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -2577,7 +2583,9 @@
       <c r="E3" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="F3" s="26"/>
+      <c r="F3" t="s">
+        <v>481</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="22">
@@ -2829,14 +2837,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="38.77734375" style="12" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.44140625" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="38.33203125" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.77734375" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.77734375" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.109375" style="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18.77734375" style="13" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="11" width="2.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="12" width="38.77734375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="13" width="12.44140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="13" width="38.33203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="13" width="11.77734375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="13" width="8.77734375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="14" width="18.109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="13" width="18.77734375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -14764,7 +14772,7 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -14789,15 +14797,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.21875" style="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.44140625" style="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="49.88671875" style="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="45.21875" style="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="14" width="22.44140625" style="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="25.21875" style="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="21" width="22.44140625" style="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="24.21875" style="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="24" width="22.44140625" style="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="17" width="25.21875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="17" width="22.44140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="17" width="49.88671875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="17" width="45.21875" collapsed="true"/>
+    <col min="5" max="14" bestFit="true" customWidth="true" style="17" width="22.44140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="17" width="25.21875" collapsed="true"/>
+    <col min="16" max="21" bestFit="true" customWidth="true" style="17" width="22.44140625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="17" width="24.21875" collapsed="true"/>
+    <col min="23" max="24" bestFit="true" customWidth="true" style="17" width="22.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Revised Test Cases for US1743
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCases.xlsx
+++ b/selenium-wd/data/TestCases.xlsx
@@ -204,7 +204,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5778" uniqueCount="622">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5784" uniqueCount="622">
   <si>
     <t>ID</t>
   </si>
@@ -3728,8 +3728,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:H1580"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1574" sqref="D1574"/>
+    <sheetView tabSelected="1" topLeftCell="A1556" workbookViewId="0">
+      <selection activeCell="F1557" sqref="F1557:F1564"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32756,7 +32756,9 @@
         <v>360</v>
       </c>
       <c r="E1557" s="26"/>
-      <c r="F1557" s="26"/>
+      <c r="F1557" s="26">
+        <v>1</v>
+      </c>
       <c r="G1557" s="27"/>
       <c r="H1557" s="31" t="s">
         <v>620</v>
@@ -32767,10 +32769,16 @@
       <c r="B1558" s="25" t="s">
         <v>608</v>
       </c>
-      <c r="C1558" s="26"/>
-      <c r="D1558" s="26"/>
+      <c r="C1558" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1558" s="26" t="s">
+        <v>360</v>
+      </c>
       <c r="E1558" s="26"/>
-      <c r="F1558" s="26"/>
+      <c r="F1558" s="26">
+        <v>1</v>
+      </c>
       <c r="G1558" s="27"/>
       <c r="H1558" s="31" t="s">
         <v>620</v>
@@ -32781,10 +32789,16 @@
       <c r="B1559" s="25" t="s">
         <v>609</v>
       </c>
-      <c r="C1559" s="26"/>
-      <c r="D1559" s="26"/>
+      <c r="C1559" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1559" s="26" t="s">
+        <v>360</v>
+      </c>
       <c r="E1559" s="26"/>
-      <c r="F1559" s="26"/>
+      <c r="F1559" s="26">
+        <v>1</v>
+      </c>
       <c r="G1559" s="27"/>
       <c r="H1559" s="31" t="s">
         <v>620</v>
@@ -32795,10 +32809,16 @@
       <c r="B1560" s="25" t="s">
         <v>610</v>
       </c>
-      <c r="C1560" s="26"/>
-      <c r="D1560" s="26"/>
+      <c r="C1560" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1560" s="26" t="s">
+        <v>360</v>
+      </c>
       <c r="E1560" s="26"/>
-      <c r="F1560" s="26"/>
+      <c r="F1560" s="26">
+        <v>1</v>
+      </c>
       <c r="G1560" s="27"/>
       <c r="H1560" s="31" t="s">
         <v>620</v>
@@ -32818,7 +32838,9 @@
         <v>360</v>
       </c>
       <c r="E1561" s="26"/>
-      <c r="F1561" s="26"/>
+      <c r="F1561" s="26">
+        <v>1</v>
+      </c>
       <c r="G1561" s="27"/>
       <c r="H1561" s="31" t="s">
         <v>620</v>
@@ -32838,7 +32860,9 @@
         <v>360</v>
       </c>
       <c r="E1562" s="26"/>
-      <c r="F1562" s="26"/>
+      <c r="F1562" s="26">
+        <v>1</v>
+      </c>
       <c r="G1562" s="27"/>
       <c r="H1562" s="31" t="s">
         <v>620</v>
@@ -32858,7 +32882,9 @@
         <v>360</v>
       </c>
       <c r="E1563" s="26"/>
-      <c r="F1563" s="26"/>
+      <c r="F1563" s="26">
+        <v>1</v>
+      </c>
       <c r="G1563" s="27"/>
       <c r="H1563" s="31" t="s">
         <v>620</v>
@@ -32878,7 +32904,9 @@
         <v>360</v>
       </c>
       <c r="E1564" s="26"/>
-      <c r="F1564" s="26"/>
+      <c r="F1564" s="26">
+        <v>1</v>
+      </c>
       <c r="G1564" s="27"/>
       <c r="H1564" s="31" t="s">
         <v>620</v>
@@ -33180,10 +33208,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D608:D609 D271:D272 D324:D325 D381:D382 D424:D425 D471:D472 D518:D519 D561:D562 D267:D268 D327:D328 D427:D428 D474:D475 D564:D565 D604:D605 D320:D321 D377:D378 D420:D421 D467:D468 D514:D515 D557:D558 D2:D262 D649:D650 D694:D695 D622:D623 D739:D740 D1002:D1039 D784:D785 D1229:D1262 D829:D830 D1047:D1084 D876:D877 D917:D918 D958:D959 D1044:D1045 D1089:D1090 D879:D912 D1134:D1135 D1179:D1180 D1352:D1385 D1226:D1227 D652:D689 D1267:D1268 D1308:D1309 D1349:D1350 D920:D953 D697:D734 D742:D779 D787:D824 D1270:D1303 D832:D871 D1092:D1129 D1137:D1174 D1182:D1221 D961:D994 D1390:D1391 D1311:D1344 D999:D1000 D1393:D1429 D1434:D1435 D1477:D1492 D1474:D1475 D1437:D1469 D1500:D1504 D1497:D1498 D1513:D1520 D1510:D1511 D1525:D1526 D1538:D1539 D1528:D1533 D1552:D1553 D1555:D1564 D1541:D1547 D1569:D1570 D1572 D1573:D1580">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D608:D609 D271:D272 D324:D325 D381:D382 D424:D425 D471:D472 D518:D519 D561:D562 D267:D268 D327:D328 D427:D428 D474:D475 D564:D565 D604:D605 D320:D321 D377:D378 D420:D421 D467:D468 D514:D515 D557:D558 D2:D262 D649:D650 D694:D695 D622:D623 D739:D740 D1002:D1039 D784:D785 D1229:D1262 D829:D830 D1047:D1084 D876:D877 D917:D918 D958:D959 D1044:D1045 D1089:D1090 D879:D912 D1134:D1135 D1179:D1180 D1352:D1385 D1226:D1227 D652:D689 D1267:D1268 D1308:D1309 D1349:D1350 D920:D953 D697:D734 D742:D779 D787:D824 D1270:D1303 D832:D871 D1092:D1129 D1137:D1174 D1182:D1221 D961:D994 D1390:D1391 D1311:D1344 D999:D1000 D1393:D1429 D1434:D1435 D1477:D1492 D1474:D1475 D1437:D1469 D1500:D1504 D1497:D1498 D1513:D1520 D1510:D1511 D1525:D1526 D1538:D1539 D1528:D1533 D1552:D1553 D1572:D1580 D1541:D1547 D1569:D1570 D1555:D1564">
       <formula1>INDIRECT(C2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1572 C1573:C4210">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C4210">
       <formula1>PageObject_Name</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Revised Again Test Cases for US1743
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCases.xlsx
+++ b/selenium-wd/data/TestCases.xlsx
@@ -2977,7 +2977,7 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3024,7 +3024,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" s="26"/>
       <c r="G2" s="26"/>
@@ -3043,7 +3043,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="26"/>
     </row>
@@ -3061,7 +3061,7 @@
         <v>4</v>
       </c>
       <c r="E4" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="26"/>
     </row>
@@ -3079,7 +3079,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="26"/>
       <c r="G5" s="6"/>
@@ -3098,7 +3098,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="26"/>
       <c r="G6" s="6"/>
@@ -3117,7 +3117,7 @@
         <v>8</v>
       </c>
       <c r="E7" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="26"/>
       <c r="G7" s="6"/>
@@ -3136,7 +3136,7 @@
         <v>8</v>
       </c>
       <c r="E8" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="26"/>
     </row>
@@ -3154,7 +3154,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="26"/>
     </row>
@@ -3172,7 +3172,7 @@
         <v>8</v>
       </c>
       <c r="E10" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="26"/>
     </row>
@@ -3190,7 +3190,7 @@
         <v>8</v>
       </c>
       <c r="E11" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="26"/>
     </row>
@@ -3208,7 +3208,7 @@
         <v>8</v>
       </c>
       <c r="E12" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="26"/>
       <c r="G12" s="26"/>
@@ -3227,7 +3227,7 @@
         <v>8</v>
       </c>
       <c r="E13" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="26"/>
     </row>
@@ -3245,7 +3245,7 @@
         <v>8</v>
       </c>
       <c r="E14" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="26"/>
     </row>
@@ -3263,7 +3263,7 @@
         <v>8</v>
       </c>
       <c r="E15" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="26"/>
     </row>
@@ -3281,7 +3281,7 @@
         <v>4</v>
       </c>
       <c r="E16" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="26"/>
     </row>
@@ -3299,7 +3299,7 @@
         <v>4</v>
       </c>
       <c r="E17" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="26"/>
     </row>
@@ -3317,7 +3317,7 @@
         <v>4</v>
       </c>
       <c r="E18" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" s="26"/>
     </row>
@@ -3335,7 +3335,7 @@
         <v>4</v>
       </c>
       <c r="E19" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" s="26"/>
     </row>
@@ -3353,7 +3353,7 @@
         <v>4</v>
       </c>
       <c r="E20" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -3370,7 +3370,7 @@
         <v>4</v>
       </c>
       <c r="E21" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -3387,7 +3387,7 @@
         <v>4</v>
       </c>
       <c r="E22" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -3404,7 +3404,7 @@
         <v>4</v>
       </c>
       <c r="E23" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -3421,7 +3421,7 @@
         <v>4</v>
       </c>
       <c r="E24" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -3438,7 +3438,7 @@
         <v>4</v>
       </c>
       <c r="E25" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -3455,7 +3455,7 @@
         <v>4</v>
       </c>
       <c r="E26" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -3472,7 +3472,7 @@
         <v>4</v>
       </c>
       <c r="E27" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -3489,7 +3489,7 @@
         <v>4</v>
       </c>
       <c r="E28" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -3506,7 +3506,7 @@
         <v>4</v>
       </c>
       <c r="E29" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -3523,7 +3523,7 @@
         <v>4</v>
       </c>
       <c r="E30" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -3540,7 +3540,7 @@
         <v>4</v>
       </c>
       <c r="E31" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -3557,7 +3557,7 @@
         <v>4</v>
       </c>
       <c r="E32" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -3574,7 +3574,7 @@
         <v>4</v>
       </c>
       <c r="E33" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -3590,7 +3590,7 @@
       <c r="D34" s="13">
         <v>4</v>
       </c>
-      <c r="E34" s="13" t="b">
+      <c r="E34" s="26" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3625,7 +3625,7 @@
         <v>4</v>
       </c>
       <c r="E36" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -3659,7 +3659,7 @@
         <v>4</v>
       </c>
       <c r="E38" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -3693,7 +3693,7 @@
         <v>4</v>
       </c>
       <c r="E40" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -3729,7 +3729,7 @@
   <dimension ref="A1:H1580"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1556" workbookViewId="0">
-      <selection activeCell="F1557" sqref="F1557:F1564"/>
+      <selection activeCell="B1572" sqref="B1572"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32765,7 +32765,9 @@
       </c>
     </row>
     <row r="1558" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
-      <c r="A1558" s="28"/>
+      <c r="A1558" s="28">
+        <v>39</v>
+      </c>
       <c r="B1558" s="25" t="s">
         <v>608</v>
       </c>
@@ -32785,7 +32787,9 @@
       </c>
     </row>
     <row r="1559" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1559" s="28"/>
+      <c r="A1559" s="28">
+        <v>39</v>
+      </c>
       <c r="B1559" s="25" t="s">
         <v>609</v>
       </c>
@@ -32805,7 +32809,9 @@
       </c>
     </row>
     <row r="1560" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1560" s="28"/>
+      <c r="A1560" s="28">
+        <v>39</v>
+      </c>
       <c r="B1560" s="25" t="s">
         <v>610</v>
       </c>

</xml_diff>

<commit_message>
Added new action methods to Excel page object methods
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCases.xlsx
+++ b/selenium-wd/data/TestCases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="910" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="910" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases-CmpReports" sheetId="1" r:id="rId1"/>
@@ -204,7 +204,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5298" uniqueCount="553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5832" uniqueCount="670">
   <si>
     <t>ID</t>
   </si>
@@ -1863,13 +1863,364 @@
   </si>
   <si>
     <t>verifySurveyInfoTimeRemainingLabelIsTickingBackward</t>
+  </si>
+  <si>
+    <t>TC1227</t>
+  </si>
+  <si>
+    <t>TC1230</t>
+  </si>
+  <si>
+    <t>TC1261</t>
+  </si>
+  <si>
+    <t>TC1269</t>
+  </si>
+  <si>
+    <t>TC1420</t>
+  </si>
+  <si>
+    <t>TC1421</t>
+  </si>
+  <si>
+    <t>TC1422</t>
+  </si>
+  <si>
+    <t>TC1428</t>
+  </si>
+  <si>
+    <t>Start Driving Survey - Curtain view</t>
+  </si>
+  <si>
+    <t>Verify restrictions on the maximum zoom level at which assets are displayed</t>
+  </si>
+  <si>
+    <t>Driver View - Returning from Curtain View should restore user selected map view combination</t>
+  </si>
+  <si>
+    <t>Navigate to Driver view when system is shutdown</t>
+  </si>
+  <si>
+    <t>Assessment mode - Satellite View - Driver view has only breadcrumb and FOV; no LISAs or indications</t>
+  </si>
+  <si>
+    <t>Assessment mode Satelite View - Reference Bottle Measurement and Isotopic Capture buttons not present</t>
+  </si>
+  <si>
+    <t>Assessment mode Satellite View - LISA, Indications, Isotopic Analysis, Field Notes not present in Display menu</t>
+  </si>
+  <si>
+    <t>Assessment mode - Map View - Driver view has only breadcrumb and FOV; no LISAs or indications</t>
+  </si>
+  <si>
+    <t>Click on Curtain View Button</t>
+  </si>
+  <si>
+    <t>Click on Curtain View Left Button</t>
+  </si>
+  <si>
+    <t>Click on Curtain View Right Button</t>
+  </si>
+  <si>
+    <t>Click on Curtain View Up Button</t>
+  </si>
+  <si>
+    <t>Click on Curtain View Down Button</t>
+  </si>
+  <si>
+    <t>Click on Curtain View Zoom Out Button</t>
+  </si>
+  <si>
+    <t>Click on Curtain View Zoom In Button</t>
+  </si>
+  <si>
+    <t>Click on Return Button</t>
+  </si>
+  <si>
+    <t>Turn Position Button OFF</t>
+  </si>
+  <si>
+    <t>Verify blue curtain appears</t>
+  </si>
+  <si>
+    <t>Verify map rotates clockwise</t>
+  </si>
+  <si>
+    <t>Verify map rotates counter-clockwise</t>
+  </si>
+  <si>
+    <t>Verify map foreground tilts up</t>
+  </si>
+  <si>
+    <t>Verify map foreground tilts down</t>
+  </si>
+  <si>
+    <t>Verify map zooms out</t>
+  </si>
+  <si>
+    <t>Verify map zooms in</t>
+  </si>
+  <si>
+    <t>Verify Position is turned OFF</t>
+  </si>
+  <si>
+    <t>Verify map moves to the right</t>
+  </si>
+  <si>
+    <t>Verify map moves to the left</t>
+  </si>
+  <si>
+    <t>Verify map moves down</t>
+  </si>
+  <si>
+    <t>Verify map moves up</t>
+  </si>
+  <si>
+    <t>Verify Assets displayed on Map</t>
+  </si>
+  <si>
+    <t>Wait for 5 seconds</t>
+  </si>
+  <si>
+    <t>Wait 2 seconds</t>
+  </si>
+  <si>
+    <t>Click on Curtain View Return Button</t>
+  </si>
+  <si>
+    <t>Click Stop Survey Button</t>
+  </si>
+  <si>
+    <t>Click Shutdown Button</t>
+  </si>
+  <si>
+    <t>Click Shutdown Confirmation Button</t>
+  </si>
+  <si>
+    <t>Verify Dashboard page</t>
+  </si>
+  <si>
+    <t>Wait 10 seconds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start Survey -&gt; Provide survey tag, select  Survey Time: Day Solar Radiation: Moderate Wind: Light Survey Type: Assessment </t>
+  </si>
+  <si>
+    <t>Start Survey -&gt; Provide survey tag, select  Survey Time: Day Solar Radiation: Moderate Wind: Light Survey Type: Assessment</t>
+  </si>
+  <si>
+    <t>Verify Indications NOT displayed on Map</t>
+  </si>
+  <si>
+    <t>Click on Mode Button</t>
+  </si>
+  <si>
+    <t>Verify Stop Survey button is present on menu</t>
+  </si>
+  <si>
+    <t>Verify Isotopic Capture button is NOT displayed on menu</t>
+  </si>
+  <si>
+    <t>Verify Reference Bottle Measurement button is NOT displayed on menu</t>
+  </si>
+  <si>
+    <t>Click on Display Button</t>
+  </si>
+  <si>
+    <t>Verify 8 Hour History option is present on menu</t>
+  </si>
+  <si>
+    <t>Verify Concentration Chart option is present on menu</t>
+  </si>
+  <si>
+    <t>Verify Windrose option is present on menu</t>
+  </si>
+  <si>
+    <t>Verify FOV option is present on menu</t>
+  </si>
+  <si>
+    <t>Verify LISA option is NOT displayed on menu</t>
+  </si>
+  <si>
+    <t>Verify Field Notes option is NOT displayed on menu</t>
+  </si>
+  <si>
+    <t>Verify Isotopic Analysis is NOT displayed on menu</t>
+  </si>
+  <si>
+    <t>Verify Indications option is NOT displayed on menu</t>
+  </si>
+  <si>
+    <t>US 2045 filed</t>
+  </si>
+  <si>
+    <t>US 2046 filed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on Mode Button </t>
+  </si>
+  <si>
+    <t>DE1636 filed</t>
+  </si>
+  <si>
+    <t>US2049 filed</t>
+  </si>
+  <si>
+    <t>US2025</t>
+  </si>
+  <si>
+    <t>DE1646 filed</t>
+  </si>
+  <si>
+    <t>verifyDisplaySwitch8HourHistoryButtonIsVisible</t>
+  </si>
+  <si>
+    <t>verifyDisplaySwitchWindroseButtonIsVisible</t>
+  </si>
+  <si>
+    <t>verifyDisplaySwitchConcentrationChartButtonIsVisible</t>
+  </si>
+  <si>
+    <t>verifyDisplaySwitchNotesButtonIsVisible</t>
+  </si>
+  <si>
+    <t>verifyDisplaySwitchIsotopicAnalysisButtonIsVisible</t>
+  </si>
+  <si>
+    <t>verifyDisplaySwitchIndicationsButtonIsVisible</t>
+  </si>
+  <si>
+    <t>verifyDisplaySwitchLisasButtonIsVisible</t>
+  </si>
+  <si>
+    <t>verifyDisplaySwitchFovsButtonIsVisible</t>
+  </si>
+  <si>
+    <t>verifyGisMaterialTypeCastIronButtonIsVisible</t>
+  </si>
+  <si>
+    <t>verifyGisMaterialTypeCopperButtonIsVisible</t>
+  </si>
+  <si>
+    <t>verifyGisMaterialTypeOtherPlasticButtonIsVisible</t>
+  </si>
+  <si>
+    <t>verifyGisMaterialTypePEPlasticButtonIsVisible</t>
+  </si>
+  <si>
+    <t>verifyGisMaterialTypeProtectedSteelButtonIsVisible</t>
+  </si>
+  <si>
+    <t>verifyGisMaterialTypeUnProtectedSteelButtonIsVisible</t>
+  </si>
+  <si>
+    <t>verifyGisUseAllPipesButtonIsVisible</t>
+  </si>
+  <si>
+    <t>verifyGisBoundaryBigBoundaryButtonIsVisible</t>
+  </si>
+  <si>
+    <t>verifyGisBoundarySmallBoundaryButtonIsVisible</t>
+  </si>
+  <si>
+    <t>verifyGisUseAllBoundariesButtonIsVisible</t>
+  </si>
+  <si>
+    <t>verifyStartSurveyButtonIsVisible</t>
+  </si>
+  <si>
+    <t>verifyStartEQSurveyButtonIsVisible</t>
+  </si>
+  <si>
+    <t>verifySystemShutdownButtonIsVisible</t>
+  </si>
+  <si>
+    <t>verifyStopDrivingSurveyButtonIsVisible</t>
+  </si>
+  <si>
+    <t>verifyStartIsotopicCaptureButtonIsVisible</t>
+  </si>
+  <si>
+    <t>verifyRefBottleMeasButtonIsVisible</t>
+  </si>
+  <si>
+    <t>verifyDisplaySwitch8HourHistoryButtonIsNotVisible</t>
+  </si>
+  <si>
+    <t>verifyDisplaySwitchWindroseButtonIsNotVisible</t>
+  </si>
+  <si>
+    <t>verifyDisplaySwitchConcentrationChartButtonIsNotVisible</t>
+  </si>
+  <si>
+    <t>verifyDisplaySwitchNotesButtonIsNotVisible</t>
+  </si>
+  <si>
+    <t>verifyDisplaySwitchIsotopicAnalysisButtonIsNotVisible</t>
+  </si>
+  <si>
+    <t>verifyDisplaySwitchIndicationsButtonIsNotVisible</t>
+  </si>
+  <si>
+    <t>verifyDisplaySwitchLisasButtonIsNotVisible</t>
+  </si>
+  <si>
+    <t>verifyDisplaySwitchFovsButtonIsNotVisible</t>
+  </si>
+  <si>
+    <t>verifyGisMaterialTypeCastIronButtonIsNotVisible</t>
+  </si>
+  <si>
+    <t>verifyGisMaterialTypeCopperButtonIsNotVisible</t>
+  </si>
+  <si>
+    <t>verifyGisMaterialTypeOtherPlasticButtonIsNotVisible</t>
+  </si>
+  <si>
+    <t>verifyGisMaterialTypePEPlasticButtonIsNotVisible</t>
+  </si>
+  <si>
+    <t>verifyGisMaterialTypeProtectedSteelButtonIsNotVisible</t>
+  </si>
+  <si>
+    <t>verifyGisMaterialTypeUnProtectedSteelButtonIsNotVisible</t>
+  </si>
+  <si>
+    <t>verifyGisUseAllPipesButtonIsNotVisible</t>
+  </si>
+  <si>
+    <t>verifyGisBoundaryBigBoundaryButtonIsNotVisible</t>
+  </si>
+  <si>
+    <t>verifyGisBoundarySmallBoundaryButtonIsNotVisible</t>
+  </si>
+  <si>
+    <t>verifyGisUseAllBoundariesButtonIsNotVisible</t>
+  </si>
+  <si>
+    <t>verifyStartSurveyButtonIsNotVisible</t>
+  </si>
+  <si>
+    <t>verifyStartEQSurveyButtonIsNotVisible</t>
+  </si>
+  <si>
+    <t>verifySystemShutdownButtonIsNotVisible</t>
+  </si>
+  <si>
+    <t>verifyStopDrivingSurveyButtonIsNotVisible</t>
+  </si>
+  <si>
+    <t>verifyStartIsotopicCaptureButtonIsNotVisible</t>
+  </si>
+  <si>
+    <t>verifyRefBottleMeasButtonIsNotVisible</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1943,8 +2294,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1962,6 +2319,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1976,7 +2339,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -2050,6 +2413,23 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -2738,10 +3118,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3341,6 +3721,145 @@
         <v>1</v>
       </c>
     </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="24">
+        <v>33</v>
+      </c>
+      <c r="B34" s="31" t="s">
+        <v>553</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>561</v>
+      </c>
+      <c r="D34" s="13">
+        <v>4</v>
+      </c>
+      <c r="E34" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="24">
+        <v>34</v>
+      </c>
+      <c r="B35" s="31" t="s">
+        <v>554</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>562</v>
+      </c>
+      <c r="D35" s="26">
+        <v>4</v>
+      </c>
+      <c r="E35" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="24">
+        <v>35</v>
+      </c>
+      <c r="B36" s="37" t="s">
+        <v>555</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>563</v>
+      </c>
+      <c r="D36" s="26">
+        <v>4</v>
+      </c>
+      <c r="E36" s="26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="24">
+        <v>36</v>
+      </c>
+      <c r="B37" s="31" t="s">
+        <v>556</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>564</v>
+      </c>
+      <c r="D37" s="26">
+        <v>4</v>
+      </c>
+      <c r="E37" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="24">
+        <v>37</v>
+      </c>
+      <c r="B38" s="37" t="s">
+        <v>557</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>565</v>
+      </c>
+      <c r="D38" s="26">
+        <v>4</v>
+      </c>
+      <c r="E38" s="26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="24">
+        <v>38</v>
+      </c>
+      <c r="B39" s="31" t="s">
+        <v>558</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>566</v>
+      </c>
+      <c r="D39" s="26">
+        <v>4</v>
+      </c>
+      <c r="E39" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="24">
+        <v>39</v>
+      </c>
+      <c r="B40" s="37" t="s">
+        <v>559</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>567</v>
+      </c>
+      <c r="D40" s="26">
+        <v>4</v>
+      </c>
+      <c r="E40" s="26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="24">
+        <v>40</v>
+      </c>
+      <c r="B41" s="37" t="s">
+        <v>560</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>568</v>
+      </c>
+      <c r="D41" s="26">
+        <v>4</v>
+      </c>
+      <c r="E41" s="26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="24"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3351,10 +3870,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:H1429"/>
+  <dimension ref="A1:H1580"/>
   <sheetViews>
-    <sheetView topLeftCell="A1402" workbookViewId="0">
-      <selection activeCell="E1424" sqref="E1424"/>
+    <sheetView topLeftCell="A1556" workbookViewId="0">
+      <selection activeCell="B1572" sqref="B1572"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30051,12 +30570,2798 @@
       <c r="G1429" s="27"/>
       <c r="H1429" s="26"/>
     </row>
+    <row r="1430" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1430" s="28">
+        <v>33</v>
+      </c>
+      <c r="B1430" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="C1430" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1430" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1430" s="26"/>
+      <c r="F1430" s="26"/>
+      <c r="G1430" s="27"/>
+      <c r="H1430" s="26"/>
+    </row>
+    <row r="1431" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1431" s="28">
+        <v>33</v>
+      </c>
+      <c r="B1431" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="C1431" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1431" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1431" s="26"/>
+      <c r="F1431" s="26"/>
+      <c r="G1431" s="27">
+        <v>4</v>
+      </c>
+      <c r="H1431" s="26"/>
+    </row>
+    <row r="1432" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1432" s="28">
+        <v>33</v>
+      </c>
+      <c r="B1432" s="25" t="s">
+        <v>478</v>
+      </c>
+      <c r="C1432" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1432" s="26" t="s">
+        <v>462</v>
+      </c>
+      <c r="E1432" s="26"/>
+      <c r="F1432" s="26"/>
+      <c r="G1432" s="27">
+        <v>3</v>
+      </c>
+      <c r="H1432" s="26"/>
+    </row>
+    <row r="1433" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1433" s="28">
+        <v>33</v>
+      </c>
+      <c r="B1433" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="C1433" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1433" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1433" s="26"/>
+      <c r="F1433" s="26"/>
+      <c r="G1433" s="27"/>
+      <c r="H1433" s="26"/>
+    </row>
+    <row r="1434" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1434" s="28">
+        <v>33</v>
+      </c>
+      <c r="B1434" s="25" t="s">
+        <v>460</v>
+      </c>
+      <c r="C1434" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1434" s="26" t="s">
+        <v>461</v>
+      </c>
+      <c r="E1434" s="26"/>
+      <c r="F1434" s="26"/>
+      <c r="G1434" s="27"/>
+      <c r="H1434" s="26"/>
+    </row>
+    <row r="1435" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1435" s="28">
+        <v>33</v>
+      </c>
+      <c r="B1435" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1435" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1435" s="26" t="s">
+        <v>459</v>
+      </c>
+      <c r="E1435" s="26"/>
+      <c r="F1435" s="26"/>
+      <c r="G1435" s="27">
+        <v>3</v>
+      </c>
+      <c r="H1435" s="26"/>
+    </row>
+    <row r="1436" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1436" s="28">
+        <v>33</v>
+      </c>
+      <c r="B1436" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1436" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1436" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1436" s="26"/>
+      <c r="F1436" s="26"/>
+      <c r="G1436" s="27"/>
+      <c r="H1436" s="26"/>
+    </row>
+    <row r="1437" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+      <c r="A1437" s="28">
+        <v>33</v>
+      </c>
+      <c r="B1437" s="25" t="s">
+        <v>367</v>
+      </c>
+      <c r="C1437" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1437" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1437" s="26"/>
+      <c r="F1437" s="26"/>
+      <c r="G1437" s="27">
+        <v>6</v>
+      </c>
+      <c r="H1437" s="26"/>
+    </row>
+    <row r="1438" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1438" s="38">
+        <v>33</v>
+      </c>
+      <c r="B1438" s="39" t="s">
+        <v>569</v>
+      </c>
+      <c r="C1438" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1438" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1438" s="29"/>
+      <c r="F1438" s="29"/>
+      <c r="G1438" s="40"/>
+      <c r="H1438" s="29"/>
+    </row>
+    <row r="1439" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1439" s="38">
+        <v>33</v>
+      </c>
+      <c r="B1439" s="39" t="s">
+        <v>578</v>
+      </c>
+      <c r="C1439" s="29" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1439" s="29" t="s">
+        <v>360</v>
+      </c>
+      <c r="E1439" s="29"/>
+      <c r="F1439" s="29">
+        <v>1</v>
+      </c>
+      <c r="G1439" s="40"/>
+      <c r="H1439" s="31" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="1440" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1440" s="28">
+        <v>33</v>
+      </c>
+      <c r="B1440" s="12" t="s">
+        <v>570</v>
+      </c>
+      <c r="C1440" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1440" s="29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1441" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1441" s="28">
+        <v>33</v>
+      </c>
+      <c r="B1441" s="25" t="s">
+        <v>579</v>
+      </c>
+      <c r="C1441" s="29" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1441" s="29" t="s">
+        <v>360</v>
+      </c>
+      <c r="E1441" s="26"/>
+      <c r="F1441" s="26">
+        <v>1</v>
+      </c>
+      <c r="G1441" s="27"/>
+      <c r="H1441" s="31" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="1442" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1442" s="28">
+        <v>33</v>
+      </c>
+      <c r="B1442" s="25" t="s">
+        <v>571</v>
+      </c>
+      <c r="C1442" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1442" s="29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="1443" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1443" s="28">
+        <v>33</v>
+      </c>
+      <c r="B1443" s="25" t="s">
+        <v>580</v>
+      </c>
+      <c r="C1443" s="29" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1443" s="29" t="s">
+        <v>360</v>
+      </c>
+      <c r="E1443" s="26"/>
+      <c r="F1443" s="26">
+        <v>1</v>
+      </c>
+      <c r="G1443" s="27"/>
+      <c r="H1443" s="31" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="1444" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1444" s="28">
+        <v>33</v>
+      </c>
+      <c r="B1444" s="25" t="s">
+        <v>572</v>
+      </c>
+      <c r="C1444" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1444" s="29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="1445" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1445" s="28">
+        <v>33</v>
+      </c>
+      <c r="B1445" s="25" t="s">
+        <v>581</v>
+      </c>
+      <c r="C1445" s="29" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1445" s="29" t="s">
+        <v>360</v>
+      </c>
+      <c r="E1445" s="26"/>
+      <c r="F1445" s="26">
+        <v>1</v>
+      </c>
+      <c r="G1445" s="27"/>
+      <c r="H1445" s="31" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="1446" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1446" s="28">
+        <v>33</v>
+      </c>
+      <c r="B1446" s="25" t="s">
+        <v>573</v>
+      </c>
+      <c r="C1446" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1446" s="29" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1447" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1447" s="28">
+        <v>33</v>
+      </c>
+      <c r="B1447" s="25" t="s">
+        <v>582</v>
+      </c>
+      <c r="C1447" s="29" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1447" s="29" t="s">
+        <v>360</v>
+      </c>
+      <c r="E1447" s="26"/>
+      <c r="F1447" s="26">
+        <v>1</v>
+      </c>
+      <c r="G1447" s="27"/>
+      <c r="H1447" s="31" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="1448" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1448" s="28">
+        <v>33</v>
+      </c>
+      <c r="B1448" s="12" t="s">
+        <v>574</v>
+      </c>
+      <c r="C1448" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1448" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="1449" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1449" s="28">
+        <v>33</v>
+      </c>
+      <c r="B1449" s="25" t="s">
+        <v>583</v>
+      </c>
+      <c r="C1449" s="29" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1449" s="29" t="s">
+        <v>360</v>
+      </c>
+      <c r="E1449" s="26"/>
+      <c r="F1449" s="26">
+        <v>1</v>
+      </c>
+      <c r="G1449" s="27"/>
+    </row>
+    <row r="1450" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1450" s="28">
+        <v>33</v>
+      </c>
+      <c r="B1450" s="25" t="s">
+        <v>575</v>
+      </c>
+      <c r="C1450" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1450" s="29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="1451" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1451" s="28">
+        <v>33</v>
+      </c>
+      <c r="B1451" s="25" t="s">
+        <v>584</v>
+      </c>
+      <c r="C1451" s="29" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1451" s="29" t="s">
+        <v>360</v>
+      </c>
+      <c r="E1451" s="26"/>
+      <c r="F1451" s="26">
+        <v>1</v>
+      </c>
+      <c r="G1451" s="27"/>
+      <c r="H1451" s="26"/>
+    </row>
+    <row r="1452" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1452" s="28">
+        <v>33</v>
+      </c>
+      <c r="B1452" s="12" t="s">
+        <v>576</v>
+      </c>
+      <c r="C1452" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1452" s="29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="1453" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1453" s="28">
+        <v>33</v>
+      </c>
+      <c r="B1453" s="25" t="s">
+        <v>577</v>
+      </c>
+      <c r="C1453" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1453" s="29" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="1454" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1454" s="28">
+        <v>33</v>
+      </c>
+      <c r="B1454" s="25" t="s">
+        <v>585</v>
+      </c>
+      <c r="C1454" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1454" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1454" s="26"/>
+      <c r="F1454" s="26"/>
+      <c r="G1454" s="27"/>
+      <c r="H1454" s="26"/>
+    </row>
+    <row r="1455" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1455" s="38">
+        <v>33</v>
+      </c>
+      <c r="B1455" s="39" t="s">
+        <v>569</v>
+      </c>
+      <c r="C1455" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1455" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1455" s="29"/>
+      <c r="F1455" s="29"/>
+      <c r="G1455" s="40"/>
+      <c r="H1455" s="29"/>
+    </row>
+    <row r="1456" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1456" s="38">
+        <v>33</v>
+      </c>
+      <c r="B1456" s="39" t="s">
+        <v>578</v>
+      </c>
+      <c r="C1456" s="29" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1456" s="29" t="s">
+        <v>360</v>
+      </c>
+      <c r="E1456" s="29"/>
+      <c r="F1456" s="29">
+        <v>1</v>
+      </c>
+      <c r="G1456" s="40"/>
+      <c r="H1456" s="29"/>
+    </row>
+    <row r="1457" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1457" s="28">
+        <v>33</v>
+      </c>
+      <c r="B1457" s="25" t="s">
+        <v>570</v>
+      </c>
+      <c r="C1457" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1457" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1457" s="26"/>
+      <c r="F1457" s="26"/>
+      <c r="G1457" s="27"/>
+      <c r="H1457" s="26"/>
+    </row>
+    <row r="1458" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1458" s="28">
+        <v>33</v>
+      </c>
+      <c r="B1458" s="25" t="s">
+        <v>586</v>
+      </c>
+      <c r="C1458" s="29" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1458" s="29" t="s">
+        <v>360</v>
+      </c>
+      <c r="E1458" s="26"/>
+      <c r="F1458" s="26">
+        <v>1</v>
+      </c>
+      <c r="G1458" s="27"/>
+      <c r="H1458" s="26"/>
+    </row>
+    <row r="1459" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1459" s="28">
+        <v>33</v>
+      </c>
+      <c r="B1459" s="25" t="s">
+        <v>571</v>
+      </c>
+      <c r="C1459" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1459" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1459" s="26"/>
+      <c r="F1459" s="26"/>
+      <c r="G1459" s="27"/>
+      <c r="H1459" s="26"/>
+    </row>
+    <row r="1460" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1460" s="28">
+        <v>33</v>
+      </c>
+      <c r="B1460" s="25" t="s">
+        <v>587</v>
+      </c>
+      <c r="C1460" s="29" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1460" s="29" t="s">
+        <v>360</v>
+      </c>
+      <c r="E1460" s="26"/>
+      <c r="F1460" s="26">
+        <v>1</v>
+      </c>
+      <c r="G1460" s="27"/>
+      <c r="H1460" s="26"/>
+    </row>
+    <row r="1461" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1461" s="28">
+        <v>33</v>
+      </c>
+      <c r="B1461" s="25" t="s">
+        <v>572</v>
+      </c>
+      <c r="C1461" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1461" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1461" s="26"/>
+      <c r="F1461" s="26"/>
+      <c r="G1461" s="27"/>
+      <c r="H1461" s="26"/>
+    </row>
+    <row r="1462" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1462" s="28">
+        <v>33</v>
+      </c>
+      <c r="B1462" s="25" t="s">
+        <v>588</v>
+      </c>
+      <c r="C1462" s="29" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1462" s="29" t="s">
+        <v>360</v>
+      </c>
+      <c r="E1462" s="26"/>
+      <c r="F1462" s="26">
+        <v>1</v>
+      </c>
+      <c r="G1462" s="27"/>
+      <c r="H1462" s="26"/>
+    </row>
+    <row r="1463" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1463" s="28">
+        <v>33</v>
+      </c>
+      <c r="B1463" s="25" t="s">
+        <v>573</v>
+      </c>
+      <c r="C1463" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1463" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1463" s="26"/>
+      <c r="F1463" s="26"/>
+      <c r="G1463" s="27"/>
+      <c r="H1463" s="26"/>
+    </row>
+    <row r="1464" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1464" s="28">
+        <v>33</v>
+      </c>
+      <c r="B1464" s="25" t="s">
+        <v>589</v>
+      </c>
+      <c r="C1464" s="29" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1464" s="29" t="s">
+        <v>360</v>
+      </c>
+      <c r="E1464" s="26"/>
+      <c r="F1464" s="26">
+        <v>1</v>
+      </c>
+      <c r="G1464" s="27"/>
+      <c r="H1464" s="26"/>
+    </row>
+    <row r="1465" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1465" s="28">
+        <v>33</v>
+      </c>
+      <c r="B1465" s="25" t="s">
+        <v>574</v>
+      </c>
+      <c r="C1465" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1465" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1465" s="26"/>
+      <c r="F1465" s="26"/>
+      <c r="G1465" s="27"/>
+      <c r="H1465" s="26"/>
+    </row>
+    <row r="1466" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1466" s="28">
+        <v>33</v>
+      </c>
+      <c r="B1466" s="25" t="s">
+        <v>583</v>
+      </c>
+      <c r="C1466" s="29" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1466" s="29" t="s">
+        <v>360</v>
+      </c>
+      <c r="E1466" s="26"/>
+      <c r="F1466" s="26">
+        <v>1</v>
+      </c>
+      <c r="G1466" s="27"/>
+      <c r="H1466" s="26"/>
+    </row>
+    <row r="1467" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1467" s="28">
+        <v>33</v>
+      </c>
+      <c r="B1467" s="25" t="s">
+        <v>575</v>
+      </c>
+      <c r="C1467" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1467" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1467" s="26"/>
+      <c r="F1467" s="26"/>
+      <c r="G1467" s="27"/>
+      <c r="H1467" s="26"/>
+    </row>
+    <row r="1468" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1468" s="28">
+        <v>33</v>
+      </c>
+      <c r="B1468" s="25" t="s">
+        <v>584</v>
+      </c>
+      <c r="C1468" s="29" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1468" s="29" t="s">
+        <v>360</v>
+      </c>
+      <c r="E1468" s="26"/>
+      <c r="F1468" s="26">
+        <v>1</v>
+      </c>
+      <c r="G1468" s="27"/>
+      <c r="H1468" s="26"/>
+    </row>
+    <row r="1469" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1469" s="28">
+        <v>33</v>
+      </c>
+      <c r="B1469" s="25" t="s">
+        <v>362</v>
+      </c>
+      <c r="C1469" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1469" s="26" t="s">
+        <v>463</v>
+      </c>
+      <c r="E1469" s="26"/>
+      <c r="F1469" s="26"/>
+      <c r="G1469" s="27"/>
+      <c r="H1469" s="26"/>
+    </row>
+    <row r="1470" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1470" s="28">
+        <v>34</v>
+      </c>
+      <c r="B1470" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="C1470" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1470" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1470" s="26"/>
+      <c r="F1470" s="26"/>
+      <c r="G1470" s="27"/>
+      <c r="H1470" s="26"/>
+    </row>
+    <row r="1471" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1471" s="28">
+        <v>34</v>
+      </c>
+      <c r="B1471" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="C1471" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1471" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1471" s="26"/>
+      <c r="F1471" s="26"/>
+      <c r="G1471" s="27">
+        <v>4</v>
+      </c>
+      <c r="H1471" s="26"/>
+    </row>
+    <row r="1472" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1472" s="28">
+        <v>34</v>
+      </c>
+      <c r="B1472" s="25" t="s">
+        <v>478</v>
+      </c>
+      <c r="C1472" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1472" s="26" t="s">
+        <v>462</v>
+      </c>
+      <c r="E1472" s="26"/>
+      <c r="F1472" s="26"/>
+      <c r="G1472" s="27">
+        <v>3</v>
+      </c>
+      <c r="H1472" s="26"/>
+    </row>
+    <row r="1473" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1473" s="28">
+        <v>34</v>
+      </c>
+      <c r="B1473" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="C1473" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1473" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1473" s="26"/>
+      <c r="F1473" s="26"/>
+      <c r="G1473" s="27"/>
+      <c r="H1473" s="26"/>
+    </row>
+    <row r="1474" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1474" s="28">
+        <v>34</v>
+      </c>
+      <c r="B1474" s="25" t="s">
+        <v>460</v>
+      </c>
+      <c r="C1474" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1474" s="26" t="s">
+        <v>461</v>
+      </c>
+      <c r="E1474" s="26"/>
+      <c r="F1474" s="26"/>
+      <c r="G1474" s="27"/>
+      <c r="H1474" s="26"/>
+    </row>
+    <row r="1475" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1475" s="28">
+        <v>34</v>
+      </c>
+      <c r="B1475" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1475" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1475" s="26" t="s">
+        <v>459</v>
+      </c>
+      <c r="E1475" s="26"/>
+      <c r="F1475" s="26"/>
+      <c r="G1475" s="27">
+        <v>3</v>
+      </c>
+      <c r="H1475" s="26"/>
+    </row>
+    <row r="1476" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1476" s="28">
+        <v>34</v>
+      </c>
+      <c r="B1476" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1476" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1476" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1476" s="26"/>
+      <c r="F1476" s="26"/>
+      <c r="G1476" s="27"/>
+      <c r="H1476" s="26"/>
+    </row>
+    <row r="1477" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+      <c r="A1477" s="28">
+        <v>34</v>
+      </c>
+      <c r="B1477" s="25" t="s">
+        <v>372</v>
+      </c>
+      <c r="C1477" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1477" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1477" s="26"/>
+      <c r="F1477" s="26"/>
+      <c r="G1477" s="27">
+        <v>3</v>
+      </c>
+      <c r="H1477" s="26"/>
+    </row>
+    <row r="1478" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1478" s="28">
+        <v>34</v>
+      </c>
+      <c r="B1478" s="26" t="s">
+        <v>361</v>
+      </c>
+      <c r="C1478" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1478" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1478" s="26"/>
+      <c r="F1478" s="26"/>
+      <c r="G1478" s="27"/>
+      <c r="H1478" s="26"/>
+    </row>
+    <row r="1479" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1479" s="28">
+        <v>34</v>
+      </c>
+      <c r="B1479" s="26" t="s">
+        <v>539</v>
+      </c>
+      <c r="C1479" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1479" s="26" t="s">
+        <v>390</v>
+      </c>
+      <c r="E1479" s="26"/>
+      <c r="F1479" s="26"/>
+      <c r="G1479" s="27"/>
+      <c r="H1479" s="26"/>
+    </row>
+    <row r="1480" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1480" s="28">
+        <v>34</v>
+      </c>
+      <c r="B1480" s="26" t="s">
+        <v>592</v>
+      </c>
+      <c r="C1480" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1480" s="26" t="s">
+        <v>360</v>
+      </c>
+      <c r="E1480" s="26"/>
+      <c r="F1480" s="26">
+        <v>2</v>
+      </c>
+      <c r="G1480" s="27"/>
+      <c r="H1480" s="26"/>
+    </row>
+    <row r="1481" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1481" s="28">
+        <v>34</v>
+      </c>
+      <c r="B1481" s="12" t="s">
+        <v>374</v>
+      </c>
+      <c r="C1481" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1481" s="26" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="1482" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1482" s="28">
+        <v>34</v>
+      </c>
+      <c r="B1482" s="12" t="s">
+        <v>469</v>
+      </c>
+      <c r="C1482" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1482" s="26" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="1483" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1483" s="28">
+        <v>34</v>
+      </c>
+      <c r="B1483" s="12" t="s">
+        <v>374</v>
+      </c>
+      <c r="C1483" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1483" s="26" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="1484" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1484" s="28">
+        <v>34</v>
+      </c>
+      <c r="B1484" s="12" t="s">
+        <v>470</v>
+      </c>
+      <c r="C1484" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1484" s="26" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="1485" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1485" s="28">
+        <v>34</v>
+      </c>
+      <c r="B1485" s="12" t="s">
+        <v>374</v>
+      </c>
+      <c r="C1485" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1485" s="26" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="1486" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1486" s="28">
+        <v>34</v>
+      </c>
+      <c r="B1486" s="12" t="s">
+        <v>470</v>
+      </c>
+      <c r="C1486" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1486" s="26" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="1487" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1487" s="28">
+        <v>34</v>
+      </c>
+      <c r="B1487" s="25" t="s">
+        <v>591</v>
+      </c>
+      <c r="C1487" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1487" s="26" t="s">
+        <v>360</v>
+      </c>
+      <c r="E1487" s="26"/>
+      <c r="F1487" s="26">
+        <v>5</v>
+      </c>
+      <c r="G1487" s="27"/>
+      <c r="H1487" s="26"/>
+    </row>
+    <row r="1488" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1488" s="28">
+        <v>34</v>
+      </c>
+      <c r="B1488" s="12" t="s">
+        <v>483</v>
+      </c>
+      <c r="C1488" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1488" s="26" t="s">
+        <v>360</v>
+      </c>
+      <c r="F1488" s="13">
+        <v>1</v>
+      </c>
+      <c r="H1488" s="31" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="1489" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1489" s="28">
+        <v>34</v>
+      </c>
+      <c r="B1489" s="12" t="s">
+        <v>545</v>
+      </c>
+      <c r="C1489" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1489" s="26" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="1490" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1490" s="28">
+        <v>34</v>
+      </c>
+      <c r="B1490" s="25" t="s">
+        <v>591</v>
+      </c>
+      <c r="C1490" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1490" s="26" t="s">
+        <v>360</v>
+      </c>
+      <c r="E1490" s="26"/>
+      <c r="F1490" s="26">
+        <v>5</v>
+      </c>
+      <c r="G1490" s="27"/>
+      <c r="H1490" s="26"/>
+    </row>
+    <row r="1491" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1491" s="28">
+        <v>34</v>
+      </c>
+      <c r="B1491" s="12" t="s">
+        <v>590</v>
+      </c>
+      <c r="C1491" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1491" s="26" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="1492" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1492" s="28">
+        <v>34</v>
+      </c>
+      <c r="B1492" s="25" t="s">
+        <v>362</v>
+      </c>
+      <c r="C1492" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1492" s="26" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="1493" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1493" s="28">
+        <v>35</v>
+      </c>
+      <c r="B1493" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="C1493" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1493" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1493" s="26"/>
+      <c r="F1493" s="26"/>
+      <c r="G1493" s="27"/>
+      <c r="H1493" s="26"/>
+    </row>
+    <row r="1494" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1494" s="28">
+        <v>35</v>
+      </c>
+      <c r="B1494" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="C1494" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1494" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1494" s="26"/>
+      <c r="F1494" s="26"/>
+      <c r="G1494" s="27">
+        <v>4</v>
+      </c>
+      <c r="H1494" s="26"/>
+    </row>
+    <row r="1495" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1495" s="28">
+        <v>35</v>
+      </c>
+      <c r="B1495" s="25" t="s">
+        <v>478</v>
+      </c>
+      <c r="C1495" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1495" s="26" t="s">
+        <v>462</v>
+      </c>
+      <c r="E1495" s="26"/>
+      <c r="F1495" s="26"/>
+      <c r="G1495" s="27">
+        <v>3</v>
+      </c>
+      <c r="H1495" s="26"/>
+    </row>
+    <row r="1496" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1496" s="28">
+        <v>35</v>
+      </c>
+      <c r="B1496" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="C1496" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1496" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1496" s="26"/>
+      <c r="F1496" s="26"/>
+      <c r="G1496" s="27"/>
+      <c r="H1496" s="26"/>
+    </row>
+    <row r="1497" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1497" s="28">
+        <v>35</v>
+      </c>
+      <c r="B1497" s="25" t="s">
+        <v>460</v>
+      </c>
+      <c r="C1497" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1497" s="26" t="s">
+        <v>461</v>
+      </c>
+      <c r="E1497" s="26"/>
+      <c r="F1497" s="26"/>
+      <c r="G1497" s="27"/>
+      <c r="H1497" s="26"/>
+    </row>
+    <row r="1498" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1498" s="28">
+        <v>35</v>
+      </c>
+      <c r="B1498" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1498" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1498" s="26" t="s">
+        <v>459</v>
+      </c>
+      <c r="E1498" s="26"/>
+      <c r="F1498" s="26"/>
+      <c r="G1498" s="27">
+        <v>3</v>
+      </c>
+      <c r="H1498" s="26"/>
+    </row>
+    <row r="1499" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1499" s="28">
+        <v>35</v>
+      </c>
+      <c r="B1499" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1499" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1499" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1499" s="26"/>
+      <c r="F1499" s="26"/>
+      <c r="G1499" s="27"/>
+      <c r="H1499" s="26"/>
+    </row>
+    <row r="1500" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+      <c r="A1500" s="28">
+        <v>35</v>
+      </c>
+      <c r="B1500" s="25" t="s">
+        <v>372</v>
+      </c>
+      <c r="C1500" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1500" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1500" s="26"/>
+      <c r="F1500" s="26"/>
+      <c r="G1500" s="27">
+        <v>3</v>
+      </c>
+      <c r="H1500" s="26"/>
+    </row>
+    <row r="1501" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1501" s="28">
+        <v>35</v>
+      </c>
+      <c r="B1501" s="26" t="s">
+        <v>357</v>
+      </c>
+      <c r="C1501" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1501" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1501" s="26"/>
+      <c r="F1501" s="26"/>
+      <c r="G1501" s="27"/>
+      <c r="H1501" s="26"/>
+    </row>
+    <row r="1502" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1502" s="28">
+        <v>35</v>
+      </c>
+      <c r="B1502" s="26" t="s">
+        <v>378</v>
+      </c>
+      <c r="C1502" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1502" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1502" s="26"/>
+      <c r="F1502" s="26"/>
+      <c r="G1502" s="27"/>
+      <c r="H1502" s="26"/>
+    </row>
+    <row r="1503" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1503" s="38">
+        <v>35</v>
+      </c>
+      <c r="B1503" s="39" t="s">
+        <v>569</v>
+      </c>
+      <c r="C1503" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1503" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1503" s="29"/>
+      <c r="F1503" s="29"/>
+      <c r="G1503" s="40"/>
+      <c r="H1503" s="29"/>
+    </row>
+    <row r="1504" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1504" s="38">
+        <v>35</v>
+      </c>
+      <c r="B1504" s="39" t="s">
+        <v>593</v>
+      </c>
+      <c r="C1504" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1504" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1504" s="29"/>
+      <c r="F1504" s="29"/>
+      <c r="G1504" s="40"/>
+      <c r="H1504" s="29"/>
+    </row>
+    <row r="1505" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1505" s="28">
+        <v>35</v>
+      </c>
+      <c r="B1505" s="12" t="s">
+        <v>450</v>
+      </c>
+      <c r="C1505" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1505" s="13" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="1506" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1506" s="28">
+        <v>36</v>
+      </c>
+      <c r="B1506" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="C1506" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1506" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1506" s="26"/>
+      <c r="F1506" s="26"/>
+      <c r="G1506" s="27"/>
+      <c r="H1506" s="26"/>
+    </row>
+    <row r="1507" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1507" s="28">
+        <v>36</v>
+      </c>
+      <c r="B1507" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="C1507" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1507" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1507" s="26"/>
+      <c r="F1507" s="26"/>
+      <c r="G1507" s="27">
+        <v>4</v>
+      </c>
+      <c r="H1507" s="26"/>
+    </row>
+    <row r="1508" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1508" s="28">
+        <v>36</v>
+      </c>
+      <c r="B1508" s="25" t="s">
+        <v>478</v>
+      </c>
+      <c r="C1508" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1508" s="26" t="s">
+        <v>462</v>
+      </c>
+      <c r="E1508" s="26"/>
+      <c r="F1508" s="26"/>
+      <c r="G1508" s="27">
+        <v>3</v>
+      </c>
+      <c r="H1508" s="26"/>
+    </row>
+    <row r="1509" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1509" s="28">
+        <v>36</v>
+      </c>
+      <c r="B1509" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="C1509" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1509" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1509" s="26"/>
+      <c r="F1509" s="26"/>
+      <c r="G1509" s="27"/>
+      <c r="H1509" s="26"/>
+    </row>
+    <row r="1510" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1510" s="28">
+        <v>36</v>
+      </c>
+      <c r="B1510" s="25" t="s">
+        <v>460</v>
+      </c>
+      <c r="C1510" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1510" s="26" t="s">
+        <v>461</v>
+      </c>
+      <c r="E1510" s="26"/>
+      <c r="F1510" s="26"/>
+      <c r="G1510" s="27"/>
+      <c r="H1510" s="26"/>
+    </row>
+    <row r="1511" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1511" s="28">
+        <v>36</v>
+      </c>
+      <c r="B1511" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1511" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1511" s="26" t="s">
+        <v>459</v>
+      </c>
+      <c r="E1511" s="26"/>
+      <c r="F1511" s="26"/>
+      <c r="G1511" s="27">
+        <v>3</v>
+      </c>
+      <c r="H1511" s="26"/>
+    </row>
+    <row r="1512" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1512" s="28">
+        <v>36</v>
+      </c>
+      <c r="B1512" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1512" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1512" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1512" s="26"/>
+      <c r="F1512" s="26"/>
+      <c r="G1512" s="27"/>
+      <c r="H1512" s="26"/>
+    </row>
+    <row r="1513" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+      <c r="A1513" s="28">
+        <v>36</v>
+      </c>
+      <c r="B1513" s="25" t="s">
+        <v>372</v>
+      </c>
+      <c r="C1513" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1513" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1513" s="26"/>
+      <c r="F1513" s="26"/>
+      <c r="G1513" s="27">
+        <v>3</v>
+      </c>
+      <c r="H1513" s="26"/>
+    </row>
+    <row r="1514" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1514" s="28">
+        <v>36</v>
+      </c>
+      <c r="B1514" s="25" t="s">
+        <v>598</v>
+      </c>
+      <c r="C1514" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1514" s="26" t="s">
+        <v>360</v>
+      </c>
+      <c r="E1514" s="26"/>
+      <c r="F1514" s="26">
+        <v>10</v>
+      </c>
+      <c r="G1514" s="27"/>
+      <c r="H1514" s="26"/>
+    </row>
+    <row r="1515" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1515" s="28">
+        <v>36</v>
+      </c>
+      <c r="B1515" s="25" t="s">
+        <v>602</v>
+      </c>
+      <c r="C1515" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1515" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1515" s="26"/>
+      <c r="F1515" s="26"/>
+      <c r="G1515" s="27"/>
+      <c r="H1515" s="26"/>
+    </row>
+    <row r="1516" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1516" s="28">
+        <v>36</v>
+      </c>
+      <c r="B1516" s="12" t="s">
+        <v>594</v>
+      </c>
+      <c r="C1516" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1516" s="26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="1517" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1517" s="28">
+        <v>36</v>
+      </c>
+      <c r="B1517" s="25" t="s">
+        <v>617</v>
+      </c>
+      <c r="C1517" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1517" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1517" s="26"/>
+      <c r="F1517" s="26"/>
+      <c r="G1517" s="27"/>
+      <c r="H1517" s="26"/>
+    </row>
+    <row r="1518" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1518" s="28">
+        <v>36</v>
+      </c>
+      <c r="B1518" s="12" t="s">
+        <v>595</v>
+      </c>
+      <c r="C1518" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1518" s="26" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="1519" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1519" s="28">
+        <v>36</v>
+      </c>
+      <c r="B1519" s="12" t="s">
+        <v>596</v>
+      </c>
+      <c r="C1519" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1519" s="26" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="1520" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1520" s="28">
+        <v>36</v>
+      </c>
+      <c r="B1520" s="42" t="s">
+        <v>597</v>
+      </c>
+      <c r="C1520" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1520" s="26" t="s">
+        <v>360</v>
+      </c>
+      <c r="F1520" s="13">
+        <v>1</v>
+      </c>
+      <c r="H1520" s="31" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="1521" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1521" s="28">
+        <v>37</v>
+      </c>
+      <c r="B1521" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="C1521" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1521" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1521" s="26"/>
+      <c r="F1521" s="26"/>
+      <c r="G1521" s="27"/>
+      <c r="H1521" s="26"/>
+    </row>
+    <row r="1522" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1522" s="28">
+        <v>37</v>
+      </c>
+      <c r="B1522" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="C1522" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1522" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1522" s="26"/>
+      <c r="F1522" s="26"/>
+      <c r="G1522" s="27">
+        <v>4</v>
+      </c>
+      <c r="H1522" s="26"/>
+    </row>
+    <row r="1523" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1523" s="28">
+        <v>37</v>
+      </c>
+      <c r="B1523" s="25" t="s">
+        <v>478</v>
+      </c>
+      <c r="C1523" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1523" s="26" t="s">
+        <v>462</v>
+      </c>
+      <c r="E1523" s="26"/>
+      <c r="F1523" s="26"/>
+      <c r="G1523" s="27">
+        <v>13</v>
+      </c>
+      <c r="H1523" s="26"/>
+    </row>
+    <row r="1524" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1524" s="28">
+        <v>37</v>
+      </c>
+      <c r="B1524" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="C1524" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1524" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1524" s="26"/>
+      <c r="F1524" s="26"/>
+      <c r="G1524" s="27"/>
+      <c r="H1524" s="26"/>
+    </row>
+    <row r="1525" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1525" s="28">
+        <v>37</v>
+      </c>
+      <c r="B1525" s="25" t="s">
+        <v>460</v>
+      </c>
+      <c r="C1525" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1525" s="26" t="s">
+        <v>461</v>
+      </c>
+      <c r="E1525" s="26"/>
+      <c r="F1525" s="26"/>
+      <c r="G1525" s="27"/>
+      <c r="H1525" s="26"/>
+    </row>
+    <row r="1526" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1526" s="28">
+        <v>37</v>
+      </c>
+      <c r="B1526" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1526" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1526" s="26" t="s">
+        <v>459</v>
+      </c>
+      <c r="E1526" s="26"/>
+      <c r="F1526" s="26"/>
+      <c r="G1526" s="27">
+        <v>13</v>
+      </c>
+      <c r="H1526" s="26"/>
+    </row>
+    <row r="1527" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1527" s="28">
+        <v>37</v>
+      </c>
+      <c r="B1527" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1527" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1527" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1527" s="26"/>
+      <c r="F1527" s="26"/>
+      <c r="G1527" s="27"/>
+      <c r="H1527" s="26"/>
+    </row>
+    <row r="1528" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+      <c r="A1528" s="28">
+        <v>37</v>
+      </c>
+      <c r="B1528" s="25" t="s">
+        <v>600</v>
+      </c>
+      <c r="C1528" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1528" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1528" s="26"/>
+      <c r="F1528" s="26"/>
+      <c r="G1528" s="27">
+        <v>30</v>
+      </c>
+      <c r="H1528" s="26"/>
+    </row>
+    <row r="1529" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1529" s="28">
+        <v>37</v>
+      </c>
+      <c r="B1529" s="25" t="s">
+        <v>476</v>
+      </c>
+      <c r="C1529" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1529" s="26" t="s">
+        <v>360</v>
+      </c>
+      <c r="E1529" s="26"/>
+      <c r="F1529" s="26">
+        <v>60</v>
+      </c>
+      <c r="G1529" s="27"/>
+      <c r="H1529" s="26"/>
+    </row>
+    <row r="1530" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1530" s="28">
+        <v>37</v>
+      </c>
+      <c r="B1530" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1530" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1530" s="26" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1530" s="26"/>
+      <c r="F1530" s="26"/>
+      <c r="G1530" s="27"/>
+      <c r="H1530" s="26"/>
+    </row>
+    <row r="1531" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1531" s="28">
+        <v>37</v>
+      </c>
+      <c r="B1531" s="25" t="s">
+        <v>346</v>
+      </c>
+      <c r="C1531" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1531" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="E1531" s="26"/>
+      <c r="F1531" s="26"/>
+      <c r="G1531" s="27"/>
+      <c r="H1531" s="26"/>
+    </row>
+    <row r="1532" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1532" s="28">
+        <v>37</v>
+      </c>
+      <c r="B1532" s="25" t="s">
+        <v>485</v>
+      </c>
+      <c r="C1532" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1532" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1532" s="26"/>
+      <c r="F1532" s="26"/>
+      <c r="G1532" s="27"/>
+      <c r="H1532" s="26"/>
+    </row>
+    <row r="1533" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1533" s="28">
+        <v>37</v>
+      </c>
+      <c r="B1533" s="25" t="s">
+        <v>601</v>
+      </c>
+      <c r="C1533" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1533" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="E1533" s="26"/>
+      <c r="F1533" s="26"/>
+      <c r="G1533" s="27"/>
+      <c r="H1533" s="26"/>
+    </row>
+    <row r="1534" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1534" s="28">
+        <v>38</v>
+      </c>
+      <c r="B1534" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="C1534" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1534" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1534" s="26"/>
+      <c r="F1534" s="26"/>
+      <c r="G1534" s="27"/>
+      <c r="H1534" s="26"/>
+    </row>
+    <row r="1535" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1535" s="28">
+        <v>38</v>
+      </c>
+      <c r="B1535" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="C1535" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1535" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1535" s="26"/>
+      <c r="F1535" s="26"/>
+      <c r="G1535" s="27">
+        <v>4</v>
+      </c>
+      <c r="H1535" s="26"/>
+    </row>
+    <row r="1536" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1536" s="28">
+        <v>38</v>
+      </c>
+      <c r="B1536" s="25" t="s">
+        <v>478</v>
+      </c>
+      <c r="C1536" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1536" s="26" t="s">
+        <v>462</v>
+      </c>
+      <c r="E1536" s="26"/>
+      <c r="F1536" s="26"/>
+      <c r="G1536" s="27">
+        <v>13</v>
+      </c>
+      <c r="H1536" s="26"/>
+    </row>
+    <row r="1537" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1537" s="28">
+        <v>38</v>
+      </c>
+      <c r="B1537" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="C1537" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1537" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1537" s="26"/>
+      <c r="F1537" s="26"/>
+      <c r="G1537" s="27"/>
+      <c r="H1537" s="26"/>
+    </row>
+    <row r="1538" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1538" s="28">
+        <v>38</v>
+      </c>
+      <c r="B1538" s="25" t="s">
+        <v>460</v>
+      </c>
+      <c r="C1538" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1538" s="26" t="s">
+        <v>461</v>
+      </c>
+      <c r="E1538" s="26"/>
+      <c r="F1538" s="26"/>
+      <c r="G1538" s="27"/>
+      <c r="H1538" s="26"/>
+    </row>
+    <row r="1539" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1539" s="28">
+        <v>38</v>
+      </c>
+      <c r="B1539" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1539" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1539" s="26" t="s">
+        <v>459</v>
+      </c>
+      <c r="E1539" s="26"/>
+      <c r="F1539" s="26"/>
+      <c r="G1539" s="27">
+        <v>13</v>
+      </c>
+      <c r="H1539" s="26"/>
+    </row>
+    <row r="1540" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1540" s="28">
+        <v>38</v>
+      </c>
+      <c r="B1540" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1540" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1540" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1540" s="26"/>
+      <c r="F1540" s="26"/>
+      <c r="G1540" s="27"/>
+      <c r="H1540" s="26"/>
+    </row>
+    <row r="1541" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+      <c r="A1541" s="28">
+        <v>38</v>
+      </c>
+      <c r="B1541" s="25" t="s">
+        <v>599</v>
+      </c>
+      <c r="C1541" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1541" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1541" s="26"/>
+      <c r="F1541" s="26"/>
+      <c r="G1541" s="27">
+        <v>30</v>
+      </c>
+      <c r="H1541" s="26"/>
+    </row>
+    <row r="1542" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1542" s="28">
+        <v>38</v>
+      </c>
+      <c r="B1542" s="25" t="s">
+        <v>602</v>
+      </c>
+      <c r="C1542" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1542" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1542" s="26"/>
+      <c r="F1542" s="26"/>
+      <c r="G1542" s="27"/>
+      <c r="H1542" s="26"/>
+    </row>
+    <row r="1543" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1543" s="28">
+        <v>38</v>
+      </c>
+      <c r="B1543" s="25" t="s">
+        <v>603</v>
+      </c>
+      <c r="C1543" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1543" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1543" s="26"/>
+      <c r="F1543" s="26"/>
+      <c r="G1543" s="27"/>
+      <c r="H1543" s="26"/>
+    </row>
+    <row r="1544" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1544" s="28">
+        <v>38</v>
+      </c>
+      <c r="B1544" s="25" t="s">
+        <v>602</v>
+      </c>
+      <c r="C1544" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1544" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1544" s="26"/>
+      <c r="F1544" s="26"/>
+      <c r="G1544" s="27"/>
+      <c r="H1544" s="26"/>
+    </row>
+    <row r="1545" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="A1545" s="28">
+        <v>38</v>
+      </c>
+      <c r="B1545" s="25" t="s">
+        <v>604</v>
+      </c>
+      <c r="C1545" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1545" s="26" t="s">
+        <v>360</v>
+      </c>
+      <c r="E1545" s="26"/>
+      <c r="F1545" s="26">
+        <v>1</v>
+      </c>
+      <c r="H1545" s="43" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="1546" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1546" s="28">
+        <v>38</v>
+      </c>
+      <c r="B1546" s="25" t="s">
+        <v>602</v>
+      </c>
+      <c r="C1546" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1546" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1546" s="26"/>
+      <c r="F1546" s="26"/>
+      <c r="G1546" s="27"/>
+      <c r="H1546" s="26"/>
+    </row>
+    <row r="1547" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="A1547" s="28">
+        <v>38</v>
+      </c>
+      <c r="B1547" s="25" t="s">
+        <v>605</v>
+      </c>
+      <c r="C1547" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1547" s="26" t="s">
+        <v>360</v>
+      </c>
+      <c r="E1547" s="26"/>
+      <c r="F1547" s="26">
+        <v>1</v>
+      </c>
+      <c r="G1547" s="27"/>
+      <c r="H1547" s="43" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="1548" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1548" s="28">
+        <v>39</v>
+      </c>
+      <c r="B1548" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="C1548" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1548" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1548" s="26"/>
+      <c r="F1548" s="26"/>
+      <c r="G1548" s="27"/>
+      <c r="H1548" s="26"/>
+    </row>
+    <row r="1549" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1549" s="28">
+        <v>39</v>
+      </c>
+      <c r="B1549" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="C1549" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1549" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1549" s="26"/>
+      <c r="F1549" s="26"/>
+      <c r="G1549" s="27">
+        <v>4</v>
+      </c>
+      <c r="H1549" s="26"/>
+    </row>
+    <row r="1550" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1550" s="28">
+        <v>39</v>
+      </c>
+      <c r="B1550" s="25" t="s">
+        <v>478</v>
+      </c>
+      <c r="C1550" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1550" s="26" t="s">
+        <v>462</v>
+      </c>
+      <c r="E1550" s="26"/>
+      <c r="F1550" s="26"/>
+      <c r="G1550" s="27">
+        <v>3</v>
+      </c>
+      <c r="H1550" s="26"/>
+    </row>
+    <row r="1551" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1551" s="28">
+        <v>39</v>
+      </c>
+      <c r="B1551" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="C1551" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1551" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1551" s="26"/>
+      <c r="F1551" s="26"/>
+      <c r="G1551" s="27"/>
+      <c r="H1551" s="26"/>
+    </row>
+    <row r="1552" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1552" s="28">
+        <v>39</v>
+      </c>
+      <c r="B1552" s="25" t="s">
+        <v>460</v>
+      </c>
+      <c r="C1552" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1552" s="26" t="s">
+        <v>461</v>
+      </c>
+      <c r="E1552" s="26"/>
+      <c r="F1552" s="26"/>
+      <c r="G1552" s="27"/>
+      <c r="H1552" s="26"/>
+    </row>
+    <row r="1553" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1553" s="28">
+        <v>39</v>
+      </c>
+      <c r="B1553" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1553" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1553" s="26" t="s">
+        <v>459</v>
+      </c>
+      <c r="E1553" s="26"/>
+      <c r="F1553" s="26"/>
+      <c r="G1553" s="27">
+        <v>13</v>
+      </c>
+      <c r="H1553" s="26"/>
+    </row>
+    <row r="1554" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1554" s="28">
+        <v>39</v>
+      </c>
+      <c r="B1554" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1554" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1554" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1554" s="26"/>
+      <c r="F1554" s="26"/>
+      <c r="G1554" s="27"/>
+      <c r="H1554" s="26"/>
+    </row>
+    <row r="1555" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+      <c r="A1555" s="28">
+        <v>39</v>
+      </c>
+      <c r="B1555" s="25" t="s">
+        <v>599</v>
+      </c>
+      <c r="C1555" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1555" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1555" s="26"/>
+      <c r="F1555" s="26"/>
+      <c r="G1555" s="27">
+        <v>30</v>
+      </c>
+      <c r="H1555" s="26"/>
+    </row>
+    <row r="1556" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1556" s="28">
+        <v>39</v>
+      </c>
+      <c r="B1556" s="25" t="s">
+        <v>606</v>
+      </c>
+      <c r="C1556" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1556" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1556" s="26"/>
+      <c r="F1556" s="26"/>
+      <c r="G1556" s="27"/>
+      <c r="H1556" s="26"/>
+    </row>
+    <row r="1557" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1557" s="28">
+        <v>39</v>
+      </c>
+      <c r="B1557" s="25" t="s">
+        <v>607</v>
+      </c>
+      <c r="C1557" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1557" s="26" t="s">
+        <v>360</v>
+      </c>
+      <c r="E1557" s="26"/>
+      <c r="F1557" s="26">
+        <v>1</v>
+      </c>
+      <c r="G1557" s="27"/>
+      <c r="H1557" s="31" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="1558" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="A1558" s="28">
+        <v>39</v>
+      </c>
+      <c r="B1558" s="25" t="s">
+        <v>608</v>
+      </c>
+      <c r="C1558" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1558" s="26" t="s">
+        <v>360</v>
+      </c>
+      <c r="E1558" s="26"/>
+      <c r="F1558" s="26">
+        <v>1</v>
+      </c>
+      <c r="G1558" s="27"/>
+      <c r="H1558" s="31" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="1559" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1559" s="28">
+        <v>39</v>
+      </c>
+      <c r="B1559" s="25" t="s">
+        <v>609</v>
+      </c>
+      <c r="C1559" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1559" s="26" t="s">
+        <v>360</v>
+      </c>
+      <c r="E1559" s="26"/>
+      <c r="F1559" s="26">
+        <v>1</v>
+      </c>
+      <c r="G1559" s="27"/>
+      <c r="H1559" s="31" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="1560" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1560" s="28">
+        <v>39</v>
+      </c>
+      <c r="B1560" s="25" t="s">
+        <v>610</v>
+      </c>
+      <c r="C1560" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1560" s="26" t="s">
+        <v>360</v>
+      </c>
+      <c r="E1560" s="26"/>
+      <c r="F1560" s="26">
+        <v>1</v>
+      </c>
+      <c r="G1560" s="27"/>
+      <c r="H1560" s="31" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="1561" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1561" s="28">
+        <v>39</v>
+      </c>
+      <c r="B1561" s="25" t="s">
+        <v>611</v>
+      </c>
+      <c r="C1561" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1561" s="26" t="s">
+        <v>360</v>
+      </c>
+      <c r="E1561" s="26"/>
+      <c r="F1561" s="26">
+        <v>1</v>
+      </c>
+      <c r="G1561" s="27"/>
+      <c r="H1561" s="31" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="1562" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="A1562" s="28">
+        <v>39</v>
+      </c>
+      <c r="B1562" s="25" t="s">
+        <v>612</v>
+      </c>
+      <c r="C1562" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1562" s="26" t="s">
+        <v>360</v>
+      </c>
+      <c r="E1562" s="26"/>
+      <c r="F1562" s="26">
+        <v>1</v>
+      </c>
+      <c r="G1562" s="27"/>
+      <c r="H1562" s="31" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="1563" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="A1563" s="28">
+        <v>39</v>
+      </c>
+      <c r="B1563" s="25" t="s">
+        <v>613</v>
+      </c>
+      <c r="C1563" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1563" s="26" t="s">
+        <v>360</v>
+      </c>
+      <c r="E1563" s="26"/>
+      <c r="F1563" s="26">
+        <v>1</v>
+      </c>
+      <c r="G1563" s="27"/>
+      <c r="H1563" s="31" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="1564" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="A1564" s="28">
+        <v>39</v>
+      </c>
+      <c r="B1564" s="25" t="s">
+        <v>614</v>
+      </c>
+      <c r="C1564" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1564" s="26" t="s">
+        <v>360</v>
+      </c>
+      <c r="E1564" s="26"/>
+      <c r="F1564" s="26">
+        <v>1</v>
+      </c>
+      <c r="G1564" s="27"/>
+      <c r="H1564" s="31" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="1565" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1565" s="28">
+        <v>40</v>
+      </c>
+      <c r="B1565" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="C1565" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1565" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1565" s="26"/>
+      <c r="F1565" s="26"/>
+      <c r="G1565" s="27"/>
+      <c r="H1565" s="26"/>
+    </row>
+    <row r="1566" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1566" s="28">
+        <v>40</v>
+      </c>
+      <c r="B1566" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="C1566" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1566" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1566" s="26"/>
+      <c r="F1566" s="26"/>
+      <c r="G1566" s="27">
+        <v>4</v>
+      </c>
+      <c r="H1566" s="26"/>
+    </row>
+    <row r="1567" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1567" s="28">
+        <v>40</v>
+      </c>
+      <c r="B1567" s="25" t="s">
+        <v>478</v>
+      </c>
+      <c r="C1567" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1567" s="26" t="s">
+        <v>462</v>
+      </c>
+      <c r="E1567" s="26"/>
+      <c r="F1567" s="26"/>
+      <c r="G1567" s="27">
+        <v>3</v>
+      </c>
+      <c r="H1567" s="26"/>
+    </row>
+    <row r="1568" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1568" s="28">
+        <v>40</v>
+      </c>
+      <c r="B1568" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="C1568" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1568" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1568" s="26"/>
+      <c r="F1568" s="26"/>
+      <c r="G1568" s="27"/>
+      <c r="H1568" s="26"/>
+    </row>
+    <row r="1569" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1569" s="28">
+        <v>40</v>
+      </c>
+      <c r="B1569" s="25" t="s">
+        <v>460</v>
+      </c>
+      <c r="C1569" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1569" s="26" t="s">
+        <v>461</v>
+      </c>
+      <c r="E1569" s="26"/>
+      <c r="F1569" s="26"/>
+      <c r="G1569" s="27"/>
+      <c r="H1569" s="26"/>
+    </row>
+    <row r="1570" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1570" s="28">
+        <v>40</v>
+      </c>
+      <c r="B1570" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1570" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1570" s="26" t="s">
+        <v>459</v>
+      </c>
+      <c r="E1570" s="26"/>
+      <c r="F1570" s="26"/>
+      <c r="G1570" s="27">
+        <v>13</v>
+      </c>
+      <c r="H1570" s="26"/>
+    </row>
+    <row r="1571" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1571" s="28">
+        <v>40</v>
+      </c>
+      <c r="B1571" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1571" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1571" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1571" s="26"/>
+      <c r="F1571" s="26"/>
+      <c r="G1571" s="27"/>
+      <c r="H1571" s="26"/>
+    </row>
+    <row r="1572" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+      <c r="A1572" s="28">
+        <v>40</v>
+      </c>
+      <c r="B1572" s="25" t="s">
+        <v>600</v>
+      </c>
+      <c r="C1572" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1572" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1572" s="26"/>
+      <c r="F1572" s="26"/>
+      <c r="G1572" s="27">
+        <v>30</v>
+      </c>
+      <c r="H1572" s="26"/>
+    </row>
+    <row r="1573" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1573" s="28">
+        <v>40</v>
+      </c>
+      <c r="B1573" s="26" t="s">
+        <v>357</v>
+      </c>
+      <c r="C1573" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1573" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1573" s="26"/>
+      <c r="F1573" s="26"/>
+      <c r="G1573" s="27"/>
+      <c r="H1573" s="26"/>
+    </row>
+    <row r="1574" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1574" s="28">
+        <v>40</v>
+      </c>
+      <c r="B1574" s="26" t="s">
+        <v>378</v>
+      </c>
+      <c r="C1574" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1574" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1574" s="26"/>
+      <c r="F1574" s="26"/>
+      <c r="G1574" s="27"/>
+      <c r="H1574" s="26"/>
+    </row>
+    <row r="1575" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1575" s="28">
+        <v>40</v>
+      </c>
+      <c r="B1575" s="25" t="s">
+        <v>476</v>
+      </c>
+      <c r="C1575" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1575" s="26" t="s">
+        <v>360</v>
+      </c>
+      <c r="E1575" s="26"/>
+      <c r="F1575" s="26">
+        <v>60</v>
+      </c>
+      <c r="G1575" s="27"/>
+      <c r="H1575" s="26"/>
+    </row>
+    <row r="1576" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1576" s="28">
+        <v>40</v>
+      </c>
+      <c r="B1576" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1576" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1576" s="26" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1576" s="26"/>
+      <c r="F1576" s="26"/>
+      <c r="G1576" s="27"/>
+      <c r="H1576" s="26"/>
+    </row>
+    <row r="1577" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1577" s="28">
+        <v>40</v>
+      </c>
+      <c r="B1577" s="25" t="s">
+        <v>346</v>
+      </c>
+      <c r="C1577" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1577" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="E1577" s="26"/>
+      <c r="F1577" s="26"/>
+      <c r="G1577" s="27"/>
+      <c r="H1577" s="26"/>
+    </row>
+    <row r="1578" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1578" s="28">
+        <v>40</v>
+      </c>
+      <c r="B1578" s="25" t="s">
+        <v>485</v>
+      </c>
+      <c r="C1578" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1578" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1578" s="26"/>
+      <c r="F1578" s="26"/>
+      <c r="G1578" s="27"/>
+      <c r="H1578" s="26"/>
+    </row>
+    <row r="1579" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1579" s="28">
+        <v>40</v>
+      </c>
+      <c r="B1579" s="25" t="s">
+        <v>601</v>
+      </c>
+      <c r="C1579" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1579" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="E1579" s="26"/>
+      <c r="F1579" s="26"/>
+      <c r="G1579" s="27"/>
+      <c r="H1579" s="26"/>
+    </row>
+    <row r="1580" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1580" s="28">
+        <v>40</v>
+      </c>
+      <c r="B1580" s="12" t="s">
+        <v>450</v>
+      </c>
+      <c r="C1580" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1580" s="26" t="s">
+        <v>385</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D608:D609 D271:D272 D324:D325 D381:D382 D424:D425 D471:D472 D518:D519 D561:D562 D267:D268 D327:D328 D427:D428 D474:D475 D564:D565 D604:D605 D320:D321 D377:D378 D420:D421 D467:D468 D514:D515 D557:D558 D2:D262 D649:D650 D694:D695 D622:D623 D739:D740 D1002:D1039 D784:D785 D1229:D1262 D829:D830 D1047:D1084 D876:D877 D917:D918 D958:D959 D1044:D1045 D1089:D1090 D879:D912 D1134:D1135 D1179:D1180 D1352:D1385 D1226:D1227 D652:D689 D1267:D1268 D1308:D1309 D1349:D1350 D920:D953 D697:D734 D742:D779 D787:D824 D1270:D1303 D832:D871 D1092:D1129 D1137:D1174 D1182:D1221 D961:D994 D1390:D1391 D1311:D1344 D999:D1000 D1393:D1429">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D608:D609 D271:D272 D324:D325 D381:D382 D424:D425 D471:D472 D518:D519 D561:D562 D267:D268 D327:D328 D427:D428 D474:D475 D564:D565 D604:D605 D320:D321 D377:D378 D420:D421 D467:D468 D514:D515 D557:D558 D2:D262 D649:D650 D694:D695 D622:D623 D739:D740 D1002:D1039 D784:D785 D1229:D1262 D829:D830 D1047:D1084 D876:D877 D917:D918 D958:D959 D1044:D1045 D1089:D1090 D879:D912 D1134:D1135 D1179:D1180 D1352:D1385 D1226:D1227 D652:D689 D1267:D1268 D1308:D1309 D1349:D1350 D920:D953 D697:D734 D742:D779 D787:D824 D1270:D1303 D832:D871 D1092:D1129 D1137:D1174 D1182:D1221 D961:D994 D1390:D1391 D1311:D1344 D999:D1000 D1393:D1429 D1434:D1435 D1477:D1492 D1474:D1475 D1437:D1469 D1500:D1504 D1497:D1498 D1513:D1520 D1510:D1511 D1525:D1526 D1538:D1539 D1528:D1533 D1552:D1553 D1572:D1580 D1541:D1547 D1569:D1570 D1555:D1564">
       <formula1>INDIRECT(C2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C4170">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C4210">
       <formula1>PageObject_Name</formula1>
     </dataValidation>
   </dataValidations>
@@ -30070,7 +33375,7 @@
           <x14:formula1>
             <xm:f>'Page Objects And Actions'!$A$2:$A$23</xm:f>
           </x14:formula1>
-          <xm:sqref>C4171:C1048576</xm:sqref>
+          <xm:sqref>C4211:C1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -30081,10 +33386,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:X171"/>
+  <dimension ref="A1:X219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A156" workbookViewId="0">
-      <selection activeCell="D171" sqref="D2:D171"/>
+    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -31738,7 +35043,7 @@
         <v>274</v>
       </c>
       <c r="D102" s="17" t="s">
-        <v>71</v>
+        <v>646</v>
       </c>
     </row>
     <row r="103" spans="3:4" x14ac:dyDescent="0.3">
@@ -31746,7 +35051,7 @@
         <v>263</v>
       </c>
       <c r="D103" s="17" t="s">
-        <v>72</v>
+        <v>622</v>
       </c>
     </row>
     <row r="104" spans="3:4" x14ac:dyDescent="0.3">
@@ -31754,7 +35059,7 @@
         <v>314</v>
       </c>
       <c r="D104" s="17" t="s">
-        <v>401</v>
+        <v>648</v>
       </c>
     </row>
     <row r="105" spans="3:4" x14ac:dyDescent="0.3">
@@ -31762,7 +35067,7 @@
         <v>315</v>
       </c>
       <c r="D105" s="17" t="s">
-        <v>183</v>
+        <v>624</v>
       </c>
     </row>
     <row r="106" spans="3:4" x14ac:dyDescent="0.3">
@@ -31770,337 +35075,577 @@
         <v>316</v>
       </c>
       <c r="D106" s="17" t="s">
-        <v>181</v>
+        <v>653</v>
       </c>
     </row>
     <row r="107" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D107" s="17" t="s">
-        <v>73</v>
+        <v>629</v>
       </c>
     </row>
     <row r="108" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D108" s="17" t="s">
-        <v>74</v>
+        <v>651</v>
       </c>
     </row>
     <row r="109" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D109" s="17" t="s">
-        <v>177</v>
+        <v>627</v>
       </c>
     </row>
     <row r="110" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D110" s="17" t="s">
-        <v>169</v>
+        <v>71</v>
       </c>
     </row>
     <row r="111" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D111" s="17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="112" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D112" s="17" t="s">
-        <v>76</v>
+        <v>650</v>
       </c>
     </row>
     <row r="113" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D113" s="17" t="s">
-        <v>77</v>
+        <v>626</v>
       </c>
     </row>
     <row r="114" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D114" s="17" t="s">
-        <v>78</v>
+        <v>652</v>
       </c>
     </row>
     <row r="115" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D115" s="17" t="s">
-        <v>79</v>
+        <v>628</v>
       </c>
     </row>
     <row r="116" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D116" s="17" t="s">
-        <v>80</v>
+        <v>649</v>
       </c>
     </row>
     <row r="117" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D117" s="17" t="s">
-        <v>174</v>
+        <v>625</v>
       </c>
     </row>
     <row r="118" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D118" s="17" t="s">
-        <v>166</v>
+        <v>647</v>
       </c>
     </row>
     <row r="119" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D119" s="17" t="s">
-        <v>173</v>
+        <v>623</v>
       </c>
     </row>
     <row r="120" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D120" s="17" t="s">
-        <v>165</v>
+        <v>401</v>
       </c>
     </row>
     <row r="121" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D121" s="17" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
     </row>
     <row r="122" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D122" s="17" t="s">
-        <v>203</v>
+        <v>181</v>
       </c>
     </row>
     <row r="123" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D123" s="17" t="s">
-        <v>385</v>
+        <v>73</v>
       </c>
     </row>
     <row r="124" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D124" s="17" t="s">
-        <v>323</v>
+        <v>74</v>
       </c>
     </row>
     <row r="125" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D125" s="17" t="s">
-        <v>81</v>
+        <v>177</v>
       </c>
     </row>
     <row r="126" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D126" s="17" t="s">
-        <v>82</v>
+        <v>169</v>
       </c>
     </row>
     <row r="127" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D127" s="17" t="s">
-        <v>83</v>
+        <v>661</v>
       </c>
     </row>
     <row r="128" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D128" s="17" t="s">
-        <v>84</v>
+        <v>637</v>
       </c>
     </row>
     <row r="129" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D129" s="17" t="s">
-        <v>85</v>
+        <v>662</v>
       </c>
     </row>
     <row r="130" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D130" s="17" t="s">
-        <v>86</v>
+        <v>638</v>
       </c>
     </row>
     <row r="131" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D131" s="17" t="s">
-        <v>87</v>
+        <v>654</v>
       </c>
     </row>
     <row r="132" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D132" s="17" t="s">
-        <v>386</v>
+        <v>630</v>
       </c>
     </row>
     <row r="133" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D133" s="17" t="s">
-        <v>88</v>
+        <v>655</v>
       </c>
     </row>
     <row r="134" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D134" s="17" t="s">
-        <v>89</v>
+        <v>631</v>
       </c>
     </row>
     <row r="135" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D135" s="17" t="s">
-        <v>90</v>
+        <v>656</v>
       </c>
     </row>
     <row r="136" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D136" s="17" t="s">
-        <v>91</v>
+        <v>632</v>
       </c>
     </row>
     <row r="137" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D137" s="17" t="s">
-        <v>321</v>
+        <v>657</v>
       </c>
     </row>
     <row r="138" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D138" s="17" t="s">
-        <v>320</v>
+        <v>633</v>
       </c>
     </row>
     <row r="139" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D139" s="17" t="s">
-        <v>92</v>
+        <v>658</v>
       </c>
     </row>
     <row r="140" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D140" s="17" t="s">
-        <v>93</v>
+        <v>634</v>
       </c>
     </row>
     <row r="141" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D141" s="17" t="s">
-        <v>209</v>
+        <v>659</v>
       </c>
     </row>
     <row r="142" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D142" s="17" t="s">
-        <v>205</v>
+        <v>635</v>
       </c>
     </row>
     <row r="143" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D143" s="17" t="s">
-        <v>206</v>
+        <v>75</v>
       </c>
     </row>
     <row r="144" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D144" s="17" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
     </row>
     <row r="145" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D145" s="17" t="s">
-        <v>95</v>
+        <v>663</v>
       </c>
     </row>
     <row r="146" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D146" s="17" t="s">
-        <v>193</v>
+        <v>639</v>
       </c>
     </row>
     <row r="147" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D147" s="17" t="s">
-        <v>192</v>
+        <v>660</v>
       </c>
     </row>
     <row r="148" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D148" s="17" t="s">
-        <v>185</v>
+        <v>636</v>
       </c>
     </row>
     <row r="149" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D149" s="17" t="s">
-        <v>191</v>
+        <v>77</v>
       </c>
     </row>
     <row r="150" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D150" s="17" t="s">
-        <v>195</v>
+        <v>78</v>
       </c>
     </row>
     <row r="151" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D151" s="17" t="s">
-        <v>186</v>
+        <v>79</v>
       </c>
     </row>
     <row r="152" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D152" s="17" t="s">
-        <v>187</v>
+        <v>80</v>
       </c>
     </row>
     <row r="153" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D153" s="17" t="s">
-        <v>550</v>
+        <v>174</v>
       </c>
     </row>
     <row r="154" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D154" s="17" t="s">
-        <v>188</v>
+        <v>166</v>
       </c>
     </row>
     <row r="155" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D155" s="17" t="s">
-        <v>207</v>
+        <v>173</v>
       </c>
     </row>
     <row r="156" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D156" s="17" t="s">
-        <v>325</v>
+        <v>165</v>
       </c>
     </row>
     <row r="157" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D157" s="17" t="s">
-        <v>551</v>
+        <v>204</v>
       </c>
     </row>
     <row r="158" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D158" s="17" t="s">
-        <v>326</v>
+        <v>203</v>
       </c>
     </row>
     <row r="159" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D159" s="17" t="s">
-        <v>189</v>
+        <v>385</v>
       </c>
     </row>
     <row r="160" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D160" s="17" t="s">
-        <v>552</v>
+        <v>323</v>
       </c>
     </row>
     <row r="161" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D161" s="17" t="s">
-        <v>208</v>
+        <v>81</v>
       </c>
     </row>
     <row r="162" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D162" s="17" t="s">
-        <v>190</v>
+        <v>82</v>
       </c>
     </row>
     <row r="163" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D163" s="17" t="s">
-        <v>319</v>
+        <v>83</v>
       </c>
     </row>
     <row r="164" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D164" s="17" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
     </row>
     <row r="165" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D165" s="17" t="s">
-        <v>324</v>
+        <v>85</v>
       </c>
     </row>
     <row r="166" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D166" s="17" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="167" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D167" s="17" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
     <row r="168" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D168" s="17" t="s">
-        <v>99</v>
+        <v>669</v>
       </c>
     </row>
     <row r="169" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D169" s="17" t="s">
-        <v>184</v>
+        <v>645</v>
       </c>
     </row>
     <row r="170" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D170" s="17" t="s">
-        <v>182</v>
+        <v>386</v>
       </c>
     </row>
     <row r="171" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D171" s="17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="172" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D172" s="17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="173" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D173" s="17" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="174" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D174" s="17" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="175" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D175" s="17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="176" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D176" s="17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="177" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D177" s="17" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="178" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D178" s="17" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="179" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D179" s="17" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="180" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D180" s="17" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="181" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D181" s="17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="182" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D182" s="17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="183" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D183" s="17" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="184" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D184" s="17" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="185" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D185" s="17" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="186" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D186" s="17" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="187" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D187" s="17" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="188" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D188" s="17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="189" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D189" s="17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="190" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D190" s="17" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="191" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D191" s="17" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="192" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D192" s="17" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="193" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D193" s="17" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="194" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D194" s="17" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="195" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D195" s="17" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="196" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D196" s="17" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="197" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D197" s="17" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="198" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D198" s="17" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="199" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D199" s="17" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="200" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D200" s="17" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="201" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D201" s="17" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="202" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D202" s="17" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="203" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D203" s="17" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="204" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D204" s="17" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="205" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D205" s="17" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="206" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D206" s="17" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="207" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D207" s="17" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="208" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D208" s="17" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="209" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D209" s="17" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="210" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D210" s="17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="211" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D211" s="17" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="212" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D212" s="17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="213" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D213" s="17" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="214" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D214" s="17" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="215" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D215" s="17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="216" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D216" s="17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="217" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D217" s="17" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="218" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D218" s="17" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="219" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D219" s="17" t="s">
         <v>461</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="D2:D171">
-    <sortCondition ref="D171"/>
+  <sortState ref="D2:D219">
+    <sortCondition ref="D219"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
US2081 - Page actions for Observer/Survey view. Refactored code
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCases.xlsx
+++ b/selenium-wd/data/TestCases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="910" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="776" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases-CmpReports" sheetId="1" r:id="rId1"/>
@@ -31,18 +31,20 @@
     <definedName name="ManageLocationsPage">'Page Objects And Actions'!$K$2:$K$50</definedName>
     <definedName name="ManageRefGasBottlesPage">'Page Objects And Actions'!$L$2:$L$50</definedName>
     <definedName name="ManageReleaseNotesPage">'Page Objects And Actions'!$M$2:$M$50</definedName>
-    <definedName name="ManageSurveyorHistoriesPage">'Page Objects And Actions'!$O$2:$BO$50</definedName>
+    <definedName name="ManageSurveyorHistoriesPage">'Page Objects And Actions'!$O$2:$BQ$50</definedName>
     <definedName name="ManageSurveyorPage">'Page Objects And Actions'!$N$2:$N$50</definedName>
     <definedName name="ManageUsersPage">'Page Objects And Actions'!$P$2:$P$50</definedName>
     <definedName name="MeasurementSessionsPage">'Page Objects And Actions'!$Q$2:$Q$50</definedName>
-    <definedName name="PageObject_Name">'Page Objects And Actions'!$A$2:$A$24</definedName>
-    <definedName name="PrimePage">'Page Objects And Actions'!$R$2:$R$50</definedName>
-    <definedName name="ReferenceGasReportsPage">'Page Objects And Actions'!$S$2:$S$50</definedName>
-    <definedName name="SendFeedbackPage">'Page Objects And Actions'!$T$2:$T$50</definedName>
-    <definedName name="SurveyorHistoryReportsPage">'Page Objects And Actions'!$V$2:$V$50</definedName>
-    <definedName name="SurveyorSystemsPage">'Page Objects And Actions'!$U$2:$U$50</definedName>
-    <definedName name="TestEnvironment">'Page Objects And Actions'!$X$2:$X$11</definedName>
-    <definedName name="UserFeedbackPage">'Page Objects And Actions'!$W$2:$W$50</definedName>
+    <definedName name="ObserverViewPage">'Page Objects And Actions'!$R$2:$R$184</definedName>
+    <definedName name="PageObject_Name">'Page Objects And Actions'!$A$2:$A$26</definedName>
+    <definedName name="PrimePage">'Page Objects And Actions'!$S$2:$S$50</definedName>
+    <definedName name="ReferenceGasReportsPage">'Page Objects And Actions'!$T$2:$T$50</definedName>
+    <definedName name="SendFeedbackPage">'Page Objects And Actions'!$U$2:$U$50</definedName>
+    <definedName name="SurveyorHistoryReportsPage">'Page Objects And Actions'!$W$2:$W$50</definedName>
+    <definedName name="SurveyorSystemsPage">'Page Objects And Actions'!$V$2:$V$50</definedName>
+    <definedName name="SurveyViewPage">'Page Objects And Actions'!$X$2:$X$139</definedName>
+    <definedName name="TestEnvironment">'Page Objects And Actions'!$Z$2:$Z$11</definedName>
+    <definedName name="UserFeedbackPage">'Page Objects And Actions'!$Y$2:$Y$50</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -204,7 +206,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5832" uniqueCount="670">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6157" uniqueCount="676">
   <si>
     <t>ID</t>
   </si>
@@ -2214,6 +2216,24 @@
   </si>
   <si>
     <t>verifyRefBottleMeasButtonIsNotVisible</t>
+  </si>
+  <si>
+    <t>ObserverViewPage</t>
+  </si>
+  <si>
+    <t>SurveyViewPage</t>
+  </si>
+  <si>
+    <t>verifyObserverViewPageIsOpened</t>
+  </si>
+  <si>
+    <t>verifyStatusButtonIsGreenWithPlus</t>
+  </si>
+  <si>
+    <t>verifyStatusButtonIsCollapsed</t>
+  </si>
+  <si>
+    <t>verifySurveyViewPageIsOpened</t>
   </si>
 </sst>
 </file>
@@ -33373,7 +33393,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'Page Objects And Actions'!$A$2:$A$23</xm:f>
+            <xm:f>'Page Objects And Actions'!$A$2:$A$25</xm:f>
           </x14:formula1>
           <xm:sqref>C4211:C1048576</xm:sqref>
         </x14:dataValidation>
@@ -33386,10 +33406,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:X219"/>
+  <dimension ref="A1:Z219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33400,12 +33420,15 @@
     <col min="4" max="4" width="45.21875" style="17" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="14" width="22.44140625" style="17" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="15" max="15" width="25.21875" style="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="21" width="22.44140625" style="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="24.21875" style="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="24" width="22.44140625" style="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="17" width="22.44140625" style="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="45.21875" style="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="22" width="22.44140625" style="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="24.21875" style="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="45.21875" style="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="26" width="22.44140625" style="17" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>7</v>
       </c>
@@ -33458,28 +33481,34 @@
         <v>23</v>
       </c>
       <c r="R1" s="16" t="s">
+        <v>670</v>
+      </c>
+      <c r="S1" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="S1" s="16" t="s">
+      <c r="T1" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="T1" s="16" t="s">
+      <c r="U1" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="U1" s="16" t="s">
+      <c r="V1" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="V1" s="16" t="s">
+      <c r="W1" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="W1" s="16" t="s">
+      <c r="X1" s="16" t="s">
+        <v>671</v>
+      </c>
+      <c r="Y1" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="X1" s="16" t="s">
+      <c r="Z1" s="16" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>8</v>
       </c>
@@ -33550,10 +33579,16 @@
         <v>39</v>
       </c>
       <c r="X2" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y2" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z2" s="17" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>9</v>
       </c>
@@ -33624,10 +33659,16 @@
         <v>41</v>
       </c>
       <c r="X3" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y3" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z3" s="17" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>10</v>
       </c>
@@ -33698,10 +33739,16 @@
         <v>40</v>
       </c>
       <c r="X4" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y4" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z4" s="17" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>11</v>
       </c>
@@ -33772,10 +33819,16 @@
         <v>42</v>
       </c>
       <c r="X5" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y5" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z5" s="17" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>12</v>
       </c>
@@ -33828,7 +33881,7 @@
         <v>43</v>
       </c>
       <c r="R6" s="17" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="S6" s="17" t="s">
         <v>43</v>
@@ -33846,10 +33899,16 @@
         <v>43</v>
       </c>
       <c r="X6" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y6" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z6" s="17" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>13</v>
       </c>
@@ -33902,7 +33961,7 @@
         <v>44</v>
       </c>
       <c r="R7" s="17" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="S7" s="17" t="s">
         <v>44</v>
@@ -33920,10 +33979,16 @@
         <v>44</v>
       </c>
       <c r="X7" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y7" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z7" s="17" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>14</v>
       </c>
@@ -33976,7 +34041,7 @@
         <v>202</v>
       </c>
       <c r="R8" s="17" t="s">
-        <v>202</v>
+        <v>52</v>
       </c>
       <c r="S8" s="17" t="s">
         <v>202</v>
@@ -33994,10 +34059,16 @@
         <v>202</v>
       </c>
       <c r="X8" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y8" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="Z8" s="17" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>15</v>
       </c>
@@ -34050,7 +34121,7 @@
         <v>45</v>
       </c>
       <c r="R9" s="17" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="S9" s="17" t="s">
         <v>45</v>
@@ -34067,8 +34138,14 @@
       <c r="W9" s="17" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X9" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y9" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>16</v>
       </c>
@@ -34121,7 +34198,7 @@
         <v>46</v>
       </c>
       <c r="R10" s="17" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="S10" s="17" t="s">
         <v>46</v>
@@ -34138,8 +34215,14 @@
       <c r="W10" s="17" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X10" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y10" s="17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>17</v>
       </c>
@@ -34192,7 +34275,7 @@
         <v>47</v>
       </c>
       <c r="R11" s="17" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="S11" s="17" t="s">
         <v>47</v>
@@ -34209,8 +34292,14 @@
       <c r="W11" s="17" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X11" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y11" s="17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>18</v>
       </c>
@@ -34263,7 +34352,7 @@
         <v>48</v>
       </c>
       <c r="R12" s="17" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="S12" s="17" t="s">
         <v>48</v>
@@ -34280,8 +34369,14 @@
       <c r="W12" s="17" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X12" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y12" s="17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>19</v>
       </c>
@@ -34294,8 +34389,14 @@
       <c r="H13" s="17" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="R13" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="X13" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>20</v>
       </c>
@@ -34308,8 +34409,14 @@
       <c r="H14" s="17" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="R14" s="17" t="s">
+        <v>473</v>
+      </c>
+      <c r="X14" s="17" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>21</v>
       </c>
@@ -34322,8 +34429,14 @@
       <c r="H15" s="17" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="R15" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="X15" s="17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>22</v>
       </c>
@@ -34333,8 +34446,14 @@
       <c r="D16" s="17" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="R16" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="X16" s="17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
         <v>23</v>
       </c>
@@ -34344,10 +34463,16 @@
       <c r="D17" s="17" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="R17" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="X17" s="17" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
-        <v>24</v>
+        <v>670</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>219</v>
@@ -34355,10 +34480,16 @@
       <c r="D18" s="17" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="R18" s="17" t="s">
+        <v>322</v>
+      </c>
+      <c r="X18" s="17" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>214</v>
@@ -34366,10 +34497,16 @@
       <c r="D19" s="17" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="R19" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="X19" s="17" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" s="17" t="s">
         <v>220</v>
@@ -34377,10 +34514,16 @@
       <c r="D20" s="17" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="R20" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="X20" s="17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C21" s="17" t="s">
         <v>240</v>
@@ -34388,10 +34531,16 @@
       <c r="D21" s="17" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="R21" s="17" t="s">
+        <v>464</v>
+      </c>
+      <c r="X21" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22" s="17" t="s">
         <v>221</v>
@@ -34399,10 +34548,16 @@
       <c r="D22" s="17" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="R22" s="17" t="s">
+        <v>465</v>
+      </c>
+      <c r="X22" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C23" s="17" t="s">
         <v>224</v>
@@ -34410,10 +34565,16 @@
       <c r="D23" s="17" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="R23" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="X23" s="17" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
-        <v>327</v>
+        <v>671</v>
       </c>
       <c r="C24" s="17" t="s">
         <v>36</v>
@@ -34421,1089 +34582,1926 @@
       <c r="D24" s="17" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="R24" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="X24" s="17" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A25" s="17" t="s">
+        <v>29</v>
+      </c>
       <c r="C25" s="17" t="s">
         <v>230</v>
       </c>
       <c r="D25" s="17" t="s">
         <v>464</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="R25" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="X25" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A26" s="17" t="s">
+        <v>327</v>
+      </c>
       <c r="C26" s="17" t="s">
         <v>231</v>
       </c>
       <c r="D26" s="17" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="R26" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="X26" s="17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C27" s="17" t="s">
         <v>232</v>
       </c>
       <c r="D27" s="17" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="R27" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="X27" s="17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C28" s="17" t="s">
         <v>228</v>
       </c>
       <c r="D28" s="17" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="R28" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="X28" s="17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C29" s="17" t="s">
         <v>241</v>
       </c>
       <c r="D29" s="17" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="R29" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="X29" s="17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C30" s="17" t="s">
         <v>242</v>
       </c>
       <c r="D30" s="17" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="R30" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="X30" s="17" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C31" s="17" t="s">
         <v>244</v>
       </c>
       <c r="D31" s="17" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="R31" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="X31" s="17" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C32" s="17" t="s">
         <v>243</v>
       </c>
       <c r="D32" s="17" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R32" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="X32" s="17" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="33" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C33" s="17" t="s">
         <v>225</v>
       </c>
       <c r="D33" s="17" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R33" s="17" t="s">
+        <v>393</v>
+      </c>
+      <c r="X33" s="17" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C34" s="17" t="s">
         <v>235</v>
       </c>
       <c r="D34" s="17" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R34" s="17" t="s">
+        <v>395</v>
+      </c>
+      <c r="X34" s="17" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="35" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C35" s="17" t="s">
         <v>234</v>
       </c>
       <c r="D35" s="17" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R35" s="17" t="s">
+        <v>394</v>
+      </c>
+      <c r="X35" s="17" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="36" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C36" s="17" t="s">
         <v>37</v>
       </c>
       <c r="D36" s="17" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R36" s="17" t="s">
+        <v>398</v>
+      </c>
+      <c r="X36" s="17" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="37" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C37" s="17" t="s">
         <v>43</v>
       </c>
       <c r="D37" s="17" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R37" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="X37" s="17" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="38" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C38" s="17" t="s">
         <v>44</v>
       </c>
       <c r="D38" s="17" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R38" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="X38" s="17" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="39" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C39" s="17" t="s">
         <v>38</v>
       </c>
       <c r="D39" s="17" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R39" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="X39" s="17" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="40" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C40" s="17" t="s">
         <v>202</v>
       </c>
       <c r="D40" s="17" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R40" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="X40" s="17" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="41" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C41" s="17" t="s">
         <v>250</v>
       </c>
       <c r="D41" s="17" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R41" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="X41" s="17" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="42" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C42" s="17" t="s">
         <v>251</v>
       </c>
       <c r="D42" s="17" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="43" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R42" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="X42" s="17" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="43" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C43" s="17" t="s">
         <v>226</v>
       </c>
       <c r="D43" s="17" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R43" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="X43" s="17" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="44" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C44" s="17" t="s">
         <v>45</v>
       </c>
       <c r="D44" s="17" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="45" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R44" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="X44" s="17" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="45" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C45" s="17" t="s">
         <v>46</v>
       </c>
       <c r="D45" s="17" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R45" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="X45" s="17" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="46" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C46" s="17" t="s">
         <v>47</v>
       </c>
       <c r="D46" s="17" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R46" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="X46" s="17" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="47" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C47" s="17" t="s">
         <v>48</v>
       </c>
       <c r="D47" s="17" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="48" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R47" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="X47" s="17" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="48" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C48" s="17" t="s">
         <v>229</v>
       </c>
       <c r="D48" s="17" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R48" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="X48" s="17" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="49" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C49" s="17" t="s">
         <v>237</v>
       </c>
       <c r="D49" s="17" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R49" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="X49" s="17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="50" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C50" s="17" t="s">
         <v>236</v>
       </c>
       <c r="D50" s="17" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R50" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="X50" s="17" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="51" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C51" s="17" t="s">
         <v>238</v>
       </c>
       <c r="D51" s="17" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R51" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="X51" s="17" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="52" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C52" s="17" t="s">
         <v>233</v>
       </c>
       <c r="D52" s="17" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="53" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R52" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="X52" s="17" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="53" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C53" s="17" t="s">
         <v>249</v>
       </c>
       <c r="D53" s="17" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R53" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="X53" s="17" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="54" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C54" s="17" t="s">
         <v>227</v>
       </c>
       <c r="D54" s="17" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="55" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R54" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="X54" s="17" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="55" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C55" s="17" t="s">
         <v>247</v>
       </c>
       <c r="D55" s="17" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="56" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R55" s="17" t="s">
+        <v>390</v>
+      </c>
+      <c r="X55" s="17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="56" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C56" s="17" t="s">
         <v>248</v>
       </c>
       <c r="D56" s="17" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R56" s="17" t="s">
+        <v>392</v>
+      </c>
+      <c r="X56" s="17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="57" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C57" s="17" t="s">
         <v>252</v>
       </c>
       <c r="D57" s="17" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="58" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R57" s="17" t="s">
+        <v>391</v>
+      </c>
+      <c r="X57" s="17" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="58" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C58" s="17" t="s">
         <v>279</v>
       </c>
       <c r="D58" s="17" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="59" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R58" s="17" t="s">
+        <v>399</v>
+      </c>
+      <c r="X58" s="17" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="59" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C59" s="17" t="s">
         <v>295</v>
       </c>
       <c r="D59" s="17" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="60" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R59" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="X59" s="17" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="60" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C60" s="17" t="s">
         <v>277</v>
       </c>
       <c r="D60" s="17" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="61" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R60" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="X60" s="17" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="61" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C61" s="17" t="s">
         <v>278</v>
       </c>
       <c r="D61" s="17" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="62" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R61" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="X61" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="62" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C62" s="17" t="s">
         <v>280</v>
       </c>
       <c r="D62" s="17" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="63" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R62" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="X62" s="17" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="63" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C63" s="17" t="s">
         <v>281</v>
       </c>
       <c r="D63" s="17" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="64" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R63" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="X63" s="17" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="64" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C64" s="17" t="s">
         <v>275</v>
       </c>
       <c r="D64" s="17" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="65" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R64" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="X64" s="17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="65" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C65" s="17" t="s">
         <v>306</v>
       </c>
       <c r="D65" s="17" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="66" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R65" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="X65" s="17" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="66" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C66" s="17" t="s">
         <v>293</v>
       </c>
       <c r="D66" s="17" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="67" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R66" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="X66" s="17" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="67" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C67" s="17" t="s">
         <v>285</v>
       </c>
       <c r="D67" s="17" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="68" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R67" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="X67" s="17" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="68" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C68" s="17" t="s">
         <v>267</v>
       </c>
       <c r="D68" s="17" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="69" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R68" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="X68" s="17" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="69" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C69" s="17" t="s">
         <v>256</v>
       </c>
       <c r="D69" s="17" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="70" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R69" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="X69" s="17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="70" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C70" s="17" t="s">
         <v>307</v>
       </c>
       <c r="D70" s="17" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="71" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R70" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="X70" s="17" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="71" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C71" s="17" t="s">
         <v>264</v>
       </c>
       <c r="D71" s="17" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="72" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R71" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="X71" s="17" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="72" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C72" s="17" t="s">
         <v>253</v>
       </c>
       <c r="D72" s="17" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="73" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R72" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="X72" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="73" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C73" s="17" t="s">
         <v>283</v>
       </c>
       <c r="D73" s="17" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="74" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R73" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="X73" s="17" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="74" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C74" s="17" t="s">
         <v>303</v>
       </c>
       <c r="D74" s="17" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="75" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R74" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="X74" s="17" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="75" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C75" s="17" t="s">
         <v>265</v>
       </c>
       <c r="D75" s="17" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="76" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R75" s="17" t="s">
+        <v>342</v>
+      </c>
+      <c r="X75" s="17" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="76" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C76" s="17" t="s">
         <v>254</v>
       </c>
       <c r="D76" s="17" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="77" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R76" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="X76" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="77" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C77" s="17" t="s">
         <v>286</v>
       </c>
       <c r="D77" s="17" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="78" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R77" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="X77" s="17" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="78" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C78" s="17" t="s">
         <v>287</v>
       </c>
       <c r="D78" s="17" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="79" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R78" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="X78" s="17" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="79" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C79" s="17" t="s">
         <v>294</v>
       </c>
       <c r="D79" s="17" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="80" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R79" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="X79" s="17" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="80" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C80" s="17" t="s">
         <v>282</v>
       </c>
       <c r="D80" s="17" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="81" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R80" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="X80" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="81" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C81" s="17" t="s">
         <v>276</v>
       </c>
       <c r="D81" s="17" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="82" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R81" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="X81" s="17" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="82" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C82" s="17" t="s">
         <v>291</v>
       </c>
       <c r="D82" s="17" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="83" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R82" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="X82" s="17" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="83" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C83" s="17" t="s">
         <v>289</v>
       </c>
       <c r="D83" s="17" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="84" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R83" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="X83" s="17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="84" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C84" s="17" t="s">
         <v>290</v>
       </c>
       <c r="D84" s="17" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="85" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R84" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="X84" s="17" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="85" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C85" s="17" t="s">
         <v>288</v>
       </c>
       <c r="D85" s="17" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="86" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R85" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="X85" s="17" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="86" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C86" s="17" t="s">
         <v>292</v>
       </c>
       <c r="D86" s="17" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="87" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R86" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="X86" s="17" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="87" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C87" s="17" t="s">
         <v>284</v>
       </c>
       <c r="D87" s="17" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="88" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R87" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="X87" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="88" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C88" s="17" t="s">
         <v>266</v>
       </c>
       <c r="D88" s="17" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="89" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R88" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="X88" s="17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="89" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C89" s="17" t="s">
         <v>255</v>
       </c>
       <c r="D89" s="17" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="90" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R89" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="X89" s="17" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="90" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C90" s="17" t="s">
         <v>268</v>
       </c>
       <c r="D90" s="17" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="91" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R90" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="X90" s="17" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="91" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C91" s="17" t="s">
         <v>257</v>
       </c>
       <c r="D91" s="17" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="92" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R91" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="X91" s="17" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="92" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C92" s="17" t="s">
         <v>269</v>
       </c>
       <c r="D92" s="17" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="93" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R92" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="X92" s="17" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="93" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C93" s="17" t="s">
         <v>258</v>
       </c>
       <c r="D93" s="17" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="94" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R93" s="17" t="s">
+        <v>646</v>
+      </c>
+      <c r="X93" s="17" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="94" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C94" s="17" t="s">
         <v>270</v>
       </c>
       <c r="D94" s="17" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="95" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R94" s="17" t="s">
+        <v>622</v>
+      </c>
+      <c r="X94" s="17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="95" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C95" s="17" t="s">
         <v>259</v>
       </c>
       <c r="D95" s="17" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="96" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R95" s="17" t="s">
+        <v>648</v>
+      </c>
+      <c r="X95" s="17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="96" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C96" s="17" t="s">
         <v>271</v>
       </c>
       <c r="D96" s="17" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="97" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R96" s="17" t="s">
+        <v>624</v>
+      </c>
+      <c r="X96" s="17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="97" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C97" s="17" t="s">
         <v>260</v>
       </c>
       <c r="D97" s="17" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="98" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R97" s="17" t="s">
+        <v>653</v>
+      </c>
+      <c r="X97" s="17" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="98" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C98" s="17" t="s">
         <v>272</v>
       </c>
       <c r="D98" s="17" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="99" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R98" s="17" t="s">
+        <v>629</v>
+      </c>
+      <c r="X98" s="17" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="99" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C99" s="17" t="s">
         <v>261</v>
       </c>
       <c r="D99" s="17" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="100" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R99" s="17" t="s">
+        <v>651</v>
+      </c>
+      <c r="X99" s="17" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="100" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C100" s="17" t="s">
         <v>273</v>
       </c>
       <c r="D100" s="17" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="101" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R100" s="17" t="s">
+        <v>627</v>
+      </c>
+      <c r="X100" s="17" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="101" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C101" s="17" t="s">
         <v>262</v>
       </c>
       <c r="D101" s="17" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="102" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R101" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="X101" s="17" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="102" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C102" s="17" t="s">
         <v>274</v>
       </c>
       <c r="D102" s="17" t="s">
         <v>646</v>
       </c>
-    </row>
-    <row r="103" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R102" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="X102" s="17" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="103" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C103" s="17" t="s">
         <v>263</v>
       </c>
       <c r="D103" s="17" t="s">
         <v>622</v>
       </c>
-    </row>
-    <row r="104" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R103" s="17" t="s">
+        <v>650</v>
+      </c>
+      <c r="X103" s="17" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="104" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C104" s="18" t="s">
         <v>314</v>
       </c>
       <c r="D104" s="17" t="s">
         <v>648</v>
       </c>
-    </row>
-    <row r="105" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R104" s="17" t="s">
+        <v>626</v>
+      </c>
+      <c r="X104" s="17" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="105" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C105" s="18" t="s">
         <v>315</v>
       </c>
       <c r="D105" s="17" t="s">
         <v>624</v>
       </c>
-    </row>
-    <row r="106" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R105" s="17" t="s">
+        <v>652</v>
+      </c>
+      <c r="X105" s="17" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="106" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C106" s="18" t="s">
         <v>316</v>
       </c>
       <c r="D106" s="17" t="s">
         <v>653</v>
       </c>
-    </row>
-    <row r="107" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R106" s="17" t="s">
+        <v>628</v>
+      </c>
+      <c r="X106" s="17" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="107" spans="3:24" x14ac:dyDescent="0.3">
       <c r="D107" s="17" t="s">
         <v>629</v>
       </c>
-    </row>
-    <row r="108" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R107" s="17" t="s">
+        <v>649</v>
+      </c>
+      <c r="X107" s="17" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="108" spans="3:24" x14ac:dyDescent="0.3">
       <c r="D108" s="17" t="s">
         <v>651</v>
       </c>
-    </row>
-    <row r="109" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R108" s="17" t="s">
+        <v>625</v>
+      </c>
+      <c r="X108" s="17" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="109" spans="3:24" x14ac:dyDescent="0.3">
       <c r="D109" s="17" t="s">
         <v>627</v>
       </c>
-    </row>
-    <row r="110" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R109" s="17" t="s">
+        <v>647</v>
+      </c>
+      <c r="X109" s="17" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="110" spans="3:24" x14ac:dyDescent="0.3">
       <c r="D110" s="17" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="111" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R110" s="17" t="s">
+        <v>623</v>
+      </c>
+      <c r="X110" s="17" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="111" spans="3:24" x14ac:dyDescent="0.3">
       <c r="D111" s="17" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="112" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="R111" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="X111" s="17" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="112" spans="3:24" x14ac:dyDescent="0.3">
       <c r="D112" s="17" t="s">
         <v>650</v>
       </c>
-    </row>
-    <row r="113" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R112" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="X112" s="17" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="113" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D113" s="17" t="s">
         <v>626</v>
       </c>
-    </row>
-    <row r="114" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R113" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="X113" s="17" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="114" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D114" s="17" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="115" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R114" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="X114" s="17" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="115" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D115" s="17" t="s">
         <v>628</v>
       </c>
-    </row>
-    <row r="116" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R115" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="X115" s="17" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="116" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D116" s="17" t="s">
         <v>649</v>
       </c>
-    </row>
-    <row r="117" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R116" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="X116" s="17" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="117" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D117" s="17" t="s">
         <v>625</v>
       </c>
-    </row>
-    <row r="118" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R117" s="17" t="s">
+        <v>661</v>
+      </c>
+      <c r="X117" s="17" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="118" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D118" s="17" t="s">
         <v>647</v>
       </c>
-    </row>
-    <row r="119" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R118" s="17" t="s">
+        <v>637</v>
+      </c>
+      <c r="X118" s="17" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="119" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D119" s="17" t="s">
         <v>623</v>
       </c>
-    </row>
-    <row r="120" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R119" s="17" t="s">
+        <v>662</v>
+      </c>
+      <c r="X119" s="17" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="120" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D120" s="17" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="121" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R120" s="17" t="s">
+        <v>638</v>
+      </c>
+      <c r="X120" s="17" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="121" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D121" s="17" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="122" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R121" s="17" t="s">
+        <v>654</v>
+      </c>
+      <c r="X121" s="17" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="122" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D122" s="17" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="123" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R122" s="17" t="s">
+        <v>630</v>
+      </c>
+      <c r="X122" s="17" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="123" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D123" s="17" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="124" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R123" s="17" t="s">
+        <v>655</v>
+      </c>
+      <c r="X123" s="17" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="124" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D124" s="17" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="125" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R124" s="17" t="s">
+        <v>631</v>
+      </c>
+      <c r="X124" s="17" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="125" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D125" s="17" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="126" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R125" s="17" t="s">
+        <v>656</v>
+      </c>
+      <c r="X125" s="17" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="126" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D126" s="17" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="127" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R126" s="17" t="s">
+        <v>632</v>
+      </c>
+      <c r="X126" s="17" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="127" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D127" s="17" t="s">
         <v>661</v>
       </c>
-    </row>
-    <row r="128" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R127" s="17" t="s">
+        <v>657</v>
+      </c>
+      <c r="X127" s="17" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="128" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D128" s="17" t="s">
         <v>637</v>
       </c>
-    </row>
-    <row r="129" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R128" s="17" t="s">
+        <v>633</v>
+      </c>
+      <c r="X128" s="17" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="129" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D129" s="17" t="s">
         <v>662</v>
       </c>
-    </row>
-    <row r="130" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R129" s="17" t="s">
+        <v>658</v>
+      </c>
+      <c r="X129" s="17" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="130" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D130" s="17" t="s">
         <v>638</v>
       </c>
-    </row>
-    <row r="131" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R130" s="17" t="s">
+        <v>634</v>
+      </c>
+      <c r="X130" s="17" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="131" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D131" s="17" t="s">
         <v>654</v>
       </c>
-    </row>
-    <row r="132" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R131" s="17" t="s">
+        <v>659</v>
+      </c>
+      <c r="X131" s="17" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="132" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D132" s="17" t="s">
         <v>630</v>
       </c>
-    </row>
-    <row r="133" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R132" s="17" t="s">
+        <v>635</v>
+      </c>
+      <c r="X132" s="17" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="133" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D133" s="17" t="s">
         <v>655</v>
       </c>
-    </row>
-    <row r="134" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R133" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="X133" s="17" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="134" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D134" s="17" t="s">
         <v>631</v>
       </c>
-    </row>
-    <row r="135" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R134" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="X134" s="17" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="135" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D135" s="17" t="s">
         <v>656</v>
       </c>
-    </row>
-    <row r="136" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R135" s="17" t="s">
+        <v>663</v>
+      </c>
+      <c r="X135" s="17" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="136" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D136" s="17" t="s">
         <v>632</v>
       </c>
-    </row>
-    <row r="137" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R136" s="17" t="s">
+        <v>639</v>
+      </c>
+      <c r="X136" s="17" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="137" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D137" s="17" t="s">
         <v>657</v>
       </c>
-    </row>
-    <row r="138" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R137" s="17" t="s">
+        <v>660</v>
+      </c>
+      <c r="X137" s="17" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="138" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D138" s="17" t="s">
         <v>633</v>
       </c>
-    </row>
-    <row r="139" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R138" s="17" t="s">
+        <v>636</v>
+      </c>
+      <c r="X138" s="17" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="139" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D139" s="17" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="140" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R139" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="X139" s="17" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="140" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D140" s="17" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="141" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R140" s="17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="141" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D141" s="17" t="s">
         <v>659</v>
       </c>
-    </row>
-    <row r="142" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R141" s="17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="142" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D142" s="17" t="s">
         <v>635</v>
       </c>
-    </row>
-    <row r="143" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R142" s="17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="143" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D143" s="17" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="144" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R143" s="17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="144" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D144" s="17" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="145" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R144" s="17" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="145" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D145" s="17" t="s">
         <v>663</v>
       </c>
-    </row>
-    <row r="146" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R145" s="17" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="146" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D146" s="17" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="147" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R146" s="17" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="147" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D147" s="17" t="s">
         <v>660</v>
       </c>
-    </row>
-    <row r="148" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R147" s="17" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="148" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D148" s="17" t="s">
         <v>636</v>
       </c>
-    </row>
-    <row r="149" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R148" s="17" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="149" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D149" s="17" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="150" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R149" s="17" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="150" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D150" s="17" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="151" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R150" s="17" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="151" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D151" s="17" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="152" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R151" s="17" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="152" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D152" s="17" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="153" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R152" s="17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="153" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D153" s="17" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="154" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R153" s="17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="154" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D154" s="17" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="155" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R154" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="155" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D155" s="17" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="156" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R155" s="17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="156" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D156" s="17" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="157" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R156" s="17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="157" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D157" s="17" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="158" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R157" s="17" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="158" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D158" s="17" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="159" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R158" s="17" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="159" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D159" s="17" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="160" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R159" s="17" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="160" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D160" s="17" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="161" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R160" s="17" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="161" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D161" s="17" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="162" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R161" s="17" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="162" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D162" s="17" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="163" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R162" s="17" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="163" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D163" s="17" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="164" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R163" s="17" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="164" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D164" s="17" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="165" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R164" s="17" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="165" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D165" s="17" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="166" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R165" s="17" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="166" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D166" s="17" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="167" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R166" s="17" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="167" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D167" s="17" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="168" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R167" s="17" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="168" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D168" s="17" t="s">
         <v>669</v>
       </c>
-    </row>
-    <row r="169" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R168" s="17" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="169" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D169" s="17" t="s">
         <v>645</v>
       </c>
-    </row>
-    <row r="170" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R169" s="17" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="170" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D170" s="17" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="171" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R170" s="17" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="171" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D171" s="17" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="172" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R171" s="17" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="172" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D172" s="17" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="173" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R172" s="17" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="173" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D173" s="17" t="s">
         <v>665</v>
       </c>
-    </row>
-    <row r="174" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R173" s="17" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="174" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D174" s="17" t="s">
         <v>641</v>
       </c>
-    </row>
-    <row r="175" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R174" s="17" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="175" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D175" s="17" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="176" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R175" s="17" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="176" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D176" s="17" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="177" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R176" s="17" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="177" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D177" s="17" t="s">
         <v>668</v>
       </c>
-    </row>
-    <row r="178" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R177" s="17" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="178" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D178" s="17" t="s">
         <v>644</v>
       </c>
-    </row>
-    <row r="179" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R178" s="17" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="179" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D179" s="17" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="180" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R179" s="17" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="180" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D180" s="17" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="181" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R180" s="17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="181" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D181" s="17" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="182" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R181" s="17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="182" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D182" s="17" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="183" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R182" s="17" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="183" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D183" s="17" t="s">
         <v>664</v>
       </c>
-    </row>
-    <row r="184" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R183" s="17" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="184" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D184" s="17" t="s">
         <v>640</v>
       </c>
-    </row>
-    <row r="185" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="R184" s="17" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="185" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D185" s="17" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="186" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="186" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D186" s="17" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="187" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="187" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D187" s="17" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="188" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="188" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D188" s="17" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="189" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="189" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D189" s="17" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="190" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="190" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D190" s="17" t="s">
         <v>667</v>
       </c>
     </row>
-    <row r="191" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="191" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D191" s="17" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="192" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="192" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D192" s="17" t="s">
         <v>193</v>
       </c>
@@ -35644,8 +36642,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="D2:D219">
-    <sortCondition ref="D219"/>
+  <sortState ref="R2:R184">
+    <sortCondition ref="R2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add missing actions in Survey view. Added HomePageActions. Fixed bugs in existing actions
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCases.xlsx
+++ b/selenium-wd/data/TestCases.xlsx
@@ -206,7 +206,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6157" uniqueCount="676">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6161" uniqueCount="679">
   <si>
     <t>ID</t>
   </si>
@@ -2234,6 +2234,15 @@
   </si>
   <si>
     <t>verifySurveyViewPageIsOpened</t>
+  </si>
+  <si>
+    <t>clickOnViewAllDrivingSurveysLink</t>
+  </si>
+  <si>
+    <t>clickOnFirstOnlineSurveyorLink</t>
+  </si>
+  <si>
+    <t>clickOnFirstMatchingDrivingSurvey</t>
   </si>
 </sst>
 </file>
@@ -33408,8 +33417,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:Z219"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="R125" workbookViewId="0">
+      <selection activeCell="X140" sqref="X2:X140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -34386,6 +34395,9 @@
       <c r="D13" s="17" t="s">
         <v>57</v>
       </c>
+      <c r="G13" s="17" t="s">
+        <v>676</v>
+      </c>
       <c r="H13" s="17" t="s">
         <v>48</v>
       </c>
@@ -34406,6 +34418,9 @@
       <c r="D14" s="17" t="s">
         <v>473</v>
       </c>
+      <c r="G14" s="17" t="s">
+        <v>677</v>
+      </c>
       <c r="H14" s="17" t="s">
         <v>197</v>
       </c>
@@ -34426,6 +34441,9 @@
       <c r="D15" s="17" t="s">
         <v>58</v>
       </c>
+      <c r="G15" s="17" t="s">
+        <v>678</v>
+      </c>
       <c r="H15" s="17" t="s">
         <v>196</v>
       </c>
@@ -34690,7 +34708,7 @@
         <v>48</v>
       </c>
       <c r="X31" s="17" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.3">
@@ -34704,7 +34722,7 @@
         <v>64</v>
       </c>
       <c r="X32" s="17" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="33" spans="3:24" x14ac:dyDescent="0.3">
@@ -34718,7 +34736,7 @@
         <v>393</v>
       </c>
       <c r="X33" s="17" t="s">
-        <v>132</v>
+        <v>398</v>
       </c>
     </row>
     <row r="34" spans="3:24" x14ac:dyDescent="0.3">
@@ -34732,7 +34750,7 @@
         <v>395</v>
       </c>
       <c r="X34" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="35" spans="3:24" x14ac:dyDescent="0.3">
@@ -34746,7 +34764,7 @@
         <v>394</v>
       </c>
       <c r="X35" s="17" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
     </row>
     <row r="36" spans="3:24" x14ac:dyDescent="0.3">
@@ -34760,7 +34778,7 @@
         <v>398</v>
       </c>
       <c r="X36" s="17" t="s">
-        <v>398</v>
+        <v>151</v>
       </c>
     </row>
     <row r="37" spans="3:24" x14ac:dyDescent="0.3">
@@ -34998,7 +35016,7 @@
         <v>141</v>
       </c>
       <c r="X53" s="17" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="54" spans="3:24" x14ac:dyDescent="0.3">
@@ -35012,7 +35030,7 @@
         <v>157</v>
       </c>
       <c r="X54" s="17" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="55" spans="3:24" x14ac:dyDescent="0.3">
@@ -35026,7 +35044,7 @@
         <v>390</v>
       </c>
       <c r="X55" s="17" t="s">
-        <v>122</v>
+        <v>399</v>
       </c>
     </row>
     <row r="56" spans="3:24" x14ac:dyDescent="0.3">
@@ -35040,7 +35058,7 @@
         <v>392</v>
       </c>
       <c r="X56" s="17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="57" spans="3:24" x14ac:dyDescent="0.3">
@@ -35054,7 +35072,7 @@
         <v>391</v>
       </c>
       <c r="X57" s="17" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
     </row>
     <row r="58" spans="3:24" x14ac:dyDescent="0.3">
@@ -35068,7 +35086,7 @@
         <v>399</v>
       </c>
       <c r="X58" s="17" t="s">
-        <v>399</v>
+        <v>143</v>
       </c>
     </row>
     <row r="59" spans="3:24" x14ac:dyDescent="0.3">
@@ -35474,7 +35492,7 @@
         <v>168</v>
       </c>
       <c r="X87" s="17" t="s">
-        <v>71</v>
+        <v>646</v>
       </c>
     </row>
     <row r="88" spans="3:24" x14ac:dyDescent="0.3">
@@ -35488,7 +35506,7 @@
         <v>194</v>
       </c>
       <c r="X88" s="17" t="s">
-        <v>72</v>
+        <v>622</v>
       </c>
     </row>
     <row r="89" spans="3:24" x14ac:dyDescent="0.3">
@@ -35502,7 +35520,7 @@
         <v>175</v>
       </c>
       <c r="X89" s="17" t="s">
-        <v>675</v>
+        <v>648</v>
       </c>
     </row>
     <row r="90" spans="3:24" x14ac:dyDescent="0.3">
@@ -35516,7 +35534,7 @@
         <v>167</v>
       </c>
       <c r="X90" s="17" t="s">
-        <v>183</v>
+        <v>624</v>
       </c>
     </row>
     <row r="91" spans="3:24" x14ac:dyDescent="0.3">
@@ -35530,7 +35548,7 @@
         <v>180</v>
       </c>
       <c r="X91" s="17" t="s">
-        <v>181</v>
+        <v>653</v>
       </c>
     </row>
     <row r="92" spans="3:24" x14ac:dyDescent="0.3">
@@ -35544,7 +35562,7 @@
         <v>172</v>
       </c>
       <c r="X92" s="17" t="s">
-        <v>177</v>
+        <v>629</v>
       </c>
     </row>
     <row r="93" spans="3:24" x14ac:dyDescent="0.3">
@@ -35558,7 +35576,7 @@
         <v>646</v>
       </c>
       <c r="X93" s="17" t="s">
-        <v>169</v>
+        <v>651</v>
       </c>
     </row>
     <row r="94" spans="3:24" x14ac:dyDescent="0.3">
@@ -35572,7 +35590,7 @@
         <v>622</v>
       </c>
       <c r="X94" s="17" t="s">
-        <v>75</v>
+        <v>627</v>
       </c>
     </row>
     <row r="95" spans="3:24" x14ac:dyDescent="0.3">
@@ -35586,7 +35604,7 @@
         <v>648</v>
       </c>
       <c r="X95" s="17" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="96" spans="3:24" x14ac:dyDescent="0.3">
@@ -35600,7 +35618,7 @@
         <v>624</v>
       </c>
       <c r="X96" s="17" t="s">
-        <v>174</v>
+        <v>72</v>
       </c>
     </row>
     <row r="97" spans="3:24" x14ac:dyDescent="0.3">
@@ -35614,7 +35632,7 @@
         <v>653</v>
       </c>
       <c r="X97" s="17" t="s">
-        <v>166</v>
+        <v>650</v>
       </c>
     </row>
     <row r="98" spans="3:24" x14ac:dyDescent="0.3">
@@ -35628,7 +35646,7 @@
         <v>629</v>
       </c>
       <c r="X98" s="17" t="s">
-        <v>173</v>
+        <v>626</v>
       </c>
     </row>
     <row r="99" spans="3:24" x14ac:dyDescent="0.3">
@@ -35642,7 +35660,7 @@
         <v>651</v>
       </c>
       <c r="X99" s="17" t="s">
-        <v>165</v>
+        <v>652</v>
       </c>
     </row>
     <row r="100" spans="3:24" x14ac:dyDescent="0.3">
@@ -35656,7 +35674,7 @@
         <v>627</v>
       </c>
       <c r="X100" s="17" t="s">
-        <v>203</v>
+        <v>628</v>
       </c>
     </row>
     <row r="101" spans="3:24" x14ac:dyDescent="0.3">
@@ -35670,7 +35688,7 @@
         <v>71</v>
       </c>
       <c r="X101" s="17" t="s">
-        <v>204</v>
+        <v>649</v>
       </c>
     </row>
     <row r="102" spans="3:24" x14ac:dyDescent="0.3">
@@ -35684,7 +35702,7 @@
         <v>72</v>
       </c>
       <c r="X102" s="17" t="s">
-        <v>385</v>
+        <v>625</v>
       </c>
     </row>
     <row r="103" spans="3:24" x14ac:dyDescent="0.3">
@@ -35698,7 +35716,7 @@
         <v>650</v>
       </c>
       <c r="X103" s="17" t="s">
-        <v>386</v>
+        <v>647</v>
       </c>
     </row>
     <row r="104" spans="3:24" x14ac:dyDescent="0.3">
@@ -35712,7 +35730,7 @@
         <v>626</v>
       </c>
       <c r="X104" s="17" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
     </row>
     <row r="105" spans="3:24" x14ac:dyDescent="0.3">
@@ -35726,7 +35744,7 @@
         <v>652</v>
       </c>
       <c r="X105" s="17" t="s">
-        <v>623</v>
+        <v>183</v>
       </c>
     </row>
     <row r="106" spans="3:24" x14ac:dyDescent="0.3">
@@ -35740,7 +35758,7 @@
         <v>628</v>
       </c>
       <c r="X106" s="17" t="s">
-        <v>624</v>
+        <v>181</v>
       </c>
     </row>
     <row r="107" spans="3:24" x14ac:dyDescent="0.3">
@@ -35751,7 +35769,7 @@
         <v>649</v>
       </c>
       <c r="X107" s="17" t="s">
-        <v>625</v>
+        <v>177</v>
       </c>
     </row>
     <row r="108" spans="3:24" x14ac:dyDescent="0.3">
@@ -35762,7 +35780,7 @@
         <v>625</v>
       </c>
       <c r="X108" s="17" t="s">
-        <v>626</v>
+        <v>169</v>
       </c>
     </row>
     <row r="109" spans="3:24" x14ac:dyDescent="0.3">
@@ -35773,7 +35791,7 @@
         <v>647</v>
       </c>
       <c r="X109" s="17" t="s">
-        <v>627</v>
+        <v>661</v>
       </c>
     </row>
     <row r="110" spans="3:24" x14ac:dyDescent="0.3">
@@ -35784,7 +35802,7 @@
         <v>623</v>
       </c>
       <c r="X110" s="17" t="s">
-        <v>628</v>
+        <v>637</v>
       </c>
     </row>
     <row r="111" spans="3:24" x14ac:dyDescent="0.3">
@@ -35795,7 +35813,7 @@
         <v>183</v>
       </c>
       <c r="X111" s="17" t="s">
-        <v>629</v>
+        <v>662</v>
       </c>
     </row>
     <row r="112" spans="3:24" x14ac:dyDescent="0.3">
@@ -35806,7 +35824,7 @@
         <v>181</v>
       </c>
       <c r="X112" s="17" t="s">
-        <v>630</v>
+        <v>638</v>
       </c>
     </row>
     <row r="113" spans="4:24" x14ac:dyDescent="0.3">
@@ -35817,7 +35835,7 @@
         <v>73</v>
       </c>
       <c r="X113" s="17" t="s">
-        <v>631</v>
+        <v>654</v>
       </c>
     </row>
     <row r="114" spans="4:24" x14ac:dyDescent="0.3">
@@ -35828,7 +35846,7 @@
         <v>74</v>
       </c>
       <c r="X114" s="17" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
     </row>
     <row r="115" spans="4:24" x14ac:dyDescent="0.3">
@@ -35839,7 +35857,7 @@
         <v>177</v>
       </c>
       <c r="X115" s="17" t="s">
-        <v>633</v>
+        <v>655</v>
       </c>
     </row>
     <row r="116" spans="4:24" x14ac:dyDescent="0.3">
@@ -35850,7 +35868,7 @@
         <v>169</v>
       </c>
       <c r="X116" s="17" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
     </row>
     <row r="117" spans="4:24" x14ac:dyDescent="0.3">
@@ -35861,7 +35879,7 @@
         <v>661</v>
       </c>
       <c r="X117" s="17" t="s">
-        <v>635</v>
+        <v>656</v>
       </c>
     </row>
     <row r="118" spans="4:24" x14ac:dyDescent="0.3">
@@ -35872,7 +35890,7 @@
         <v>637</v>
       </c>
       <c r="X118" s="17" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
     </row>
     <row r="119" spans="4:24" x14ac:dyDescent="0.3">
@@ -35883,7 +35901,7 @@
         <v>662</v>
       </c>
       <c r="X119" s="17" t="s">
-        <v>637</v>
+        <v>657</v>
       </c>
     </row>
     <row r="120" spans="4:24" x14ac:dyDescent="0.3">
@@ -35894,7 +35912,7 @@
         <v>638</v>
       </c>
       <c r="X120" s="17" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
     </row>
     <row r="121" spans="4:24" x14ac:dyDescent="0.3">
@@ -35905,7 +35923,7 @@
         <v>654</v>
       </c>
       <c r="X121" s="17" t="s">
-        <v>639</v>
+        <v>658</v>
       </c>
     </row>
     <row r="122" spans="4:24" x14ac:dyDescent="0.3">
@@ -35916,7 +35934,7 @@
         <v>630</v>
       </c>
       <c r="X122" s="17" t="s">
-        <v>646</v>
+        <v>634</v>
       </c>
     </row>
     <row r="123" spans="4:24" x14ac:dyDescent="0.3">
@@ -35927,7 +35945,7 @@
         <v>655</v>
       </c>
       <c r="X123" s="17" t="s">
-        <v>647</v>
+        <v>659</v>
       </c>
     </row>
     <row r="124" spans="4:24" x14ac:dyDescent="0.3">
@@ -35938,7 +35956,7 @@
         <v>631</v>
       </c>
       <c r="X124" s="17" t="s">
-        <v>648</v>
+        <v>635</v>
       </c>
     </row>
     <row r="125" spans="4:24" x14ac:dyDescent="0.3">
@@ -35949,7 +35967,7 @@
         <v>656</v>
       </c>
       <c r="X125" s="17" t="s">
-        <v>649</v>
+        <v>75</v>
       </c>
     </row>
     <row r="126" spans="4:24" x14ac:dyDescent="0.3">
@@ -35960,7 +35978,7 @@
         <v>632</v>
       </c>
       <c r="X126" s="17" t="s">
-        <v>650</v>
+        <v>76</v>
       </c>
     </row>
     <row r="127" spans="4:24" x14ac:dyDescent="0.3">
@@ -35971,7 +35989,7 @@
         <v>657</v>
       </c>
       <c r="X127" s="17" t="s">
-        <v>651</v>
+        <v>663</v>
       </c>
     </row>
     <row r="128" spans="4:24" x14ac:dyDescent="0.3">
@@ -35982,7 +36000,7 @@
         <v>633</v>
       </c>
       <c r="X128" s="17" t="s">
-        <v>652</v>
+        <v>639</v>
       </c>
     </row>
     <row r="129" spans="4:24" x14ac:dyDescent="0.3">
@@ -35993,7 +36011,7 @@
         <v>658</v>
       </c>
       <c r="X129" s="17" t="s">
-        <v>653</v>
+        <v>660</v>
       </c>
     </row>
     <row r="130" spans="4:24" x14ac:dyDescent="0.3">
@@ -36004,7 +36022,7 @@
         <v>634</v>
       </c>
       <c r="X130" s="17" t="s">
-        <v>654</v>
+        <v>636</v>
       </c>
     </row>
     <row r="131" spans="4:24" x14ac:dyDescent="0.3">
@@ -36015,7 +36033,7 @@
         <v>659</v>
       </c>
       <c r="X131" s="17" t="s">
-        <v>655</v>
+        <v>174</v>
       </c>
     </row>
     <row r="132" spans="4:24" x14ac:dyDescent="0.3">
@@ -36026,7 +36044,7 @@
         <v>635</v>
       </c>
       <c r="X132" s="17" t="s">
-        <v>656</v>
+        <v>166</v>
       </c>
     </row>
     <row r="133" spans="4:24" x14ac:dyDescent="0.3">
@@ -36037,7 +36055,7 @@
         <v>75</v>
       </c>
       <c r="X133" s="17" t="s">
-        <v>657</v>
+        <v>173</v>
       </c>
     </row>
     <row r="134" spans="4:24" x14ac:dyDescent="0.3">
@@ -36048,7 +36066,7 @@
         <v>76</v>
       </c>
       <c r="X134" s="17" t="s">
-        <v>658</v>
+        <v>165</v>
       </c>
     </row>
     <row r="135" spans="4:24" x14ac:dyDescent="0.3">
@@ -36059,7 +36077,7 @@
         <v>663</v>
       </c>
       <c r="X135" s="17" t="s">
-        <v>659</v>
+        <v>204</v>
       </c>
     </row>
     <row r="136" spans="4:24" x14ac:dyDescent="0.3">
@@ -36070,7 +36088,7 @@
         <v>639</v>
       </c>
       <c r="X136" s="17" t="s">
-        <v>660</v>
+        <v>203</v>
       </c>
     </row>
     <row r="137" spans="4:24" x14ac:dyDescent="0.3">
@@ -36081,7 +36099,7 @@
         <v>660</v>
       </c>
       <c r="X137" s="17" t="s">
-        <v>661</v>
+        <v>385</v>
       </c>
     </row>
     <row r="138" spans="4:24" x14ac:dyDescent="0.3">
@@ -36092,7 +36110,7 @@
         <v>636</v>
       </c>
       <c r="X138" s="17" t="s">
-        <v>662</v>
+        <v>323</v>
       </c>
     </row>
     <row r="139" spans="4:24" x14ac:dyDescent="0.3">
@@ -36103,7 +36121,7 @@
         <v>77</v>
       </c>
       <c r="X139" s="17" t="s">
-        <v>663</v>
+        <v>386</v>
       </c>
     </row>
     <row r="140" spans="4:24" x14ac:dyDescent="0.3">
@@ -36113,6 +36131,9 @@
       <c r="R140" s="17" t="s">
         <v>78</v>
       </c>
+      <c r="X140" s="17" t="s">
+        <v>675</v>
+      </c>
     </row>
     <row r="141" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D141" s="17" t="s">
@@ -36642,8 +36663,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="R2:R184">
-    <sortCondition ref="R2"/>
+  <sortState ref="X2:X140">
+    <sortCondition ref="X140"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added SurveyPageTest to regression suite. Added new actions to excelsheet
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCases.xlsx
+++ b/selenium-wd/data/TestCases.xlsx
@@ -206,7 +206,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6161" uniqueCount="679">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6175" uniqueCount="685">
   <si>
     <t>ID</t>
   </si>
@@ -2243,6 +2243,24 @@
   </si>
   <si>
     <t>clickOnFirstMatchingDrivingSurvey</t>
+  </si>
+  <si>
+    <t>verifyIsotopicCaptureResultIsPresentOnMap</t>
+  </si>
+  <si>
+    <t>verifyIsotopicCaptureResultIsNotPresentOnMap</t>
+  </si>
+  <si>
+    <t>verifyRefGasCaptureResultIsPresentOnMap</t>
+  </si>
+  <si>
+    <t>verifyRefGasCaptureResultIsNotPresentOnMap</t>
+  </si>
+  <si>
+    <t>verifySurveyInfoStartTimeLabelHasCorrectTimeFormat</t>
+  </si>
+  <si>
+    <t>verifySurveyInfoEndTimeLabelHasCorrectTimeFormat</t>
   </si>
 </sst>
 </file>
@@ -3901,8 +3919,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:H1580"/>
   <sheetViews>
-    <sheetView topLeftCell="A1556" workbookViewId="0">
-      <selection activeCell="B1572" sqref="B1572"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33415,10 +33433,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:Z219"/>
+  <dimension ref="A1:Z223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R125" workbookViewId="0">
-      <selection activeCell="X140" sqref="X2:X140"/>
+    <sheetView tabSelected="1" topLeftCell="R173" workbookViewId="0">
+      <selection activeCell="R188" sqref="R2:R188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -36055,7 +36073,7 @@
         <v>75</v>
       </c>
       <c r="X133" s="17" t="s">
-        <v>173</v>
+        <v>680</v>
       </c>
     </row>
     <row r="134" spans="4:24" x14ac:dyDescent="0.3">
@@ -36066,7 +36084,7 @@
         <v>76</v>
       </c>
       <c r="X134" s="17" t="s">
-        <v>165</v>
+        <v>679</v>
       </c>
     </row>
     <row r="135" spans="4:24" x14ac:dyDescent="0.3">
@@ -36077,7 +36095,7 @@
         <v>663</v>
       </c>
       <c r="X135" s="17" t="s">
-        <v>204</v>
+        <v>173</v>
       </c>
     </row>
     <row r="136" spans="4:24" x14ac:dyDescent="0.3">
@@ -36088,7 +36106,7 @@
         <v>639</v>
       </c>
       <c r="X136" s="17" t="s">
-        <v>203</v>
+        <v>165</v>
       </c>
     </row>
     <row r="137" spans="4:24" x14ac:dyDescent="0.3">
@@ -36099,7 +36117,7 @@
         <v>660</v>
       </c>
       <c r="X137" s="17" t="s">
-        <v>385</v>
+        <v>204</v>
       </c>
     </row>
     <row r="138" spans="4:24" x14ac:dyDescent="0.3">
@@ -36110,7 +36128,7 @@
         <v>636</v>
       </c>
       <c r="X138" s="17" t="s">
-        <v>323</v>
+        <v>203</v>
       </c>
     </row>
     <row r="139" spans="4:24" x14ac:dyDescent="0.3">
@@ -36121,7 +36139,7 @@
         <v>77</v>
       </c>
       <c r="X139" s="17" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="140" spans="4:24" x14ac:dyDescent="0.3">
@@ -36132,7 +36150,7 @@
         <v>78</v>
       </c>
       <c r="X140" s="17" t="s">
-        <v>675</v>
+        <v>323</v>
       </c>
     </row>
     <row r="141" spans="4:24" x14ac:dyDescent="0.3">
@@ -36142,6 +36160,9 @@
       <c r="R141" s="17" t="s">
         <v>79</v>
       </c>
+      <c r="X141" s="17" t="s">
+        <v>682</v>
+      </c>
     </row>
     <row r="142" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D142" s="17" t="s">
@@ -36150,6 +36171,9 @@
       <c r="R142" s="17" t="s">
         <v>80</v>
       </c>
+      <c r="X142" s="17" t="s">
+        <v>681</v>
+      </c>
     </row>
     <row r="143" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D143" s="17" t="s">
@@ -36158,6 +36182,9 @@
       <c r="R143" s="17" t="s">
         <v>174</v>
       </c>
+      <c r="X143" s="17" t="s">
+        <v>386</v>
+      </c>
     </row>
     <row r="144" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D144" s="17" t="s">
@@ -36166,505 +36193,546 @@
       <c r="R144" s="17" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="145" spans="4:18" x14ac:dyDescent="0.3">
+      <c r="X144" s="17" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="145" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D145" s="17" t="s">
         <v>663</v>
       </c>
       <c r="R145" s="17" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="146" spans="4:18" x14ac:dyDescent="0.3">
+        <v>680</v>
+      </c>
+      <c r="X145" s="17" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="146" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D146" s="17" t="s">
         <v>639</v>
       </c>
       <c r="R146" s="17" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="147" spans="4:18" x14ac:dyDescent="0.3">
+        <v>679</v>
+      </c>
+      <c r="X146" s="17" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="147" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D147" s="17" t="s">
         <v>660</v>
       </c>
       <c r="R147" s="17" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="148" spans="4:18" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="148" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D148" s="17" t="s">
         <v>636</v>
       </c>
       <c r="R148" s="17" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="149" spans="4:18" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="149" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D149" s="17" t="s">
         <v>77</v>
       </c>
       <c r="R149" s="17" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="150" spans="4:18" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="150" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D150" s="17" t="s">
         <v>78</v>
       </c>
       <c r="R150" s="17" t="s">
-        <v>672</v>
-      </c>
-    </row>
-    <row r="151" spans="4:18" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="151" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D151" s="17" t="s">
         <v>79</v>
       </c>
       <c r="R151" s="17" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="152" spans="4:18" x14ac:dyDescent="0.3">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="152" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D152" s="17" t="s">
         <v>80</v>
       </c>
       <c r="R152" s="17" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="153" spans="4:18" x14ac:dyDescent="0.3">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="153" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D153" s="17" t="s">
         <v>174</v>
       </c>
       <c r="R153" s="17" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="154" spans="4:18" x14ac:dyDescent="0.3">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="154" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D154" s="17" t="s">
         <v>166</v>
       </c>
       <c r="R154" s="17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="155" spans="4:24" x14ac:dyDescent="0.3">
+      <c r="D155" s="17" t="s">
+        <v>680</v>
+      </c>
+      <c r="R155" s="17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="156" spans="4:24" x14ac:dyDescent="0.3">
+      <c r="D156" s="17" t="s">
+        <v>679</v>
+      </c>
+      <c r="R156" s="17" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="155" spans="4:18" x14ac:dyDescent="0.3">
-      <c r="D155" s="17" t="s">
+    <row r="157" spans="4:24" x14ac:dyDescent="0.3">
+      <c r="D157" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="R155" s="17" t="s">
+      <c r="R157" s="17" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="156" spans="4:18" x14ac:dyDescent="0.3">
-      <c r="D156" s="17" t="s">
+    <row r="158" spans="4:24" x14ac:dyDescent="0.3">
+      <c r="D158" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="R156" s="17" t="s">
+      <c r="R158" s="17" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="157" spans="4:18" x14ac:dyDescent="0.3">
-      <c r="D157" s="17" t="s">
+    <row r="159" spans="4:24" x14ac:dyDescent="0.3">
+      <c r="D159" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="R157" s="17" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="158" spans="4:18" x14ac:dyDescent="0.3">
-      <c r="D158" s="17" t="s">
+      <c r="R159" s="17" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="160" spans="4:24" x14ac:dyDescent="0.3">
+      <c r="D160" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="R158" s="17" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="159" spans="4:18" x14ac:dyDescent="0.3">
-      <c r="D159" s="17" t="s">
-        <v>385</v>
-      </c>
-      <c r="R159" s="17" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="160" spans="4:18" x14ac:dyDescent="0.3">
-      <c r="D160" s="17" t="s">
-        <v>323</v>
-      </c>
       <c r="R160" s="17" t="s">
-        <v>205</v>
+        <v>681</v>
       </c>
     </row>
     <row r="161" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D161" s="17" t="s">
-        <v>81</v>
+        <v>385</v>
       </c>
       <c r="R161" s="17" t="s">
-        <v>673</v>
+        <v>386</v>
       </c>
     </row>
     <row r="162" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D162" s="17" t="s">
-        <v>82</v>
+        <v>323</v>
       </c>
       <c r="R162" s="17" t="s">
-        <v>206</v>
+        <v>674</v>
       </c>
     </row>
     <row r="163" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D163" s="17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="R163" s="17" t="s">
-        <v>193</v>
+        <v>209</v>
       </c>
     </row>
     <row r="164" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D164" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="R164" s="17" t="s">
-        <v>192</v>
+        <v>205</v>
       </c>
     </row>
     <row r="165" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D165" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="R165" s="17" t="s">
-        <v>185</v>
+        <v>673</v>
       </c>
     </row>
     <row r="166" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D166" s="17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="R166" s="17" t="s">
-        <v>191</v>
+        <v>206</v>
       </c>
     </row>
     <row r="167" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D167" s="17" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="R167" s="17" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="168" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D168" s="17" t="s">
-        <v>669</v>
+        <v>86</v>
       </c>
       <c r="R168" s="17" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
     </row>
     <row r="169" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D169" s="17" t="s">
-        <v>645</v>
+        <v>87</v>
       </c>
       <c r="R169" s="17" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="170" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D170" s="17" t="s">
-        <v>386</v>
+        <v>669</v>
       </c>
       <c r="R170" s="17" t="s">
-        <v>550</v>
+        <v>191</v>
       </c>
     </row>
     <row r="171" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D171" s="17" t="s">
-        <v>88</v>
+        <v>645</v>
       </c>
       <c r="R171" s="17" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
     </row>
     <row r="172" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D172" s="17" t="s">
-        <v>89</v>
+        <v>682</v>
       </c>
       <c r="R172" s="17" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
     </row>
     <row r="173" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D173" s="17" t="s">
-        <v>665</v>
+        <v>681</v>
       </c>
       <c r="R173" s="17" t="s">
-        <v>325</v>
+        <v>187</v>
       </c>
     </row>
     <row r="174" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D174" s="17" t="s">
-        <v>641</v>
+        <v>386</v>
       </c>
       <c r="R174" s="17" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="175" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D175" s="17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R175" s="17" t="s">
-        <v>326</v>
+        <v>188</v>
       </c>
     </row>
     <row r="176" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D176" s="17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R176" s="17" t="s">
-        <v>189</v>
+        <v>207</v>
       </c>
     </row>
     <row r="177" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D177" s="17" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="R177" s="17" t="s">
-        <v>552</v>
+        <v>325</v>
       </c>
     </row>
     <row r="178" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D178" s="17" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="R178" s="17" t="s">
-        <v>208</v>
+        <v>551</v>
       </c>
     </row>
     <row r="179" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D179" s="17" t="s">
-        <v>321</v>
+        <v>90</v>
       </c>
       <c r="R179" s="17" t="s">
-        <v>190</v>
+        <v>326</v>
       </c>
     </row>
     <row r="180" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D180" s="17" t="s">
-        <v>320</v>
+        <v>91</v>
       </c>
       <c r="R180" s="17" t="s">
-        <v>98</v>
+        <v>189</v>
       </c>
     </row>
     <row r="181" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D181" s="17" t="s">
-        <v>92</v>
+        <v>668</v>
       </c>
       <c r="R181" s="17" t="s">
-        <v>99</v>
+        <v>552</v>
       </c>
     </row>
     <row r="182" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D182" s="17" t="s">
-        <v>93</v>
+        <v>644</v>
       </c>
       <c r="R182" s="17" t="s">
-        <v>184</v>
+        <v>208</v>
       </c>
     </row>
     <row r="183" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D183" s="17" t="s">
-        <v>664</v>
+        <v>321</v>
       </c>
       <c r="R183" s="17" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
     </row>
     <row r="184" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D184" s="17" t="s">
-        <v>640</v>
+        <v>320</v>
       </c>
       <c r="R184" s="17" t="s">
-        <v>461</v>
+        <v>98</v>
       </c>
     </row>
     <row r="185" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D185" s="17" t="s">
-        <v>209</v>
+        <v>92</v>
+      </c>
+      <c r="R185" s="17" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="186" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D186" s="17" t="s">
-        <v>205</v>
+        <v>93</v>
+      </c>
+      <c r="R186" s="17" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="187" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D187" s="17" t="s">
-        <v>206</v>
+        <v>664</v>
+      </c>
+      <c r="R187" s="17" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="188" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D188" s="17" t="s">
-        <v>94</v>
+        <v>640</v>
+      </c>
+      <c r="R188" s="17" t="s">
+        <v>461</v>
       </c>
     </row>
     <row r="189" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D189" s="17" t="s">
-        <v>95</v>
+        <v>209</v>
       </c>
     </row>
     <row r="190" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D190" s="17" t="s">
-        <v>667</v>
+        <v>205</v>
       </c>
     </row>
     <row r="191" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D191" s="17" t="s">
-        <v>643</v>
+        <v>206</v>
       </c>
     </row>
     <row r="192" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D192" s="17" t="s">
-        <v>193</v>
+        <v>94</v>
       </c>
     </row>
     <row r="193" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D193" s="17" t="s">
-        <v>192</v>
+        <v>95</v>
       </c>
     </row>
     <row r="194" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D194" s="17" t="s">
-        <v>185</v>
+        <v>667</v>
       </c>
     </row>
     <row r="195" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D195" s="17" t="s">
-        <v>191</v>
+        <v>643</v>
       </c>
     </row>
     <row r="196" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D196" s="17" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="197" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D197" s="17" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
     </row>
     <row r="198" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D198" s="17" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="199" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D199" s="17" t="s">
-        <v>550</v>
+        <v>191</v>
       </c>
     </row>
     <row r="200" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D200" s="17" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
     </row>
     <row r="201" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D201" s="17" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
     </row>
     <row r="202" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D202" s="17" t="s">
-        <v>325</v>
+        <v>187</v>
       </c>
     </row>
     <row r="203" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D203" s="17" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="204" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D204" s="17" t="s">
-        <v>326</v>
+        <v>188</v>
       </c>
     </row>
     <row r="205" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D205" s="17" t="s">
-        <v>189</v>
+        <v>207</v>
       </c>
     </row>
     <row r="206" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D206" s="17" t="s">
-        <v>552</v>
+        <v>325</v>
       </c>
     </row>
     <row r="207" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D207" s="17" t="s">
-        <v>208</v>
+        <v>551</v>
       </c>
     </row>
     <row r="208" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D208" s="17" t="s">
-        <v>190</v>
+        <v>326</v>
       </c>
     </row>
     <row r="209" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D209" s="17" t="s">
-        <v>319</v>
+        <v>189</v>
       </c>
     </row>
     <row r="210" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D210" s="17" t="s">
-        <v>96</v>
+        <v>552</v>
       </c>
     </row>
     <row r="211" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D211" s="17" t="s">
-        <v>324</v>
+        <v>208</v>
       </c>
     </row>
     <row r="212" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D212" s="17" t="s">
-        <v>97</v>
+        <v>190</v>
       </c>
     </row>
     <row r="213" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D213" s="17" t="s">
-        <v>666</v>
+        <v>319</v>
       </c>
     </row>
     <row r="214" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D214" s="17" t="s">
-        <v>642</v>
+        <v>96</v>
       </c>
     </row>
     <row r="215" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D215" s="17" t="s">
-        <v>98</v>
+        <v>324</v>
       </c>
     </row>
     <row r="216" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D216" s="17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="217" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D217" s="17" t="s">
-        <v>184</v>
+        <v>666</v>
       </c>
     </row>
     <row r="218" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D218" s="17" t="s">
-        <v>182</v>
+        <v>642</v>
       </c>
     </row>
     <row r="219" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D219" s="17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="220" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D220" s="17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="221" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D221" s="17" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="222" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D222" s="17" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="223" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D223" s="17" t="s">
         <v>461</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="X2:X140">
-    <sortCondition ref="X140"/>
+  <sortState ref="R2:R188">
+    <sortCondition ref="R188"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Classes for making report tests data-driven
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCases.xlsx
+++ b/selenium-wd/data/TestCases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="776" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="776" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases-CmpReports" sheetId="1" r:id="rId1"/>
@@ -206,7 +206,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7597" uniqueCount="753">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7635" uniqueCount="790">
   <si>
     <t>ID</t>
   </si>
@@ -2465,6 +2465,117 @@
   </si>
   <si>
     <t>DE1803</t>
+  </si>
+  <si>
+    <t>clickOnComplianceViewerMetaZIP</t>
+  </si>
+  <si>
+    <t>clickOnComplianceViewerPDFZIP</t>
+  </si>
+  <si>
+    <t>clickOnComplianceViewerShapeZIP</t>
+  </si>
+  <si>
+    <t>clickOnComplianceViewerPDF</t>
+  </si>
+  <si>
+    <t>clickOnComplianceViewerView1</t>
+  </si>
+  <si>
+    <t>clickOnComplianceViewerView2</t>
+  </si>
+  <si>
+    <t>clickOnComplianceViewerView3</t>
+  </si>
+  <si>
+    <t>clickOnComplianceViewerView4</t>
+  </si>
+  <si>
+    <t>clickOnComplianceViewerView5</t>
+  </si>
+  <si>
+    <t>clickOnComplianceViewerView6</t>
+  </si>
+  <si>
+    <t>clickOnComplianceViewerView7</t>
+  </si>
+  <si>
+    <t>clickNoOnChangeReportDialog</t>
+  </si>
+  <si>
+    <t>extractPDFZIP</t>
+  </si>
+  <si>
+    <t>extractMetaZIP</t>
+  </si>
+  <si>
+    <t>extractShapeZIP</t>
+  </si>
+  <si>
+    <t>createNewCustomer</t>
+  </si>
+  <si>
+    <t>createNewUser</t>
+  </si>
+  <si>
+    <t>waitForPDFDownloadToComplete</t>
+  </si>
+  <si>
+    <t>waitForPDFZIPDownloadToComplete</t>
+  </si>
+  <si>
+    <t>waitForMetaZIPDownloadToComplete</t>
+  </si>
+  <si>
+    <t>waitForShapeZIPDownloadToComplete</t>
+  </si>
+  <si>
+    <t>waitForView1DownloadToComplete</t>
+  </si>
+  <si>
+    <t>waitForView2DownloadToComplete</t>
+  </si>
+  <si>
+    <t>waitForView3DownloadToComplete</t>
+  </si>
+  <si>
+    <t>waitForView4DownloadToComplete</t>
+  </si>
+  <si>
+    <t>waitForView5DownloadToComplete</t>
+  </si>
+  <si>
+    <t>waitForView6DownloadToComplete</t>
+  </si>
+  <si>
+    <t>waitForView7DownloadToComplete</t>
+  </si>
+  <si>
+    <t>verifyViewsAreInCorrectSequence</t>
+  </si>
+  <si>
+    <t>verifyView1ThumbnailIsCorrect</t>
+  </si>
+  <si>
+    <t>verifyView2ThumbnailIsCorrect</t>
+  </si>
+  <si>
+    <t>verifyView3ThumbnailIsCorrect</t>
+  </si>
+  <si>
+    <t>verifyView4ThumbnailIsCorrect</t>
+  </si>
+  <si>
+    <t>verifyView5ThumbnailIsCorrect</t>
+  </si>
+  <si>
+    <t>verifyView6ThumbnailIsCorrect</t>
+  </si>
+  <si>
+    <t>verifyView7ThumbnailIsCorrect</t>
+  </si>
+  <si>
+    <t>verifyGapShapeFilesHaveCorrectData</t>
   </si>
 </sst>
 </file>
@@ -3365,7 +3476,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -42350,8 +42461,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:Z223"/>
   <sheetViews>
-    <sheetView topLeftCell="P86" workbookViewId="0">
-      <selection activeCell="R107" sqref="R107"/>
+    <sheetView tabSelected="1" topLeftCell="B94" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C148" sqref="C148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -42799,7 +42910,7 @@
         <v>43</v>
       </c>
       <c r="J6" s="16" t="s">
-        <v>43</v>
+        <v>768</v>
       </c>
       <c r="K6" s="16" t="s">
         <v>43</v>
@@ -42879,7 +42990,7 @@
         <v>44</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K7" s="16" t="s">
         <v>44</v>
@@ -42959,7 +43070,7 @@
         <v>202</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>202</v>
+        <v>44</v>
       </c>
       <c r="K8" s="16" t="s">
         <v>202</v>
@@ -43039,7 +43150,7 @@
         <v>45</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>45</v>
+        <v>202</v>
       </c>
       <c r="K9" s="16" t="s">
         <v>45</v>
@@ -43116,7 +43227,7 @@
         <v>46</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K10" s="16" t="s">
         <v>46</v>
@@ -43193,7 +43304,7 @@
         <v>47</v>
       </c>
       <c r="J11" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K11" s="16" t="s">
         <v>47</v>
@@ -43270,7 +43381,7 @@
         <v>48</v>
       </c>
       <c r="J12" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K12" s="16" t="s">
         <v>48</v>
@@ -43334,6 +43445,12 @@
       <c r="H13" s="16" t="s">
         <v>48</v>
       </c>
+      <c r="J13" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="P13" s="16" t="s">
+        <v>769</v>
+      </c>
       <c r="R13" s="16" t="s">
         <v>57</v>
       </c>
@@ -44695,6 +44812,9 @@
       </c>
     </row>
     <row r="107" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C107" s="16" t="s">
+        <v>756</v>
+      </c>
       <c r="D107" s="16" t="s">
         <v>628</v>
       </c>
@@ -44706,6 +44826,9 @@
       </c>
     </row>
     <row r="108" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C108" s="16" t="s">
+        <v>754</v>
+      </c>
       <c r="D108" s="16" t="s">
         <v>650</v>
       </c>
@@ -44717,6 +44840,9 @@
       </c>
     </row>
     <row r="109" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C109" s="16" t="s">
+        <v>753</v>
+      </c>
       <c r="D109" s="16" t="s">
         <v>626</v>
       </c>
@@ -44728,6 +44854,9 @@
       </c>
     </row>
     <row r="110" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C110" s="16" t="s">
+        <v>755</v>
+      </c>
       <c r="D110" s="16" t="s">
         <v>71</v>
       </c>
@@ -44739,6 +44868,9 @@
       </c>
     </row>
     <row r="111" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C111" s="16" t="s">
+        <v>755</v>
+      </c>
       <c r="D111" s="16" t="s">
         <v>72</v>
       </c>
@@ -44750,6 +44882,9 @@
       </c>
     </row>
     <row r="112" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C112" s="16" t="s">
+        <v>757</v>
+      </c>
       <c r="D112" s="16" t="s">
         <v>649</v>
       </c>
@@ -44760,7 +44895,10 @@
         <v>637</v>
       </c>
     </row>
-    <row r="113" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="113" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C113" s="16" t="s">
+        <v>758</v>
+      </c>
       <c r="D113" s="16" t="s">
         <v>625</v>
       </c>
@@ -44771,7 +44909,10 @@
         <v>653</v>
       </c>
     </row>
-    <row r="114" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="114" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C114" s="16" t="s">
+        <v>759</v>
+      </c>
       <c r="D114" s="16" t="s">
         <v>651</v>
       </c>
@@ -44782,7 +44923,10 @@
         <v>629</v>
       </c>
     </row>
-    <row r="115" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="115" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C115" s="16" t="s">
+        <v>760</v>
+      </c>
       <c r="D115" s="16" t="s">
         <v>627</v>
       </c>
@@ -44793,7 +44937,10 @@
         <v>654</v>
       </c>
     </row>
-    <row r="116" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="116" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C116" s="16" t="s">
+        <v>761</v>
+      </c>
       <c r="D116" s="16" t="s">
         <v>648</v>
       </c>
@@ -44804,7 +44951,10 @@
         <v>630</v>
       </c>
     </row>
-    <row r="117" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="117" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C117" s="16" t="s">
+        <v>762</v>
+      </c>
       <c r="D117" s="16" t="s">
         <v>624</v>
       </c>
@@ -44815,7 +44965,10 @@
         <v>655</v>
       </c>
     </row>
-    <row r="118" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="118" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C118" s="16" t="s">
+        <v>763</v>
+      </c>
       <c r="D118" s="16" t="s">
         <v>646</v>
       </c>
@@ -44826,7 +44979,10 @@
         <v>631</v>
       </c>
     </row>
-    <row r="119" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="119" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C119" s="16" t="s">
+        <v>764</v>
+      </c>
       <c r="D119" s="16" t="s">
         <v>622</v>
       </c>
@@ -44837,7 +44993,10 @@
         <v>656</v>
       </c>
     </row>
-    <row r="120" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="120" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C120" s="16" t="s">
+        <v>770</v>
+      </c>
       <c r="D120" s="16" t="s">
         <v>401</v>
       </c>
@@ -44848,7 +45007,10 @@
         <v>632</v>
       </c>
     </row>
-    <row r="121" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="121" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C121" s="16" t="s">
+        <v>771</v>
+      </c>
       <c r="D121" s="16" t="s">
         <v>183</v>
       </c>
@@ -44859,7 +45021,10 @@
         <v>657</v>
       </c>
     </row>
-    <row r="122" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="122" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C122" s="16" t="s">
+        <v>772</v>
+      </c>
       <c r="D122" s="16" t="s">
         <v>181</v>
       </c>
@@ -44870,7 +45035,10 @@
         <v>633</v>
       </c>
     </row>
-    <row r="123" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="123" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C123" s="16" t="s">
+        <v>773</v>
+      </c>
       <c r="D123" s="16" t="s">
         <v>73</v>
       </c>
@@ -44881,7 +45049,10 @@
         <v>658</v>
       </c>
     </row>
-    <row r="124" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="124" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C124" s="16" t="s">
+        <v>774</v>
+      </c>
       <c r="D124" s="16" t="s">
         <v>74</v>
       </c>
@@ -44892,7 +45063,10 @@
         <v>634</v>
       </c>
     </row>
-    <row r="125" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="125" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C125" s="16" t="s">
+        <v>775</v>
+      </c>
       <c r="D125" s="16" t="s">
         <v>177</v>
       </c>
@@ -44903,7 +45077,10 @@
         <v>75</v>
       </c>
     </row>
-    <row r="126" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="126" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C126" s="16" t="s">
+        <v>776</v>
+      </c>
       <c r="D126" s="16" t="s">
         <v>169</v>
       </c>
@@ -44914,7 +45091,10 @@
         <v>76</v>
       </c>
     </row>
-    <row r="127" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="127" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C127" s="16" t="s">
+        <v>777</v>
+      </c>
       <c r="D127" s="16" t="s">
         <v>660</v>
       </c>
@@ -44925,7 +45105,10 @@
         <v>662</v>
       </c>
     </row>
-    <row r="128" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="128" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C128" s="16" t="s">
+        <v>778</v>
+      </c>
       <c r="D128" s="16" t="s">
         <v>636</v>
       </c>
@@ -44936,7 +45119,10 @@
         <v>638</v>
       </c>
     </row>
-    <row r="129" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="129" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C129" s="16" t="s">
+        <v>779</v>
+      </c>
       <c r="D129" s="16" t="s">
         <v>661</v>
       </c>
@@ -44947,7 +45133,10 @@
         <v>659</v>
       </c>
     </row>
-    <row r="130" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="130" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C130" s="16" t="s">
+        <v>780</v>
+      </c>
       <c r="D130" s="16" t="s">
         <v>637</v>
       </c>
@@ -44958,7 +45147,10 @@
         <v>635</v>
       </c>
     </row>
-    <row r="131" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="131" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C131" s="16" t="s">
+        <v>765</v>
+      </c>
       <c r="D131" s="16" t="s">
         <v>653</v>
       </c>
@@ -44969,7 +45161,10 @@
         <v>174</v>
       </c>
     </row>
-    <row r="132" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="132" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C132" s="16" t="s">
+        <v>766</v>
+      </c>
       <c r="D132" s="16" t="s">
         <v>629</v>
       </c>
@@ -44980,7 +45175,10 @@
         <v>166</v>
       </c>
     </row>
-    <row r="133" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="133" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C133" s="16" t="s">
+        <v>767</v>
+      </c>
       <c r="D133" s="16" t="s">
         <v>654</v>
       </c>
@@ -44991,7 +45189,10 @@
         <v>679</v>
       </c>
     </row>
-    <row r="134" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="134" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C134" s="16" t="s">
+        <v>781</v>
+      </c>
       <c r="D134" s="16" t="s">
         <v>630</v>
       </c>
@@ -45002,7 +45203,10 @@
         <v>678</v>
       </c>
     </row>
-    <row r="135" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="135" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C135" s="16" t="s">
+        <v>782</v>
+      </c>
       <c r="D135" s="16" t="s">
         <v>655</v>
       </c>
@@ -45013,7 +45217,10 @@
         <v>173</v>
       </c>
     </row>
-    <row r="136" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="136" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C136" s="16" t="s">
+        <v>783</v>
+      </c>
       <c r="D136" s="16" t="s">
         <v>631</v>
       </c>
@@ -45024,7 +45231,10 @@
         <v>165</v>
       </c>
     </row>
-    <row r="137" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="137" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C137" s="16" t="s">
+        <v>784</v>
+      </c>
       <c r="D137" s="16" t="s">
         <v>656</v>
       </c>
@@ -45035,7 +45245,10 @@
         <v>204</v>
       </c>
     </row>
-    <row r="138" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="138" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C138" s="16" t="s">
+        <v>785</v>
+      </c>
       <c r="D138" s="16" t="s">
         <v>632</v>
       </c>
@@ -45046,7 +45259,10 @@
         <v>203</v>
       </c>
     </row>
-    <row r="139" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="139" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C139" s="16" t="s">
+        <v>786</v>
+      </c>
       <c r="D139" s="16" t="s">
         <v>657</v>
       </c>
@@ -45057,7 +45273,10 @@
         <v>385</v>
       </c>
     </row>
-    <row r="140" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="140" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C140" s="16" t="s">
+        <v>787</v>
+      </c>
       <c r="D140" s="16" t="s">
         <v>633</v>
       </c>
@@ -45068,7 +45287,10 @@
         <v>323</v>
       </c>
     </row>
-    <row r="141" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="141" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C141" s="16" t="s">
+        <v>788</v>
+      </c>
       <c r="D141" s="16" t="s">
         <v>658</v>
       </c>
@@ -45079,7 +45301,10 @@
         <v>681</v>
       </c>
     </row>
-    <row r="142" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="142" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C142" s="16" t="s">
+        <v>789</v>
+      </c>
       <c r="D142" s="16" t="s">
         <v>634</v>
       </c>
@@ -45090,7 +45315,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="143" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="143" spans="3:24" x14ac:dyDescent="0.3">
       <c r="D143" s="16" t="s">
         <v>75</v>
       </c>
@@ -45101,7 +45326,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="144" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="144" spans="3:24" x14ac:dyDescent="0.3">
       <c r="D144" s="16" t="s">
         <v>76</v>
       </c>
@@ -45646,8 +45871,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="R2:R188">
-    <sortCondition ref="R188"/>
+  <sortState ref="J2:J13">
+    <sortCondition ref="J2:J13"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Methods for copy reports test
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCases.xlsx
+++ b/selenium-wd/data/TestCases.xlsx
@@ -206,7 +206,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7635" uniqueCount="790">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7638" uniqueCount="793">
   <si>
     <t>ID</t>
   </si>
@@ -2576,6 +2576,15 @@
   </si>
   <si>
     <t>verifyGapShapeFilesHaveCorrectData</t>
+  </si>
+  <si>
+    <t>copyReport</t>
+  </si>
+  <si>
+    <t>modifyReport</t>
+  </si>
+  <si>
+    <t>verifyReportPageFieldsAreCorrect</t>
   </si>
 </sst>
 </file>
@@ -42461,8 +42470,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:Z223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B94" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C148" sqref="C148"/>
+    <sheetView tabSelected="1" topLeftCell="B126" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C145" sqref="C145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -45316,6 +45325,9 @@
       </c>
     </row>
     <row r="143" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C143" s="16" t="s">
+        <v>790</v>
+      </c>
       <c r="D143" s="16" t="s">
         <v>75</v>
       </c>
@@ -45327,6 +45339,9 @@
       </c>
     </row>
     <row r="144" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C144" s="16" t="s">
+        <v>791</v>
+      </c>
       <c r="D144" s="16" t="s">
         <v>76</v>
       </c>
@@ -45337,7 +45352,10 @@
         <v>683</v>
       </c>
     </row>
-    <row r="145" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="145" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C145" s="16" t="s">
+        <v>792</v>
+      </c>
       <c r="D145" s="16" t="s">
         <v>662</v>
       </c>
@@ -45348,7 +45366,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="146" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="146" spans="3:24" x14ac:dyDescent="0.3">
       <c r="D146" s="16" t="s">
         <v>638</v>
       </c>
@@ -45359,7 +45377,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="147" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="147" spans="3:24" x14ac:dyDescent="0.3">
       <c r="D147" s="16" t="s">
         <v>659</v>
       </c>
@@ -45367,7 +45385,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="148" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="148" spans="3:24" x14ac:dyDescent="0.3">
       <c r="D148" s="16" t="s">
         <v>635</v>
       </c>
@@ -45375,7 +45393,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="149" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="149" spans="3:24" x14ac:dyDescent="0.3">
       <c r="D149" s="16" t="s">
         <v>77</v>
       </c>
@@ -45383,7 +45401,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="150" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="150" spans="3:24" x14ac:dyDescent="0.3">
       <c r="D150" s="16" t="s">
         <v>78</v>
       </c>
@@ -45391,7 +45409,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="151" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="151" spans="3:24" x14ac:dyDescent="0.3">
       <c r="D151" s="16" t="s">
         <v>79</v>
       </c>
@@ -45399,7 +45417,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="152" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="152" spans="3:24" x14ac:dyDescent="0.3">
       <c r="D152" s="16" t="s">
         <v>80</v>
       </c>
@@ -45407,7 +45425,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="153" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="153" spans="3:24" x14ac:dyDescent="0.3">
       <c r="D153" s="16" t="s">
         <v>174</v>
       </c>
@@ -45415,7 +45433,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="154" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="154" spans="3:24" x14ac:dyDescent="0.3">
       <c r="D154" s="16" t="s">
         <v>166</v>
       </c>
@@ -45423,7 +45441,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="155" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="155" spans="3:24" x14ac:dyDescent="0.3">
       <c r="D155" s="16" t="s">
         <v>679</v>
       </c>
@@ -45431,7 +45449,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="156" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="156" spans="3:24" x14ac:dyDescent="0.3">
       <c r="D156" s="16" t="s">
         <v>678</v>
       </c>
@@ -45439,7 +45457,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="157" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="157" spans="3:24" x14ac:dyDescent="0.3">
       <c r="D157" s="16" t="s">
         <v>173</v>
       </c>
@@ -45447,7 +45465,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="158" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="158" spans="3:24" x14ac:dyDescent="0.3">
       <c r="D158" s="16" t="s">
         <v>165</v>
       </c>
@@ -45455,7 +45473,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="159" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="159" spans="3:24" x14ac:dyDescent="0.3">
       <c r="D159" s="16" t="s">
         <v>204</v>
       </c>
@@ -45463,7 +45481,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="160" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="160" spans="3:24" x14ac:dyDescent="0.3">
       <c r="D160" s="16" t="s">
         <v>203</v>
       </c>

</xml_diff>

<commit_message>
Updates to data reader and test cases for copy reports
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCases.xlsx
+++ b/selenium-wd/data/TestCases.xlsx
@@ -206,7 +206,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7638" uniqueCount="793">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7640" uniqueCount="795">
   <si>
     <t>ID</t>
   </si>
@@ -2585,6 +2585,12 @@
   </si>
   <si>
     <t>verifyReportPageFieldsAreCorrect</t>
+  </si>
+  <si>
+    <t>startNetworkProxy</t>
+  </si>
+  <si>
+    <t>stopNetworkProxy</t>
   </si>
 </sst>
 </file>
@@ -42470,8 +42476,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:Z223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B126" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C145" sqref="C145"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="X18" sqref="X18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -42727,7 +42733,7 @@
         <v>41</v>
       </c>
       <c r="Z3" s="16" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.3">
@@ -42807,7 +42813,7 @@
         <v>40</v>
       </c>
       <c r="Z4" s="16" t="s">
-        <v>462</v>
+        <v>793</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.3">
@@ -42887,7 +42893,7 @@
         <v>42</v>
       </c>
       <c r="Z5" s="16" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.3">
@@ -42967,7 +42973,7 @@
         <v>43</v>
       </c>
       <c r="Z6" s="16" t="s">
-        <v>328</v>
+        <v>463</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.3">
@@ -43047,7 +43053,7 @@
         <v>44</v>
       </c>
       <c r="Z7" s="16" t="s">
-        <v>329</v>
+        <v>794</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.3">
@@ -43127,7 +43133,7 @@
         <v>202</v>
       </c>
       <c r="Z8" s="16" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.3">
@@ -43206,6 +43212,9 @@
       <c r="Y9" s="16" t="s">
         <v>45</v>
       </c>
+      <c r="Z9" s="16" t="s">
+        <v>329</v>
+      </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
@@ -43283,6 +43292,9 @@
       <c r="Y10" s="16" t="s">
         <v>46</v>
       </c>
+      <c r="Z10" s="16" t="s">
+        <v>332</v>
+      </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
@@ -45889,8 +45901,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="J2:J13">
-    <sortCondition ref="J2:J13"/>
+  <sortState ref="Z2:Z10">
+    <sortCondition ref="Z2:Z10"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
initial set of changes for uploading survey data to environments
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCases.xlsx
+++ b/selenium-wd/data/TestCases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="776" firstSheet="1" activeTab="3"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="776" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases-CmpReports" sheetId="1" r:id="rId1"/>
@@ -3566,8 +3566,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4679,7 +4679,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:H2422"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2395" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2311" workbookViewId="0">
       <selection activeCell="G2400" sqref="G2400"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
turn on tests in xlsx
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCases.xlsx
+++ b/selenium-wd/data/TestCases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="776" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="776" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases-CmpReports" sheetId="1" r:id="rId1"/>
@@ -3598,8 +3598,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3646,7 +3646,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2"/>
       <c r="G2" s="25"/>
@@ -3665,7 +3665,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="25"/>
     </row>
@@ -3683,7 +3683,7 @@
         <v>4</v>
       </c>
       <c r="E4" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="25"/>
     </row>
@@ -3701,7 +3701,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="25"/>
       <c r="G5" s="6"/>
@@ -3720,7 +3720,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="25"/>
       <c r="G6" s="6"/>
@@ -3739,7 +3739,7 @@
         <v>8</v>
       </c>
       <c r="E7" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="25"/>
       <c r="G7" s="6"/>
@@ -3758,7 +3758,7 @@
         <v>8</v>
       </c>
       <c r="E8" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="25"/>
     </row>
@@ -3776,7 +3776,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="25"/>
     </row>
@@ -3794,7 +3794,7 @@
         <v>8</v>
       </c>
       <c r="E10" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="25"/>
     </row>
@@ -3812,7 +3812,7 @@
         <v>8</v>
       </c>
       <c r="E11" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="25"/>
     </row>
@@ -3830,7 +3830,7 @@
         <v>8</v>
       </c>
       <c r="E12" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="25"/>
       <c r="G12" s="25"/>
@@ -3849,7 +3849,7 @@
         <v>8</v>
       </c>
       <c r="E13" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13"/>
     </row>
@@ -3867,7 +3867,7 @@
         <v>8</v>
       </c>
       <c r="E14" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="25"/>
     </row>
@@ -3885,7 +3885,7 @@
         <v>8</v>
       </c>
       <c r="E15" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="25"/>
     </row>
@@ -3903,7 +3903,7 @@
         <v>4</v>
       </c>
       <c r="E16" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="25"/>
     </row>
@@ -3921,7 +3921,7 @@
         <v>4</v>
       </c>
       <c r="E17" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="25"/>
     </row>
@@ -3939,7 +3939,7 @@
         <v>4</v>
       </c>
       <c r="E18" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" s="25"/>
     </row>
@@ -3957,7 +3957,7 @@
         <v>4</v>
       </c>
       <c r="E19" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" s="25"/>
     </row>
@@ -3975,7 +3975,7 @@
         <v>4</v>
       </c>
       <c r="E20" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -3992,7 +3992,7 @@
         <v>4</v>
       </c>
       <c r="E21" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -4009,7 +4009,7 @@
         <v>4</v>
       </c>
       <c r="E22" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -4026,7 +4026,7 @@
         <v>4</v>
       </c>
       <c r="E23" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -4043,7 +4043,7 @@
         <v>4</v>
       </c>
       <c r="E24" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -4060,7 +4060,7 @@
         <v>4</v>
       </c>
       <c r="E25" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -4077,7 +4077,7 @@
         <v>4</v>
       </c>
       <c r="E26" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -4094,7 +4094,7 @@
         <v>4</v>
       </c>
       <c r="E27" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -4111,7 +4111,7 @@
         <v>4</v>
       </c>
       <c r="E28" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -4128,7 +4128,7 @@
         <v>4</v>
       </c>
       <c r="E29" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29"/>
     </row>
@@ -4146,7 +4146,7 @@
         <v>4</v>
       </c>
       <c r="E30" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -4163,7 +4163,7 @@
         <v>4</v>
       </c>
       <c r="E31" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -4180,7 +4180,7 @@
         <v>4</v>
       </c>
       <c r="E32" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -4197,7 +4197,7 @@
         <v>4</v>
       </c>
       <c r="E33" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -4214,7 +4214,7 @@
         <v>4</v>
       </c>
       <c r="E34" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -4231,7 +4231,7 @@
         <v>4</v>
       </c>
       <c r="E35" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -4248,7 +4248,7 @@
         <v>4</v>
       </c>
       <c r="E36" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -4265,7 +4265,7 @@
         <v>4</v>
       </c>
       <c r="E37" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -4282,7 +4282,7 @@
         <v>4</v>
       </c>
       <c r="E38" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -4299,7 +4299,7 @@
         <v>4</v>
       </c>
       <c r="E39" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -4316,7 +4316,7 @@
         <v>4</v>
       </c>
       <c r="E40" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -4333,7 +4333,7 @@
         <v>4</v>
       </c>
       <c r="E41" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -4350,7 +4350,7 @@
         <v>4</v>
       </c>
       <c r="E42" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -4367,7 +4367,7 @@
         <v>4</v>
       </c>
       <c r="E43" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -4384,7 +4384,7 @@
         <v>4</v>
       </c>
       <c r="E44" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -4401,7 +4401,7 @@
         <v>4</v>
       </c>
       <c r="E45" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -4418,7 +4418,7 @@
         <v>4</v>
       </c>
       <c r="E46" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -4435,7 +4435,7 @@
         <v>4</v>
       </c>
       <c r="E47" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -4452,7 +4452,7 @@
         <v>4</v>
       </c>
       <c r="E48" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -4469,7 +4469,7 @@
         <v>4</v>
       </c>
       <c r="E49" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -4486,7 +4486,7 @@
         <v>4</v>
       </c>
       <c r="E50" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -4503,7 +4503,7 @@
         <v>4</v>
       </c>
       <c r="E51" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -4520,7 +4520,7 @@
         <v>4</v>
       </c>
       <c r="E52" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -4537,7 +4537,7 @@
         <v>4</v>
       </c>
       <c r="E53" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -4571,7 +4571,7 @@
         <v>8</v>
       </c>
       <c r="E55" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -4588,7 +4588,7 @@
         <v>5</v>
       </c>
       <c r="E56" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
@@ -4605,7 +4605,7 @@
         <v>6</v>
       </c>
       <c r="E57" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -4622,7 +4622,7 @@
         <v>8</v>
       </c>
       <c r="E58" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
@@ -4639,7 +4639,7 @@
         <v>8</v>
       </c>
       <c r="E59" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
@@ -4656,7 +4656,7 @@
         <v>8</v>
       </c>
       <c r="E60" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -4673,7 +4673,7 @@
         <v>8</v>
       </c>
       <c r="E61" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
@@ -4690,7 +4690,7 @@
         <v>6</v>
       </c>
       <c r="E62" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -4712,7 +4712,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:M2493"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2217" workbookViewId="0">
+    <sheetView topLeftCell="A2217" workbookViewId="0">
       <selection activeCell="G2086" sqref="G2086"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added new db3s and test data updates
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCases.xlsx
+++ b/selenium-wd/data/TestCases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="776" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="776" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases-CmpReports" sheetId="1" r:id="rId1"/>
@@ -3598,8 +3598,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E62"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4712,8 +4712,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:M2493"/>
   <sheetViews>
-    <sheetView topLeftCell="A2217" workbookViewId="0">
-      <selection activeCell="G2086" sqref="G2086"/>
+    <sheetView tabSelected="1" topLeftCell="A1399" workbookViewId="0">
+      <selection activeCell="B1417" sqref="B1417:F1417"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9285,7 +9285,7 @@
         <v>6</v>
       </c>
       <c r="B239" s="25" t="s">
-        <v>478</v>
+        <v>749</v>
       </c>
       <c r="C239" s="25" t="s">
         <v>327</v>
@@ -9295,7 +9295,7 @@
       </c>
       <c r="E239" s="25"/>
       <c r="F239" s="25">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="G239" s="26"/>
       <c r="H239" s="25"/>
@@ -10127,7 +10127,7 @@
         <v>7</v>
       </c>
       <c r="B284" s="25" t="s">
-        <v>478</v>
+        <v>749</v>
       </c>
       <c r="C284" s="25" t="s">
         <v>327</v>
@@ -10137,7 +10137,7 @@
       </c>
       <c r="E284" s="25"/>
       <c r="F284" s="25">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="G284" s="26"/>
       <c r="H284" s="25"/>
@@ -14165,7 +14165,7 @@
         <v>11</v>
       </c>
       <c r="B495" s="25" t="s">
-        <v>478</v>
+        <v>749</v>
       </c>
       <c r="C495" s="25" t="s">
         <v>327</v>
@@ -14175,7 +14175,7 @@
       </c>
       <c r="E495" s="25"/>
       <c r="F495" s="25">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="G495" s="26"/>
       <c r="H495" s="25"/>
@@ -15108,7 +15108,7 @@
         <v>12</v>
       </c>
       <c r="B543" s="25" t="s">
-        <v>478</v>
+        <v>749</v>
       </c>
       <c r="C543" s="25" t="s">
         <v>327</v>
@@ -15982,7 +15982,7 @@
         <v>13</v>
       </c>
       <c r="B589" s="25" t="s">
-        <v>478</v>
+        <v>749</v>
       </c>
       <c r="C589" s="25" t="s">
         <v>327</v>
@@ -15992,7 +15992,7 @@
       </c>
       <c r="E589" s="25"/>
       <c r="F589" s="25">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="G589" s="26"/>
       <c r="H589" s="25"/>
@@ -16925,7 +16925,7 @@
         <v>14</v>
       </c>
       <c r="B637" s="25" t="s">
-        <v>478</v>
+        <v>749</v>
       </c>
       <c r="C637" s="25" t="s">
         <v>327</v>
@@ -16935,7 +16935,7 @@
       </c>
       <c r="E637" s="25"/>
       <c r="F637" s="25">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="G637" s="26"/>
       <c r="H637" s="25"/>
@@ -24833,7 +24833,7 @@
         <v>23</v>
       </c>
       <c r="B1048" s="25" t="s">
-        <v>474</v>
+        <v>749</v>
       </c>
       <c r="C1048" s="25" t="s">
         <v>327</v>
@@ -24843,7 +24843,7 @@
       </c>
       <c r="E1048" s="25"/>
       <c r="F1048" s="25">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="G1048" s="26"/>
       <c r="H1048" s="25"/>
@@ -25677,7 +25677,7 @@
         <v>24</v>
       </c>
       <c r="B1093" s="25" t="s">
-        <v>474</v>
+        <v>749</v>
       </c>
       <c r="C1093" s="25" t="s">
         <v>327</v>
@@ -25687,7 +25687,7 @@
       </c>
       <c r="E1093" s="25"/>
       <c r="F1093" s="25">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="G1093" s="26"/>
       <c r="H1093" s="25"/>
@@ -26521,7 +26521,7 @@
         <v>25</v>
       </c>
       <c r="B1138" s="25" t="s">
-        <v>474</v>
+        <v>749</v>
       </c>
       <c r="C1138" s="25" t="s">
         <v>327</v>
@@ -26531,7 +26531,7 @@
       </c>
       <c r="E1138" s="25"/>
       <c r="F1138" s="25">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="G1138" s="26"/>
       <c r="H1138" s="25"/>
@@ -27365,7 +27365,7 @@
         <v>26</v>
       </c>
       <c r="B1183" s="25" t="s">
-        <v>474</v>
+        <v>749</v>
       </c>
       <c r="C1183" s="25" t="s">
         <v>327</v>
@@ -27375,7 +27375,7 @@
       </c>
       <c r="E1183" s="25"/>
       <c r="F1183" s="25">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="G1183" s="26"/>
       <c r="H1183" s="25"/>
@@ -28263,7 +28263,7 @@
         <v>27</v>
       </c>
       <c r="B1231" s="25" t="s">
-        <v>474</v>
+        <v>749</v>
       </c>
       <c r="C1231" s="25" t="s">
         <v>327</v>
@@ -28273,7 +28273,7 @@
       </c>
       <c r="E1231" s="25"/>
       <c r="F1231" s="25">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="G1231" s="26"/>
       <c r="H1231" s="25"/>
@@ -29263,7 +29263,7 @@
         <v>28</v>
       </c>
       <c r="B1282" s="25" t="s">
-        <v>474</v>
+        <v>749</v>
       </c>
       <c r="C1282" s="25" t="s">
         <v>327</v>
@@ -29273,7 +29273,7 @@
       </c>
       <c r="E1282" s="25"/>
       <c r="F1282" s="25">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="G1282" s="26"/>
       <c r="H1282" s="25"/>
@@ -30166,7 +30166,7 @@
         <v>29</v>
       </c>
       <c r="B1327" s="25" t="s">
-        <v>474</v>
+        <v>749</v>
       </c>
       <c r="C1327" s="25" t="s">
         <v>327</v>
@@ -30176,7 +30176,7 @@
       </c>
       <c r="E1327" s="25"/>
       <c r="F1327" s="25">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="G1327" s="26"/>
       <c r="H1327" s="25"/>
@@ -31058,7 +31058,7 @@
         <v>30</v>
       </c>
       <c r="B1372" s="25" t="s">
-        <v>474</v>
+        <v>749</v>
       </c>
       <c r="C1372" s="25" t="s">
         <v>327</v>
@@ -31068,7 +31068,7 @@
       </c>
       <c r="E1372" s="25"/>
       <c r="F1372" s="25">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="G1372" s="26"/>
       <c r="H1372" s="25"/>
@@ -31950,7 +31950,7 @@
         <v>31</v>
       </c>
       <c r="B1417" s="25" t="s">
-        <v>474</v>
+        <v>749</v>
       </c>
       <c r="C1417" s="25" t="s">
         <v>327</v>
@@ -31960,7 +31960,7 @@
       </c>
       <c r="E1417" s="25"/>
       <c r="F1417" s="25">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="G1417" s="26"/>
       <c r="H1417" s="25"/>
@@ -52334,7 +52334,7 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D635:D636 D282:D283 D338:D339 D396:D397 D442:D443 D493:D494 D541:D542 D587:D588 D2049:D2493 J2482 J2459:J2461 D341:D343 D445:D447 D631:D632 D2:D270 D392:D393 D331:D335 D435:D439 D537:D538 D486:D490 D1622:D1631 D676:D677 D721:D722 D649:D650 D766:D767 D1045:D1082 D811:D812 J1257 D580:D584 D1090:D1127 D856:D860 D907:D911 D952:D956 D1087:D1088 D1132:D1133 J891 D1177:D1178 D997:D1001 J1392 D1222:D1226 D679:D716 D1273:D1277 D1318:D1322 D1363:D1367 J936 D724:D761 D769:D806 D814:D851 J1302 D615 D1135:D1172 D1180:D1217 J1026 J981 D1408:D1412 J1347 D1042:D1043 J1437 D1501:D1502 D1544:D1559 D1541:D1542 D1504:D1536 D1567:D1571 D1564:D1565 D1580:D1587 D1577:D1578 D1592:D1593 D1605:D1606 D1595:D1600 D1619:D1620 D1639:D1647 D1608:D1614 D1636:D1637 J1485 D1872:D1883 D1730:D1731 D1652:D1653 D1733:D1752 D1691:D1692 D1810:D1811 D1675:D1686 D1714:D1725 D1771:D1772 D1828:D1829 D1849:D1850 D1831:D1844 D1888:D1889 D1655:D1672 D1694:D1711 D1756:D1766 D1774:D1791 D1794:D1805 D1813:D1823 D1852:D1869 D1891:D1908 D1911:D1922 D1927:D1928 D1930:D1947 D1950:D1961 D1966:D1967 D1969:D1986 D1989:D2000 D2005:D2006 D2008:D2041 D2046:D2047 J16:J18 J36 J375 D375 J470 D470 J521 D521 J615 D496:D498 D275:D279 J660 J2295 J90 D419 J419 D564 J564 D660 J2341 J2386 J2431 J66:J68 J341:J343 J445:J447 J496:J498 J590:J592 J866:J868 J917:J919 J962:J964 J1007:J1009 J1232:J1234 J1328:J1330 J1373:J1375 J1418:J1420 J1464:J1466 D590:D592 D862:D902 D913:D947 D958:D992 D1003:D1037 D1228:D1268 D1324:D1358 D1369:D1403 D1414:D1448 D1459:D1496 D1453:D1457 K1283:K1285 D1279:D1313">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D635:D636 D282:D283 D338:D339 D396:D397 D442:D443 D493:D494 D541:D542 D587:D588 D2049:D2493 J2482 J2459:J2461 D341:D343 D445:D447 D631:D632 D2:D270 D392:D393 D331:D335 D435:D439 D537:D538 D486:D490 D1622:D1631 D676:D677 D721:D722 D649:D650 D766:D767 D1045:D1082 D811:D812 J1257 D580:D584 D1228:D1268 D856:D860 D907:D911 D952:D956 D1087:D1088 D1132:D1133 J891 D1177:D1178 D997:D1001 J1392 D1222:D1226 D679:D716 D1273:D1277 D1318:D1322 D1363:D1367 J936 D724:D761 D769:D806 D814:D851 J1302 D615 D1090:D1127 D1135:D1172 J1026 J981 D1408:D1412 J1347 D1042:D1043 J1437 D1501:D1502 D1544:D1559 D1541:D1542 D1504:D1536 D1567:D1571 D1564:D1565 D1580:D1587 D1577:D1578 D1592:D1593 D1605:D1606 D1595:D1600 D1619:D1620 D1639:D1647 D1608:D1614 D1636:D1637 J1485 D1872:D1883 D1730:D1731 D1652:D1653 D1733:D1752 D1691:D1692 D1810:D1811 D1675:D1686 D1714:D1725 D1771:D1772 D1828:D1829 D1849:D1850 D1831:D1844 D1888:D1889 D1655:D1672 D1694:D1711 D1756:D1766 D1774:D1791 D1794:D1805 D1813:D1823 D1852:D1869 D1891:D1908 D1911:D1922 D1927:D1928 D1930:D1947 D1950:D1961 D1966:D1967 D1969:D1986 D1989:D2000 D2005:D2006 D2008:D2041 D2046:D2047 J16:J18 J36 J375 D375 J470 D470 J521 D521 J615 D496:D498 D275:D279 J660 J2295 J90 D419 J419 D564 J564 D660 J2341 J2386 J2431 J66:J68 J341:J343 J445:J447 J496:J498 J590:J592 J866:J868 J917:J919 J962:J964 J1007:J1009 J1232:J1234 J1328:J1330 J1373:J1375 J1418:J1420 J1464:J1466 D590:D592 D862:D902 D913:D947 D958:D992 D1003:D1037 D1180:D1217 D1279:D1313 D1324:D1358 D1369:D1403 D1459:D1496 D1453:D1457 K1283:K1285 D1414:D1448">
       <formula1>INDIRECT(C2)</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I16:I18 I36 I375 I470 I521 I615 I891 I936 I981 I1026 I1257 I1302 I1347 I1392 I1437 I1485 I90 I2295 I419 I564 I660 I2341 I2386 I2431 I2482 I66:I68 I341:I343 I445:I447 I496:I498 I590:I592 I866:I868 I917:I919 I962:I964 I1007:I1009 I1232:I1234 I1328:I1330 I1373:I1375 I1418:I1420 I1464:I1466 I2459:I2461 J1283:J1285 C1:C4281">

</xml_diff>

<commit_message>
enable all action execution tests
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCases.xlsx
+++ b/selenium-wd/data/TestCases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="776" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="776" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases-CmpReports" sheetId="1" r:id="rId1"/>
@@ -3604,8 +3604,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58:E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3652,7 +3652,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2"/>
       <c r="G2" s="25"/>
@@ -3671,7 +3671,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="25"/>
     </row>
@@ -3689,7 +3689,7 @@
         <v>4</v>
       </c>
       <c r="E4" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="25"/>
     </row>
@@ -3707,7 +3707,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="25"/>
       <c r="G5" s="6"/>
@@ -3726,7 +3726,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="25"/>
       <c r="G6" s="6"/>
@@ -3745,7 +3745,7 @@
         <v>8</v>
       </c>
       <c r="E7" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="25"/>
       <c r="G7" s="6"/>
@@ -3764,7 +3764,7 @@
         <v>8</v>
       </c>
       <c r="E8" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="25"/>
     </row>
@@ -3782,7 +3782,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="25"/>
     </row>
@@ -3800,7 +3800,7 @@
         <v>8</v>
       </c>
       <c r="E10" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="25"/>
     </row>
@@ -3818,7 +3818,7 @@
         <v>8</v>
       </c>
       <c r="E11" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="25"/>
     </row>
@@ -3836,7 +3836,7 @@
         <v>8</v>
       </c>
       <c r="E12" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="25"/>
       <c r="G12" s="25"/>
@@ -3855,7 +3855,7 @@
         <v>8</v>
       </c>
       <c r="E13" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13"/>
     </row>
@@ -3873,7 +3873,7 @@
         <v>8</v>
       </c>
       <c r="E14" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="25"/>
     </row>
@@ -3891,7 +3891,7 @@
         <v>8</v>
       </c>
       <c r="E15" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="25"/>
     </row>
@@ -3909,7 +3909,7 @@
         <v>4</v>
       </c>
       <c r="E16" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="25"/>
     </row>
@@ -3927,7 +3927,7 @@
         <v>4</v>
       </c>
       <c r="E17" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="25"/>
     </row>
@@ -3945,7 +3945,7 @@
         <v>4</v>
       </c>
       <c r="E18" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" s="25"/>
     </row>
@@ -3963,7 +3963,7 @@
         <v>4</v>
       </c>
       <c r="E19" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" s="25"/>
     </row>
@@ -3981,7 +3981,7 @@
         <v>4</v>
       </c>
       <c r="E20" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -3998,7 +3998,7 @@
         <v>4</v>
       </c>
       <c r="E21" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -4015,7 +4015,7 @@
         <v>4</v>
       </c>
       <c r="E22" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -4032,7 +4032,7 @@
         <v>4</v>
       </c>
       <c r="E23" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -4049,7 +4049,7 @@
         <v>4</v>
       </c>
       <c r="E24" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -4066,7 +4066,7 @@
         <v>4</v>
       </c>
       <c r="E25" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -4083,7 +4083,7 @@
         <v>4</v>
       </c>
       <c r="E26" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -4100,7 +4100,7 @@
         <v>4</v>
       </c>
       <c r="E27" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -4117,7 +4117,7 @@
         <v>4</v>
       </c>
       <c r="E28" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -4134,7 +4134,7 @@
         <v>4</v>
       </c>
       <c r="E29" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29"/>
     </row>
@@ -4152,7 +4152,7 @@
         <v>4</v>
       </c>
       <c r="E30" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -4169,7 +4169,7 @@
         <v>4</v>
       </c>
       <c r="E31" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -4186,7 +4186,7 @@
         <v>4</v>
       </c>
       <c r="E32" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -4203,7 +4203,7 @@
         <v>4</v>
       </c>
       <c r="E33" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -4220,7 +4220,7 @@
         <v>4</v>
       </c>
       <c r="E34" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -4237,7 +4237,7 @@
         <v>4</v>
       </c>
       <c r="E35" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -4254,7 +4254,7 @@
         <v>4</v>
       </c>
       <c r="E36" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -4271,7 +4271,7 @@
         <v>4</v>
       </c>
       <c r="E37" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -4288,7 +4288,7 @@
         <v>4</v>
       </c>
       <c r="E38" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -4305,7 +4305,7 @@
         <v>4</v>
       </c>
       <c r="E39" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -4322,7 +4322,7 @@
         <v>4</v>
       </c>
       <c r="E40" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -4339,7 +4339,7 @@
         <v>4</v>
       </c>
       <c r="E41" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -4356,7 +4356,7 @@
         <v>4</v>
       </c>
       <c r="E42" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -4373,7 +4373,7 @@
         <v>4</v>
       </c>
       <c r="E43" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -4390,7 +4390,7 @@
         <v>4</v>
       </c>
       <c r="E44" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G44" s="6"/>
     </row>
@@ -4408,7 +4408,7 @@
         <v>4</v>
       </c>
       <c r="E45" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -4425,7 +4425,7 @@
         <v>4</v>
       </c>
       <c r="E46" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G46" s="6"/>
     </row>
@@ -4443,7 +4443,7 @@
         <v>4</v>
       </c>
       <c r="E47" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -4460,7 +4460,7 @@
         <v>4</v>
       </c>
       <c r="E48" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -4477,7 +4477,7 @@
         <v>4</v>
       </c>
       <c r="E49" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -4494,7 +4494,7 @@
         <v>4</v>
       </c>
       <c r="E50" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -4511,7 +4511,7 @@
         <v>4</v>
       </c>
       <c r="E51" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -4528,7 +4528,7 @@
         <v>4</v>
       </c>
       <c r="E52" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -4545,7 +4545,7 @@
         <v>4</v>
       </c>
       <c r="E53" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -4562,7 +4562,7 @@
         <v>8</v>
       </c>
       <c r="E54" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -4596,7 +4596,7 @@
         <v>5</v>
       </c>
       <c r="E56" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
@@ -4613,7 +4613,7 @@
         <v>6</v>
       </c>
       <c r="E57" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -4647,7 +4647,7 @@
         <v>8</v>
       </c>
       <c r="E59" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
@@ -4664,7 +4664,7 @@
         <v>8</v>
       </c>
       <c r="E60" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -4681,7 +4681,7 @@
         <v>8</v>
       </c>
       <c r="E61" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
@@ -4698,7 +4698,7 @@
         <v>6</v>
       </c>
       <c r="E62" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -4720,7 +4720,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:M2495"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2260" workbookViewId="0">
+    <sheetView topLeftCell="A2260" workbookViewId="0">
       <selection activeCell="E2129" sqref="E2129"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
DriverViewPageTest class test fixes + other cleanup for simulator based view tests
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCases.xlsx
+++ b/selenium-wd/data/TestCases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="776" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="776" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases-CmpReports" sheetId="1" r:id="rId1"/>
@@ -3604,7 +3604,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+    <sheetView topLeftCell="A44" workbookViewId="0">
       <selection activeCell="E58" sqref="E58:E62"/>
     </sheetView>
   </sheetViews>
@@ -4720,8 +4720,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:M2495"/>
   <sheetViews>
-    <sheetView topLeftCell="A2260" workbookViewId="0">
-      <selection activeCell="E2129" sqref="E2129"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
enable all actionexecution driverview tests
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCases.xlsx
+++ b/selenium-wd/data/TestCases.xlsx
@@ -3613,8 +3613,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3661,7 +3661,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2"/>
       <c r="G2" s="25"/>
@@ -3680,7 +3680,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="25"/>
     </row>
@@ -3698,7 +3698,7 @@
         <v>4</v>
       </c>
       <c r="E4" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="25"/>
     </row>
@@ -3716,7 +3716,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="25"/>
       <c r="G5" s="6"/>
@@ -3735,7 +3735,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="25"/>
       <c r="G6" s="6"/>
@@ -3754,7 +3754,7 @@
         <v>8</v>
       </c>
       <c r="E7" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="25"/>
       <c r="G7" s="6"/>
@@ -3773,7 +3773,7 @@
         <v>8</v>
       </c>
       <c r="E8" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="25"/>
     </row>
@@ -3791,7 +3791,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="25"/>
     </row>
@@ -3809,7 +3809,7 @@
         <v>8</v>
       </c>
       <c r="E10" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="25"/>
     </row>
@@ -3827,7 +3827,7 @@
         <v>8</v>
       </c>
       <c r="E11" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="25"/>
     </row>
@@ -3864,7 +3864,7 @@
         <v>8</v>
       </c>
       <c r="E13" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13"/>
     </row>
@@ -3882,7 +3882,7 @@
         <v>8</v>
       </c>
       <c r="E14" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="25"/>
     </row>
@@ -3900,7 +3900,7 @@
         <v>8</v>
       </c>
       <c r="E15" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="25"/>
     </row>
@@ -3918,7 +3918,7 @@
         <v>4</v>
       </c>
       <c r="E16" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="25"/>
     </row>
@@ -3936,7 +3936,7 @@
         <v>4</v>
       </c>
       <c r="E17" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="25"/>
     </row>
@@ -3954,7 +3954,7 @@
         <v>4</v>
       </c>
       <c r="E18" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" s="25"/>
     </row>
@@ -3972,7 +3972,7 @@
         <v>4</v>
       </c>
       <c r="E19" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" s="25"/>
     </row>
@@ -3990,7 +3990,7 @@
         <v>4</v>
       </c>
       <c r="E20" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -4007,7 +4007,7 @@
         <v>4</v>
       </c>
       <c r="E21" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -4024,7 +4024,7 @@
         <v>4</v>
       </c>
       <c r="E22" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -4041,7 +4041,7 @@
         <v>4</v>
       </c>
       <c r="E23" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -4058,7 +4058,7 @@
         <v>4</v>
       </c>
       <c r="E24" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -4075,7 +4075,7 @@
         <v>4</v>
       </c>
       <c r="E25" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -4092,7 +4092,7 @@
         <v>4</v>
       </c>
       <c r="E26" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -4109,7 +4109,7 @@
         <v>4</v>
       </c>
       <c r="E27" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -4126,7 +4126,7 @@
         <v>4</v>
       </c>
       <c r="E28" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -4143,7 +4143,7 @@
         <v>4</v>
       </c>
       <c r="E29" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29"/>
     </row>
@@ -4161,7 +4161,7 @@
         <v>4</v>
       </c>
       <c r="E30" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -4178,7 +4178,7 @@
         <v>4</v>
       </c>
       <c r="E31" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -4195,7 +4195,7 @@
         <v>4</v>
       </c>
       <c r="E32" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -4212,7 +4212,7 @@
         <v>4</v>
       </c>
       <c r="E33" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -4229,7 +4229,7 @@
         <v>4</v>
       </c>
       <c r="E34" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -4246,7 +4246,7 @@
         <v>4</v>
       </c>
       <c r="E35" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -4263,7 +4263,7 @@
         <v>4</v>
       </c>
       <c r="E36" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -4280,7 +4280,7 @@
         <v>4</v>
       </c>
       <c r="E37" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -4297,7 +4297,7 @@
         <v>4</v>
       </c>
       <c r="E38" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -4314,7 +4314,7 @@
         <v>4</v>
       </c>
       <c r="E39" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -4331,7 +4331,7 @@
         <v>4</v>
       </c>
       <c r="E40" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -4348,7 +4348,7 @@
         <v>4</v>
       </c>
       <c r="E41" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -4365,7 +4365,7 @@
         <v>4</v>
       </c>
       <c r="E42" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -4382,7 +4382,7 @@
         <v>4</v>
       </c>
       <c r="E43" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -4399,7 +4399,7 @@
         <v>4</v>
       </c>
       <c r="E44" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G44" s="6"/>
     </row>
@@ -4417,7 +4417,7 @@
         <v>4</v>
       </c>
       <c r="E45" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -4434,7 +4434,7 @@
         <v>4</v>
       </c>
       <c r="E46" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G46" s="6"/>
     </row>
@@ -4452,7 +4452,7 @@
         <v>4</v>
       </c>
       <c r="E47" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -4469,7 +4469,7 @@
         <v>4</v>
       </c>
       <c r="E48" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -4486,7 +4486,7 @@
         <v>4</v>
       </c>
       <c r="E49" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -4503,7 +4503,7 @@
         <v>4</v>
       </c>
       <c r="E50" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -4520,7 +4520,7 @@
         <v>4</v>
       </c>
       <c r="E51" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -4537,7 +4537,7 @@
         <v>4</v>
       </c>
       <c r="E52" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -4554,7 +4554,7 @@
         <v>4</v>
       </c>
       <c r="E53" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -4571,7 +4571,7 @@
         <v>8</v>
       </c>
       <c r="E54" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -4588,7 +4588,7 @@
         <v>8</v>
       </c>
       <c r="E55" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -4605,7 +4605,7 @@
         <v>5</v>
       </c>
       <c r="E56" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
@@ -4622,7 +4622,7 @@
         <v>6</v>
       </c>
       <c r="E57" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -4639,7 +4639,7 @@
         <v>8</v>
       </c>
       <c r="E58" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
@@ -4656,7 +4656,7 @@
         <v>8</v>
       </c>
       <c r="E59" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
@@ -4673,7 +4673,7 @@
         <v>8</v>
       </c>
       <c r="E60" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -4690,7 +4690,7 @@
         <v>8</v>
       </c>
       <c r="E61" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
@@ -4707,7 +4707,7 @@
         <v>6</v>
       </c>
       <c r="E62" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
enable all tests for actionexecution driver
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCases.xlsx
+++ b/selenium-wd/data/TestCases.xlsx
@@ -3616,8 +3616,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3664,7 +3664,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2"/>
       <c r="G2" s="25"/>
@@ -3683,7 +3683,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="25"/>
     </row>
@@ -3701,7 +3701,7 @@
         <v>4</v>
       </c>
       <c r="E4" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="25"/>
     </row>
@@ -3719,7 +3719,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="25"/>
       <c r="G5" s="6"/>
@@ -3738,7 +3738,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="25"/>
       <c r="G6" s="6"/>
@@ -3757,7 +3757,7 @@
         <v>8</v>
       </c>
       <c r="E7" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="25"/>
       <c r="G7" s="6"/>
@@ -3776,7 +3776,7 @@
         <v>8</v>
       </c>
       <c r="E8" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="25"/>
     </row>
@@ -3794,7 +3794,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="25"/>
     </row>
@@ -3812,7 +3812,7 @@
         <v>8</v>
       </c>
       <c r="E10" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="25"/>
     </row>
@@ -3830,7 +3830,7 @@
         <v>8</v>
       </c>
       <c r="E11" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="25"/>
     </row>
@@ -3848,7 +3848,7 @@
         <v>8</v>
       </c>
       <c r="E12" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="25"/>
       <c r="G12" s="25"/>
@@ -3867,7 +3867,7 @@
         <v>8</v>
       </c>
       <c r="E13" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13"/>
     </row>
@@ -3885,7 +3885,7 @@
         <v>8</v>
       </c>
       <c r="E14" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="25"/>
     </row>
@@ -3903,7 +3903,7 @@
         <v>8</v>
       </c>
       <c r="E15" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="25"/>
     </row>
@@ -3921,7 +3921,7 @@
         <v>4</v>
       </c>
       <c r="E16" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="25"/>
     </row>
@@ -3939,7 +3939,7 @@
         <v>4</v>
       </c>
       <c r="E17" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="25"/>
     </row>
@@ -3957,7 +3957,7 @@
         <v>4</v>
       </c>
       <c r="E18" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" s="25"/>
     </row>
@@ -3975,7 +3975,7 @@
         <v>4</v>
       </c>
       <c r="E19" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" s="25"/>
     </row>
@@ -3993,7 +3993,7 @@
         <v>4</v>
       </c>
       <c r="E20" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -4010,7 +4010,7 @@
         <v>4</v>
       </c>
       <c r="E21" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -4027,7 +4027,7 @@
         <v>4</v>
       </c>
       <c r="E22" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -4044,7 +4044,7 @@
         <v>4</v>
       </c>
       <c r="E23" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -4078,7 +4078,7 @@
         <v>4</v>
       </c>
       <c r="E25" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -4095,7 +4095,7 @@
         <v>4</v>
       </c>
       <c r="E26" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -4112,7 +4112,7 @@
         <v>4</v>
       </c>
       <c r="E27" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -4129,7 +4129,7 @@
         <v>4</v>
       </c>
       <c r="E28" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -4146,7 +4146,7 @@
         <v>4</v>
       </c>
       <c r="E29" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29"/>
     </row>
@@ -4164,7 +4164,7 @@
         <v>4</v>
       </c>
       <c r="E30" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -4181,7 +4181,7 @@
         <v>4</v>
       </c>
       <c r="E31" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -4198,7 +4198,7 @@
         <v>4</v>
       </c>
       <c r="E32" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -4215,7 +4215,7 @@
         <v>4</v>
       </c>
       <c r="E33" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -4232,7 +4232,7 @@
         <v>4</v>
       </c>
       <c r="E34" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -4249,7 +4249,7 @@
         <v>4</v>
       </c>
       <c r="E35" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -4266,7 +4266,7 @@
         <v>4</v>
       </c>
       <c r="E36" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -4283,7 +4283,7 @@
         <v>4</v>
       </c>
       <c r="E37" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -4300,7 +4300,7 @@
         <v>4</v>
       </c>
       <c r="E38" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -4317,7 +4317,7 @@
         <v>4</v>
       </c>
       <c r="E39" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -4334,7 +4334,7 @@
         <v>4</v>
       </c>
       <c r="E40" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -4351,7 +4351,7 @@
         <v>4</v>
       </c>
       <c r="E41" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -4368,7 +4368,7 @@
         <v>4</v>
       </c>
       <c r="E42" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -4385,7 +4385,7 @@
         <v>4</v>
       </c>
       <c r="E43" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -4402,7 +4402,7 @@
         <v>4</v>
       </c>
       <c r="E44" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G44" s="6"/>
     </row>
@@ -4420,7 +4420,7 @@
         <v>4</v>
       </c>
       <c r="E45" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -4437,7 +4437,7 @@
         <v>4</v>
       </c>
       <c r="E46" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G46" s="6"/>
     </row>
@@ -4455,7 +4455,7 @@
         <v>4</v>
       </c>
       <c r="E47" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -4472,7 +4472,7 @@
         <v>4</v>
       </c>
       <c r="E48" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -4489,7 +4489,7 @@
         <v>4</v>
       </c>
       <c r="E49" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -4506,7 +4506,7 @@
         <v>4</v>
       </c>
       <c r="E50" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -4523,7 +4523,7 @@
         <v>4</v>
       </c>
       <c r="E51" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -4540,7 +4540,7 @@
         <v>4</v>
       </c>
       <c r="E52" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -4557,7 +4557,7 @@
         <v>4</v>
       </c>
       <c r="E53" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -4574,7 +4574,7 @@
         <v>8</v>
       </c>
       <c r="E54" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -4591,7 +4591,7 @@
         <v>8</v>
       </c>
       <c r="E55" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -4608,7 +4608,7 @@
         <v>5</v>
       </c>
       <c r="E56" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
@@ -4625,7 +4625,7 @@
         <v>6</v>
       </c>
       <c r="E57" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -4642,7 +4642,7 @@
         <v>8</v>
       </c>
       <c r="E58" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
@@ -4659,7 +4659,7 @@
         <v>8</v>
       </c>
       <c r="E59" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
@@ -4676,7 +4676,7 @@
         <v>8</v>
       </c>
       <c r="E60" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -4693,7 +4693,7 @@
         <v>8</v>
       </c>
       <c r="E61" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
@@ -4710,7 +4710,7 @@
         <v>6</v>
       </c>
       <c r="E62" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -4732,8 +4732,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:M2497"/>
   <sheetViews>
-    <sheetView topLeftCell="A1035" workbookViewId="0">
-      <selection activeCell="C1053" sqref="C1053"/>
+    <sheetView topLeftCell="A653" workbookViewId="0">
+      <selection activeCell="F667" sqref="F667"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16804,7 +16804,7 @@
       <c r="E629" s="25"/>
       <c r="F629" s="25"/>
       <c r="G629" s="26">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H629" s="25"/>
     </row>
@@ -17523,7 +17523,7 @@
       </c>
       <c r="E667" s="25"/>
       <c r="F667" s="25" t="s">
-        <v>831</v>
+        <v>372</v>
       </c>
       <c r="G667" s="26"/>
       <c r="H667" s="25"/>

</xml_diff>

<commit_message>
test case data updates for failing test cases
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCases.xlsx
+++ b/selenium-wd/data/TestCases.xlsx
@@ -3617,7 +3617,7 @@
   <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3664,7 +3664,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2"/>
       <c r="G2" s="25"/>
@@ -3683,7 +3683,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" s="25"/>
     </row>
@@ -3701,7 +3701,7 @@
         <v>4</v>
       </c>
       <c r="E4" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" s="25"/>
     </row>
@@ -3719,7 +3719,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" s="25"/>
       <c r="G5" s="6"/>
@@ -3738,7 +3738,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="25"/>
       <c r="G6" s="6"/>
@@ -3757,7 +3757,7 @@
         <v>8</v>
       </c>
       <c r="E7" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" s="25"/>
       <c r="G7" s="6"/>
@@ -3776,7 +3776,7 @@
         <v>8</v>
       </c>
       <c r="E8" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="25"/>
     </row>
@@ -3794,7 +3794,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="25"/>
     </row>
@@ -3812,7 +3812,7 @@
         <v>8</v>
       </c>
       <c r="E10" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" s="25"/>
     </row>
@@ -3830,7 +3830,7 @@
         <v>8</v>
       </c>
       <c r="E11" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" s="25"/>
     </row>
@@ -3848,7 +3848,7 @@
         <v>8</v>
       </c>
       <c r="E12" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" s="25"/>
       <c r="G12" s="25"/>
@@ -3867,7 +3867,7 @@
         <v>8</v>
       </c>
       <c r="E13" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13"/>
     </row>
@@ -3885,7 +3885,7 @@
         <v>8</v>
       </c>
       <c r="E14" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" s="25"/>
     </row>
@@ -3921,7 +3921,7 @@
         <v>4</v>
       </c>
       <c r="E16" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" s="25"/>
     </row>
@@ -3939,7 +3939,7 @@
         <v>4</v>
       </c>
       <c r="E17" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" s="25"/>
     </row>
@@ -3957,7 +3957,7 @@
         <v>4</v>
       </c>
       <c r="E18" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18" s="25"/>
     </row>
@@ -3975,7 +3975,7 @@
         <v>4</v>
       </c>
       <c r="E19" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19" s="25"/>
     </row>
@@ -3993,7 +3993,7 @@
         <v>4</v>
       </c>
       <c r="E20" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -4010,7 +4010,7 @@
         <v>4</v>
       </c>
       <c r="E21" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -4027,7 +4027,7 @@
         <v>4</v>
       </c>
       <c r="E22" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -4044,7 +4044,7 @@
         <v>4</v>
       </c>
       <c r="E23" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -4061,7 +4061,7 @@
         <v>4</v>
       </c>
       <c r="E24" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -4078,7 +4078,7 @@
         <v>4</v>
       </c>
       <c r="E25" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -4095,7 +4095,7 @@
         <v>4</v>
       </c>
       <c r="E26" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -4112,7 +4112,7 @@
         <v>4</v>
       </c>
       <c r="E27" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -4129,7 +4129,7 @@
         <v>4</v>
       </c>
       <c r="E28" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -4146,7 +4146,7 @@
         <v>4</v>
       </c>
       <c r="E29" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F29"/>
     </row>
@@ -4164,7 +4164,7 @@
         <v>4</v>
       </c>
       <c r="E30" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -4181,7 +4181,7 @@
         <v>4</v>
       </c>
       <c r="E31" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -4198,7 +4198,7 @@
         <v>4</v>
       </c>
       <c r="E32" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -4215,7 +4215,7 @@
         <v>4</v>
       </c>
       <c r="E33" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -4232,7 +4232,7 @@
         <v>4</v>
       </c>
       <c r="E34" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -4249,7 +4249,7 @@
         <v>4</v>
       </c>
       <c r="E35" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -4266,7 +4266,7 @@
         <v>4</v>
       </c>
       <c r="E36" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -4283,7 +4283,7 @@
         <v>4</v>
       </c>
       <c r="E37" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -4300,7 +4300,7 @@
         <v>4</v>
       </c>
       <c r="E38" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -4317,7 +4317,7 @@
         <v>4</v>
       </c>
       <c r="E39" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -4334,7 +4334,7 @@
         <v>4</v>
       </c>
       <c r="E40" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -4351,7 +4351,7 @@
         <v>4</v>
       </c>
       <c r="E41" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -4368,7 +4368,7 @@
         <v>4</v>
       </c>
       <c r="E42" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -4385,7 +4385,7 @@
         <v>4</v>
       </c>
       <c r="E43" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -4402,7 +4402,7 @@
         <v>4</v>
       </c>
       <c r="E44" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G44" s="6"/>
     </row>
@@ -4420,7 +4420,7 @@
         <v>4</v>
       </c>
       <c r="E45" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -4437,7 +4437,7 @@
         <v>4</v>
       </c>
       <c r="E46" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G46" s="6"/>
     </row>
@@ -4455,7 +4455,7 @@
         <v>4</v>
       </c>
       <c r="E47" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -4472,7 +4472,7 @@
         <v>4</v>
       </c>
       <c r="E48" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -4489,7 +4489,7 @@
         <v>4</v>
       </c>
       <c r="E49" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -4506,7 +4506,7 @@
         <v>4</v>
       </c>
       <c r="E50" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -4523,7 +4523,7 @@
         <v>4</v>
       </c>
       <c r="E51" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -4540,7 +4540,7 @@
         <v>4</v>
       </c>
       <c r="E52" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -4557,7 +4557,7 @@
         <v>4</v>
       </c>
       <c r="E53" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -4574,7 +4574,7 @@
         <v>8</v>
       </c>
       <c r="E54" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -4591,7 +4591,7 @@
         <v>8</v>
       </c>
       <c r="E55" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -4608,7 +4608,7 @@
         <v>5</v>
       </c>
       <c r="E56" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
@@ -4625,7 +4625,7 @@
         <v>6</v>
       </c>
       <c r="E57" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -4642,7 +4642,7 @@
         <v>8</v>
       </c>
       <c r="E58" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
@@ -4659,7 +4659,7 @@
         <v>8</v>
       </c>
       <c r="E59" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
@@ -4676,7 +4676,7 @@
         <v>8</v>
       </c>
       <c r="E60" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -4693,7 +4693,7 @@
         <v>8</v>
       </c>
       <c r="E61" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
@@ -4710,7 +4710,7 @@
         <v>6</v>
       </c>
       <c r="E62" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -4732,8 +4732,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:M2497"/>
   <sheetViews>
-    <sheetView topLeftCell="A653" workbookViewId="0">
-      <selection activeCell="F667" sqref="F667"/>
+    <sheetView topLeftCell="A222" workbookViewId="0">
+      <selection activeCell="G230" sqref="G230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9146,7 +9146,7 @@
       <c r="E230" s="25"/>
       <c r="F230" s="25"/>
       <c r="G230" s="26">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H230" s="25"/>
     </row>
@@ -9315,7 +9315,7 @@
       </c>
       <c r="E239" s="25"/>
       <c r="F239" s="25">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="G239" s="26"/>
       <c r="H239" s="25"/>
@@ -9547,7 +9547,7 @@
         <v>10</v>
       </c>
       <c r="D252" s="25" t="s">
-        <v>122</v>
+        <v>391</v>
       </c>
       <c r="E252" s="25"/>
       <c r="F252" s="25"/>
@@ -9797,7 +9797,7 @@
       </c>
       <c r="E265" s="25"/>
       <c r="F265" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="G265" s="26"/>
       <c r="H265" s="25"/>
@@ -12975,7 +12975,7 @@
       <c r="E432" s="25"/>
       <c r="F432" s="25"/>
       <c r="G432" s="26">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H432" s="25"/>
     </row>
@@ -13198,7 +13198,7 @@
       </c>
       <c r="E444" s="25"/>
       <c r="F444" s="25">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G444" s="26"/>
       <c r="H444" s="25"/>
@@ -13835,7 +13835,7 @@
       </c>
       <c r="E476" s="25"/>
       <c r="F476" s="25" t="s">
-        <v>429</v>
+        <v>372</v>
       </c>
       <c r="G476" s="26"/>
       <c r="H476" s="25"/>

</xml_diff>

<commit_message>
turn on all driver view tests in xlsx
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCases.xlsx
+++ b/selenium-wd/data/TestCases.xlsx
@@ -3617,7 +3617,7 @@
   <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E15" sqref="E15:E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3664,7 +3664,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2"/>
       <c r="G2" s="25"/>
@@ -3683,7 +3683,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="25"/>
     </row>
@@ -3701,7 +3701,7 @@
         <v>4</v>
       </c>
       <c r="E4" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="25"/>
     </row>
@@ -3719,7 +3719,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="25"/>
       <c r="G5" s="6"/>
@@ -3738,7 +3738,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="25"/>
       <c r="G6" s="6"/>
@@ -3757,7 +3757,7 @@
         <v>8</v>
       </c>
       <c r="E7" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="25"/>
       <c r="G7" s="6"/>
@@ -3776,7 +3776,7 @@
         <v>8</v>
       </c>
       <c r="E8" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="25"/>
     </row>
@@ -3794,7 +3794,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="25"/>
     </row>
@@ -3812,7 +3812,7 @@
         <v>8</v>
       </c>
       <c r="E10" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="25"/>
     </row>
@@ -3830,7 +3830,7 @@
         <v>8</v>
       </c>
       <c r="E11" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="25"/>
     </row>
@@ -3848,7 +3848,7 @@
         <v>8</v>
       </c>
       <c r="E12" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="25"/>
       <c r="G12" s="25"/>
@@ -3867,7 +3867,7 @@
         <v>8</v>
       </c>
       <c r="E13" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13"/>
     </row>
@@ -3885,7 +3885,7 @@
         <v>8</v>
       </c>
       <c r="E14" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="25"/>
     </row>
@@ -3921,7 +3921,7 @@
         <v>4</v>
       </c>
       <c r="E16" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="25"/>
     </row>
@@ -3939,7 +3939,7 @@
         <v>4</v>
       </c>
       <c r="E17" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="25"/>
     </row>
@@ -3957,7 +3957,7 @@
         <v>4</v>
       </c>
       <c r="E18" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" s="25"/>
     </row>
@@ -3975,7 +3975,7 @@
         <v>4</v>
       </c>
       <c r="E19" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" s="25"/>
     </row>
@@ -3993,7 +3993,7 @@
         <v>4</v>
       </c>
       <c r="E20" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -4010,7 +4010,7 @@
         <v>4</v>
       </c>
       <c r="E21" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -4027,7 +4027,7 @@
         <v>4</v>
       </c>
       <c r="E22" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -4044,7 +4044,7 @@
         <v>4</v>
       </c>
       <c r="E23" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -4061,7 +4061,7 @@
         <v>4</v>
       </c>
       <c r="E24" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -4078,7 +4078,7 @@
         <v>4</v>
       </c>
       <c r="E25" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -4095,7 +4095,7 @@
         <v>4</v>
       </c>
       <c r="E26" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -4112,7 +4112,7 @@
         <v>4</v>
       </c>
       <c r="E27" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -4129,7 +4129,7 @@
         <v>4</v>
       </c>
       <c r="E28" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -4146,7 +4146,7 @@
         <v>4</v>
       </c>
       <c r="E29" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29"/>
     </row>
@@ -4164,7 +4164,7 @@
         <v>4</v>
       </c>
       <c r="E30" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -4181,7 +4181,7 @@
         <v>4</v>
       </c>
       <c r="E31" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -4198,7 +4198,7 @@
         <v>4</v>
       </c>
       <c r="E32" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -4215,7 +4215,7 @@
         <v>4</v>
       </c>
       <c r="E33" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -4232,7 +4232,7 @@
         <v>4</v>
       </c>
       <c r="E34" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -4249,7 +4249,7 @@
         <v>4</v>
       </c>
       <c r="E35" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -4266,7 +4266,7 @@
         <v>4</v>
       </c>
       <c r="E36" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -4283,7 +4283,7 @@
         <v>4</v>
       </c>
       <c r="E37" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -4300,7 +4300,7 @@
         <v>4</v>
       </c>
       <c r="E38" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -4317,7 +4317,7 @@
         <v>4</v>
       </c>
       <c r="E39" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -4334,7 +4334,7 @@
         <v>4</v>
       </c>
       <c r="E40" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -4351,7 +4351,7 @@
         <v>4</v>
       </c>
       <c r="E41" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -4368,7 +4368,7 @@
         <v>4</v>
       </c>
       <c r="E42" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -4385,7 +4385,7 @@
         <v>4</v>
       </c>
       <c r="E43" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -4402,7 +4402,7 @@
         <v>4</v>
       </c>
       <c r="E44" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G44" s="6"/>
     </row>
@@ -4420,7 +4420,7 @@
         <v>4</v>
       </c>
       <c r="E45" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -4437,7 +4437,7 @@
         <v>4</v>
       </c>
       <c r="E46" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G46" s="6"/>
     </row>
@@ -4455,7 +4455,7 @@
         <v>4</v>
       </c>
       <c r="E47" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -4472,7 +4472,7 @@
         <v>4</v>
       </c>
       <c r="E48" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -4489,7 +4489,7 @@
         <v>4</v>
       </c>
       <c r="E49" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -4506,7 +4506,7 @@
         <v>4</v>
       </c>
       <c r="E50" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -4523,7 +4523,7 @@
         <v>4</v>
       </c>
       <c r="E51" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -4540,7 +4540,7 @@
         <v>4</v>
       </c>
       <c r="E52" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -4557,7 +4557,7 @@
         <v>4</v>
       </c>
       <c r="E53" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -4574,7 +4574,7 @@
         <v>8</v>
       </c>
       <c r="E54" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -4591,7 +4591,7 @@
         <v>8</v>
       </c>
       <c r="E55" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -4608,7 +4608,7 @@
         <v>5</v>
       </c>
       <c r="E56" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
@@ -4625,7 +4625,7 @@
         <v>6</v>
       </c>
       <c r="E57" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -4642,7 +4642,7 @@
         <v>8</v>
       </c>
       <c r="E58" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
@@ -4659,7 +4659,7 @@
         <v>8</v>
       </c>
       <c r="E59" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
@@ -4676,7 +4676,7 @@
         <v>8</v>
       </c>
       <c r="E60" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -4693,7 +4693,7 @@
         <v>8</v>
       </c>
       <c r="E61" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
@@ -4710,7 +4710,7 @@
         <v>6</v>
       </c>
       <c r="E62" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
turn off FOV checks in xlsx based tests
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCases.xlsx
+++ b/selenium-wd/data/TestCases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="776" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="776" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases-CmpReports" sheetId="1" r:id="rId1"/>
@@ -206,7 +206,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9386" uniqueCount="831">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9391" uniqueCount="832">
   <si>
     <t>ID</t>
   </si>
@@ -2699,6 +2699,9 @@
   </si>
   <si>
     <t>DE1867 - Field Notes disabled</t>
+  </si>
+  <si>
+    <t>TURN OFF FOV</t>
   </si>
 </sst>
 </file>
@@ -2830,7 +2833,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -2911,6 +2914,12 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -3601,8 +3610,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E62"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4717,8 +4726,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:M2498"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="D607" workbookViewId="0">
+      <selection activeCell="F611" sqref="F611"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7233,15 +7242,19 @@
         <v>346</v>
       </c>
       <c r="C130" s="25" t="s">
-        <v>10</v>
+        <v>327</v>
       </c>
       <c r="D130" s="25" t="s">
-        <v>169</v>
+        <v>360</v>
       </c>
       <c r="E130" s="25"/>
-      <c r="F130" s="25"/>
+      <c r="F130" s="25">
+        <v>1</v>
+      </c>
       <c r="G130" s="26"/>
-      <c r="H130" s="26"/>
+      <c r="H130" s="42" t="s">
+        <v>831</v>
+      </c>
     </row>
     <row r="131" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A131" s="27">
@@ -8017,15 +8030,19 @@
         <v>346</v>
       </c>
       <c r="C172" s="25" t="s">
-        <v>10</v>
+        <v>327</v>
       </c>
       <c r="D172" s="25" t="s">
-        <v>169</v>
+        <v>360</v>
       </c>
       <c r="E172" s="25"/>
-      <c r="F172" s="25"/>
+      <c r="F172" s="25">
+        <v>1</v>
+      </c>
       <c r="G172" s="26"/>
-      <c r="H172" s="26"/>
+      <c r="H172" s="42" t="s">
+        <v>831</v>
+      </c>
     </row>
     <row r="173" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A173" s="27">
@@ -8801,15 +8818,19 @@
         <v>346</v>
       </c>
       <c r="C214" s="25" t="s">
-        <v>10</v>
+        <v>327</v>
       </c>
       <c r="D214" s="25" t="s">
-        <v>169</v>
+        <v>360</v>
       </c>
       <c r="E214" s="25"/>
-      <c r="F214" s="25"/>
+      <c r="F214" s="25">
+        <v>1</v>
+      </c>
       <c r="G214" s="26"/>
-      <c r="H214" s="26"/>
+      <c r="H214" s="42" t="s">
+        <v>831</v>
+      </c>
     </row>
     <row r="215" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A215" s="27">
@@ -11746,15 +11767,19 @@
         <v>446</v>
       </c>
       <c r="C371" s="25" t="s">
-        <v>10</v>
+        <v>327</v>
       </c>
       <c r="D371" s="25" t="s">
-        <v>169</v>
+        <v>360</v>
       </c>
       <c r="E371" s="25"/>
-      <c r="F371" s="25"/>
+      <c r="F371" s="25">
+        <v>1</v>
+      </c>
       <c r="G371" s="26"/>
-      <c r="H371" s="26"/>
+      <c r="H371" s="42" t="s">
+        <v>831</v>
+      </c>
     </row>
     <row r="372" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A372" s="27">
@@ -16395,15 +16420,19 @@
         <v>446</v>
       </c>
       <c r="C612" s="25" t="s">
-        <v>10</v>
+        <v>327</v>
       </c>
       <c r="D612" s="25" t="s">
-        <v>169</v>
+        <v>360</v>
       </c>
       <c r="E612" s="25"/>
-      <c r="F612" s="25"/>
+      <c r="F612" s="25">
+        <v>1</v>
+      </c>
       <c r="G612" s="26"/>
-      <c r="H612" s="26"/>
+      <c r="H612" s="43" t="s">
+        <v>831</v>
+      </c>
     </row>
     <row r="613" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A613" s="27">

</xml_diff>

<commit_message>
fixed test case as per test data pushed to blank DB
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCases.xlsx
+++ b/selenium-wd/data/TestCases.xlsx
@@ -2680,9 +2680,6 @@
     <t>Run the survey for 10 seconds</t>
   </si>
   <si>
-    <t>Surveyor: White Dodge - FDDS2037</t>
-  </si>
-  <si>
     <t>Click on GIS Button again to hide menu</t>
   </si>
   <si>
@@ -2702,12 +2699,15 @@
   </si>
   <si>
     <t>TURN OFF FOV</t>
+  </si>
+  <si>
+    <t>Surveyor: Software Car - FDDS2037</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3014,6 +3014,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3049,6 +3066,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3611,7 +3645,7 @@
   <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="A4:B4"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3658,7 +3692,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2"/>
       <c r="G2" s="25"/>
@@ -3677,7 +3711,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" s="25"/>
     </row>
@@ -3695,7 +3729,7 @@
         <v>4</v>
       </c>
       <c r="E4" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" s="25"/>
     </row>
@@ -3713,7 +3747,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" s="25"/>
       <c r="G5" s="6"/>
@@ -3732,7 +3766,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="25"/>
       <c r="G6" s="6"/>
@@ -3751,7 +3785,7 @@
         <v>8</v>
       </c>
       <c r="E7" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" s="25"/>
       <c r="G7" s="6"/>
@@ -3770,7 +3804,7 @@
         <v>8</v>
       </c>
       <c r="E8" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="25"/>
     </row>
@@ -3788,7 +3822,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="25"/>
     </row>
@@ -3806,7 +3840,7 @@
         <v>8</v>
       </c>
       <c r="E10" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" s="25"/>
     </row>
@@ -3824,7 +3858,7 @@
         <v>8</v>
       </c>
       <c r="E11" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" s="25"/>
     </row>
@@ -3842,7 +3876,7 @@
         <v>8</v>
       </c>
       <c r="E12" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" s="25"/>
       <c r="G12" s="25"/>
@@ -3915,7 +3949,7 @@
         <v>4</v>
       </c>
       <c r="E16" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" s="25"/>
     </row>
@@ -3933,7 +3967,7 @@
         <v>4</v>
       </c>
       <c r="E17" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" s="25"/>
     </row>
@@ -3951,7 +3985,7 @@
         <v>4</v>
       </c>
       <c r="E18" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18" s="25"/>
     </row>
@@ -3969,7 +4003,7 @@
         <v>4</v>
       </c>
       <c r="E19" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19" s="25"/>
     </row>
@@ -3987,7 +4021,7 @@
         <v>4</v>
       </c>
       <c r="E20" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -4004,7 +4038,7 @@
         <v>4</v>
       </c>
       <c r="E21" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -4021,7 +4055,7 @@
         <v>4</v>
       </c>
       <c r="E22" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -4038,7 +4072,7 @@
         <v>4</v>
       </c>
       <c r="E23" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -4089,7 +4123,7 @@
         <v>4</v>
       </c>
       <c r="E26" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -4106,7 +4140,7 @@
         <v>4</v>
       </c>
       <c r="E27" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -4123,7 +4157,7 @@
         <v>4</v>
       </c>
       <c r="E28" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -4140,7 +4174,7 @@
         <v>4</v>
       </c>
       <c r="E29" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F29"/>
     </row>
@@ -4158,7 +4192,7 @@
         <v>4</v>
       </c>
       <c r="E30" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -4175,7 +4209,7 @@
         <v>4</v>
       </c>
       <c r="E31" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -4192,7 +4226,7 @@
         <v>4</v>
       </c>
       <c r="E32" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -4209,7 +4243,7 @@
         <v>4</v>
       </c>
       <c r="E33" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -4226,7 +4260,7 @@
         <v>4</v>
       </c>
       <c r="E34" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -4243,7 +4277,7 @@
         <v>4</v>
       </c>
       <c r="E35" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -4260,7 +4294,7 @@
         <v>4</v>
       </c>
       <c r="E36" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -4277,7 +4311,7 @@
         <v>4</v>
       </c>
       <c r="E37" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -4294,7 +4328,7 @@
         <v>4</v>
       </c>
       <c r="E38" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -4311,7 +4345,7 @@
         <v>4</v>
       </c>
       <c r="E39" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -4328,7 +4362,7 @@
         <v>4</v>
       </c>
       <c r="E40" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -4345,7 +4379,7 @@
         <v>4</v>
       </c>
       <c r="E41" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -4362,7 +4396,7 @@
         <v>4</v>
       </c>
       <c r="E42" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -4379,7 +4413,7 @@
         <v>4</v>
       </c>
       <c r="E43" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -4396,7 +4430,7 @@
         <v>4</v>
       </c>
       <c r="E44" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G44" s="6"/>
     </row>
@@ -4414,7 +4448,7 @@
         <v>4</v>
       </c>
       <c r="E45" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -4431,7 +4465,7 @@
         <v>4</v>
       </c>
       <c r="E46" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G46" s="6"/>
     </row>
@@ -4449,7 +4483,7 @@
         <v>4</v>
       </c>
       <c r="E47" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -4466,7 +4500,7 @@
         <v>4</v>
       </c>
       <c r="E48" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -4483,7 +4517,7 @@
         <v>4</v>
       </c>
       <c r="E49" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -4500,7 +4534,7 @@
         <v>4</v>
       </c>
       <c r="E50" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -4517,7 +4551,7 @@
         <v>4</v>
       </c>
       <c r="E51" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -4534,7 +4568,7 @@
         <v>4</v>
       </c>
       <c r="E52" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -4551,7 +4585,7 @@
         <v>4</v>
       </c>
       <c r="E53" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -4568,7 +4602,7 @@
         <v>8</v>
       </c>
       <c r="E54" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -4585,7 +4619,7 @@
         <v>8</v>
       </c>
       <c r="E55" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -4602,7 +4636,7 @@
         <v>5</v>
       </c>
       <c r="E56" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
@@ -4619,7 +4653,7 @@
         <v>6</v>
       </c>
       <c r="E57" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -4636,7 +4670,7 @@
         <v>8</v>
       </c>
       <c r="E58" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
@@ -4653,7 +4687,7 @@
         <v>8</v>
       </c>
       <c r="E59" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
@@ -4670,7 +4704,7 @@
         <v>8</v>
       </c>
       <c r="E60" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -4687,7 +4721,7 @@
         <v>8</v>
       </c>
       <c r="E61" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
@@ -4704,7 +4738,7 @@
         <v>6</v>
       </c>
       <c r="E62" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -4726,8 +4760,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:M2498"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D607" workbookViewId="0">
-      <selection activeCell="F611" sqref="F611"/>
+    <sheetView tabSelected="1" topLeftCell="A694" workbookViewId="0">
+      <selection activeCell="F575" sqref="F575"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7253,7 +7287,7 @@
       </c>
       <c r="G130" s="26"/>
       <c r="H130" s="42" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="131" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -8041,7 +8075,7 @@
       </c>
       <c r="G172" s="26"/>
       <c r="H172" s="42" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="173" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -8829,7 +8863,7 @@
       </c>
       <c r="G214" s="26"/>
       <c r="H214" s="42" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="215" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -11778,7 +11812,7 @@
       </c>
       <c r="G371" s="26"/>
       <c r="H371" s="42" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="372" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -14500,7 +14534,7 @@
         <v>11</v>
       </c>
       <c r="B512" s="25" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C512" s="25" t="s">
         <v>10</v>
@@ -14850,7 +14884,7 @@
       </c>
       <c r="E530" s="25"/>
       <c r="F530" s="25" t="s">
-        <v>824</v>
+        <v>831</v>
       </c>
       <c r="G530" s="26"/>
       <c r="H530" s="25"/>
@@ -15716,7 +15750,7 @@
       </c>
       <c r="E575" s="25"/>
       <c r="F575" s="25" t="s">
-        <v>824</v>
+        <v>831</v>
       </c>
       <c r="G575" s="26"/>
       <c r="H575" s="25"/>
@@ -16431,7 +16465,7 @@
       </c>
       <c r="G612" s="26"/>
       <c r="H612" s="43" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="613" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -25055,7 +25089,7 @@
         <v>23</v>
       </c>
       <c r="B1063" s="25" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C1063" s="25" t="s">
         <v>10</v>
@@ -25237,7 +25271,7 @@
         <v>23</v>
       </c>
       <c r="B1073" s="24" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="C1073" s="25" t="s">
         <v>10</v>
@@ -34574,7 +34608,7 @@
         <v>34</v>
       </c>
       <c r="B1556" s="24" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="C1556" s="25" t="s">
         <v>327</v>
@@ -34632,7 +34666,7 @@
         <v>34</v>
       </c>
       <c r="B1559" s="24" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="C1559" s="25" t="s">
         <v>327</v>
@@ -43918,7 +43952,7 @@
         <v>52</v>
       </c>
       <c r="B2054" s="24" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="C2054" s="25" t="s">
         <v>10</v>
@@ -44396,7 +44430,7 @@
       </c>
       <c r="E2079" s="25"/>
       <c r="F2079" s="25" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="G2079" s="26"/>
       <c r="H2079" s="25"/>
@@ -46851,7 +46885,7 @@
       </c>
       <c r="E2211" s="25"/>
       <c r="F2211" s="25" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="G2211" s="26"/>
       <c r="H2211" s="25"/>
@@ -48081,7 +48115,7 @@
       </c>
       <c r="G2276" s="26"/>
       <c r="H2276" s="29" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="2277" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
turned on all test from xlsx for driver view
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCases.xlsx
+++ b/selenium-wd/data/TestCases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="776" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="776" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases-CmpReports" sheetId="1" r:id="rId1"/>
@@ -3644,8 +3644,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15:E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3692,7 +3692,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2"/>
       <c r="G2" s="25"/>
@@ -3711,7 +3711,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="25"/>
     </row>
@@ -3729,7 +3729,7 @@
         <v>4</v>
       </c>
       <c r="E4" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="25"/>
     </row>
@@ -3747,7 +3747,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="25"/>
       <c r="G5" s="6"/>
@@ -3766,7 +3766,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="25"/>
       <c r="G6" s="6"/>
@@ -3785,7 +3785,7 @@
         <v>8</v>
       </c>
       <c r="E7" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="25"/>
       <c r="G7" s="6"/>
@@ -3804,7 +3804,7 @@
         <v>8</v>
       </c>
       <c r="E8" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="25"/>
     </row>
@@ -3822,7 +3822,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="25"/>
     </row>
@@ -3840,7 +3840,7 @@
         <v>8</v>
       </c>
       <c r="E10" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="25"/>
     </row>
@@ -3858,7 +3858,7 @@
         <v>8</v>
       </c>
       <c r="E11" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="25"/>
     </row>
@@ -3876,7 +3876,7 @@
         <v>8</v>
       </c>
       <c r="E12" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="25"/>
       <c r="G12" s="25"/>
@@ -3949,7 +3949,7 @@
         <v>4</v>
       </c>
       <c r="E16" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="25"/>
     </row>
@@ -3967,7 +3967,7 @@
         <v>4</v>
       </c>
       <c r="E17" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="25"/>
     </row>
@@ -3985,7 +3985,7 @@
         <v>4</v>
       </c>
       <c r="E18" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" s="25"/>
     </row>
@@ -4003,7 +4003,7 @@
         <v>4</v>
       </c>
       <c r="E19" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" s="25"/>
     </row>
@@ -4021,7 +4021,7 @@
         <v>4</v>
       </c>
       <c r="E20" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -4038,7 +4038,7 @@
         <v>4</v>
       </c>
       <c r="E21" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -4055,7 +4055,7 @@
         <v>4</v>
       </c>
       <c r="E22" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -4072,7 +4072,7 @@
         <v>4</v>
       </c>
       <c r="E23" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -4123,7 +4123,7 @@
         <v>4</v>
       </c>
       <c r="E26" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -4140,7 +4140,7 @@
         <v>4</v>
       </c>
       <c r="E27" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -4157,7 +4157,7 @@
         <v>4</v>
       </c>
       <c r="E28" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -4174,7 +4174,7 @@
         <v>4</v>
       </c>
       <c r="E29" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29"/>
     </row>
@@ -4192,7 +4192,7 @@
         <v>4</v>
       </c>
       <c r="E30" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -4209,7 +4209,7 @@
         <v>4</v>
       </c>
       <c r="E31" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -4226,7 +4226,7 @@
         <v>4</v>
       </c>
       <c r="E32" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -4243,7 +4243,7 @@
         <v>4</v>
       </c>
       <c r="E33" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -4260,7 +4260,7 @@
         <v>4</v>
       </c>
       <c r="E34" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -4277,7 +4277,7 @@
         <v>4</v>
       </c>
       <c r="E35" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -4294,7 +4294,7 @@
         <v>4</v>
       </c>
       <c r="E36" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -4311,7 +4311,7 @@
         <v>4</v>
       </c>
       <c r="E37" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -4328,7 +4328,7 @@
         <v>4</v>
       </c>
       <c r="E38" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -4345,7 +4345,7 @@
         <v>4</v>
       </c>
       <c r="E39" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -4362,7 +4362,7 @@
         <v>4</v>
       </c>
       <c r="E40" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -4379,7 +4379,7 @@
         <v>4</v>
       </c>
       <c r="E41" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -4396,7 +4396,7 @@
         <v>4</v>
       </c>
       <c r="E42" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -4413,7 +4413,7 @@
         <v>4</v>
       </c>
       <c r="E43" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -4430,7 +4430,7 @@
         <v>4</v>
       </c>
       <c r="E44" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G44" s="6"/>
     </row>
@@ -4448,7 +4448,7 @@
         <v>4</v>
       </c>
       <c r="E45" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -4465,7 +4465,7 @@
         <v>4</v>
       </c>
       <c r="E46" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G46" s="6"/>
     </row>
@@ -4483,7 +4483,7 @@
         <v>4</v>
       </c>
       <c r="E47" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -4500,7 +4500,7 @@
         <v>4</v>
       </c>
       <c r="E48" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -4517,7 +4517,7 @@
         <v>4</v>
       </c>
       <c r="E49" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -4534,7 +4534,7 @@
         <v>4</v>
       </c>
       <c r="E50" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -4551,7 +4551,7 @@
         <v>4</v>
       </c>
       <c r="E51" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -4568,7 +4568,7 @@
         <v>4</v>
       </c>
       <c r="E52" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -4585,7 +4585,7 @@
         <v>4</v>
       </c>
       <c r="E53" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -4602,7 +4602,7 @@
         <v>8</v>
       </c>
       <c r="E54" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -4619,7 +4619,7 @@
         <v>8</v>
       </c>
       <c r="E55" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -4636,7 +4636,7 @@
         <v>5</v>
       </c>
       <c r="E56" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
@@ -4653,7 +4653,7 @@
         <v>6</v>
       </c>
       <c r="E57" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -4670,7 +4670,7 @@
         <v>8</v>
       </c>
       <c r="E58" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
@@ -4687,7 +4687,7 @@
         <v>8</v>
       </c>
       <c r="E59" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
@@ -4704,7 +4704,7 @@
         <v>8</v>
       </c>
       <c r="E60" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -4721,7 +4721,7 @@
         <v>8</v>
       </c>
       <c r="E61" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
@@ -4738,7 +4738,7 @@
         <v>6</v>
       </c>
       <c r="E62" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -4760,7 +4760,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:M2498"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A694" workbookViewId="0">
+    <sheetView topLeftCell="A694" workbookViewId="0">
       <selection activeCell="F575" sqref="F575"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updates to TestCaseData and TestCases xlsx
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCases.xlsx
+++ b/selenium-wd/data/TestCases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="776" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="776" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases-CmpReports" sheetId="1" r:id="rId1"/>
@@ -3644,7 +3644,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+    <sheetView topLeftCell="A32" workbookViewId="0">
       <selection activeCell="E15" sqref="E15:E62"/>
     </sheetView>
   </sheetViews>
@@ -4760,8 +4760,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:M2498"/>
   <sheetViews>
-    <sheetView topLeftCell="A694" workbookViewId="0">
-      <selection activeCell="F575" sqref="F575"/>
+    <sheetView tabSelected="1" topLeftCell="A536" workbookViewId="0">
+      <selection activeCell="G536" sqref="G536"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
fixes for cross customer analyzer use
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCases.xlsx
+++ b/selenium-wd/data/TestCases.xlsx
@@ -206,7 +206,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9391" uniqueCount="832">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9391" uniqueCount="834">
   <si>
     <t>ID</t>
   </si>
@@ -2702,6 +2702,12 @@
   </si>
   <si>
     <t>Surveyor: Software Car - FDDS2037</t>
+  </si>
+  <si>
+    <t>Surveyor: SimAuto-Surveyor5 - SimAuto-Analyzer5</t>
+  </si>
+  <si>
+    <t>Surveyor: SimAuto-Surveyor4 - SimAuto-Analyzer4</t>
   </si>
 </sst>
 </file>
@@ -3644,8 +3650,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15:E62"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4760,16 +4766,16 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:M2498"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A536" workbookViewId="0">
-      <selection activeCell="G536" sqref="G536"/>
+    <sheetView tabSelected="1" topLeftCell="A387" workbookViewId="0">
+      <selection activeCell="C428" sqref="C428"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.77734375" style="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="38.77734375" style="12" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31.5546875" style="12" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="12.44140625" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="38.33203125" style="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.5546875" style="13" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="11.77734375" style="13" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="8.77734375" style="13" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="18.109375" style="14" bestFit="1" customWidth="1" collapsed="1"/>
@@ -5833,7 +5839,7 @@
       <c r="E54" s="25"/>
       <c r="F54" s="25"/>
       <c r="G54" s="26">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="H54" s="25"/>
     </row>
@@ -5889,7 +5895,7 @@
       <c r="E57" s="25"/>
       <c r="F57" s="25"/>
       <c r="G57" s="26">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="H57" s="25"/>
     </row>
@@ -6749,7 +6755,7 @@
       </c>
       <c r="E101" s="25"/>
       <c r="F101" s="25" t="s">
-        <v>355</v>
+        <v>833</v>
       </c>
       <c r="G101" s="26"/>
       <c r="H101" s="25"/>
@@ -7614,7 +7620,7 @@
       <c r="E147" s="25"/>
       <c r="F147" s="25"/>
       <c r="G147" s="26">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="H147" s="25"/>
     </row>
@@ -7670,7 +7676,7 @@
       <c r="E150" s="25"/>
       <c r="F150" s="25"/>
       <c r="G150" s="26">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="H150" s="25"/>
     </row>
@@ -8325,7 +8331,7 @@
       </c>
       <c r="E185" s="25"/>
       <c r="F185" s="25" t="s">
-        <v>355</v>
+        <v>832</v>
       </c>
       <c r="G185" s="26"/>
       <c r="H185" s="25"/>
@@ -8402,7 +8408,7 @@
       <c r="E189" s="25"/>
       <c r="F189" s="25"/>
       <c r="G189" s="26">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="H189" s="25"/>
     </row>
@@ -8458,7 +8464,7 @@
       <c r="E192" s="25"/>
       <c r="F192" s="25"/>
       <c r="G192" s="26">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="H192" s="25"/>
     </row>
@@ -9113,7 +9119,7 @@
       </c>
       <c r="E227" s="25"/>
       <c r="F227" s="25" t="s">
-        <v>355</v>
+        <v>832</v>
       </c>
       <c r="G227" s="26"/>
       <c r="H227" s="25"/>
@@ -9974,7 +9980,7 @@
       <c r="E273" s="25"/>
       <c r="F273" s="25"/>
       <c r="G273" s="26">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="H273" s="25"/>
     </row>
@@ -10030,7 +10036,7 @@
       <c r="E276" s="25"/>
       <c r="F276" s="25"/>
       <c r="G276" s="26">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="H276" s="25"/>
     </row>
@@ -10915,7 +10921,7 @@
       </c>
       <c r="E324" s="25"/>
       <c r="F324" s="25" t="s">
-        <v>355</v>
+        <v>832</v>
       </c>
       <c r="G324" s="26"/>
       <c r="H324" s="25"/>
@@ -11012,7 +11018,7 @@
       <c r="E329" s="25"/>
       <c r="F329" s="25"/>
       <c r="G329" s="26">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="H329" s="25"/>
     </row>
@@ -11068,7 +11074,7 @@
       <c r="E332" s="25"/>
       <c r="F332" s="25"/>
       <c r="G332" s="26">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="H332" s="25"/>
     </row>
@@ -12094,7 +12100,7 @@
       </c>
       <c r="E385" s="25"/>
       <c r="F385" s="25" t="s">
-        <v>355</v>
+        <v>832</v>
       </c>
       <c r="G385" s="26"/>
       <c r="H385" s="25"/>
@@ -12191,7 +12197,7 @@
       <c r="E390" s="25"/>
       <c r="F390" s="25"/>
       <c r="G390" s="26">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="H390" s="25"/>
     </row>
@@ -12213,7 +12219,7 @@
       <c r="G391" s="26"/>
       <c r="H391" s="25"/>
     </row>
-    <row r="392" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A392" s="27">
         <v>9</v>
       </c>
@@ -12247,7 +12253,7 @@
       <c r="E393" s="25"/>
       <c r="F393" s="25"/>
       <c r="G393" s="26">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="H393" s="25"/>
     </row>
@@ -12269,7 +12275,7 @@
       <c r="G394" s="26"/>
       <c r="H394" s="25"/>
     </row>
-    <row r="395" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A395" s="27">
         <v>9</v>
       </c>
@@ -12930,7 +12936,7 @@
       </c>
       <c r="E429" s="25"/>
       <c r="F429" s="25" t="s">
-        <v>355</v>
+        <v>832</v>
       </c>
       <c r="G429" s="26"/>
       <c r="H429" s="25"/>
@@ -13029,7 +13035,7 @@
       <c r="G434" s="26"/>
       <c r="H434" s="25"/>
     </row>
-    <row r="435" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:12" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A435" s="27">
         <v>10</v>
       </c>
@@ -13139,7 +13145,7 @@
       <c r="G440" s="26"/>
       <c r="H440" s="25"/>
     </row>
-    <row r="441" spans="1:12" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:12" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A441" s="27">
         <v>10</v>
       </c>
@@ -14022,7 +14028,7 @@
       <c r="G485" s="26"/>
       <c r="H485" s="25"/>
     </row>
-    <row r="486" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="486" spans="1:10" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A486" s="27">
         <v>11</v>
       </c>
@@ -14132,7 +14138,7 @@
       <c r="G491" s="26"/>
       <c r="H491" s="25"/>
     </row>
-    <row r="492" spans="1:10" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="492" spans="1:10" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A492" s="27">
         <v>11</v>
       </c>
@@ -15011,7 +15017,7 @@
       <c r="E536" s="25"/>
       <c r="F536" s="25"/>
       <c r="G536" s="26">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="H536" s="25"/>
     </row>
@@ -15033,7 +15039,7 @@
       <c r="G537" s="26"/>
       <c r="H537" s="25"/>
     </row>
-    <row r="538" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="538" spans="1:12" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A538" s="27">
         <v>12</v>
       </c>
@@ -15067,7 +15073,7 @@
       <c r="E539" s="25"/>
       <c r="F539" s="25"/>
       <c r="G539" s="26">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="H539" s="25"/>
     </row>
@@ -15089,7 +15095,7 @@
       <c r="G540" s="26"/>
       <c r="H540" s="25"/>
     </row>
-    <row r="541" spans="1:12" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="541" spans="1:12" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A541" s="27">
         <v>12</v>
       </c>
@@ -15750,7 +15756,7 @@
       </c>
       <c r="E575" s="25"/>
       <c r="F575" s="25" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="G575" s="26"/>
       <c r="H575" s="25"/>
@@ -15827,7 +15833,7 @@
       <c r="E579" s="25"/>
       <c r="F579" s="25"/>
       <c r="G579" s="26">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="H579" s="25"/>
     </row>
@@ -15849,7 +15855,7 @@
       <c r="G580" s="26"/>
       <c r="H580" s="25"/>
     </row>
-    <row r="581" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="581" spans="1:10" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A581" s="27">
         <v>13</v>
       </c>
@@ -15883,7 +15889,7 @@
       <c r="E582" s="25"/>
       <c r="F582" s="25"/>
       <c r="G582" s="26">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="H582" s="25"/>
     </row>
@@ -15959,7 +15965,7 @@
       <c r="G586" s="26"/>
       <c r="H586" s="25"/>
     </row>
-    <row r="587" spans="1:10" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="587" spans="1:10" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A587" s="27">
         <v>13</v>
       </c>
@@ -16747,7 +16753,7 @@
       </c>
       <c r="E626" s="25"/>
       <c r="F626" s="25" t="s">
-        <v>355</v>
+        <v>832</v>
       </c>
       <c r="G626" s="26"/>
       <c r="H626" s="25"/>
@@ -16846,7 +16852,7 @@
       <c r="G631" s="26"/>
       <c r="H631" s="25"/>
     </row>
-    <row r="632" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="632" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A632" s="27">
         <v>14</v>
       </c>
@@ -16902,7 +16908,7 @@
       <c r="G634" s="26"/>
       <c r="H634" s="25"/>
     </row>
-    <row r="635" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="635" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A635" s="27">
         <v>14</v>
       </c>
@@ -17698,7 +17704,7 @@
       <c r="G676" s="26"/>
       <c r="H676" s="25"/>
     </row>
-    <row r="677" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="677" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A677" s="27">
         <v>15</v>
       </c>
@@ -17754,7 +17760,7 @@
       <c r="G679" s="26"/>
       <c r="H679" s="25"/>
     </row>
-    <row r="680" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="680" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A680" s="27">
         <v>15</v>
       </c>
@@ -18538,7 +18544,7 @@
       <c r="G721" s="26"/>
       <c r="H721" s="25"/>
     </row>
-    <row r="722" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="722" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A722" s="27">
         <v>16</v>
       </c>
@@ -18594,7 +18600,7 @@
       <c r="G724" s="26"/>
       <c r="H724" s="25"/>
     </row>
-    <row r="725" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="725" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A725" s="27">
         <v>16</v>
       </c>
@@ -19378,7 +19384,7 @@
       <c r="G766" s="26"/>
       <c r="H766" s="25"/>
     </row>
-    <row r="767" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="767" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A767" s="27">
         <v>17</v>
       </c>
@@ -19434,7 +19440,7 @@
       <c r="G769" s="26"/>
       <c r="H769" s="25"/>
     </row>
-    <row r="770" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="770" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A770" s="27">
         <v>17</v>
       </c>
@@ -20218,7 +20224,7 @@
       <c r="G811" s="26"/>
       <c r="H811" s="25"/>
     </row>
-    <row r="812" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="812" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A812" s="27">
         <v>18</v>
       </c>
@@ -20274,7 +20280,7 @@
       <c r="G814" s="26"/>
       <c r="H814" s="25"/>
     </row>
-    <row r="815" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="815" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A815" s="27">
         <v>18</v>
       </c>
@@ -21058,7 +21064,7 @@
       <c r="G856" s="26"/>
       <c r="H856" s="25"/>
     </row>
-    <row r="857" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="857" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A857" s="27">
         <v>19</v>
       </c>
@@ -21168,7 +21174,7 @@
       <c r="G862" s="26"/>
       <c r="H862" s="25"/>
     </row>
-    <row r="863" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="863" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A863" s="27">
         <v>19</v>
       </c>
@@ -22054,7 +22060,7 @@
       <c r="G907" s="26"/>
       <c r="H907" s="25"/>
     </row>
-    <row r="908" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="908" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A908" s="27">
         <v>20</v>
       </c>
@@ -22164,7 +22170,7 @@
       <c r="G913" s="26"/>
       <c r="H913" s="25"/>
     </row>
-    <row r="914" spans="1:12" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="914" spans="1:12" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A914" s="27">
         <v>20</v>
       </c>
@@ -22942,7 +22948,7 @@
       <c r="G952" s="26"/>
       <c r="H952" s="25"/>
     </row>
-    <row r="953" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="953" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A953" s="27">
         <v>21</v>
       </c>
@@ -23052,7 +23058,7 @@
       <c r="G958" s="26"/>
       <c r="H958" s="25"/>
     </row>
-    <row r="959" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="959" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A959" s="27">
         <v>21</v>
       </c>
@@ -23830,7 +23836,7 @@
       <c r="G997" s="26"/>
       <c r="H997" s="25"/>
     </row>
-    <row r="998" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="998" spans="1:10" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A998" s="27">
         <v>22</v>
       </c>
@@ -23940,7 +23946,7 @@
       <c r="G1003" s="26"/>
       <c r="H1003" s="25"/>
     </row>
-    <row r="1004" spans="1:10" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="1004" spans="1:10" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A1004" s="27">
         <v>22</v>
       </c>
@@ -24718,7 +24724,7 @@
       <c r="G1042" s="26"/>
       <c r="H1042" s="25"/>
     </row>
-    <row r="1043" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1043" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1043" s="27">
         <v>23</v>
       </c>
@@ -24774,7 +24780,7 @@
       <c r="G1045" s="26"/>
       <c r="H1045" s="25"/>
     </row>
-    <row r="1046" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="1046" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A1046" s="27">
         <v>23</v>
       </c>
@@ -25576,7 +25582,7 @@
       <c r="G1088" s="26"/>
       <c r="H1088" s="25"/>
     </row>
-    <row r="1089" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1089" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1089" s="27">
         <v>24</v>
       </c>
@@ -25632,7 +25638,7 @@
       <c r="G1091" s="26"/>
       <c r="H1091" s="25"/>
     </row>
-    <row r="1092" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="1092" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A1092" s="27">
         <v>24</v>
       </c>
@@ -26416,7 +26422,7 @@
       <c r="G1133" s="26"/>
       <c r="H1133" s="25"/>
     </row>
-    <row r="1134" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1134" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1134" s="27">
         <v>25</v>
       </c>
@@ -26472,7 +26478,7 @@
       <c r="G1136" s="26"/>
       <c r="H1136" s="25"/>
     </row>
-    <row r="1137" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="1137" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A1137" s="27">
         <v>25</v>
       </c>
@@ -27256,7 +27262,7 @@
       <c r="G1178" s="26"/>
       <c r="H1178" s="25"/>
     </row>
-    <row r="1179" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1179" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1179" s="27">
         <v>26</v>
       </c>
@@ -27312,7 +27318,7 @@
       <c r="G1181" s="26"/>
       <c r="H1181" s="25"/>
     </row>
-    <row r="1182" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="1182" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A1182" s="27">
         <v>26</v>
       </c>
@@ -28096,7 +28102,7 @@
       <c r="G1223" s="26"/>
       <c r="H1223" s="25"/>
     </row>
-    <row r="1224" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1224" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1224" s="27">
         <v>27</v>
       </c>
@@ -28206,7 +28212,7 @@
       <c r="G1229" s="26"/>
       <c r="H1229" s="25"/>
     </row>
-    <row r="1230" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="1230" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A1230" s="27">
         <v>27</v>
       </c>
@@ -29092,7 +29098,7 @@
       <c r="G1274" s="26"/>
       <c r="H1274" s="25"/>
     </row>
-    <row r="1275" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1275" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1275" s="27">
         <v>28</v>
       </c>
@@ -29202,7 +29208,7 @@
       <c r="G1280" s="26"/>
       <c r="H1280" s="25"/>
     </row>
-    <row r="1281" spans="1:13" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="1281" spans="1:13" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A1281" s="27">
         <v>28</v>
       </c>
@@ -29991,7 +29997,7 @@
       <c r="G1319" s="26"/>
       <c r="H1319" s="25"/>
     </row>
-    <row r="1320" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1320" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1320" s="27">
         <v>29</v>
       </c>
@@ -30101,7 +30107,7 @@
       <c r="G1325" s="26"/>
       <c r="H1325" s="25"/>
     </row>
-    <row r="1326" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="1326" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A1326" s="27">
         <v>29</v>
       </c>
@@ -30879,7 +30885,7 @@
       <c r="G1364" s="26"/>
       <c r="H1364" s="25"/>
     </row>
-    <row r="1365" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1365" spans="1:12" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1365" s="27">
         <v>30</v>
       </c>
@@ -30989,7 +30995,7 @@
       <c r="G1370" s="26"/>
       <c r="H1370" s="25"/>
     </row>
-    <row r="1371" spans="1:12" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="1371" spans="1:12" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A1371" s="27">
         <v>30</v>
       </c>
@@ -31767,7 +31773,7 @@
       <c r="G1409" s="26"/>
       <c r="H1409" s="25"/>
     </row>
-    <row r="1410" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1410" spans="1:12" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1410" s="27">
         <v>31</v>
       </c>
@@ -31877,7 +31883,7 @@
       <c r="G1415" s="26"/>
       <c r="H1415" s="25"/>
     </row>
-    <row r="1416" spans="1:12" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="1416" spans="1:12" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A1416" s="27">
         <v>31</v>
       </c>
@@ -32655,7 +32661,7 @@
       <c r="G1454" s="26"/>
       <c r="H1454" s="25"/>
     </row>
-    <row r="1455" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1455" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1455" s="27">
         <v>32</v>
       </c>
@@ -32765,7 +32771,7 @@
       <c r="G1460" s="26"/>
       <c r="H1460" s="25"/>
     </row>
-    <row r="1461" spans="1:12" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="1461" spans="1:12" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A1461" s="27">
         <v>32</v>
       </c>
@@ -33597,7 +33603,7 @@
       <c r="G1502" s="26"/>
       <c r="H1502" s="25"/>
     </row>
-    <row r="1503" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1503" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1503" s="27">
         <v>33</v>
       </c>
@@ -33653,7 +33659,7 @@
       <c r="G1505" s="26"/>
       <c r="H1505" s="25"/>
     </row>
-    <row r="1506" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="1506" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A1506" s="27">
         <v>33</v>
       </c>
@@ -34363,7 +34369,7 @@
       <c r="G1542" s="26"/>
       <c r="H1542" s="25"/>
     </row>
-    <row r="1543" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1543" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1543" s="27">
         <v>34</v>
       </c>
@@ -34419,7 +34425,7 @@
       <c r="G1545" s="26"/>
       <c r="H1545" s="25"/>
     </row>
-    <row r="1546" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="1546" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A1546" s="27">
         <v>34</v>
       </c>
@@ -34793,7 +34799,7 @@
       <c r="G1565" s="26"/>
       <c r="H1565" s="25"/>
     </row>
-    <row r="1566" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1566" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1566" s="27">
         <v>35</v>
       </c>
@@ -34849,7 +34855,7 @@
       <c r="G1568" s="26"/>
       <c r="H1568" s="25"/>
     </row>
-    <row r="1569" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="1569" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A1569" s="27">
         <v>35</v>
       </c>
@@ -35035,7 +35041,7 @@
       <c r="G1578" s="26"/>
       <c r="H1578" s="25"/>
     </row>
-    <row r="1579" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1579" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1579" s="27">
         <v>36</v>
       </c>
@@ -35091,7 +35097,7 @@
       <c r="G1581" s="26"/>
       <c r="H1581" s="25"/>
     </row>
-    <row r="1582" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="1582" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A1582" s="27">
         <v>36</v>
       </c>
@@ -35343,7 +35349,7 @@
       <c r="G1594" s="26"/>
       <c r="H1594" s="25"/>
     </row>
-    <row r="1595" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1595" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1595" s="27">
         <v>37</v>
       </c>
@@ -35399,7 +35405,7 @@
       <c r="G1597" s="26"/>
       <c r="H1597" s="25"/>
     </row>
-    <row r="1598" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="1598" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A1598" s="27">
         <v>37</v>
       </c>
@@ -35493,7 +35499,7 @@
       <c r="G1602" s="26"/>
       <c r="H1602" s="25"/>
     </row>
-    <row r="1603" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1603" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1603" s="27">
         <v>37</v>
       </c>
@@ -35605,7 +35611,7 @@
       <c r="G1608" s="26"/>
       <c r="H1608" s="25"/>
     </row>
-    <row r="1609" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1609" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1609" s="27">
         <v>38</v>
       </c>
@@ -35661,7 +35667,7 @@
       <c r="G1611" s="26"/>
       <c r="H1611" s="25"/>
     </row>
-    <row r="1612" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="1612" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A1612" s="27">
         <v>38</v>
       </c>
@@ -35699,7 +35705,7 @@
       <c r="G1613" s="26"/>
       <c r="H1613" s="25"/>
     </row>
-    <row r="1614" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1614" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1614" s="27">
         <v>38</v>
       </c>
@@ -35847,7 +35853,7 @@
       <c r="G1621" s="26"/>
       <c r="H1621" s="25"/>
     </row>
-    <row r="1622" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1622" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1622" s="27">
         <v>39</v>
       </c>
@@ -35903,7 +35909,7 @@
       <c r="G1624" s="26"/>
       <c r="H1624" s="25"/>
     </row>
-    <row r="1625" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="1625" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A1625" s="27">
         <v>39</v>
       </c>
@@ -35941,7 +35947,7 @@
       <c r="G1626" s="26"/>
       <c r="H1626" s="25"/>
     </row>
-    <row r="1627" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1627" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1627" s="27">
         <v>39</v>
       </c>
@@ -35979,7 +35985,7 @@
       </c>
       <c r="G1628" s="26"/>
     </row>
-    <row r="1629" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1629" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1629" s="27">
         <v>39</v>
       </c>
@@ -36017,7 +36023,7 @@
       </c>
       <c r="G1630" s="26"/>
     </row>
-    <row r="1631" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1631" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1631" s="27">
         <v>39</v>
       </c>
@@ -36169,7 +36175,7 @@
       <c r="G1638" s="26"/>
       <c r="H1638" s="25"/>
     </row>
-    <row r="1639" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1639" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1639" s="27">
         <v>40</v>
       </c>
@@ -36225,7 +36231,7 @@
       <c r="G1641" s="26"/>
       <c r="H1641" s="25"/>
     </row>
-    <row r="1642" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="1642" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A1642" s="27">
         <v>40</v>
       </c>
@@ -36391,7 +36397,7 @@
       <c r="G1650" s="26"/>
       <c r="H1650" s="25"/>
     </row>
-    <row r="1651" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1651" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1651" s="27">
         <v>40</v>
       </c>
@@ -36503,7 +36509,7 @@
       <c r="G1656" s="26"/>
       <c r="H1656" s="25"/>
     </row>
-    <row r="1657" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1657" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1657" s="27">
         <v>41</v>
       </c>
@@ -36559,7 +36565,7 @@
       <c r="G1659" s="26"/>
       <c r="H1659" s="25"/>
     </row>
-    <row r="1660" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="1660" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A1660" s="27">
         <v>41</v>
       </c>
@@ -36869,7 +36875,7 @@
       <c r="G1676" s="26"/>
       <c r="H1676" s="25"/>
     </row>
-    <row r="1677" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1677" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1677" s="27">
         <v>41</v>
       </c>
@@ -37233,7 +37239,7 @@
       <c r="G1695" s="26"/>
       <c r="H1695" s="25"/>
     </row>
-    <row r="1696" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1696" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1696" s="27">
         <v>42</v>
       </c>
@@ -37289,7 +37295,7 @@
       <c r="G1698" s="26"/>
       <c r="H1698" s="25"/>
     </row>
-    <row r="1699" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="1699" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A1699" s="27">
         <v>42</v>
       </c>
@@ -37599,7 +37605,7 @@
       <c r="G1715" s="26"/>
       <c r="H1715" s="25"/>
     </row>
-    <row r="1716" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1716" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1716" s="27">
         <v>42</v>
       </c>
@@ -37963,7 +37969,7 @@
       <c r="G1734" s="26"/>
       <c r="H1734" s="25"/>
     </row>
-    <row r="1735" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1735" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1735" s="27">
         <v>43</v>
       </c>
@@ -38019,7 +38025,7 @@
       <c r="G1737" s="26"/>
       <c r="H1737" s="25"/>
     </row>
-    <row r="1738" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="1738" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A1738" s="27">
         <v>43</v>
       </c>
@@ -38347,7 +38353,7 @@
       <c r="G1755" s="26"/>
       <c r="H1755" s="25"/>
     </row>
-    <row r="1756" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1756" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1756" s="27">
         <v>43</v>
       </c>
@@ -38729,7 +38735,7 @@
       <c r="G1775" s="26"/>
       <c r="H1775" s="25"/>
     </row>
-    <row r="1776" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1776" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1776" s="27">
         <v>44</v>
       </c>
@@ -38785,7 +38791,7 @@
       <c r="G1778" s="26"/>
       <c r="H1778" s="25"/>
     </row>
-    <row r="1779" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="1779" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A1779" s="27">
         <v>44</v>
       </c>
@@ -39095,7 +39101,7 @@
       <c r="G1795" s="26"/>
       <c r="H1795" s="25"/>
     </row>
-    <row r="1796" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1796" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1796" s="27">
         <v>44</v>
       </c>
@@ -39459,7 +39465,7 @@
       <c r="G1814" s="26"/>
       <c r="H1814" s="25"/>
     </row>
-    <row r="1815" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1815" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1815" s="27">
         <v>45</v>
       </c>
@@ -39515,7 +39521,7 @@
       <c r="G1817" s="26"/>
       <c r="H1817" s="25"/>
     </row>
-    <row r="1818" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="1818" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A1818" s="27">
         <v>45</v>
       </c>
@@ -39793,7 +39799,7 @@
       <c r="G1832" s="26"/>
       <c r="H1832" s="25"/>
     </row>
-    <row r="1833" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1833" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1833" s="27">
         <v>46</v>
       </c>
@@ -39849,7 +39855,7 @@
       <c r="G1835" s="26"/>
       <c r="H1835" s="25"/>
     </row>
-    <row r="1836" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="1836" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A1836" s="27">
         <v>46</v>
       </c>
@@ -39961,7 +39967,7 @@
       <c r="G1841" s="26"/>
       <c r="H1841" s="25"/>
     </row>
-    <row r="1842" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1842" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1842" s="27">
         <v>46</v>
       </c>
@@ -40195,7 +40201,7 @@
       <c r="G1853" s="26"/>
       <c r="H1853" s="25"/>
     </row>
-    <row r="1854" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1854" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1854" s="27">
         <v>47</v>
       </c>
@@ -40251,7 +40257,7 @@
       <c r="G1856" s="26"/>
       <c r="H1856" s="25"/>
     </row>
-    <row r="1857" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="1857" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A1857" s="27">
         <v>47</v>
       </c>
@@ -40561,7 +40567,7 @@
       <c r="G1873" s="26"/>
       <c r="H1873" s="25"/>
     </row>
-    <row r="1874" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1874" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1874" s="27">
         <v>47</v>
       </c>
@@ -40925,7 +40931,7 @@
       <c r="G1892" s="26"/>
       <c r="H1892" s="25"/>
     </row>
-    <row r="1893" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1893" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1893" s="27">
         <v>48</v>
       </c>
@@ -40981,7 +40987,7 @@
       <c r="G1895" s="26"/>
       <c r="H1895" s="25"/>
     </row>
-    <row r="1896" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="1896" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A1896" s="27">
         <v>48</v>
       </c>
@@ -41291,7 +41297,7 @@
       <c r="G1912" s="26"/>
       <c r="H1912" s="25"/>
     </row>
-    <row r="1913" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1913" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1913" s="27">
         <v>48</v>
       </c>
@@ -41655,7 +41661,7 @@
       <c r="G1931" s="26"/>
       <c r="H1931" s="25"/>
     </row>
-    <row r="1932" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1932" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1932" s="27">
         <v>49</v>
       </c>
@@ -41711,7 +41717,7 @@
       <c r="G1934" s="26"/>
       <c r="H1934" s="25"/>
     </row>
-    <row r="1935" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="1935" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A1935" s="27">
         <v>49</v>
       </c>
@@ -42021,7 +42027,7 @@
       <c r="G1951" s="26"/>
       <c r="H1951" s="25"/>
     </row>
-    <row r="1952" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1952" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1952" s="27">
         <v>49</v>
       </c>
@@ -42385,7 +42391,7 @@
       <c r="G1970" s="26"/>
       <c r="H1970" s="25"/>
     </row>
-    <row r="1971" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1971" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1971" s="27">
         <v>50</v>
       </c>
@@ -42441,7 +42447,7 @@
       <c r="G1973" s="26"/>
       <c r="H1973" s="25"/>
     </row>
-    <row r="1974" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="1974" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A1974" s="27">
         <v>50</v>
       </c>
@@ -42751,7 +42757,7 @@
       <c r="G1990" s="26"/>
       <c r="H1990" s="25"/>
     </row>
-    <row r="1991" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1991" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1991" s="27">
         <v>50</v>
       </c>
@@ -43115,7 +43121,7 @@
       <c r="G2009" s="26"/>
       <c r="H2009" s="25"/>
     </row>
-    <row r="2010" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2010" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A2010" s="27">
         <v>51</v>
       </c>
@@ -43171,7 +43177,7 @@
       <c r="G2012" s="26"/>
       <c r="H2012" s="25"/>
     </row>
-    <row r="2013" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="2013" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A2013" s="27">
         <v>51</v>
       </c>
@@ -43499,7 +43505,7 @@
       <c r="G2030" s="26"/>
       <c r="H2030" s="25"/>
     </row>
-    <row r="2031" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2031" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A2031" s="27">
         <v>51</v>
       </c>
@@ -43891,7 +43897,7 @@
       <c r="G2050" s="26"/>
       <c r="H2050" s="25"/>
     </row>
-    <row r="2051" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2051" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A2051" s="27">
         <v>52</v>
       </c>
@@ -43947,7 +43953,7 @@
       <c r="G2053" s="26"/>
       <c r="H2053" s="25"/>
     </row>
-    <row r="2054" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="2054" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A2054" s="27">
         <v>52</v>
       </c>
@@ -44275,7 +44281,7 @@
       <c r="G2071" s="26"/>
       <c r="H2071" s="25"/>
     </row>
-    <row r="2072" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2072" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A2072" s="27">
         <v>52</v>
       </c>
@@ -44647,7 +44653,7 @@
       <c r="E2090" s="25"/>
       <c r="F2090" s="25"/>
       <c r="G2090" s="26">
-        <v>20</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2091" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -44668,7 +44674,7 @@
       <c r="G2091" s="26"/>
       <c r="H2091" s="25"/>
     </row>
-    <row r="2092" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2092" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A2092" s="27">
         <v>53</v>
       </c>
@@ -44702,7 +44708,7 @@
       <c r="E2093" s="25"/>
       <c r="F2093" s="25"/>
       <c r="G2093" s="26">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="H2093" s="25"/>
     </row>
@@ -44724,7 +44730,7 @@
       <c r="G2094" s="26"/>
       <c r="H2094" s="25"/>
     </row>
-    <row r="2095" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="2095" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A2095" s="27">
         <v>53</v>
       </c>
@@ -45388,7 +45394,7 @@
       </c>
       <c r="E2130" s="25"/>
       <c r="F2130" s="25" t="s">
-        <v>792</v>
+        <v>832</v>
       </c>
       <c r="G2130" s="26"/>
       <c r="H2130" s="25"/>
@@ -45465,7 +45471,7 @@
       <c r="E2134" s="25"/>
       <c r="F2134" s="25"/>
       <c r="G2134" s="26">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="H2134" s="25"/>
     </row>
@@ -45487,7 +45493,7 @@
       <c r="G2135" s="26"/>
       <c r="H2135" s="25"/>
     </row>
-    <row r="2136" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2136" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A2136" s="27">
         <v>54</v>
       </c>
@@ -45521,7 +45527,7 @@
       <c r="E2137" s="25"/>
       <c r="F2137" s="25"/>
       <c r="G2137" s="26">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="H2137" s="25"/>
     </row>
@@ -45543,7 +45549,7 @@
       <c r="G2138" s="26"/>
       <c r="H2138" s="25"/>
     </row>
-    <row r="2139" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="2139" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A2139" s="27">
         <v>54</v>
       </c>
@@ -46207,7 +46213,7 @@
       </c>
       <c r="E2174" s="25"/>
       <c r="F2174" s="25" t="s">
-        <v>792</v>
+        <v>832</v>
       </c>
       <c r="G2174" s="26"/>
       <c r="H2174" s="25"/>
@@ -46305,7 +46311,7 @@
       <c r="G2179" s="26"/>
       <c r="H2179" s="25"/>
     </row>
-    <row r="2180" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2180" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A2180" s="27">
         <v>55</v>
       </c>
@@ -46361,7 +46367,7 @@
       <c r="G2182" s="26"/>
       <c r="H2182" s="25"/>
     </row>
-    <row r="2183" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="2183" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A2183" s="27">
         <v>55</v>
       </c>
@@ -47123,7 +47129,7 @@
       <c r="G2223" s="26"/>
       <c r="H2223" s="25"/>
     </row>
-    <row r="2224" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2224" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A2224" s="27">
         <v>56</v>
       </c>
@@ -47179,7 +47185,7 @@
       <c r="G2226" s="26"/>
       <c r="H2226" s="25"/>
     </row>
-    <row r="2227" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="2227" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A2227" s="27">
         <v>56</v>
       </c>
@@ -47920,7 +47926,7 @@
       <c r="E2266" s="25"/>
       <c r="F2266" s="25"/>
       <c r="G2266" s="26">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="H2266" s="25"/>
     </row>
@@ -47942,7 +47948,7 @@
       <c r="G2267" s="26"/>
       <c r="H2267" s="25"/>
     </row>
-    <row r="2268" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2268" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A2268" s="27">
         <v>57</v>
       </c>
@@ -47976,7 +47982,7 @@
       <c r="E2269" s="25"/>
       <c r="F2269" s="25"/>
       <c r="G2269" s="26">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="H2269" s="25"/>
     </row>
@@ -47998,7 +48004,7 @@
       <c r="G2270" s="26"/>
       <c r="H2270" s="25"/>
     </row>
-    <row r="2271" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="2271" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A2271" s="27">
         <v>57</v>
       </c>
@@ -48756,7 +48762,7 @@
       </c>
       <c r="E2310" s="25"/>
       <c r="F2310" s="25" t="s">
-        <v>792</v>
+        <v>832</v>
       </c>
       <c r="G2310" s="26"/>
       <c r="H2310" s="25"/>
@@ -48851,7 +48857,7 @@
       <c r="E2315" s="25"/>
       <c r="F2315" s="25"/>
       <c r="G2315" s="26">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="H2315" s="25"/>
     </row>
@@ -48873,7 +48879,7 @@
       <c r="G2316" s="26"/>
       <c r="H2316" s="25"/>
     </row>
-    <row r="2317" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2317" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A2317" s="27">
         <v>58</v>
       </c>
@@ -48907,7 +48913,7 @@
       <c r="E2318" s="25"/>
       <c r="F2318" s="25"/>
       <c r="G2318" s="26">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="H2318" s="25"/>
     </row>
@@ -48929,7 +48935,7 @@
       <c r="G2319" s="26"/>
       <c r="H2319" s="25"/>
     </row>
-    <row r="2320" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="2320" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A2320" s="27">
         <v>58</v>
       </c>
@@ -49625,7 +49631,7 @@
       </c>
       <c r="E2356" s="25"/>
       <c r="F2356" s="25" t="s">
-        <v>792</v>
+        <v>832</v>
       </c>
       <c r="G2356" s="26"/>
       <c r="H2356" s="25"/>
@@ -49702,7 +49708,7 @@
       <c r="E2360" s="25"/>
       <c r="F2360" s="25"/>
       <c r="G2360" s="26">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="H2360" s="25"/>
     </row>
@@ -49724,7 +49730,7 @@
       <c r="G2361" s="26"/>
       <c r="H2361" s="25"/>
     </row>
-    <row r="2362" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2362" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A2362" s="27">
         <v>59</v>
       </c>
@@ -49758,7 +49764,7 @@
       <c r="E2363" s="25"/>
       <c r="F2363" s="25"/>
       <c r="G2363" s="26">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="H2363" s="25"/>
     </row>
@@ -49780,7 +49786,7 @@
       <c r="G2364" s="26"/>
       <c r="H2364" s="25"/>
     </row>
-    <row r="2365" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="2365" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A2365" s="27">
         <v>59</v>
       </c>
@@ -50476,7 +50482,7 @@
       </c>
       <c r="E2401" s="25"/>
       <c r="F2401" s="25" t="s">
-        <v>792</v>
+        <v>832</v>
       </c>
       <c r="G2401" s="26"/>
       <c r="H2401" s="25"/>
@@ -50553,7 +50559,7 @@
       <c r="E2405" s="25"/>
       <c r="F2405" s="25"/>
       <c r="G2405" s="26">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="H2405" s="25"/>
     </row>
@@ -50575,7 +50581,7 @@
       <c r="G2406" s="26"/>
       <c r="H2406" s="25"/>
     </row>
-    <row r="2407" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2407" spans="1:8" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A2407" s="27">
         <v>60</v>
       </c>
@@ -50609,7 +50615,7 @@
       <c r="E2408" s="25"/>
       <c r="F2408" s="25"/>
       <c r="G2408" s="26">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="H2408" s="25"/>
     </row>
@@ -50631,7 +50637,7 @@
       <c r="G2409" s="26"/>
       <c r="H2409" s="25"/>
     </row>
-    <row r="2410" spans="1:8" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="2410" spans="1:8" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A2410" s="27">
         <v>60</v>
       </c>
@@ -51327,7 +51333,7 @@
       </c>
       <c r="E2446" s="25"/>
       <c r="F2446" s="25" t="s">
-        <v>792</v>
+        <v>832</v>
       </c>
       <c r="G2446" s="26"/>
       <c r="H2446" s="25"/>
@@ -51425,7 +51431,7 @@
       <c r="G2451" s="26"/>
       <c r="H2451" s="25"/>
     </row>
-    <row r="2452" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2452" spans="1:10" s="6" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A2452" s="27">
         <v>61</v>
       </c>
@@ -51535,7 +51541,7 @@
       <c r="G2457" s="26"/>
       <c r="H2457" s="25"/>
     </row>
-    <row r="2458" spans="1:10" s="6" customFormat="1" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="2458" spans="1:10" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A2458" s="27">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
fixes for driverview tests cases XLSX
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCases.xlsx
+++ b/selenium-wd/data/TestCases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="776" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="776" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases-CmpReports" sheetId="1" r:id="rId1"/>
@@ -3644,8 +3644,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3692,7 +3692,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2"/>
       <c r="G2" s="25"/>
@@ -3711,7 +3711,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="25"/>
     </row>
@@ -3729,7 +3729,7 @@
         <v>4</v>
       </c>
       <c r="E4" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="25"/>
     </row>
@@ -3747,7 +3747,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="25"/>
       <c r="G5" s="6"/>
@@ -3766,7 +3766,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="25"/>
       <c r="G6" s="6"/>
@@ -3785,7 +3785,7 @@
         <v>8</v>
       </c>
       <c r="E7" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="25"/>
       <c r="G7" s="6"/>
@@ -3804,7 +3804,7 @@
         <v>8</v>
       </c>
       <c r="E8" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="25"/>
     </row>
@@ -3822,7 +3822,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="25"/>
     </row>
@@ -3840,7 +3840,7 @@
         <v>8</v>
       </c>
       <c r="E10" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="25"/>
     </row>
@@ -3858,7 +3858,7 @@
         <v>8</v>
       </c>
       <c r="E11" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="25"/>
     </row>
@@ -3876,7 +3876,7 @@
         <v>8</v>
       </c>
       <c r="E12" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="25"/>
       <c r="G12" s="25"/>
@@ -3895,7 +3895,7 @@
         <v>8</v>
       </c>
       <c r="E13" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13"/>
     </row>
@@ -3913,7 +3913,7 @@
         <v>8</v>
       </c>
       <c r="E14" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="25"/>
     </row>
@@ -3931,7 +3931,7 @@
         <v>8</v>
       </c>
       <c r="E15" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="25"/>
     </row>
@@ -3949,7 +3949,7 @@
         <v>4</v>
       </c>
       <c r="E16" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="25"/>
     </row>
@@ -3967,7 +3967,7 @@
         <v>4</v>
       </c>
       <c r="E17" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="25"/>
     </row>
@@ -3985,7 +3985,7 @@
         <v>4</v>
       </c>
       <c r="E18" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" s="25"/>
     </row>
@@ -4003,7 +4003,7 @@
         <v>4</v>
       </c>
       <c r="E19" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" s="25"/>
     </row>
@@ -4021,7 +4021,7 @@
         <v>4</v>
       </c>
       <c r="E20" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -4038,7 +4038,7 @@
         <v>4</v>
       </c>
       <c r="E21" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -4055,7 +4055,7 @@
         <v>4</v>
       </c>
       <c r="E22" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -4072,7 +4072,7 @@
         <v>4</v>
       </c>
       <c r="E23" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -4089,7 +4089,7 @@
         <v>4</v>
       </c>
       <c r="E24" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -4106,7 +4106,7 @@
         <v>4</v>
       </c>
       <c r="E25" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -4123,7 +4123,7 @@
         <v>4</v>
       </c>
       <c r="E26" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -4140,7 +4140,7 @@
         <v>4</v>
       </c>
       <c r="E27" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -4157,7 +4157,7 @@
         <v>4</v>
       </c>
       <c r="E28" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -4174,7 +4174,7 @@
         <v>4</v>
       </c>
       <c r="E29" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29"/>
     </row>
@@ -4192,7 +4192,7 @@
         <v>4</v>
       </c>
       <c r="E30" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -4209,7 +4209,7 @@
         <v>4</v>
       </c>
       <c r="E31" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -4226,7 +4226,7 @@
         <v>4</v>
       </c>
       <c r="E32" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -4243,7 +4243,7 @@
         <v>4</v>
       </c>
       <c r="E33" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -4260,7 +4260,7 @@
         <v>4</v>
       </c>
       <c r="E34" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -4277,7 +4277,7 @@
         <v>4</v>
       </c>
       <c r="E35" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -4294,7 +4294,7 @@
         <v>4</v>
       </c>
       <c r="E36" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -4311,7 +4311,7 @@
         <v>4</v>
       </c>
       <c r="E37" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -4328,7 +4328,7 @@
         <v>4</v>
       </c>
       <c r="E38" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -4345,7 +4345,7 @@
         <v>4</v>
       </c>
       <c r="E39" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -4362,7 +4362,7 @@
         <v>4</v>
       </c>
       <c r="E40" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -4379,7 +4379,7 @@
         <v>4</v>
       </c>
       <c r="E41" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -4396,7 +4396,7 @@
         <v>4</v>
       </c>
       <c r="E42" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -4413,7 +4413,7 @@
         <v>4</v>
       </c>
       <c r="E43" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -4430,7 +4430,7 @@
         <v>4</v>
       </c>
       <c r="E44" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G44" s="6"/>
     </row>
@@ -4448,7 +4448,7 @@
         <v>4</v>
       </c>
       <c r="E45" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -4465,7 +4465,7 @@
         <v>4</v>
       </c>
       <c r="E46" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G46" s="6"/>
     </row>
@@ -4483,7 +4483,7 @@
         <v>4</v>
       </c>
       <c r="E47" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -4500,7 +4500,7 @@
         <v>4</v>
       </c>
       <c r="E48" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -4517,7 +4517,7 @@
         <v>4</v>
       </c>
       <c r="E49" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -4534,7 +4534,7 @@
         <v>4</v>
       </c>
       <c r="E50" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -4551,7 +4551,7 @@
         <v>4</v>
       </c>
       <c r="E51" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -4568,7 +4568,7 @@
         <v>4</v>
       </c>
       <c r="E52" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -4585,7 +4585,7 @@
         <v>4</v>
       </c>
       <c r="E53" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -4602,7 +4602,7 @@
         <v>8</v>
       </c>
       <c r="E54" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -4619,7 +4619,7 @@
         <v>8</v>
       </c>
       <c r="E55" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -4636,7 +4636,7 @@
         <v>5</v>
       </c>
       <c r="E56" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
@@ -4670,7 +4670,7 @@
         <v>8</v>
       </c>
       <c r="E58" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
@@ -4687,7 +4687,7 @@
         <v>8</v>
       </c>
       <c r="E59" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
@@ -4704,7 +4704,7 @@
         <v>8</v>
       </c>
       <c r="E60" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -4721,7 +4721,7 @@
         <v>8</v>
       </c>
       <c r="E61" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
@@ -4738,7 +4738,7 @@
         <v>6</v>
       </c>
       <c r="E62" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -4760,7 +4760,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:M2499"/>
   <sheetViews>
-    <sheetView topLeftCell="A2211" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A451" workbookViewId="0">
       <selection activeCell="B2228" sqref="B2228"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
test case fixes xlsx tests
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCases.xlsx
+++ b/selenium-wd/data/TestCases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="776" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="776" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases-CmpReports" sheetId="1" r:id="rId1"/>
@@ -206,7 +206,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9394" uniqueCount="832">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9394" uniqueCount="833">
   <si>
     <t>ID</t>
   </si>
@@ -2702,6 +2702,9 @@
   </si>
   <si>
     <t>Start Survey -&gt; Provide survey tag, select  Survey Time: Day Solar Radiation: Moderate Wind: Light Survey Type: Manual</t>
+  </si>
+  <si>
+    <t>Manual Survey - Satellite - All ON</t>
   </si>
 </sst>
 </file>
@@ -3644,8 +3647,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3692,7 +3695,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2"/>
       <c r="G2" s="25"/>
@@ -3711,7 +3714,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" s="25"/>
     </row>
@@ -3729,7 +3732,7 @@
         <v>4</v>
       </c>
       <c r="E4" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" s="25"/>
     </row>
@@ -3747,7 +3750,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" s="25"/>
       <c r="G5" s="6"/>
@@ -3785,7 +3788,7 @@
         <v>8</v>
       </c>
       <c r="E7" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" s="25"/>
       <c r="G7" s="6"/>
@@ -3804,7 +3807,7 @@
         <v>8</v>
       </c>
       <c r="E8" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="25"/>
     </row>
@@ -3822,7 +3825,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="25"/>
     </row>
@@ -3840,7 +3843,7 @@
         <v>8</v>
       </c>
       <c r="E10" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" s="25"/>
     </row>
@@ -3858,7 +3861,7 @@
         <v>8</v>
       </c>
       <c r="E11" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" s="25"/>
     </row>
@@ -3876,7 +3879,7 @@
         <v>8</v>
       </c>
       <c r="E12" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" s="25"/>
       <c r="G12" s="25"/>
@@ -3895,7 +3898,7 @@
         <v>8</v>
       </c>
       <c r="E13" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13"/>
     </row>
@@ -3913,7 +3916,7 @@
         <v>8</v>
       </c>
       <c r="E14" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" s="25"/>
     </row>
@@ -3931,7 +3934,7 @@
         <v>8</v>
       </c>
       <c r="E15" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" s="25"/>
     </row>
@@ -3949,7 +3952,7 @@
         <v>4</v>
       </c>
       <c r="E16" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" s="25"/>
     </row>
@@ -3967,7 +3970,7 @@
         <v>4</v>
       </c>
       <c r="E17" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" s="25"/>
     </row>
@@ -3985,7 +3988,7 @@
         <v>4</v>
       </c>
       <c r="E18" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18" s="25"/>
     </row>
@@ -4003,7 +4006,7 @@
         <v>4</v>
       </c>
       <c r="E19" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19" s="25"/>
     </row>
@@ -4021,7 +4024,7 @@
         <v>4</v>
       </c>
       <c r="E20" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -4038,7 +4041,7 @@
         <v>4</v>
       </c>
       <c r="E21" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -4055,7 +4058,7 @@
         <v>4</v>
       </c>
       <c r="E22" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -4072,7 +4075,7 @@
         <v>4</v>
       </c>
       <c r="E23" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -4089,7 +4092,7 @@
         <v>4</v>
       </c>
       <c r="E24" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -4106,7 +4109,7 @@
         <v>4</v>
       </c>
       <c r="E25" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -4123,7 +4126,7 @@
         <v>4</v>
       </c>
       <c r="E26" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -4140,7 +4143,7 @@
         <v>4</v>
       </c>
       <c r="E27" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -4157,7 +4160,7 @@
         <v>4</v>
       </c>
       <c r="E28" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -4174,7 +4177,7 @@
         <v>4</v>
       </c>
       <c r="E29" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F29"/>
     </row>
@@ -4192,7 +4195,7 @@
         <v>4</v>
       </c>
       <c r="E30" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -4209,7 +4212,7 @@
         <v>4</v>
       </c>
       <c r="E31" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -4226,7 +4229,7 @@
         <v>4</v>
       </c>
       <c r="E32" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -4243,7 +4246,7 @@
         <v>4</v>
       </c>
       <c r="E33" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -4260,7 +4263,7 @@
         <v>4</v>
       </c>
       <c r="E34" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -4277,7 +4280,7 @@
         <v>4</v>
       </c>
       <c r="E35" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -4294,7 +4297,7 @@
         <v>4</v>
       </c>
       <c r="E36" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -4311,7 +4314,7 @@
         <v>4</v>
       </c>
       <c r="E37" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -4328,7 +4331,7 @@
         <v>4</v>
       </c>
       <c r="E38" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -4345,7 +4348,7 @@
         <v>4</v>
       </c>
       <c r="E39" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -4362,7 +4365,7 @@
         <v>4</v>
       </c>
       <c r="E40" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -4379,7 +4382,7 @@
         <v>4</v>
       </c>
       <c r="E41" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -4396,7 +4399,7 @@
         <v>4</v>
       </c>
       <c r="E42" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -4413,7 +4416,7 @@
         <v>4</v>
       </c>
       <c r="E43" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -4430,7 +4433,7 @@
         <v>4</v>
       </c>
       <c r="E44" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G44" s="6"/>
     </row>
@@ -4448,7 +4451,7 @@
         <v>4</v>
       </c>
       <c r="E45" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -4465,7 +4468,7 @@
         <v>4</v>
       </c>
       <c r="E46" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G46" s="6"/>
     </row>
@@ -4483,7 +4486,7 @@
         <v>4</v>
       </c>
       <c r="E47" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -4500,7 +4503,7 @@
         <v>4</v>
       </c>
       <c r="E48" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -4517,7 +4520,7 @@
         <v>4</v>
       </c>
       <c r="E49" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -4534,7 +4537,7 @@
         <v>4</v>
       </c>
       <c r="E50" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -4551,7 +4554,7 @@
         <v>4</v>
       </c>
       <c r="E51" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -4568,7 +4571,7 @@
         <v>4</v>
       </c>
       <c r="E52" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -4585,7 +4588,7 @@
         <v>4</v>
       </c>
       <c r="E53" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -4602,7 +4605,7 @@
         <v>8</v>
       </c>
       <c r="E54" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -4619,7 +4622,7 @@
         <v>8</v>
       </c>
       <c r="E55" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -4636,7 +4639,7 @@
         <v>5</v>
       </c>
       <c r="E56" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
@@ -4647,13 +4650,13 @@
         <v>707</v>
       </c>
       <c r="C57" s="25" t="s">
-        <v>101</v>
+        <v>832</v>
       </c>
       <c r="D57" s="25">
         <v>6</v>
       </c>
       <c r="E57" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -4670,7 +4673,7 @@
         <v>8</v>
       </c>
       <c r="E58" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
@@ -4687,7 +4690,7 @@
         <v>8</v>
       </c>
       <c r="E59" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
@@ -4704,7 +4707,7 @@
         <v>8</v>
       </c>
       <c r="E60" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -4721,7 +4724,7 @@
         <v>8</v>
       </c>
       <c r="E61" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
@@ -4738,7 +4741,7 @@
         <v>6</v>
       </c>
       <c r="E62" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -4760,8 +4763,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:M2499"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A451" workbookViewId="0">
-      <selection activeCell="B2228" sqref="B2228"/>
+    <sheetView topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="D187" sqref="D187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Fixed driverviewpagetest failure - location wrong
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCases.xlsx
+++ b/selenium-wd/data/TestCases.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\surveyor-qa\selenium-wd\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sxiang\dev\surveyor-qa\selenium-wd\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="776" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="776" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases-CmpReports" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -206,7 +206,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9394" uniqueCount="833">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9397" uniqueCount="835">
   <si>
     <t>ID</t>
   </si>
@@ -2705,12 +2705,19 @@
   </si>
   <si>
     <t>Surveyor: SimAuto-Surveyor5 - SimAuto-Analyzer5</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3247,12 +3254,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="46.21875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.77734375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.21875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="28" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="2.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="46.21875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="23.77734375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="21.21875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="28.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -3360,14 +3367,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="59.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.77734375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.77734375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.44140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.44140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="20.21875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="2.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="59.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.77734375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.77734375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.44140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="20.21875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -3647,18 +3654,18 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E62"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.5546875" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="68" style="13" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.33203125" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="6.21875" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="26.6640625" style="13" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="20" width="2.77734375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="13" width="15.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="13" width="68.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="13" width="9.33203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="13" width="6.21875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="13" width="26.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -3695,7 +3702,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2"/>
       <c r="G2" s="25"/>
@@ -3714,7 +3721,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" s="25"/>
     </row>
@@ -3732,7 +3739,7 @@
         <v>4</v>
       </c>
       <c r="E4" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" s="25"/>
     </row>
@@ -3750,7 +3757,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" s="25"/>
       <c r="G5" s="6"/>
@@ -3769,7 +3776,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="25"/>
       <c r="G6" s="6"/>
@@ -3788,7 +3795,7 @@
         <v>8</v>
       </c>
       <c r="E7" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" s="25"/>
       <c r="G7" s="6"/>
@@ -3807,7 +3814,7 @@
         <v>8</v>
       </c>
       <c r="E8" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="25"/>
     </row>
@@ -3825,7 +3832,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="25"/>
     </row>
@@ -3845,7 +3852,9 @@
       <c r="E10" s="25" t="b">
         <v>1</v>
       </c>
-      <c r="F10" s="25"/>
+      <c r="F10" s="25" t="s">
+        <v>833</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="23">
@@ -3863,7 +3872,9 @@
       <c r="E11" s="25" t="b">
         <v>1</v>
       </c>
-      <c r="F11" s="25"/>
+      <c r="F11" s="25" t="s">
+        <v>834</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="23">
@@ -3879,7 +3890,7 @@
         <v>8</v>
       </c>
       <c r="E12" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" s="25"/>
       <c r="G12" s="25"/>
@@ -3898,7 +3909,7 @@
         <v>8</v>
       </c>
       <c r="E13" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13"/>
     </row>
@@ -3918,7 +3929,9 @@
       <c r="E14" s="25" t="b">
         <v>1</v>
       </c>
-      <c r="F14" s="25"/>
+      <c r="F14" s="25" t="s">
+        <v>833</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="23">
@@ -3936,7 +3949,9 @@
       <c r="E15" s="25" t="b">
         <v>1</v>
       </c>
-      <c r="F15" s="25"/>
+      <c r="F15" s="25" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="23">
@@ -3952,7 +3967,7 @@
         <v>4</v>
       </c>
       <c r="E16" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" s="25"/>
     </row>
@@ -3970,7 +3985,7 @@
         <v>4</v>
       </c>
       <c r="E17" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" s="25"/>
     </row>
@@ -3988,7 +4003,7 @@
         <v>4</v>
       </c>
       <c r="E18" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18" s="25"/>
     </row>
@@ -4006,7 +4021,7 @@
         <v>4</v>
       </c>
       <c r="E19" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19" s="25"/>
     </row>
@@ -4024,7 +4039,7 @@
         <v>4</v>
       </c>
       <c r="E20" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -4041,7 +4056,7 @@
         <v>4</v>
       </c>
       <c r="E21" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -4058,7 +4073,7 @@
         <v>4</v>
       </c>
       <c r="E22" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -4075,7 +4090,7 @@
         <v>4</v>
       </c>
       <c r="E23" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -4094,6 +4109,9 @@
       <c r="E24" s="25" t="b">
         <v>1</v>
       </c>
+      <c r="F24" s="13" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="23">
@@ -4111,6 +4129,9 @@
       <c r="E25" s="25" t="b">
         <v>1</v>
       </c>
+      <c r="F25" s="13" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="23">
@@ -4126,7 +4147,7 @@
         <v>4</v>
       </c>
       <c r="E26" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -4143,7 +4164,7 @@
         <v>4</v>
       </c>
       <c r="E27" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -4160,7 +4181,7 @@
         <v>4</v>
       </c>
       <c r="E28" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -4177,7 +4198,7 @@
         <v>4</v>
       </c>
       <c r="E29" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F29"/>
     </row>
@@ -4195,7 +4216,7 @@
         <v>4</v>
       </c>
       <c r="E30" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -4212,7 +4233,7 @@
         <v>4</v>
       </c>
       <c r="E31" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -4229,7 +4250,7 @@
         <v>4</v>
       </c>
       <c r="E32" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -4246,7 +4267,7 @@
         <v>4</v>
       </c>
       <c r="E33" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -4263,7 +4284,7 @@
         <v>4</v>
       </c>
       <c r="E34" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -4280,7 +4301,7 @@
         <v>4</v>
       </c>
       <c r="E35" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -4297,7 +4318,7 @@
         <v>4</v>
       </c>
       <c r="E36" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -4314,7 +4335,7 @@
         <v>4</v>
       </c>
       <c r="E37" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -4331,7 +4352,7 @@
         <v>4</v>
       </c>
       <c r="E38" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -4348,7 +4369,7 @@
         <v>4</v>
       </c>
       <c r="E39" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -4365,7 +4386,7 @@
         <v>4</v>
       </c>
       <c r="E40" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -4382,7 +4403,7 @@
         <v>4</v>
       </c>
       <c r="E41" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -4399,7 +4420,7 @@
         <v>4</v>
       </c>
       <c r="E42" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -4433,7 +4454,7 @@
         <v>4</v>
       </c>
       <c r="E44" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G44" s="6"/>
     </row>
@@ -4451,7 +4472,7 @@
         <v>4</v>
       </c>
       <c r="E45" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -4468,7 +4489,7 @@
         <v>4</v>
       </c>
       <c r="E46" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G46" s="6"/>
     </row>
@@ -4486,7 +4507,7 @@
         <v>4</v>
       </c>
       <c r="E47" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -4503,7 +4524,7 @@
         <v>4</v>
       </c>
       <c r="E48" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -4520,7 +4541,7 @@
         <v>4</v>
       </c>
       <c r="E49" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -4537,7 +4558,7 @@
         <v>4</v>
       </c>
       <c r="E50" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -4554,7 +4575,7 @@
         <v>4</v>
       </c>
       <c r="E51" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -4571,7 +4592,7 @@
         <v>4</v>
       </c>
       <c r="E52" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -4588,7 +4609,7 @@
         <v>4</v>
       </c>
       <c r="E53" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -4605,7 +4626,7 @@
         <v>8</v>
       </c>
       <c r="E54" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -4622,7 +4643,7 @@
         <v>8</v>
       </c>
       <c r="E55" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -4639,7 +4660,7 @@
         <v>5</v>
       </c>
       <c r="E56" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
@@ -4656,7 +4677,7 @@
         <v>6</v>
       </c>
       <c r="E57" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -4673,7 +4694,7 @@
         <v>8</v>
       </c>
       <c r="E58" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
@@ -4690,7 +4711,7 @@
         <v>8</v>
       </c>
       <c r="E59" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
@@ -4707,7 +4728,7 @@
         <v>8</v>
       </c>
       <c r="E60" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -4724,7 +4745,7 @@
         <v>8</v>
       </c>
       <c r="E61" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
@@ -4741,7 +4762,7 @@
         <v>6</v>
       </c>
       <c r="E62" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -4763,21 +4784,21 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:M2499"/>
   <sheetViews>
-    <sheetView topLeftCell="A2396" workbookViewId="0">
-      <selection activeCell="G2405" sqref="G2405"/>
+    <sheetView topLeftCell="A265" workbookViewId="0">
+      <selection activeCell="C2162" sqref="C2162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="38.77734375" style="12" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.44140625" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="38.33203125" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.77734375" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.77734375" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.109375" style="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18.77734375" style="13" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="11" width="2.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="12" width="38.77734375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="13" width="12.44140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="13" width="38.33203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="13" width="11.77734375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="13" width="8.77734375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="14" width="18.109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="13" width="18.77734375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.5546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -52375,7 +52396,7 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -52400,18 +52421,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.21875" style="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.44140625" style="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="49.88671875" style="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="45.21875" style="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="14" width="22.44140625" style="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="25.21875" style="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="17" width="22.44140625" style="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="45.21875" style="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="22" width="22.44140625" style="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="24.21875" style="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="45.21875" style="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="26" width="22.44140625" style="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="16" width="25.21875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="16" width="22.44140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="16" width="49.88671875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="16" width="45.21875" collapsed="true"/>
+    <col min="5" max="14" bestFit="true" customWidth="true" style="16" width="22.44140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="16" width="25.21875" collapsed="true"/>
+    <col min="16" max="17" bestFit="true" customWidth="true" style="16" width="22.44140625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="16" width="45.21875" collapsed="true"/>
+    <col min="19" max="22" bestFit="true" customWidth="true" style="16" width="22.44140625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="16" width="24.21875" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="16" width="45.21875" collapsed="true"/>
+    <col min="25" max="26" bestFit="true" customWidth="true" style="16" width="22.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add method to post survey session from DB3 in TestEnvironmentActions
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCases.xlsx
+++ b/selenium-wd/data/TestCases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="776" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="776" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases-CmpReports" sheetId="1" r:id="rId1"/>
@@ -206,7 +206,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9568" uniqueCount="834">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9569" uniqueCount="835">
   <si>
     <t>ID</t>
   </si>
@@ -2708,6 +2708,9 @@
   </si>
   <si>
     <t>Wait</t>
+  </si>
+  <si>
+    <t>postSurveySessionsFromDB3ToCloud</t>
   </si>
 </sst>
 </file>
@@ -3650,7 +3653,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E62"/>
     </sheetView>
   </sheetViews>
@@ -4766,8 +4769,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:M2557"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="B146" sqref="B146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -53447,8 +53450,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:Z230"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D230" sqref="D230"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Z11" sqref="Z11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -54343,6 +54346,9 @@
       <c r="Y11" s="16" t="s">
         <v>47</v>
       </c>
+      <c r="Z11" s="16" t="s">
+        <v>834</v>
+      </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">

</xml_diff>